<commit_message>
needed to restore data(module_stats)
</commit_message>
<xml_diff>
--- a/tables/Swip_TMT_Module_GLM_Results.xlsx
+++ b/tables/Swip_TMT_Module_GLM_Results.xlsx
@@ -33,2296 +33,2296 @@
     <t xml:space="preserve">M1</t>
   </si>
   <si>
-    <t xml:space="preserve">Ipo7|Q9EPL8;Tnpo2|Q99LG2;Gnpda2|Q9CRC9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dpysl2|O08553;Ro60|O08848;Dpysl4|O35098;Kpna3|O35344;Kpna6|O35345;Chka|O54804;Csnk2a2|O54833;Reps1|O54916;Ubr1|O70481;Klc1|O88447;Pak1|O88643;Gnpda1|O88958;Coro1a|O89053;Aldoc|P05063;Hspa2|P17156;Plaa|P27612;Braf|P28028;Aco1|P28271;Map2k1|P31938;Map2k4|P47809;Pkm|P52480;Ctbp2|P56546;Ube2m|P61082;Ppp2cb|P62715;Sult4a1|P63046;Ppp2ca|P63330;Csnk2b|P67871;Ctps|P70698;Crmp1|P97427;Pde4d|Q01063;Abraxas2|Q3TCJ1;Pde12|Q3TIU4;Ctu2|Q3U308;Limch1|Q3UH68;Nt5c2|Q3V1L4;Tom1l2|Q5SRX1;Abr|Q5SSL4;Ubr3|Q5U430;Cttn|Q60598;Kpna1|Q60960;Myh10|Q61879;Plcg1|Q62077;Ralbp1|Q62172;Dpysl3|Q62188;Gart|Q64737;Ppp2r2a|Q6P1F6;Ado|Q6PDY2;Ubr2|Q6WKZ8;Ppp2r1a|Q76MZ3;Ubfd1|Q78JW9;Ppp6r1|Q7TSI3;Sestd1|Q80UK0;Reps2|Q80XA6;Atg2b|Q80XK6;Ddhd2|Q80Y98;Ubash3b|Q8BGG7;Oscp1|Q8BHW2;Flna|Q8BTM8;Arrb1|Q8BWG8;Arhgap12|Q8C0D4;Crbn|Q8C7D2;Acat2|Q8CAY6;Pygb|Q8CI94;Prmt5|Q8CIG8;Oplah|Q8K010;Hspa12a|Q8K0U4;Trnt1|Q8K1J6;Spire2|Q8K1S6;Apeh|Q8R146;Ppp6r2|Q8R3Q2;Ipo4|Q8VI75;Ipo9|Q91YE6;Asl|Q91YI0;Fgd4|Q91ZT5;Ppp6r3|Q922D4;Atg5|Q99J83;Tnpo2|Q99LG2;Ogfr|Q99PG2;Gnpda2|Q9CRC9;Snf8|Q9CZ28;Cul5|Q9D5V5;Atg101|Q9D8Z6;Atg7|Q9D906;Dtd1|Q9DD18;Ipo7|Q9EPL8;Dpysl5|Q9EQF6;Ngly1|Q9JI78;Psmg1|Q9JK23;Ggps1|Q9WTN0;Pygm|Q9WUB3;Coro1b|Q9WUM3;Rps6ka2|Q9WUT3;Carm1|Q9WVG6;Rasal1|Q9Z268;Hdac6|Q9Z2V5;Psmd10|Q9Z2X2;Plcl2|Q8K394</t>
+    <t xml:space="preserve">|Q9EPL8;|Q99LG2;|Q9CRC9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08553;|O08848;|O35098;|O35344;|O35345;|O54804;|O54833;|O54916;|O70481;|O88447;|O88643;|O88958;|O89053;|P05063;|P17156;|P27612;|P28028;|P28271;|P31938;|P47809;|P52480;|P56546;|P61082;|P62715;|P63046;|P63330;|P67871;|P70698;|P97427;|Q01063;|Q3TCJ1;|Q3TIU4;|Q3U308;|Q3UH68;|Q3V1L4;|Q5SRX1;|Q5SSL4;|Q5U430;|Q60598;|Q60960;|Q61879;|Q62077;|Q62172;|Q62188;|Q64737;|Q6P1F6;|Q6PDY2;|Q6WKZ8;|Q76MZ3;|Q78JW9;|Q7TSI3;|Q80UK0;|Q80XA6;|Q80XK6;|Q80Y98;|Q8BGG7;|Q8BHW2;|Q8BTM8;|Q8BWG8;|Q8C0D4;|Q8C7D2;|Q8CAY6;|Q8CI94;|Q8CIG8;|Q8K010;|Q8K0U4;|Q8K1J6;|Q8K1S6;|Q8R146;|Q8R3Q2;|Q8VI75;|Q91YE6;|Q91YI0;|Q91ZT5;|Q922D4;|Q99J83;|Q99LG2;|Q99PG2;|Q9CRC9;|Q9CZ28;|Q9D5V5;|Q9D8Z6;|Q9D906;|Q9DD18;|Q9EPL8;|Q9EQF6;|Q9JI78;|Q9JK23;|Q9WTN0;|Q9WUB3;|Q9WUM3;|Q9WUT3;|Q9WVG6;|Q9Z268;|Q9Z2V5;|Q9Z2X2;|Q8K394</t>
   </si>
   <si>
     <t xml:space="preserve">M2</t>
   </si>
   <si>
-    <t xml:space="preserve">Vstm2b|Q9JME9;Mmp17|Q9R0S3;C1ql3|Q9ESN4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abcc1|O35379;Neu1|O35657;Ctss|O70370;Pdlim1|O70400;Scrg1|O88745;Lgmn|O89017;Vav1|P27870;Drp2|Q05AA6;Nell2|Q61220;Arhgdib|Q61599;Ehbp1|Q69ZW3;Tnc|Q80YX1;Pex19|Q8VCI5;Rab40c|Q8VHQ4;Tmem132a|Q922P8;Epdr1|Q99M71;Trim26|Q99PN3;Atp13a2|Q9CTG6;Kctd4|Q9D7X1;Cdh13|Q9WTR5;Tbc1d8|Q9Z1A9;Matn2|O08746;Gpld1|O70362;Adam15|O88839;Itga5|P11688;Ptpn6|P29351;Rab22a|P35285;Ret|P35546;Abca1|P41233;Dab1|P97318;Anxa4|P97429;Ids|Q08890;Ncf1|Q09014;Vav2|Q60992;Rhoc|Q62159;Cltb|Q6IRU5;Tmeff1|Q6PFE7;Pcdh8|Q7TSK3;Ndrg4|Q8BTG7;Scyl2|Q8CFE4;Nradd|Q8CJ26;Nckap1l|Q8K1X4;Stxbp5|Q8K400;Fam129b|Q8R1F1;Phospho1|Q8R2H9;Abca3|Q8R420;Apbb1ip|Q8R5A3;Flnc|Q8VHX6;Serpina3n|Q91WP6;Mcoln1|Q99J21;Necab3|Q9D6J4;Caly|Q9DCA7;Sorcs1|Q9JLC4;Ecel1|Q9JMI0;Dkk3|Q9QUN9;Syt5|Q9R0N5;Ehd1|Q9WVK4;Rnaset2b|C0HKG6;Unc5c|O08747;Sdcbp|O08992;Acvr1|P37172;Tmod1|P49813;Kcnb1|Q03717;Ptprg|Q05909;Fbxo7|Q3U7U3;Cacna1e|Q61290;Cbarp|Q66L44;Nav3|Q80TN7;Cd99l2|Q8BIF0;Ncs1|Q8BNY6;Cc2d1b|Q8BRN9;Acvr1c|Q8K348;Kcnq3|Q8K3F6;Glra3|Q91XP5;Fuca1|Q99LJ1;Cdh22|Q9WTP5;Prkag1|O54950;Car11|O70354;Ctsl|P06797;Clu|Q06890;Znrf2|Q71FD5;Agfg2|Q80WC7;Plppr2|Q8VCY8;Adcy3|Q8VHH7;C1ql3|Q9ESN4;Vstm2b|Q9JME9;Rnf11|Q9QYK7;Mmp17|Q9R0S3;Abi3|Q8BYZ1;Matn4|O89029;Grn|P28798;Gla|P51569;Sorcs3|Q8VI51;Man2b1|O09159;Lrp11|Q8CB67</t>
+    <t xml:space="preserve">|Q9JME9;|Q9R0S3;|Q9ESN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35379;|O35657;|O70370;|O70400;|O88745;|O89017;|P27870;|Q05AA6;|Q61220;|Q61599;|Q69ZW3;|Q80YX1;|Q8VCI5;|Q8VHQ4;|Q922P8;|Q99M71;|Q99PN3;|Q9CTG6;|Q9D7X1;|Q9WTR5;|Q9Z1A9;|O08746;|O70362;|O88839;|P11688;|P29351;|P35285;|P35546;|P41233;|P97318;|P97429;|Q08890;|Q09014;|Q60992;|Q62159;|Q6IRU5;|Q6PFE7;|Q7TSK3;|Q8BTG7;|Q8CFE4;|Q8CJ26;|Q8K1X4;|Q8K400;|Q8R1F1;|Q8R2H9;|Q8R420;|Q8R5A3;|Q8VHX6;|Q91WP6;|Q99J21;|Q9D6J4;|Q9DCA7;|Q9JLC4;|Q9JMI0;|Q9QUN9;|Q9R0N5;|Q9WVK4;|C0HKG6;|O08747;|O08992;|P37172;|P49813;|Q03717;|Q05909;|Q3U7U3;|Q61290;|Q66L44;|Q80TN7;|Q8BIF0;|Q8BNY6;|Q8BRN9;|Q8K348;|Q8K3F6;|Q91XP5;|Q99LJ1;|Q9WTP5;|O54950;|O70354;|P06797;|Q06890;|Q71FD5;|Q80WC7;|Q8VCY8;|Q8VHH7;|Q9ESN4;|Q9JME9;|Q9QYK7;|Q9R0S3;|Q8BYZ1;|O89029;|P28798;|P51569;|Q8VI51;|O09159;|Q8CB67</t>
   </si>
   <si>
     <t xml:space="preserve">M3</t>
   </si>
   <si>
-    <t xml:space="preserve">Cic|Q924A2;Bex2|Q9WTZ8;Cd5l|Q9QWK4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gpatch8|A2A6A1;Rsrc2|A2RTL5;Itih4|A6X935;Irf2bp2|E9Q1P8;Nolc1|E9Q5C9;Tpr|F6ZDS4;Ntn1|O09118;Ess2|O70279;C3|P01027;Cfp|P11680;Plg|P20918;Csk|P41241;Pbx1|P41778;Mapkapk2|P49138;Pcyt1a|P49586;Rrp1|P56183;Tdg|P56581;Wdr5|P61965;Hmgb1|P63158;Ncoa1|P70365;Fgf13|P70377;Rit2|P70425;Naca|P70670;Serping1|P97290;Ppp4c|P97470;Sap30bp|Q02614;Smarcad1|Q04692;Map6d1|Q14BB9;BC005624|Q3TQI7;Ccdc174|Q3U155;Foxk2|Q3UCQ1;Gpatch11|Q3UFS4;Ankrd34b|Q3UUF8;2210016L21Rik|Q3UY34;Psd|Q5DTT2;Bcan|Q61361;Nup62|Q63850;Btf3|Q64152;Wapl|Q65Z40;Pcnp|Q6P8I4;Nup98|Q6PFD9;Synm|Q70IV5;Dek|Q7TNV0;Cep104|Q80V31;F12|Q80YC5;Ccdc50|Q810U5;Elmo1|Q8BPU7;Cnot4|Q8BT14;Plekha1|Q8BUL6;Synpo|Q8CC35;Tceal5|Q8CCT4;Nup88|Q8CEC0;Ccdc59|Q8R2N0;Irf2bp1|Q8R3Y8;Pdcd10|Q8VE70;Dus3l|Q91XI1;Wrnip1|Q91XU0;Mapk8|Q91Y86;Cic|Q924A2;Psip1|Q99JF8;Stk24|Q99KH8;Grk2|Q99MK8;Gigyf1|Q99MR1;Pard3|Q99NH2;Npm3|Q9CPP0;Ramac|Q9CQY2;Rprd1b|Q9CSU0;Cacybp|Q9CXW3;Mmachc|Q9CZD0;2310057M21Rik|Q9D2Q3;Ppil3|Q9D6L8;Nosip|Q9D6T0;Wdr12|Q9JJA4;Nrip3|Q9JJR9;Scly|Q9JLI6;Cd2ap|Q9JLQ0;Dusp14|Q9JLY7;Hdgfl3|Q9JMG7;Cd5l|Q9QWK4;Dnajb1|Q9QYJ3;Zranb2|Q9R020;Sorbs3|Q9R1Z8;Mad1l1|Q9WTX8;Bex2|Q9WTZ8;Stk25|Q9Z2W1</t>
+    <t xml:space="preserve">|Q924A2;|Q9WTZ8;|Q9QWK4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A6A1;|A2RTL5;|A6X935;|E9Q1P8;|E9Q5C9;|F6ZDS4;|O09118;|O70279;|P01027;|P11680;|P20918;|P41241;|P41778;|P49138;|P49586;|P56183;|P56581;|P61965;|P63158;|P70365;|P70377;|P70425;|P70670;|P97290;|P97470;|Q02614;|Q04692;|Q14BB9;|Q3TQI7;|Q3U155;|Q3UCQ1;|Q3UFS4;|Q3UUF8;|Q3UY34;|Q5DTT2;|Q61361;|Q63850;|Q64152;|Q65Z40;|Q6P8I4;|Q6PFD9;|Q70IV5;|Q7TNV0;|Q80V31;|Q80YC5;|Q810U5;|Q8BPU7;|Q8BT14;|Q8BUL6;|Q8CC35;|Q8CCT4;|Q8CEC0;|Q8R2N0;|Q8R3Y8;|Q8VE70;|Q91XI1;|Q91XU0;|Q91Y86;|Q924A2;|Q99JF8;|Q99KH8;|Q99MK8;|Q99MR1;|Q99NH2;|Q9CPP0;|Q9CQY2;|Q9CSU0;|Q9CXW3;|Q9CZD0;|Q9D2Q3;|Q9D6L8;|Q9D6T0;|Q9JJA4;|Q9JJR9;|Q9JLI6;|Q9JLQ0;|Q9JLY7;|Q9JMG7;|Q9QWK4;|Q9QYJ3;|Q9R020;|Q9R1Z8;|Q9WTX8;|Q9WTZ8;|Q9Z2W1</t>
   </si>
   <si>
     <t xml:space="preserve">M4</t>
   </si>
   <si>
-    <t xml:space="preserve">Cul2|Q9D4H8;Gmpr|Q9DCZ1;Gps1|Q99LD4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usp24|B1AY13;Ccdc6|D3YZP9;Map3k4|O08648;Cops5|O35864;Cops3|O88543;Cops4|O88544;Cops6|O88545;Aldoa|P05064;Me1|P06801;Pde11a|P0C1Q2;Alad|P10518;Glul|P15105;Ass1|P16460;Fasn|P19096;Aldh1a1|P24549;Cap1|P40124;Gfpt1|P47856;Adsl|P54822;Cops2|P61202;Rbx1|P62878;Pfkfb2|P70265;Ctps2|P70303;Usp9x|P70398;F8a|Q00558;Prkcz|Q02956;Enah|Q03173;Relch|Q148V7;Ankrd28|Q505D1;Rabl6|Q5U3K5;Csnk2a1|Q60737;Mapre1|Q61166;Lasp1|Q61792;Fnip1|Q68FD7;Hectd1|Q69ZR2;Ncoa7|Q6DFV7;Ppp1r9b|Q6R891;Cand1|Q6ZQ38;Fcsk|Q7TMC8;Huwe1|Q7TMY8;Rpap1|Q80TE0;Zer1|Q80ZJ6;Katnb1|Q8BG40;Psmd5|Q8BJY1;Gphn|Q8BUV3;Cops7b|Q8BV13;Pdcl3|Q8BVF2;Fsd1l|Q8BYN5;Trmt6|Q8CE96;Vwf|Q8CIZ8;Amdhd2|Q8JZV7;Eipr1|Q8K0G5;Katnal1|Q8K0T4;Dnm1l|Q8K1M6;Blmh|Q8R016;Aldh1l1|Q8R0Y6;Tbc1d22a|Q8R5A6;Aspscr1|Q8VBT9;Cops8|Q8VBV7;Lrrc14|Q8VC16;Wdr13|Q91V09;Man2c1|Q91W89;Lrrfip2|Q91WK0;Twf1|Q91YR1;Ugp2|Q91ZJ5;Gmppa|Q922H4;Ppp2r2d|Q925E7;Wdr77|Q99J09;Klhl22|Q99JN2;Gmpr2|Q99L27;Gps1|Q99LD4;Ubxn6|Q99PL6;Vps25|Q9CQ80;Denr|Q9CQJ6;Cap2|Q9CYT6;Cops7a|Q9CZ04;Mms19|Q9D071;Cul2|Q9D4H8;Appbp2|Q9DAX9;Pdcl|Q9DBX2;Gmpr|Q9DCZ1;Nbea|Q9EPN1;Kif21a|Q9QXL2;Twf2|Q9Z0P5</t>
+    <t xml:space="preserve">|Q9D4H8;|Q9DCZ1;|Q99LD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B1AY13;|D3YZP9;|O08648;|O35864;|O88543;|O88544;|O88545;|P05064;|P06801;|P0C1Q2;|P10518;|P15105;|P16460;|P19096;|P24549;|P40124;|P47856;|P54822;|P61202;|P62878;|P70265;|P70303;|P70398;|Q00558;|Q02956;|Q03173;|Q148V7;|Q505D1;|Q5U3K5;|Q60737;|Q61166;|Q61792;|Q68FD7;|Q69ZR2;|Q6DFV7;|Q6R891;|Q6ZQ38;|Q7TMC8;|Q7TMY8;|Q80TE0;|Q80ZJ6;|Q8BG40;|Q8BJY1;|Q8BUV3;|Q8BV13;|Q8BVF2;|Q8BYN5;|Q8CE96;|Q8CIZ8;|Q8JZV7;|Q8K0G5;|Q8K0T4;|Q8K1M6;|Q8R016;|Q8R0Y6;|Q8R5A6;|Q8VBT9;|Q8VBV7;|Q8VC16;|Q91V09;|Q91W89;|Q91WK0;|Q91YR1;|Q91ZJ5;|Q922H4;|Q925E7;|Q99J09;|Q99JN2;|Q99L27;|Q99LD4;|Q99PL6;|Q9CQ80;|Q9CQJ6;|Q9CYT6;|Q9CZ04;|Q9D071;|Q9D4H8;|Q9DAX9;|Q9DBX2;|Q9DCZ1;|Q9EPN1;|Q9QXL2;|Q9Z0P5</t>
   </si>
   <si>
     <t xml:space="preserve">M5</t>
   </si>
   <si>
-    <t xml:space="preserve">Ssbp3|Q9D032;Gtf2e2|Q9D902;Rcc2|Q8BK67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cdc27|A2A6Q5;Plcxd2|B2RXA1;Rbm25|B2RY56;Chd2|E9PZM4;Akap13|E9Q394;Gtpbp1|O08582;Metap2|O08663;Stag2|O35638;Cfh|P06909;Gas2|P11862;Polr3b|P59470;Surf6|P70279;C1qa|P98086;Rplp2|P99027;Cdk7|Q03147;Mcrip1|Q3UGS4;Mtcl1|Q3UHU5;Lrch2|Q3UMG5;Rc3h1|Q4VGL6;Usp22|Q5DU02;Zfp91|Q62511;Nuak1|Q641K5;Plekhg5|Q66T02;Jmjd1c|Q69ZK6;Togaram1|Q6A070;Smarca2|Q6DIC0;Arhgap20|Q6IFT4;Gpbp1|Q6NXH3;Dnajc8|Q6NZB0;Smchd1|Q6P5D8;Txlna|Q6PAM1;Wipf2|Q6PEV3;Rasa4|Q6PFQ7;Zc3h4|Q6ZPZ3;Lsm8|Q6ZWM4;Luc7l2|Q7TNC4;Mybbp1a|Q7TPV4;Ppp1r10|Q80W00;Samd4b|Q80XS6;Ddx42|Q810A7;Cwf19l2|Q8BG79;Cdkn2aip|Q8BI72;Rcc2|Q8BK67;Nyap2|Q8BM65;Anapc5|Q8BTZ4;Etf1|Q8BWY3;Nkrf|Q8BY02;Trim35|Q8C006;Grsf1|Q8C5Q4;Svil|Q8K4L3;Ilkap|Q8R0F6;Nol6|Q8R5K4;Wdr74|Q8VCG3;Rpp25|Q91WE3;Rrp9|Q91WM3;Ythdf2|Q91YT7;Hspa14|Q99M31;Cd2bp2|Q9CWK3;Prkrip1|Q9CWV6;Ssbp3|Q9D032;Zfp706|Q9D115;Dnajb4|Q9D832;Gtf2e2|Q9D902;Prpf4|Q9DAW6;Zfp287|Q9EQB9;Aff4|Q9ESC8;Gtf2h2|Q9JIB4;Trpc4ap|Q9JLV2;Mageh1|Q9NWG9;Maged1|Q9QYH6;Fzr1|Q9R1K5;Rps6ka4|Q9Z2B9;Sart1|Q9Z315;Gpx1|P11352;Mprip|P97434;Patl1|Q3TC46;Eif2d|Q61211;Tnrc6b|Q8BKI2;Exosc7|Q9D0M0;Mkrn2|Q9ERV1;Cnot9|Q9JKY0</t>
+    <t xml:space="preserve">|Q9D032;|Q9D902;|Q8BK67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A6Q5;|B2RXA1;|B2RY56;|E9PZM4;|E9Q394;|O08582;|O08663;|O35638;|P06909;|P11862;|P59470;|P70279;|P98086;|P99027;|Q03147;|Q3UGS4;|Q3UHU5;|Q3UMG5;|Q4VGL6;|Q5DU02;|Q62511;|Q641K5;|Q66T02;|Q69ZK6;|Q6A070;|Q6DIC0;|Q6IFT4;|Q6NXH3;|Q6NZB0;|Q6P5D8;|Q6PAM1;|Q6PEV3;|Q6PFQ7;|Q6ZPZ3;|Q6ZWM4;|Q7TNC4;|Q7TPV4;|Q80W00;|Q80XS6;|Q810A7;|Q8BG79;|Q8BI72;|Q8BK67;|Q8BM65;|Q8BTZ4;|Q8BWY3;|Q8BY02;|Q8C006;|Q8C5Q4;|Q8K4L3;|Q8R0F6;|Q8R5K4;|Q8VCG3;|Q91WE3;|Q91WM3;|Q91YT7;|Q99M31;|Q9CWK3;|Q9CWV6;|Q9D032;|Q9D115;|Q9D832;|Q9D902;|Q9DAW6;|Q9EQB9;|Q9ESC8;|Q9JIB4;|Q9JLV2;|Q9NWG9;|Q9QYH6;|Q9R1K5;|Q9Z2B9;|Q9Z315;|P11352;|P97434;|Q3TC46;|Q61211;|Q8BKI2;|Q9D0M0;|Q9ERV1;|Q9JKY0</t>
   </si>
   <si>
     <t xml:space="preserve">M6</t>
   </si>
   <si>
-    <t xml:space="preserve">Dctn3|Q9Z0Y1;Arpc3|Q9JM76;Arpc1b|Q9WV32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cul4b|A2A432;Ube3a|O08759;Map2k3|O09110;Kif3c|O35066;Ift81|O35594;Psmb10|O35955;Impact|O55091;Grk6|O70293;Fhl2|O70433;Dync1i2|O88487;Hdac3|O88895;Wipf3|P0C7L0;Hexb|P20060;Kif3a|P28741;Wars|P32921;Cast|P51125;Polr1c|P52432;Arpp19|P56212;Eif5|P59325;Nploc4|P60670;Dynlrb1|P62627;Tpt1|P63028;Mapk1|P63085;Kifap3|P70188;Psme1|P97371;Ddr1|Q03146;Eml1|Q05BC3;Cdv3|Q4VAA2;Wdr81|Q5ND34;Hars|Q61035;Shc3|Q61120;Hspa1a|Q61696;Kif3b|Q61771;Pdcd4|Q61823;Tfe3|Q64092;Eif3j2|Q66JS6;Usp7|Q6A4J8;Ppp2r5b|Q6PD28;Ccdc85b|Q6PDY0;Mapre3|Q6PER3;Dalrd3|Q6PJN8;Ppp2r2b|Q6ZWR4;Ccdc25|Q78PG9;Ube3c|Q80U95;Naa15|Q80UM3;Ppp1r12b|Q8BG95;Limd2|Q8BGB5;Pan2|Q8BGF7;Olfml3|Q8BK62;Peli2|Q8BST6;Dcun1d2|Q8BZJ7;Tango6|Q8C3S2;Glcci1|Q8K3I9;Cdc16|Q8R349;Nrbf2|Q8VCQ3;Dcaf11|Q91VU6;Sh3d19|Q91X43;Wasl|Q91YD9;Lims1|Q99JW4;Cttnbp2nl|Q99LJ0;Lpin2|Q99PI5;Arpc5|Q9CPW4;3110082I17Rik|Q9CXL3;Tars|Q9D0R2;Get4|Q9D1H7;Necap2|Q9D1J1;Aacs|Q9D2R0;Ppp1r12a|Q9DBR7;Ccdc97|Q9DBT3;Telo2|Q9DC40;Crip2|Q9DCT8;Capn10|Q9ESK3;Lztfl1|Q9JHQ5;Bag3|Q9JLV1;Arpc3|Q9JM76;Ptk2b|Q9QVP9;Dctn6|Q9WUB4;Arpc1b|Q9WV32;Dctn3|Q9Z0Y1</t>
+    <t xml:space="preserve">|Q9Z0Y1;|Q9JM76;|Q9WV32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A432;|O08759;|O09110;|O35066;|O35594;|O35955;|O55091;|O70293;|O70433;|O88487;|O88895;|P0C7L0;|P20060;|P28741;|P32921;|P51125;|P52432;|P56212;|P59325;|P60670;|P62627;|P63028;|P63085;|P70188;|P97371;|Q03146;|Q05BC3;|Q4VAA2;|Q5ND34;|Q61035;|Q61120;|Q61696;|Q61771;|Q61823;|Q64092;|Q66JS6;|Q6A4J8;|Q6PD28;|Q6PDY0;|Q6PER3;|Q6PJN8;|Q6ZWR4;|Q78PG9;|Q80U95;|Q80UM3;|Q8BG95;|Q8BGB5;|Q8BGF7;|Q8BK62;|Q8BST6;|Q8BZJ7;|Q8C3S2;|Q8K3I9;|Q8R349;|Q8VCQ3;|Q91VU6;|Q91X43;|Q91YD9;|Q99JW4;|Q99LJ0;|Q99PI5;|Q9CPW4;|Q9CXL3;|Q9D0R2;|Q9D1H7;|Q9D1J1;|Q9D2R0;|Q9DBR7;|Q9DBT3;|Q9DC40;|Q9DCT8;|Q9ESK3;|Q9JHQ5;|Q9JLV1;|Q9JM76;|Q9QVP9;|Q9WUB4;|Q9WV32;|Q9Z0Y1</t>
   </si>
   <si>
     <t xml:space="preserve">M7</t>
   </si>
   <si>
-    <t xml:space="preserve">Eif3g|Q9Z1D1;Rpl37|Q9D823;Eif3i|Q9QZD9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ythdc1|E9Q5K9;Hmgb3|O54879;Eif3d|O70194;Eef1b2|O70251;Nr3c1|P06537;Eif4a2|P10630;Mdk|P12025;Eif3a|P23116;Col18a1|P39061;Rpl29|P47915;Ube2e1|P52482;Cnbp|P53996;Paxbp1|P58501;Eif3e|P60229;Eif4a1|P60843;Uba52|P62984;Crip1|P63254;Rps12|P63323;Myo7a|P97479;Mex3c|Q05A36;Wdr18|Q4VBE8;Gpkow|Q56A08;Rbbp7|Q60973;Papola|Q61183;Npm1|Q61937;Speg|Q62407;Aktip|Q64362;Zrsr1|Q64707;Isy1|Q69ZQ2;Helz|Q6DFV5;Rprd2|Q6NXI6;Klhdc10|Q6PAR0;Srsf1|Q6PDM2;Rnf220|Q6PDX6;Gm2000|Q6ZWV7;Prpf40b|Q80W14;Vrk1|Q80X41;Ubap2l|Q80X50;Hook1|Q8BIL5;Pum3|Q8BKS9;Srsf7|Q8BL97;Eif1ax|Q8BMJ3;Metap1|Q8BP48;Hpf1|Q8CFE2;Eif3b|Q8JZQ9;Polb|Q8K409;Eif3l|Q8QZY1;Eif3c|Q8R1B4;D8Ertd738e|Q8R1F0;Hexim1|Q8R409;Spon1|Q8VCC9;Zgpat|Q8VDM1;Rpa1|Q8VEE4;Recql5|Q8VID5;Eif3h|Q91WK2;Arrb2|Q91YI4;Thyn1|Q91YJ3;Ddx27|Q921N6;Cmas|Q99KK2;Srrt|Q99MR6;Zcchc8|Q9CYA6;Tomm34|Q9CYG7;Nol7|Q9D7Z3;Rpl37|Q9D823;Eif3k|Q9DBZ5;Eif3f|Q9DCH4;Pes1|Q9EQ61;Hrg|Q9ESB3;Zfp207|Q9JMD0;Edf1|Q9JMG1;Eif3i|Q9QZD9;Ppie|Q9QZH3;Prpf40a|Q9R1C7;Eif3g|Q9Z1D1</t>
+    <t xml:space="preserve">|Q9Z1D1;|Q9D823;|Q9QZD9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9Q5K9;|O54879;|O70194;|O70251;|P06537;|P10630;|P12025;|P23116;|P39061;|P47915;|P52482;|P53996;|P58501;|P60229;|P60843;|P62984;|P63254;|P63323;|P97479;|Q05A36;|Q4VBE8;|Q56A08;|Q60973;|Q61183;|Q61937;|Q62407;|Q64362;|Q64707;|Q69ZQ2;|Q6DFV5;|Q6NXI6;|Q6PAR0;|Q6PDM2;|Q6PDX6;|Q6ZWV7;|Q80W14;|Q80X41;|Q80X50;|Q8BIL5;|Q8BKS9;|Q8BL97;|Q8BMJ3;|Q8BP48;|Q8CFE2;|Q8JZQ9;|Q8K409;|Q8QZY1;|Q8R1B4;|Q8R1F0;|Q8R409;|Q8VCC9;|Q8VDM1;|Q8VEE4;|Q8VID5;|Q91WK2;|Q91YI4;|Q91YJ3;|Q921N6;|Q99KK2;|Q99MR6;|Q9CYA6;|Q9CYG7;|Q9D7Z3;|Q9D823;|Q9DBZ5;|Q9DCH4;|Q9EQ61;|Q9ESB3;|Q9JMD0;|Q9JMG1;|Q9QZD9;|Q9QZH3;|Q9R1C7;|Q9Z1D1</t>
   </si>
   <si>
     <t xml:space="preserve">M8</t>
   </si>
   <si>
-    <t xml:space="preserve">Extl2|Q9ES89;Rabac1|Q9Z0S9;Tm9sf1|Q9DBU0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fut9|O88819;Cdk16|Q04735;Lingo3|Q6GQU6;Armh3|Q6PD19;Slit1|Q80TR4;Gulp1|Q8K2A1;Abca8b|Q8K440;Chmp2a|Q9DB34;Tmf1|B9EKI3;Bet1l|O35153;Cyp2j6|O54750;Gosr1|O88630;Mgat1|P27808;Man1a2|P39098;Acsl1|P41216;Psen1|P49769;H4c1|P62806;Pald1|P70261;Ext2|P70428;Kcnab3|P97382;Yipf3|Q3UDR8;Galnt2|Q6PB93;Galnt17|Q7TT15;Abhd13|Q80UX8;Arl5a|Q80ZU0;Elmod2|Q8BGF6;Micall1|Q8BGT6;Arfrp1|Q8BXL7;Fkrp|Q8CG64;Cmtm4|Q8CJ61;Rab15|Q8K386;Fyco1|Q8VDC1;Tm9sf1|Q9DBU0;Glmp|Q9JHJ3;Galnt16|Q9JJ61;Large1|Q9Z1M7;Tbc1d23|Q8K0F1;Rab39b|Q8BHC1;B3galt6|Q91Z92;Ugcg|O88693;H2-K1|P01901;Rab5c|P35278;B3gat3|P58158;Sgcd|P82347;Stxbp5l|Q5DQR4;Chsy3|Q5DTK1;Gpr17|Q6NS65;Abhd17b|Q7M759;Chst2|Q80WV3;Miga2|Q8BK03;Man2a2|Q8BRK9;Aifm2|Q8BUE4;Golim4|Q8BXA1;Fam20b|Q8VCS3;Fam3c|Q91VU0;B3galnt1|Q920V1;Smurf1|Q9CUN6;Fam3a|Q9D8T0;Zfpl1|Q9DB43;Tpcn1|Q9EQJ0;Gpc6|Q9R087;Rabac1|Q9Z0S9;Borcs6|Q9D6W8;Sema4g|Q9WUH7;Xylt1|Q811B1;Slc30a5|Q8R4H9;Dhrs1|Q99L04;Dipk1b|Q99ML4;B3gat1|Q9CW73;Extl2|Q9ES89</t>
+    <t xml:space="preserve">|Q9ES89;|Q9Z0S9;|Q9DBU0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88819;|Q04735;|Q6GQU6;|Q6PD19;|Q80TR4;|Q8K2A1;|Q8K440;|Q9DB34;|B9EKI3;|O35153;|O54750;|O88630;|P27808;|P39098;|P41216;|P49769;|P62806;|P70261;|P70428;|P97382;|Q3UDR8;|Q6PB93;|Q7TT15;|Q80UX8;|Q80ZU0;|Q8BGF6;|Q8BGT6;|Q8BXL7;|Q8CG64;|Q8CJ61;|Q8K386;|Q8VDC1;|Q9DBU0;|Q9JHJ3;|Q9JJ61;|Q9Z1M7;|Q8K0F1;|Q8BHC1;|Q91Z92;|O88693;|P01901;|P35278;|P58158;|P82347;|Q5DQR4;|Q5DTK1;|Q6NS65;|Q7M759;|Q80WV3;|Q8BK03;|Q8BRK9;|Q8BUE4;|Q8BXA1;|Q8VCS3;|Q91VU0;|Q920V1;|Q9CUN6;|Q9D8T0;|Q9DB43;|Q9EQJ0;|Q9R087;|Q9Z0S9;|Q9D6W8;|Q9WUH7;|Q811B1;|Q8R4H9;|Q99L04;|Q99ML4;|Q9CW73;|Q9ES89</t>
   </si>
   <si>
     <t xml:space="preserve">M9</t>
   </si>
   <si>
-    <t xml:space="preserve">Copg1|Q9QZE5;Copg2|Q9QXK3;Zwint|Q9CQU5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agrn|A2ASQ1;Copb2|O55029;Cope|O89079;C4b|P01029;Igkv6-17|P01633;Nid1|P10493;Fn1|P11276;Psmd3|P14685;Hmga1|P17095;F2|P19221;Xrcc5|P27641;Mug1|P28665;Vtn|P29788;Eif1|P48024;Ncan|P55066;Psmc1|P62192;Lsm3|P62311;Ptn|P63089;Ube2i|P63280;Evl|P70429;Serpine2|Q07235;Fam172a|Q3TNH5;Dop1b|Q3UHQ6;Pxdn|Q3UQ28;Arcn1|Q5XJY5;Reln|Q60841;Lamb2|Q61292;Itih3|Q61704;Vcan|Q62059;Aldh1a2|Q62148;Fkbp5|Q64378;Sphkap|Q6NSW3;Ecpas|Q6PDI5;Pja2|Q80U04;Hapln4|Q80WM4;Fam160b2|Q80YR2;F13a1|Q8BH61;Rapgef5|Q8C0Q9;Ccdc186|Q8C9S4;Copa|Q8CIE6;Flcn|Q8QZS3;Vps18|Q8R307;Nup85|Q8R480;Rem2|Q8VEL9;Golga4|Q91VW5;Vps11|Q91W86;Vps16|Q920Q4;Zfp330|Q922H9;Xpo6|Q924Z6;Psmd6|Q99JI4;2610002M06Rik|Q9CQD4;Zwint|Q9CQU5;Atp6v1g1|Q9CR51;Smyd3|Q9CWR2;Psmd8|Q9CX56;Cep97|Q9CZ62;Vps33a|Q9D2N9;Srp19|Q9D7A6;Psmd12|Q9D8W5;Copb1|Q9JIF7;Hapln1|Q9QUP5;Copg2|Q9QXK3;Copg1|Q9QZE5;Uchl5|Q9WUP7;Cxcl14|Q9WUQ5;Slit3|Q9WVB4;Psmd13|Q9WVJ2</t>
+    <t xml:space="preserve">|Q9QZE5;|Q9QXK3;|Q9CQU5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2ASQ1;|O55029;|O89079;|P01029;|P01633;|P10493;|P11276;|P14685;|P17095;|P19221;|P27641;|P28665;|P29788;|P48024;|P55066;|P62192;|P62311;|P63089;|P63280;|P70429;|Q07235;|Q3TNH5;|Q3UHQ6;|Q3UQ28;|Q5XJY5;|Q60841;|Q61292;|Q61704;|Q62059;|Q62148;|Q64378;|Q6NSW3;|Q6PDI5;|Q80U04;|Q80WM4;|Q80YR2;|Q8BH61;|Q8C0Q9;|Q8C9S4;|Q8CIE6;|Q8QZS3;|Q8R307;|Q8R480;|Q8VEL9;|Q91VW5;|Q91W86;|Q920Q4;|Q922H9;|Q924Z6;|Q99JI4;|Q9CQD4;|Q9CQU5;|Q9CR51;|Q9CWR2;|Q9CX56;|Q9CZ62;|Q9D2N9;|Q9D7A6;|Q9D8W5;|Q9JIF7;|Q9QUP5;|Q9QXK3;|Q9QZE5;|Q9WUP7;|Q9WUQ5;|Q9WVB4;|Q9WVJ2</t>
   </si>
   <si>
     <t xml:space="preserve">M10</t>
   </si>
   <si>
-    <t xml:space="preserve">Impa2|Q91UZ5;Mid1ip1|Q9CQ20;Pts|Q9R1Z7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C77080|A2A7S8;Myo10|F8VQB6;Chkb|O55229;Stat5b|P42232;Efnb2|P52800;Ube2d2a|P62838;Smad4|P97471;Apba2|P98084;Kcnc2|Q14B80;Zyg11b|Q3UFS0;Pacs2|Q3V3Q7;Islr2|Q5RKR3;Patj|Q63ZW7;Pde1c|Q64338;Atg2a|Q6P4T0;Herc4|Q6PAV2;Plekhm2|Q80TQ5;Thnsl2|Q80W22;Sergef|Q80YD6;Dusp28|Q8BTR5;Phlpp2|Q8BXA7;Tigar|Q8BZA9;Paox|Q8C0L6;Unc119b|Q8C4B4;Rtkn|Q8C6B2;Fermt2|Q8CIB5;Dcun1d3|Q8K0V2;Ipo11|Q8K2V6;Inpp5b|Q8K337;Ntmt1|Q8R2U4;Exoc6|Q8R313;Arhgef12|Q8R4H2;Hip1|Q8VD75;Pafah2|Q8VDG7;Fbxo21|Q8VDH1;Rab3il1|Q8VDV3;Caskin2|Q8VHK1;Impa2|Q91UZ5;Memo1|Q91VH6;Wdr45|Q91VM3;Fbxl15|Q91W61;Traf7|Q922B6;Nup155|Q99P88;Mid1ip1|Q9CQ20;Arhgef25|Q9CWR0;Lysmd1|Q9D0E3;Pir|Q9D711;Eef1akmt2|Q9D853;Ccdc91|Q9D8L5;Fbxo3|Q9DC63;Slc29a1|Q9JIM1;Pts|Q9R1Z7;Ccs|Q9WU84;Stxbp4|Q9WV89;Gipc1|Q9Z0G0;Mtm1|Q9Z2C5;Gng4|P50153;Cdc42ep1|Q91W92;Fbxo31|Q3TQF0;Wipi2|Q80W47</t>
+    <t xml:space="preserve">|Q91UZ5;|Q9CQ20;|Q9R1Z7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A7S8;|F8VQB6;|O55229;|P42232;|P52800;|P62838;|P97471;|P98084;|Q14B80;|Q3UFS0;|Q3V3Q7;|Q5RKR3;|Q63ZW7;|Q64338;|Q6P4T0;|Q6PAV2;|Q80TQ5;|Q80W22;|Q80YD6;|Q8BTR5;|Q8BXA7;|Q8BZA9;|Q8C0L6;|Q8C4B4;|Q8C6B2;|Q8CIB5;|Q8K0V2;|Q8K2V6;|Q8K337;|Q8R2U4;|Q8R313;|Q8R4H2;|Q8VD75;|Q8VDG7;|Q8VDH1;|Q8VDV3;|Q8VHK1;|Q91UZ5;|Q91VH6;|Q91VM3;|Q91W61;|Q922B6;|Q99P88;|Q9CQ20;|Q9CWR0;|Q9D0E3;|Q9D711;|Q9D853;|Q9D8L5;|Q9DC63;|Q9JIM1;|Q9R1Z7;|Q9WU84;|Q9WV89;|Q9Z0G0;|Q9Z2C5;|P50153;|Q91W92;|Q3TQF0;|Q80W47</t>
   </si>
   <si>
     <t xml:space="preserve">M11</t>
   </si>
   <si>
-    <t xml:space="preserve">Ap2b1|Q9DBG3;Atp6v1c1|Q9Z1G3;Tprgl|Q9DBS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numbl|O08919;Ap2a2|P17427;Sh3rf1|Q69ZI1;Pik3r4|Q8VD65;Mzt2|Q9CQ25;Rfc5|Q9D0F6;Nos1ap|Q9D3A8;Ap2b1|Q9DBG3;Unc13b|Q9Z1N9;Sh3yl1|O08641;Slc32a1|O35633;Ulk1|O70405;Ap2a1|P17426;Atp6v1a|P50516;Atp6v1e1|P50518;Ap2s1|P62743;Atp6v1b2|P62814;Ap2m1|P84091;Rogdi|Q3TDK6;Gdpd5|Q640M6;Sv2c|Q69ZS6;Dgkq|Q6P5E8;Arhgap10|Q6Y5D8;Rusc2|Q80U22;Synpr|Q8BGN8;Dmxl2|Q8BPN8;Ralgapb|Q8BQZ4;Atp6v1h|Q8BVE3;Vps13c|Q8BX70;Slc7a14|Q8BXR1;Synj1|Q8CHC4;Wdr7|Q920I9;Atp6v1f|Q9D1K2;Tprgl|Q9DBS2;Atp6v1g2|Q9WTT4;Atp6v1c1|Q9Z1G3;Dennd4c|A6H8H2;Ptpn9|O35239;Syngr1|O55100;Syn1|O88935;Atp6v0c|P63082;Slc30a3|P97441;Ppp2r5e|Q61151;Syp|Q62277;Sh3gl1|Q62419;Avl9|Q80U56;Napepld|Q8BH82;Slc17a6|Q8BLE7;2900026A02Rik|Q8BRV5;Syngr3|Q8R191;Syt12|Q920N7;Rab30|Q923S9;Hint3|Q9CPS6;Snx7|Q9CY18;Sv2a|Q9JIS5;Scamp5|Q9JKD3;Reep6|Q9JM62;Atp6v0a1|Q9Z1G4</t>
+    <t xml:space="preserve">|Q9DBG3;|Q9Z1G3;|Q9DBS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08919;|P17427;|Q69ZI1;|Q8VD65;|Q9CQ25;|Q9D0F6;|Q9D3A8;|Q9DBG3;|Q9Z1N9;|O08641;|O35633;|O70405;|P17426;|P50516;|P50518;|P62743;|P62814;|P84091;|Q3TDK6;|Q640M6;|Q69ZS6;|Q6P5E8;|Q6Y5D8;|Q80U22;|Q8BGN8;|Q8BPN8;|Q8BQZ4;|Q8BVE3;|Q8BX70;|Q8BXR1;|Q8CHC4;|Q920I9;|Q9D1K2;|Q9DBS2;|Q9WTT4;|Q9Z1G3;|A6H8H2;|O35239;|O55100;|O88935;|P63082;|P97441;|Q61151;|Q62277;|Q62419;|Q80U56;|Q8BH82;|Q8BLE7;|Q8BRV5;|Q8R191;|Q920N7;|Q923S9;|Q9CPS6;|Q9CY18;|Q9JIS5;|Q9JKD3;|Q9JM62;|Q9Z1G4</t>
   </si>
   <si>
     <t xml:space="preserve">M12</t>
   </si>
   <si>
-    <t xml:space="preserve">Gsk3b|Q9WV60;Csnk1d|Q9DC28;Mink1|Q9JM52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cttnbp2|B9EJA2;Dctn1|O08788;Nf1|Q04690;Gsk3a|Q2NL51;Mast3|Q3U214;Agap2|Q3UHD9;Btrc|Q3ULA2;0610010F05Rik|Q68FF0;Cep170|Q6A065;Ttbk1|Q6PCN3;Map6|Q7TSJ2;Btbd8|Q80TK0;Clec16a|Q80U30;Cep170b|Q80U49;Dtx3|Q80V91;Cnksr2|Q80YA9;Arhgap32|Q811P8;Frmd4a|Q8BIE6;Map4k5|Q8BPM2;Map1s|Q8C052;Dock3|Q8CIQ7;Uvrag|Q8K245;Itpka|Q8R071;Ascc2|Q91WR3;Zmym2|Q9CU65;Dync1h1|Q9JHU4;Mink1|Q9JM52;Asap1|Q9QWY8;Nme7|Q9QXL8;Mast1|Q9R1L5;Tbk1|Q9WUN2;Gsk3b|Q9WV60;Clip2|Q9Z0H8;Focad|A2AKG8;Parp4|E9PYK3;Kif2a|P28740;Cryz|P47199;Tubgcp3|P58854;Rab10|P61027;Xrn1|P97789;Mark3|Q03141;Brsk1|Q5RJI5;Zc2hc1a|Q8BJH1;Clasp2|Q8BRT1;Sipa1l1|Q8C0T5;Eri3|Q8C460;Mark4|Q8CIP4;Dync1li1|Q8R1Q8;Actr1b|Q8R5C5;Mark1|Q8VHJ5;Tubgcp2|Q921G8;Ntpcr|Q9CQA9;Gar1|Q9CY66;Csnk1d|Q9DC28;Wdr43|Q6ZQL4;Ap4b1|Q9WV76;Ap4e1|Q80V94;Cpsf3|Q9QXK7</t>
+    <t xml:space="preserve">|Q9WV60;|Q9DC28;|Q9JM52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B9EJA2;|O08788;|Q04690;|Q2NL51;|Q3U214;|Q3UHD9;|Q3ULA2;|Q68FF0;|Q6A065;|Q6PCN3;|Q7TSJ2;|Q80TK0;|Q80U30;|Q80U49;|Q80V91;|Q80YA9;|Q811P8;|Q8BIE6;|Q8BPM2;|Q8C052;|Q8CIQ7;|Q8K245;|Q8R071;|Q91WR3;|Q9CU65;|Q9JHU4;|Q9JM52;|Q9QWY8;|Q9QXL8;|Q9R1L5;|Q9WUN2;|Q9WV60;|Q9Z0H8;|A2AKG8;|E9PYK3;|P28740;|P47199;|P58854;|P61027;|P97789;|Q03141;|Q5RJI5;|Q8BJH1;|Q8BRT1;|Q8C0T5;|Q8C460;|Q8CIP4;|Q8R1Q8;|Q8R5C5;|Q8VHJ5;|Q921G8;|Q9CQA9;|Q9CY66;|Q9DC28;|Q6ZQL4;|Q9WV76;|Q80V94;|Q9QXK7</t>
   </si>
   <si>
     <t xml:space="preserve">M13</t>
   </si>
   <si>
-    <t xml:space="preserve">Arhgap35|Q91YM2;Pfkp|Q9WUA3;Afdn|Q9QZQ1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Idh1|O88844;Eno1|P17182;Rps6ka1|P18653;Rock2|P70336;Arf1|P84078;Cep76|Q0VEJ0;Iqsec3|Q3TES0;Prickle1|Q3U5C7;Wnk2|Q3UH66;Gpd1l|Q3ULJ0;Vps51|Q3UVL4;Ttc9|Q3V038;Acaca|Q5SWU9;Arhgap23|Q69ZH9;Inppl1|Q6P549;Magi1|Q6RHR9;Fsd1|Q7TPM6;Tppp|Q7TQD2;Cyld|Q80TQ2;Whrn|Q80VW5;Pip4k2b|Q80XI4;Ddhd1|Q80YA3;Kbtbd11|Q8BNW9;Arhgef33|Q8BW86;Camk1d|Q8BW96;Vps52|Q8C754;Gan|Q8CA72;Vps53|Q8CCB4;Vcpip1|Q8CDG3;Vps50|Q8CI71;Samd14|Q8K070;Otud7a|Q8R554;Rapgef3|Q8VCC8;Sgip1|Q8VD37;Arhgap35|Q91YM2;Parva|Q9EPC1;Xpo7|Q9EPK7;Xpo4|Q9ESJ0;Rcan1|Q9JHG6;Add3|Q9QYB5;Afdn|Q9QZQ1;Pfkp|Q9WUA3</t>
+    <t xml:space="preserve">|Q91YM2;|Q9WUA3;|Q9QZQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88844;|P17182;|P18653;|P70336;|P84078;|Q0VEJ0;|Q3TES0;|Q3U5C7;|Q3UH66;|Q3ULJ0;|Q3UVL4;|Q3V038;|Q5SWU9;|Q69ZH9;|Q6P549;|Q6RHR9;|Q7TPM6;|Q7TQD2;|Q80TQ2;|Q80VW5;|Q80XI4;|Q80YA3;|Q8BNW9;|Q8BW86;|Q8BW96;|Q8C754;|Q8CA72;|Q8CCB4;|Q8CDG3;|Q8CI71;|Q8K070;|Q8R554;|Q8VCC8;|Q8VD37;|Q91YM2;|Q9EPC1;|Q9EPK7;|Q9ESJ0;|Q9JHG6;|Q9QYB5;|Q9QZQ1;|Q9WUA3</t>
   </si>
   <si>
     <t xml:space="preserve">M14</t>
   </si>
   <si>
-    <t xml:space="preserve">Tspan31|Q9CQ88;Vps29|Q9QZ88;Crocc|Q8CJ40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snx3|O70492;Fcgr2b|P08101;Lmnb2|P21619;Ggt1|Q60928;Enpp6|Q8BGN3;Mfsd6|Q8CBH5;Slc9a8|Q8R4D1;Tspan31|Q9CQ88;Abhd2|Q9QXM0;Syndig1|A2ANU3;Prkcd|P28867;Ap1m1|P35585;Clgn|P52194;Ap1s1|P61967;Vldlr|P98156;6430571L13Rik|Q8BGK9;Crocc|Q8CJ40;Atp6v0a2|P15920;Clcn3|P51791;Spryd7|Q3TFQ1;9330182L06Rik|Q3UZV7;Cpm|Q80V42;Ranbp6|Q8BIV3;Lnpep|Q8C129;Vps35|Q9EQH3;Vps29|Q9QZ88;5330417C22Rik|A2AFS3;Ptgis|O35074;Pitpnm1|O35954;Rab4a|P56371;Pcnx2|Q5DU28;Fa2h|Q5MPP0;Atp2c1|Q80XR2;Stx16|Q8BVI5;Kctd2|Q8CEZ0;Adpgk|Q8VDL4;Slc41a3|Q921R8;Mettl9|Q9EPL4;Stx6|Q9JKK1;Scamp4|Q9JKV5;Sema4f|Q9Z123;Etnk1|Q9D4V0</t>
+    <t xml:space="preserve">|Q9CQ88;|Q9QZ88;|Q8CJ40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O70492;|P08101;|P21619;|Q60928;|Q8BGN3;|Q8CBH5;|Q8R4D1;|Q9CQ88;|Q9QXM0;|A2ANU3;|P28867;|P35585;|P52194;|P61967;|P98156;|Q8BGK9;|Q8CJ40;|P15920;|P51791;|Q3TFQ1;|Q3UZV7;|Q80V42;|Q8BIV3;|Q8C129;|Q9EQH3;|Q9QZ88;|A2AFS3;|O35074;|O35954;|P56371;|Q5DU28;|Q5MPP0;|Q80XR2;|Q8BVI5;|Q8CEZ0;|Q8VDL4;|Q921R8;|Q9EPL4;|Q9JKK1;|Q9JKV5;|Q9Z123;|Q9D4V0</t>
   </si>
   <si>
     <t xml:space="preserve">M15</t>
   </si>
   <si>
-    <t xml:space="preserve">Hs6st1|Q9QYK5;Ccdc167|Q9D162;Fam174a|Q9D3L0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rab11fip2|G3XA57;Usp46|P62069;Eps15l1|Q60902;Coch|Q62507;Aftph|Q80WT5;Cwc22|Q8C5N3;Rab11fip5|Q8R361;Ccdc167|Q9D162;Rab11fip1|Q9D620;Gtf2i|Q9ESZ8;Sptlc1|O35704;Lsg1|Q3UM18;Pigh|Q5M9N4;Scap|Q6GQT6;Dpy19l3|Q71B07;Creg2|Q8BGC9;Wdr48|Q8BH57;Lss|Q8BLN5;Vps9d1|Q8C190;Dnajc9|Q91WN1;Fam174a|Q9D3L0;Gpr89|Q8BS95;Hs6st3|Q9QYK4;Mttp|O08601;Manea|Q6NXH2;Ostm1|Q8BGT0;Bicd1|Q8BR07;Hs6st1|Q9QYK5;Cx3cl1|O35188;Sigmar1|O55242;Tmem254c|P0DN91;Srprb|P47758;Txndc15|Q6P6J9;Tm7sf2|Q71KT5;Clptm1l|Q8BXA5;Dst|Q91ZU6;Ap1s2|Q9DB50;Tmem9b|Q9JJR8;Tacc1|Q6Y685</t>
+    <t xml:space="preserve">|Q9QYK5;|Q9D162;|Q9D3L0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|G3XA57;|P62069;|Q60902;|Q62507;|Q80WT5;|Q8C5N3;|Q8R361;|Q9D162;|Q9D620;|Q9ESZ8;|O35704;|Q3UM18;|Q5M9N4;|Q6GQT6;|Q71B07;|Q8BGC9;|Q8BH57;|Q8BLN5;|Q8C190;|Q91WN1;|Q9D3L0;|Q8BS95;|Q9QYK4;|O08601;|Q6NXH2;|Q8BGT0;|Q8BR07;|Q9QYK5;|O35188;|O55242;|P0DN91;|P47758;|Q6P6J9;|Q71KT5;|Q8BXA5;|Q91ZU6;|Q9DB50;|Q9JJR8;|Q6Y685</t>
   </si>
   <si>
     <t xml:space="preserve">M16</t>
   </si>
   <si>
-    <t xml:space="preserve">Atp11c|Q9QZW0;Srpr|Q9DBG7;Spg21|Q9CQC8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enpep|P16406;Sez6|Q7TSK2;Cd163|Q2VLH6;Slc23a2|Q9EPR4;Slc6a13|P31649;Elmod1|Q3V1U8;Slc48a1|Q9D8M3;Vamp4|O70480;Csf1r|P09581;Abcb1a|P21447;Ccn2|P29268;Itga6|Q61739;Mrc1|Q61830;Islr|Q6GU68;Vstm2l|Q6PDS0;Jph4|Q80WT0;Fndc3a|Q8BX90;Lmf2|Q8C3X8;Mmgt1|Q8K273;Alg3|Q8K2A8;Pigu|Q8K358;Slc12a6|Q924N4;Spg21|Q9CQC8;Emc2|Q9CRD2;Sec11c|Q9D8V7;Srpr|Q9DBG7;Pigo|Q9JJI6;Atp11c|Q9QZW0;Bcam|Q9R069;Slc35a2|Q9R0M8;Chrna4|O70174;H2-D1|P01899;Ptgs1|P22437;Armcx3|Q8BHS6;Lemd3|Q9WU40</t>
+    <t xml:space="preserve">|Q9QZW0;|Q9DBG7;|Q9CQC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P16406;|Q7TSK2;|Q2VLH6;|Q9EPR4;|P31649;|Q3V1U8;|Q9D8M3;|O70480;|P09581;|P21447;|P29268;|Q61739;|Q61830;|Q6GU68;|Q6PDS0;|Q80WT0;|Q8BX90;|Q8C3X8;|Q8K273;|Q8K2A8;|Q8K358;|Q924N4;|Q9CQC8;|Q9CRD2;|Q9D8V7;|Q9DBG7;|Q9JJI6;|Q9QZW0;|Q9R069;|Q9R0M8;|O70174;|P01899;|P22437;|Q8BHS6;|Q9WU40</t>
   </si>
   <si>
     <t xml:space="preserve">M17</t>
   </si>
   <si>
-    <t xml:space="preserve">Osbpl1a|Q91XL9;Gstt3|Q99L20;Rgs6|Q9Z2H2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptpn11|P35235;Adss|P46664;Prkcg|P63318;Map2k6|P70236;Mpp1|P70290;Diras2|Q5PR73;Gstt2|Q61133;Bcar1|Q61140;Irak1|Q62406;Gstt1|Q64471;Sik3|Q6P4S6;Wdfy2|Q8BUB4;Camkk2|Q8C078;Pitpnc1|Q8K4R4;Serpinb1b|Q8VHP7;Osbpl1a|Q91XL9;Gstt3|Q99L20;Dusp3|Q9D7X3;Bola1|Q9D8S9;Selenoo|Q9DBC0;Gucy1a1|Q9ERL9;Ide|Q9JHR7;Akr1a1|Q9JII6;Rpgr|Q9R0X5;Stk11|Q9WTK7;Dmtn|Q9WV69;Epb41l3|Q9WV92;Rgs6|Q9Z2H2;Arfgap3|Q9D8S3;Sptb|P15508;Sptan1|P16546;Pak7|Q8C015;4833439L19Rik|Q9DBN4;Mrpl22|Q8BU88;Ablim2|Q8BL65</t>
+    <t xml:space="preserve">|Q91XL9;|Q99L20;|Q9Z2H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P35235;|P46664;|P63318;|P70236;|P70290;|Q5PR73;|Q61133;|Q61140;|Q62406;|Q64471;|Q6P4S6;|Q8BUB4;|Q8C078;|Q8K4R4;|Q8VHP7;|Q91XL9;|Q99L20;|Q9D7X3;|Q9D8S9;|Q9DBC0;|Q9ERL9;|Q9JHR7;|Q9JII6;|Q9R0X5;|Q9WTK7;|Q9WV69;|Q9WV92;|Q9Z2H2;|Q9D8S3;|P15508;|P16546;|Q8C015;|Q9DBN4;|Q8BU88;|Q8BL65</t>
   </si>
   <si>
     <t xml:space="preserve">M18</t>
   </si>
   <si>
-    <t xml:space="preserve">Mtmr14|Q8VEL2;Abca7|Q91V24;Kank2|Q8BX02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fggy|A2AJL3;Mtr|A6H5Y3;Otud7b|B2RUR8;Ttl|P38585;Pkn1|P70268;S100a13|P97352;Cbfb|Q08024;Akt2|Q60823;Rrm2b|Q6PEE3;Dock1|Q8BUR4;Kank2|Q8BX02;Pgm5|Q8BZF8;Adgrg1|Q8K209;Bbox1|Q924Y0;Ppp1r3g|Q9CW07;Apip|Q9WVQ5;Pld4|Q8BG07;Tom1l1|Q923U0;Ankrd27|Q3UMR0;Smurf2|A2A5Z6;Arhgap27|A2AB59;Ptrhd1|D3Z4S3;Serpinb8|O08800;Noct|O35710;Sema6b|O54951;Sh3pxd2a|O89032;Slc6a4|Q60857;Rab34|Q64008;Lrfn2|Q80TG9;Zadh2|Q8BGC4;Flrt2|Q8BLU0;Tmem143|Q8VD26;Mtmr14|Q8VEL2;Abca7|Q91V24</t>
+    <t xml:space="preserve">|Q8VEL2;|Q91V24;|Q8BX02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AJL3;|A6H5Y3;|B2RUR8;|P38585;|P70268;|P97352;|Q08024;|Q60823;|Q6PEE3;|Q8BUR4;|Q8BX02;|Q8BZF8;|Q8K209;|Q924Y0;|Q9CW07;|Q9WVQ5;|Q8BG07;|Q923U0;|Q3UMR0;|A2A5Z6;|A2AB59;|D3Z4S3;|O08800;|O35710;|O54951;|O89032;|Q60857;|Q64008;|Q80TG9;|Q8BGC4;|Q8BLU0;|Q8VD26;|Q8VEL2;|Q91V24</t>
   </si>
   <si>
     <t xml:space="preserve">M19</t>
   </si>
   <si>
-    <t xml:space="preserve">Ccdc22|Q9JIG7;Fam45a|Q9D8N2;Commd2|Q8BXC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kifc2|O08672;Vps26c|O35075;Dcn|P28654;Syt2|P46097;Hspg2|Q05793;Vps8|Q0P5W1;Washc4|Q3UMB9;Cdc42bpa|Q3UU96;Commd6|Q3V4B5;Commd3|Q63829;Tnks|Q6PFX9;Washc2|Q6PGL7;Tiam2|Q6ZPF3;Ccdc93|Q7TQK5;Ttc9c|Q810A3;Commd7|Q8BG94;Vps35l|Q8BWQ6;Commd2|Q8BXC6;Ttc39b|Q8BYY4;Wwp1|Q8BZZ3;Washc5|Q8C2E7;Dock2|Q8C3J5;Bag5|Q8CI32;Commd9|Q8K2Q0;Lgi3|Q8K406;Commd1|Q8K4M5;Zcchc18|Q8VD24;Washc1|Q8VDD8;Bicd2|Q921C5;Fam45a|Q9D8N2;Klc4|Q9DBS5;Ccdc22|Q9JIG7;Rab37|Q9JKM7;Tmem163|Q8C996</t>
+    <t xml:space="preserve">|Q9JIG7;|Q9D8N2;|Q8BXC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08672;|O35075;|P28654;|P46097;|Q05793;|Q0P5W1;|Q3UMB9;|Q3UU96;|Q3V4B5;|Q63829;|Q6PFX9;|Q6PGL7;|Q6ZPF3;|Q7TQK5;|Q810A3;|Q8BG94;|Q8BWQ6;|Q8BXC6;|Q8BYY4;|Q8BZZ3;|Q8C2E7;|Q8C3J5;|Q8CI32;|Q8K2Q0;|Q8K406;|Q8K4M5;|Q8VD24;|Q8VDD8;|Q921C5;|Q9D8N2;|Q9DBS5;|Q9JIG7;|Q9JKM7;|Q8C996</t>
   </si>
   <si>
     <t xml:space="preserve">M20</t>
   </si>
   <si>
-    <t xml:space="preserve">Acsbg1|Q99PU5;Arfgap1|Q9EPJ9;Rab27b|Q99P58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sh2d3c|Q9QZS8;Mgll|O35678;Atp6v0d1|P51863;Dnajc5|P60904;Vamp2|P63044;Rab33a|P97950;Map3k13|Q1HKZ5;Rab26|Q504M8;Arg1|Q61176;Gpam|Q61586;Vat1|Q62465;Cltc|Q68FD5;Ocrl|Q6NVF0;Trim37|Q6PCX9;Mfsd4a|Q6PDC8;Zfyve1|Q810J8;Slc35d3|Q8BGF8;Iffo1|Q8BXL9;Ston2|Q8BZ60;Syn3|Q8JZP2;Myrip|Q8K3I4;Abhd4|Q8VD66;Syt17|Q920M7;Rab27b|Q99P58;Acsbg1|Q99PU5;Arfgap1|Q9EPJ9;Ube3b|Q9ES34;Vps13a|Q5H8C4;Slc5a7|Q8BGY9;Olfm2|Q8BM13</t>
+    <t xml:space="preserve">|Q99PU5;|Q9EPJ9;|Q99P58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9QZS8;|O35678;|P51863;|P60904;|P63044;|P97950;|Q1HKZ5;|Q504M8;|Q61176;|Q61586;|Q62465;|Q68FD5;|Q6NVF0;|Q6PCX9;|Q6PDC8;|Q810J8;|Q8BGF8;|Q8BXL9;|Q8BZ60;|Q8JZP2;|Q8K3I4;|Q8VD66;|Q920M7;|Q99P58;|Q99PU5;|Q9EPJ9;|Q9ES34;|Q5H8C4;|Q8BGY9;|Q8BM13</t>
   </si>
   <si>
     <t xml:space="preserve">M21</t>
   </si>
   <si>
-    <t xml:space="preserve">Rdh14|Q9ERI6;Gria4|Q9Z2W8;Atad1|Q9D5T0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akap1|O08715;Golga5|Q9QYE6;Myadm|O35682;Rab33b|O35963;Rmdn3|Q3UJU9;Miga1|Q4QQM5;Snph|Q80U23;Mfn1|Q811U4;Sybu|Q8BHS8;Comtd1|Q8BIG7;Exd2|Q8VEG4;Atad1|Q9D5T0;Rab24|P35290;Olfm3|P63056;Cdh6|P97326;March5|Q3KNM2;Fam173a|Q501J2;Dbh|Q64237;Panx2|Q6IMP4;Minar1|Q8K3V7;Mavs|Q8VCF0;Rdh14|Q9ERI6;Gria4|Q9Z2W8;Ehbp1l1|Q99MS7;Fbxl2|Q8BH16;Agpat5|Q9D1E8;Cyb5b|Q9CQX2</t>
+    <t xml:space="preserve">|Q9ERI6;|Q9Z2W8;|Q9D5T0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08715;|Q9QYE6;|O35682;|O35963;|Q3UJU9;|Q4QQM5;|Q80U23;|Q811U4;|Q8BHS8;|Q8BIG7;|Q8VEG4;|Q9D5T0;|P35290;|P63056;|P97326;|Q3KNM2;|Q501J2;|Q64237;|Q6IMP4;|Q8K3V7;|Q8VCF0;|Q9ERI6;|Q9Z2W8;|Q99MS7;|Q8BH16;|Q9D1E8;|Q9CQX2</t>
   </si>
   <si>
     <t xml:space="preserve">M22</t>
   </si>
   <si>
-    <t xml:space="preserve">H1f3|P43277;Mecp2|Q9Z2D6;H2bu2|Q9D2U9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tcof1|O08784;Cavin1|O54724;H1f0|P10922;H1f2|P15864;H2afx|P27661;H1f4|P43274;H1f1|P43275;H1f5|P43276;H1f3|P43277;Cdk5r1|P61809;H2afv|Q3THW5;Fbxw11|Q5SRY7;Cavin2|Q63918;H2ac20|Q64523;H2bc18|Q64525;Nexn|Q7TPW1;Rab3gap1|Q80UJ7;Cavin3|Q91VJ2;Mecp2|Q9Z2D6;Hnrnpf|Q9Z2X1;Macroh2a2|Q8CCK0;H2bu2|Q9D2U9</t>
+    <t xml:space="preserve">|P43277;|Q9Z2D6;|Q9D2U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08784;|O54724;|P10922;|P15864;|P27661;|P43274;|P43275;|P43276;|P43277;|P61809;|Q3THW5;|Q5SRY7;|Q63918;|Q64523;|Q64525;|Q7TPW1;|Q80UJ7;|Q91VJ2;|Q9Z2D6;|Q9Z2X1;|Q8CCK0;|Q9D2U9</t>
   </si>
   <si>
     <t xml:space="preserve">M23</t>
   </si>
   <si>
-    <t xml:space="preserve">Rin1|Q921Q7;Rhobtb2|Q91V93;Nsmf|Q99NF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uhrf1bp1l|A2RSJ4;Limk2|O54785;Dtnb|O70585;Sh3bp1|P55194;Cdk18|Q04899;Rab3ip|Q68EF0;Wdcp|Q6NV72;Kank4|Q6P9J5;Arhgef4|Q7TNR9;Ppp2r2c|Q8BG02;Pi4kb|Q8BKC8;Fam110b|Q8C739;Tma7|Q8K003;Rhobtb2|Q91V93;Farp2|Q91VS8;Rin1|Q921Q7;Nsmf|Q99NF2;Ttc9b|Q9D6E4;Scyl1|Q9EQC5;Hltf|Q6PCN7;Mapk8ip1|Q9WVI9</t>
+    <t xml:space="preserve">|Q921Q7;|Q91V93;|Q99NF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2RSJ4;|O54785;|O70585;|P55194;|Q04899;|Q68EF0;|Q6NV72;|Q6P9J5;|Q7TNR9;|Q8BG02;|Q8BKC8;|Q8C739;|Q8K003;|Q91V93;|Q91VS8;|Q921Q7;|Q99NF2;|Q9D6E4;|Q9EQC5;|Q6PCN7;|Q9WVI9</t>
   </si>
   <si>
     <t xml:space="preserve">M24</t>
   </si>
   <si>
-    <t xml:space="preserve">Akr7a5|Q8CG76;Pithd1|Q8BWR2;Naxe|Q8K4Z3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acot1|O55137;Nudt11|P0C028;Bcat1|P24288;Akr1b8|P45377;Pcbd1|P61458;Wdr41|Q3UDP0;Nudt9|Q8BVU5;Pithd1|Q8BWR2;Nit2|Q9JHW2;Tulp3|O88413;Nudt2|P56380;Lypla1|P97823;Hsdl2|Q2TPA8;Akr7a5|Q8CG76;Naxe|Q8K4Z3;Dhrs4|Q99LB2;Dph2|Q9CR25;Eci2|Q9WUR2</t>
+    <t xml:space="preserve">|Q8CG76;|Q8BWR2;|Q8K4Z3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55137;|P0C028;|P24288;|P45377;|P61458;|Q3UDP0;|Q8BVU5;|Q8BWR2;|Q9JHW2;|O88413;|P56380;|P97823;|Q2TPA8;|Q8CG76;|Q8K4Z3;|Q99LB2;|Q9CR25;|Q9WUR2</t>
   </si>
   <si>
     <t xml:space="preserve">M25</t>
   </si>
   <si>
-    <t xml:space="preserve">Sh3glb1|Q9JK48;Sh3glb2|Q8R3V5;Fbxo45|Q8K3B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lzts3|A2AHG0;Carmil3|Q3UFQ8;Ddn|Q80TS7;Aak1|Q3UHJ0;Jakmip3|Q5DTN8;Msi1|Q61474;Mycbp2|Q7TPH6;Tecpr1|Q80VP0;Kctd13|Q8BGV7;Lsm11|Q8BUV6;Arfip2|Q8K221;Fbxo45|Q8K3B1;Sh3glb2|Q8R3V5;Tubg2|Q8VCK3;Acot11|Q8VHQ9;Lrrc49|Q91YK0;Sh3glb1|Q9JK48</t>
+    <t xml:space="preserve">|Q9JK48;|Q8R3V5;|Q8K3B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AHG0;|Q3UFQ8;|Q80TS7;|Q3UHJ0;|Q5DTN8;|Q61474;|Q7TPH6;|Q80VP0;|Q8BGV7;|Q8BUV6;|Q8K221;|Q8K3B1;|Q8R3V5;|Q8VCK3;|Q8VHQ9;|Q91YK0;|Q9JK48</t>
   </si>
   <si>
     <t xml:space="preserve">M26</t>
   </si>
   <si>
-    <t xml:space="preserve">Flad1|Q8R123;Nme3|Q9WV85;Aldh7a1|Q9DBF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glmn|Q8BZM1;Echdc1|Q9D9V3;Aldh7a1|Q9DBF1;Nif3l1|Q9EQ80;Tyw5|A2RSX7;Mpv17|P19258;Lyplal1|Q3UFF7;C9orf72|Q6DFW0;Atpaf1|Q811I0;Flad1|Q8R123;Sdhd|Q9CXV1;Bcs1l|Q9CZP5;Rexo2|Q9D8S4;Htra2|Q9JIY5;Nme3|Q9WV85</t>
+    <t xml:space="preserve">|Q8R123;|Q9WV85;|Q9DBF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8BZM1;|Q9D9V3;|Q9DBF1;|Q9EQ80;|A2RSX7;|P19258;|Q3UFF7;|Q6DFW0;|Q811I0;|Q8R123;|Q9CXV1;|Q9CZP5;|Q9D8S4;|Q9JIY5;|Q9WV85</t>
   </si>
   <si>
     <t xml:space="preserve">M27</t>
   </si>
   <si>
-    <t xml:space="preserve">Suclg1|Q9WUM5;Pdhb|Q9D051;Oxct1|Q9D0K2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nipsnap2|O55126;Mmut|P16332;Fech|P22315;Pdha1|P35486;Acadm|P45952;H2-Ke6|P50171;Acadl|P51174;Mccc2|Q3ULD5;Sdr39u1|Q5M8N4;Lrpprc|Q6PB66;Abhd10|Q6PE15;Echs1|Q8BH95;Pitrm1|Q8K411;Abhd11|Q8K4F5;Cbr4|Q91VT4;L2hgdh|Q91YP0;Pdk3|Q922H2;Pycr2|Q922Q4;Dnaja3|Q99M87;Mrps16|Q9CPX7;Decr1|Q9CQ62;Uqcc1|Q9CWU6;Pmpcb|Q9CXT8;Cs|Q9CZU6;Pdhb|Q9D051;Oxct1|Q9D0K2;Acad8|Q9D7B6;Ivd|Q9JHI5;Ndufaf3|Q9JKL4;Acot9|Q9R0X4;Suclg1|Q9WUM5;Timm44|O35857;Eci1|P42125;Tst|P52196;Cox7b|P56393;Idh3g|P70404;Pdp1|Q3UV70;Mars2|Q499X9;Tln2|Q71LX4;Ndufa12|Q7TMF3;Mrpl38|Q8K2M0;Coa7|Q921H9;Hadhb|Q99JY0;Mccc1|Q99MR8;Mrpl45|Q9D0Q7;Txnrd2|Q9JLT4;Suclg2|Q9Z2I8;Hadha|Q8BMS1;Clybl|Q8R4N0</t>
+    <t xml:space="preserve">|Q9WUM5;|Q9D051;|Q9D0K2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55126;|P16332;|P22315;|P35486;|P45952;|P50171;|P51174;|Q3ULD5;|Q5M8N4;|Q6PB66;|Q6PE15;|Q8BH95;|Q8K411;|Q8K4F5;|Q91VT4;|Q91YP0;|Q922H2;|Q922Q4;|Q99M87;|Q9CPX7;|Q9CQ62;|Q9CWU6;|Q9CXT8;|Q9CZU6;|Q9D051;|Q9D0K2;|Q9D7B6;|Q9JHI5;|Q9JKL4;|Q9R0X4;|Q9WUM5;|O35857;|P42125;|P52196;|P56393;|P70404;|Q3UV70;|Q499X9;|Q71LX4;|Q7TMF3;|Q8K2M0;|Q921H9;|Q99JY0;|Q99MR8;|Q9D0Q7;|Q9JLT4;|Q9Z2I8;|Q8BMS1;|Q8R4N0</t>
   </si>
   <si>
     <t xml:space="preserve">M28</t>
   </si>
   <si>
-    <t xml:space="preserve">Atp5d|Q9D3D9;Aifm1|Q9Z0X1;Ndufb9|Q9CQJ8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ech1|O35459;ATP6|P00848;ND4|P03911;Cox4i1|P19783;Slc25a4|P48962;Slc25a5|P51881;Atp5mpl|P56379;Cox6b1|P56391;Atp5b|P56480;Atp5a1|Q03265;Mcu|Q3UMR5;Ndufa4|Q62425;Gpd2|Q64521;Bdh1|Q80XN0;Samm50|Q8BGH2;Timm29|Q8BGX2;Immt|Q8CAQ8;Sdha|Q8K2B3;Ndufs8|Q8K3J1;Slc25a3|Q8VEM8;Ghitm|Q91VC9;Atp5c1|Q91VR2;Atad3a|Q925I1;Sfxn1|Q99JR1;Ndufa10|Q99LC3;Etfa|Q99LC5;Ndufa5|Q9CPP6;Cox6c|Q9CPQ1;Sdhb|Q9CQA3;Ndufb9|Q9CQJ8;Uqcrc1|Q9CZ13;Tomm40l|Q9CZR3;Atp5d|Q9D3D9;Uqcrc2|Q9DB77;Ndufa9|Q9DC69;Ndufb10|Q9DCS9;Ndufs3|Q9DCT2;Rapgef4|Q9EQZ6;Aifm1|Q9Z0X1</t>
+    <t xml:space="preserve">|Q9D3D9;|Q9Z0X1;|Q9CQJ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35459;|P00848;|P03911;|P19783;|P48962;|P51881;|P56379;|P56391;|P56480;|Q03265;|Q3UMR5;|Q62425;|Q64521;|Q80XN0;|Q8BGH2;|Q8BGX2;|Q8CAQ8;|Q8K2B3;|Q8K3J1;|Q8VEM8;|Q91VC9;|Q91VR2;|Q925I1;|Q99JR1;|Q99LC3;|Q99LC5;|Q9CPP6;|Q9CPQ1;|Q9CQA3;|Q9CQJ8;|Q9CZ13;|Q9CZR3;|Q9D3D9;|Q9DB77;|Q9DC69;|Q9DCS9;|Q9DCT2;|Q9EQZ6;|Q9Z0X1</t>
   </si>
   <si>
     <t xml:space="preserve">M29</t>
   </si>
   <si>
-    <t xml:space="preserve">Mecr|Q9DCS3;Ak4|Q9WUR9;Ak3|Q9WTP7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poldip2|Q91VA6;Nipsnap1|O55125;Sod2|P09671;Prdx3|P20108;Hspd1|P63038;Phb|P67778;Ccdc51|Q3URS9;Tmem65|Q4VAE3;Slc30a9|Q5IRJ6;Erc2|Q6PH08;Amph|Q7TQF7;Tufm|Q8BFR5;Gpt2|Q8BGT5;Thnsl1|Q8BH55;Me3|Q8BMF3;Spata2l|Q8BNN1;Cars2|Q8BYM8;Exog|Q8C163;Iba57|Q8CAK1;Acat1|Q8QZT1;Bphl|Q8R164;Sfxn3|Q91V61;Mtif2|Q91YJ5;Mlycd|Q99J39;Stoml2|Q99JB2;Aco2|Q99KI0;Hibadh|Q99L13;Ndufc2|Q9CQ54;Acot13|Q9CQR4;Fam136a|Q9CR98;Idh3a|Q9D6R2;Isca2|Q9DCB8;Mecr|Q9DCS3;Agk|Q9ESW4;Nfu1|Q9QZ23;Ak3|Q9WTP7;Ak4|Q9WUR9</t>
+    <t xml:space="preserve">|Q9DCS3;|Q9WUR9;|Q9WTP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q91VA6;|O55125;|P09671;|P20108;|P63038;|P67778;|Q3URS9;|Q4VAE3;|Q5IRJ6;|Q6PH08;|Q7TQF7;|Q8BFR5;|Q8BGT5;|Q8BH55;|Q8BMF3;|Q8BNN1;|Q8BYM8;|Q8C163;|Q8CAK1;|Q8QZT1;|Q8R164;|Q91V61;|Q91YJ5;|Q99J39;|Q99JB2;|Q99KI0;|Q99L13;|Q9CQ54;|Q9CQR4;|Q9CR98;|Q9D6R2;|Q9DCB8;|Q9DCS3;|Q9ESW4;|Q9QZ23;|Q9WTP7;|Q9WUR9</t>
   </si>
   <si>
     <t xml:space="preserve">M30</t>
   </si>
   <si>
-    <t xml:space="preserve">Ppif|Q99KR7;Aldh6a1|Q9EQ20;Acss1|Q99NB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Got2|P05202;Surf1|P09925;Th|P24529;Tfam|P40630;Fh1|P97807;Pcx|Q05920;Fahd2a|Q3TC72;Tamm41|Q3TUH1;Them4|Q3UUI3;Abcb7|Q61102;Sptbn1|Q62261;Hspe1|Q64433;Pdpr|Q7TSQ8;Glrx5|Q80Y14;Slc25a12|Q8BH59;Dars2|Q8BIP0;Nadk2|Q8C5H8;Taco1|Q8K0Z7;Fahd1|Q8R0F8;Acsf2|Q8VCW8;Lars2|Q8VDC0;Mpst|Q99J99;Ppif|Q99KR7;Acss1|Q99NB1;Ndufa6|Q9CQZ5;Mcee|Q9D1I5;Aldh6a1|Q9EQ20;Pdk2|Q9JK42</t>
+    <t xml:space="preserve">|Q99KR7;|Q9EQ20;|Q99NB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P05202;|P09925;|P24529;|P40630;|P97807;|Q05920;|Q3TC72;|Q3TUH1;|Q3UUI3;|Q61102;|Q62261;|Q64433;|Q7TSQ8;|Q80Y14;|Q8BH59;|Q8BIP0;|Q8C5H8;|Q8K0Z7;|Q8R0F8;|Q8VCW8;|Q8VDC0;|Q99J99;|Q99KR7;|Q99NB1;|Q9CQZ5;|Q9D1I5;|Q9EQ20;|Q9JK42</t>
   </si>
   <si>
     <t xml:space="preserve">M31</t>
   </si>
   <si>
-    <t xml:space="preserve">Lactb|Q9EP89;Slc25a10|Q9QZD8;Apoo|Q9DCZ4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mtx2|O88441;Yme1l1|O88967;Cox6a1|P43024;Nlrx1|Q3TL44;Ndufb6|Q3UIU2;Spg7|Q3ULF4;Opa3|Q505D7;Dnajc11|Q5U458;Micos10|Q7TNS2;Coa6|Q8BGD8;Rdh13|Q8CEE7;Acad9|Q8JZN5;Gfm1|Q8K0D5;Prelid3a|Q8VE85;Atp5l|Q9CPQ8;Slc25a11|Q9CR62;Sdhc|Q9CZB0;Ndufv2|Q9D6J6;Uqcrb|Q9D855;Timm50|Q9D880;Tmem160|Q9D938;Apoo|Q9DCZ4;Lactb|Q9EP89;Ndufa13|Q9ERS2;Slc25a10|Q9QZD8;Ndufa7|Q9Z1P6;Letm1|Q9Z2I0</t>
+    <t xml:space="preserve">|Q9EP89;|Q9QZD8;|Q9DCZ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88441;|O88967;|P43024;|Q3TL44;|Q3UIU2;|Q3ULF4;|Q505D7;|Q5U458;|Q7TNS2;|Q8BGD8;|Q8CEE7;|Q8JZN5;|Q8K0D5;|Q8VE85;|Q9CPQ8;|Q9CR62;|Q9CZB0;|Q9D6J6;|Q9D855;|Q9D880;|Q9D938;|Q9DCZ4;|Q9EP89;|Q9ERS2;|Q9QZD8;|Q9Z1P6;|Q9Z2I0</t>
   </si>
   <si>
     <t xml:space="preserve">M32</t>
   </si>
   <si>
-    <t xml:space="preserve">Mical3|Q8CJ19;Tsfm|Q9CZR8;Lonp1|Q8CGK3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prex1|Q69ZK0;Ank2|Q8C8R3;Dlgap1|Q9D415;Gatm|Q9D964;Plch2|A2AP18;Dld|O08749;Mdh2|P08249;Hspa9|P38647;Abat|P61922;Acsf3|Q3URE1;Arhgap21|Q6DFV3;Lrrc7|Q80TE7;Rimbp2|Q80U40;Pck2|Q8BH04;Iars2|Q8BIJ6;Dlgap2|Q8BJ42;Aldh5a1|Q8BWF0;Ptges2|Q8BWM0;Scai|Q8C8N2;Lonp1|Q8CGK3;Mical3|Q8CJ19;Ablim1|Q8K4G5;Hibch|Q8QZS1;Me2|Q99KE1;Tsfm|Q9CZR8;Mrrf|Q9D6S7;Sucla2|Q9Z2I9</t>
+    <t xml:space="preserve">|Q8CJ19;|Q9CZR8;|Q8CGK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q69ZK0;|Q8C8R3;|Q9D415;|Q9D964;|A2AP18;|O08749;|P08249;|P38647;|P61922;|Q3URE1;|Q6DFV3;|Q80TE7;|Q80U40;|Q8BH04;|Q8BIJ6;|Q8BJ42;|Q8BWF0;|Q8BWM0;|Q8C8N2;|Q8CGK3;|Q8CJ19;|Q8K4G5;|Q8QZS1;|Q99KE1;|Q9CZR8;|Q9D6S7;|Q9Z2I9</t>
   </si>
   <si>
     <t xml:space="preserve">M33</t>
   </si>
   <si>
-    <t xml:space="preserve">Oxsm|Q9D404;Nubpl|Q9CWD8;Hint2|Q9D0S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cox15|Q8BJ03;Nubpl|Q9CWD8;Plgrkt|Q9D3P8;Fhit|O89106;Gfer|P56213;Mpc1|P63030;Prdx5|P99029;Rars2|Q3U186;Cmpk2|Q3U5Q7;Cryzl2|Q3UNZ8;Cox7a2l|Q61387;Kyat3|Q71RI9;Dglucy|Q8BH86;Vwa8|Q8CC88;Afg3l2|Q8JZQ2;Hscb|Q8K3A0;Gdap1l1|Q8VE33;Chchd6|Q91VN4;Gcsh|Q91WK5;Ndufa2|Q9CQ75;Hint2|Q9D0S9;Mmab|Q9D273;Oxsm|Q9D404;Acadsb|Q9DBL1;Aldh18a1|Q9Z110</t>
+    <t xml:space="preserve">|Q9D404;|Q9CWD8;|Q9D0S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8BJ03;|Q9CWD8;|Q9D3P8;|O89106;|P56213;|P63030;|P99029;|Q3U186;|Q3U5Q7;|Q3UNZ8;|Q61387;|Q71RI9;|Q8BH86;|Q8CC88;|Q8JZQ2;|Q8K3A0;|Q8VE33;|Q91VN4;|Q91WK5;|Q9CQ75;|Q9D0S9;|Q9D273;|Q9D404;|Q9DBL1;|Q9Z110</t>
   </si>
   <si>
     <t xml:space="preserve">M34</t>
   </si>
   <si>
-    <t xml:space="preserve">Dmac2l|Q9CRA7;Ethe1|Q9DCM0;Ndufaf4|Q9D1H6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajm1|A2AJA9;Mipep|A6H611;ND1|P03888;Hmgcl|P38060;Aldh2|P47738;Cycs|P62897;Isoc2a|P85094;Unc13a|Q4KUS2;Hadh|Q61425;Acaa2|Q8BWT1;Micu1|Q8VCX5;Hars2|Q99KK9;Ndufs5|Q99LY9;Nipsnap3b|Q9CQE1;Trap1|Q9CQN1;Dmac2l|Q9CRA7;Ndufs4|Q9CXZ1;Mpc2|Q9D023;Ndufaf4|Q9D1H6;Ethe1|Q9DCM0;Ptpn4|Q9WU22</t>
+    <t xml:space="preserve">|Q9CRA7;|Q9DCM0;|Q9D1H6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AJA9;|A6H611;|P03888;|P38060;|P47738;|P62897;|P85094;|Q4KUS2;|Q61425;|Q8BWT1;|Q8VCX5;|Q99KK9;|Q99LY9;|Q9CQE1;|Q9CQN1;|Q9CRA7;|Q9CXZ1;|Q9D023;|Q9D1H6;|Q9DCM0;|Q9WU22</t>
   </si>
   <si>
     <t xml:space="preserve">M35</t>
   </si>
   <si>
-    <t xml:space="preserve">Homer2|Q9QWW1;Plcxd3|Q8BLJ3;Begain|Q68EF6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srcin1|Q9QWI6;Kalrn|A2CG49;Gpx4|O70325;Ctbp1|O88712;Dnm1|P39053;Grid2ip|Q0QWG9;Traf3|Q60803;Dlg4|Q62108;Begain|Q68EF6;Plcxd3|Q8BLJ3;Dlg2|Q91XM9;Macrod1|Q922B1;Homer2|Q9QWW1</t>
+    <t xml:space="preserve">|Q9QWW1;|Q8BLJ3;|Q68EF6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9QWI6;|A2CG49;|O70325;|O88712;|P39053;|Q0QWG9;|Q60803;|Q62108;|Q68EF6;|Q8BLJ3;|Q91XM9;|Q922B1;|Q9QWW1</t>
   </si>
   <si>
     <t xml:space="preserve">M36</t>
   </si>
   <si>
-    <t xml:space="preserve">Pclo|Q9QYX7;Ndufb7|Q9CR61;Atp5pb|Q9CQQ7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ndufb11|O09111;Bsn|O88737;Grin2a|P35436;Grin2b|Q01097;Ndufaf2|Q59J78;Pgam5|Q8BX10;Atp5pb|Q9CQQ7;Ndufb7|Q9CR61;Uqcrfs1|Q9CR68;Pclo|Q9QYX7</t>
+    <t xml:space="preserve">|Q9QYX7;|Q9CR61;|Q9CQQ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09111;|O88737;|P35436;|Q01097;|Q59J78;|Q8BX10;|Q9CQQ7;|Q9CR61;|Q9CR68;|Q9QYX7</t>
   </si>
   <si>
     <t xml:space="preserve">M37</t>
   </si>
   <si>
-    <t xml:space="preserve">Gstz1|Q9WVL0;Cyc1|Q9D0M3;Etfb|Q9DCW4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ndufs1|Q91VD9;Mtfp1|Q9CRB8;Cyc1|Q9D0M3;Etfb|Q9DCW4;Gstz1|Q9WVL0</t>
+    <t xml:space="preserve">|Q9WVL0;|Q9D0M3;|Q9DCW4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q91VD9;|Q9CRB8;|Q9D0M3;|Q9DCW4;|Q9WVL0</t>
   </si>
   <si>
     <t xml:space="preserve">M38</t>
   </si>
   <si>
-    <t xml:space="preserve">Stard10|Q9JMD3;Pfn2|Q9JJV2;Tubb2b|Q9CWF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gpd1|P13707;Eno2|P17183;Tpi1|P17751;Hspa4l|P48722;Gdi1|P50396;Usp5|P56399;Tuba4a|P68368;Tuba1a|P68369;Gclc|P97494;Uba1|Q02053;Smyd5|Q3TYX3;Prdx2|Q61171;Pafah1b3|Q61205;Xpnpep1|Q6P1B1;Ube2o|Q6ZPJ3;Tubb2a|Q7TMM9;Cpped1|Q8BFS6;Sh3bgrl2|Q8BG73;Pggt1b|Q8BUY9;Nhlrc2|Q8BZW8;Yod1|Q8CB27;Pdxk|Q8K183;4931406C07Rik|Q91V76;Csdc2|Q91YQ3;Ddo|Q922Z0;Mien1|Q9CQ86;Tubb2b|Q9CWF2;Ola1|Q9CZ30;Acp1|Q9D358;Itpa|Q9D892;Csad|Q9DBE0;Cmpk1|Q9DBP5;Pfn2|Q9JJV2;Nt5c|Q9JM14;Stard10|Q9JMD3;Esd|Q9R0P3;Akt3|Q9WUA6</t>
+    <t xml:space="preserve">|Q9JMD3;|Q9JJV2;|Q9CWF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P13707;|P17183;|P17751;|P48722;|P50396;|P56399;|P68368;|P68369;|P97494;|Q02053;|Q3TYX3;|Q61171;|Q61205;|Q6P1B1;|Q6ZPJ3;|Q7TMM9;|Q8BFS6;|Q8BG73;|Q8BUY9;|Q8BZW8;|Q8CB27;|Q8K183;|Q91V76;|Q91YQ3;|Q922Z0;|Q9CQ86;|Q9CWF2;|Q9CZ30;|Q9D358;|Q9D892;|Q9DBE0;|Q9DBP5;|Q9JJV2;|Q9JM14;|Q9JMD3;|Q9R0P3;|Q9WUA6</t>
   </si>
   <si>
     <t xml:space="preserve">M39</t>
   </si>
   <si>
-    <t xml:space="preserve">Lhpp|Q9D7I5;Srr|Q9QZX7;Pgam1|Q9DBJ1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Got1|P05201;Fabp3|P11404;Acyp1|P56376;Actn4|P57780;Kpnb1|P70168;Ric8a|Q3TIR3;Ttll12|Q3UDE2;Hspa4|Q61316;Gdi2|Q61598;Dbnl|Q62418;Wdr44|Q6NVE8;Gapvd1|Q6PAR5;Phyhipl|Q8BGT8;AW549877|Q8BR90;Pgm2l1|Q8CAA7;Ppm1f|Q8CGA0;Pak2|Q8CIN4;Hnmt|Q91VF2;Rabep2|Q91WG2;Camk1|Q91YS8;Park7|Q99LX0;Nanp|Q9CPT3;Mri1|Q9CQT1;Vta1|Q9CR26;Arl2|Q9D0J4;Lhpp|Q9D7I5;Pgam1|Q9DBJ1;Mettl26|Q9DCS2;Srr|Q9QZX7;Crlf3|Q9Z2L7</t>
+    <t xml:space="preserve">|Q9D7I5;|Q9QZX7;|Q9DBJ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P05201;|P11404;|P56376;|P57780;|P70168;|Q3TIR3;|Q3UDE2;|Q61316;|Q61598;|Q62418;|Q6NVE8;|Q6PAR5;|Q8BGT8;|Q8BR90;|Q8CAA7;|Q8CGA0;|Q8CIN4;|Q91VF2;|Q91WG2;|Q91YS8;|Q99LX0;|Q9CPT3;|Q9CQT1;|Q9CR26;|Q9D0J4;|Q9D7I5;|Q9DBJ1;|Q9DCS2;|Q9QZX7;|Q9Z2L7</t>
   </si>
   <si>
     <t xml:space="preserve">M40</t>
   </si>
   <si>
-    <t xml:space="preserve">Phpt1|Q9DAK9;Sh3bgrl|Q9JJU8;Ak1|Q9R0Y5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gsto1|O09131;Rbbp9|O88851;Ranbp1|P34022;Akr1b3|P45376;Ube2n|P61089;Nutf2|P61971;Pebp1|P70296;Jpt1|P97825;Rela|Q04207;Fabp5|Q05816;Otub1|Q7TQI3;Ube2q1|Q7TSS2;Tiprl|Q8BH58;Gga1|Q8R0H9;Gca|Q8VC88;As3mt|Q91WU5;Sncb|Q91ZZ3;Pcyt2|Q922E4;Dpp3|Q99KK7;Nudcd2|Q9CQ48;Ccdc43|Q9CR29;Ube2f|Q9CY34;Eef1akmt1|Q9CY45;Gbe1|Q9D6Y9;Phpt1|Q9DAK9;Sh3bgrl|Q9JJU8;Prep|Q9QUR6;Ak1|Q9R0Y5</t>
+    <t xml:space="preserve">|Q9DAK9;|Q9JJU8;|Q9R0Y5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09131;|O88851;|P34022;|P45376;|P61089;|P61971;|P70296;|P97825;|Q04207;|Q05816;|Q7TQI3;|Q7TSS2;|Q8BH58;|Q8R0H9;|Q8VC88;|Q91WU5;|Q91ZZ3;|Q922E4;|Q99KK7;|Q9CQ48;|Q9CR29;|Q9CY34;|Q9CY45;|Q9D6Y9;|Q9DAK9;|Q9JJU8;|Q9QUR6;|Q9R0Y5</t>
   </si>
   <si>
     <t xml:space="preserve">M41</t>
   </si>
   <si>
-    <t xml:space="preserve">Pgm3|Q9CYR6;Cygb|Q9CX80;Nudt3|Q9JI46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armt1|A6H630;Ddt|O35215;Shd|O88834;Mdh1|P14152;Selenbp1|P17563;Tsta3|P23591;Adh5|P28474;Ptpa|P58389;Tubb4b|P68372;Prkcb|P68404;Anxa7|Q07076;Scrn3|Q3TMH2;Hdhd2|Q3UGR5;Ppp1r7|Q3UM45;Crppa|Q5RJG7;Serpinb6a|Q60854;Fscn1|Q61553;Acap2|Q6ZQK5;Cpne4|Q8BLR2;Grhpr|Q91Z53;Arhgdia|Q99PT1;Cygb|Q9CX80;Pgm3|Q9CYR6;Ube2v1|Q9CZY3;Ube2v2|Q9D2M8;Paics|Q9DCL9;Nudt3|Q9JI46;Gsdme|Q9Z2D3</t>
+    <t xml:space="preserve">|Q9CYR6;|Q9CX80;|Q9JI46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A6H630;|O35215;|O88834;|P14152;|P17563;|P23591;|P28474;|P58389;|P68372;|P68404;|Q07076;|Q3TMH2;|Q3UGR5;|Q3UM45;|Q5RJG7;|Q60854;|Q61553;|Q6ZQK5;|Q8BLR2;|Q91Z53;|Q99PT1;|Q9CX80;|Q9CYR6;|Q9CZY3;|Q9D2M8;|Q9DCL9;|Q9JI46;|Q9Z2D3</t>
   </si>
   <si>
     <t xml:space="preserve">M42</t>
   </si>
   <si>
-    <t xml:space="preserve">Ncdn|Q9Z0E0;Lypla2|Q9WTL7;Uchl3|Q9JKB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabgap1l|A6H6A9;Prdx6|O08709;Rabep1|O35551;Slk|O54988;Cfl1|P18760;Mif|P34884;Ywhag|P61982;Pfn1|P62962;2610301B20Rik|Q3UJP5;Hsph1|Q61699;Vcl|Q64727;Ppm1e|Q80TL0;Ipo5|Q8BKC5;Rnpep|Q8VCT3;Mpi|Q924M7;Rab28|Q99KL7;Pgls|Q9CQ60;Gmfb|Q9CQI3;Ywhab|Q9CQV8;Cndp2|Q9D1A2;Cnn3|Q9DAW9;Hikeshi|Q9DD02;Oga|Q9EQQ9;Uchl3|Q9JKB1;Lypla2|Q9WTL7;Pdcd6ip|Q9WU78;Ncdn|Q9Z0E0</t>
+    <t xml:space="preserve">|Q9Z0E0;|Q9WTL7;|Q9JKB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A6H6A9;|O08709;|O35551;|O54988;|P18760;|P34884;|P61982;|P62962;|Q3UJP5;|Q61699;|Q64727;|Q80TL0;|Q8BKC5;|Q8VCT3;|Q924M7;|Q99KL7;|Q9CQ60;|Q9CQI3;|Q9CQV8;|Q9D1A2;|Q9DAW9;|Q9DD02;|Q9EQQ9;|Q9JKB1;|Q9WTL7;|Q9WU78;|Q9Z0E0</t>
   </si>
   <si>
     <t xml:space="preserve">M43</t>
   </si>
   <si>
-    <t xml:space="preserve">Lysmd2|Q9D7V2;Dhdh|Q9DBB8;Nagk|Q9QZ08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabgap1|A2AWA9;Tpmt|O55060;Cbr1|P48758;Cpne2|P59108;Ywhaz|P63101;Macrod2|Q3UYG8;Dnajc6|Q80TZ3;Chmp7|Q8R1T1;Sh3bgrl3|Q91VW3;Pnpo|Q91XF0;Gak|Q99KY4;Cotl1|Q9CQI6;Lysmd2|Q9D7V2;Efhd2|Q9D8Y0;Dhdh|Q9DBB8;Npl|Q9DCJ9;Drg2|Q9QXB9;Nagk|Q9QZ08;Hebp1|Q9R257</t>
+    <t xml:space="preserve">|Q9D7V2;|Q9DBB8;|Q9QZ08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AWA9;|O55060;|P48758;|P59108;|P63101;|Q3UYG8;|Q80TZ3;|Q8R1T1;|Q91VW3;|Q91XF0;|Q99KY4;|Q9CQI6;|Q9D7V2;|Q9D8Y0;|Q9DBB8;|Q9DCJ9;|Q9QXB9;|Q9QZ08;|Q9R257</t>
   </si>
   <si>
     <t xml:space="preserve">M44</t>
   </si>
   <si>
-    <t xml:space="preserve">Rabggta|Q9JHK4;Lap3|Q9CPY7;Fam49b|Q921M7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apba1|B2RUJ5;Wdr1|O88342;Gpi1|P06745;Ephx2|P34914;Gsr|P47791;Npepps|Q11011;Guk1|Q64520;Prune1|Q8BIW1;Armc6|Q8BNU0;Thtpa|Q8JZL3;Cbr3|Q8K354;Ptgr2|Q8VDQ1;Fam49b|Q921M7;Lap3|Q9CPY7;Pgm2|Q9D0F9;Rabggta|Q9JHK4</t>
+    <t xml:space="preserve">|Q9JHK4;|Q9CPY7;|Q921M7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RUJ5;|O88342;|P06745;|P34914;|P47791;|Q11011;|Q64520;|Q8BIW1;|Q8BNU0;|Q8JZL3;|Q8K354;|Q8VDQ1;|Q921M7;|Q9CPY7;|Q9D0F9;|Q9JHK4</t>
   </si>
   <si>
     <t xml:space="preserve">M45</t>
   </si>
   <si>
-    <t xml:space="preserve">Glrx|Q9QUH0;Glo1|Q9CPU0;Rabif|Q91X96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impa1|O55023;Lta4h|P24527;Adk|P55264;Ywhaq|P68254;Hint1|P70349;Tubb5|P99024;Ckb|Q04447;Adprhl2|Q8CG72;Pgp|Q8CHP8;Rpe|Q8VEE0;Rabif|Q91X96;Glo1|Q9CPU0;Glrx|Q9QUH0</t>
+    <t xml:space="preserve">|Q9QUH0;|Q9CPU0;|Q91X96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55023;|P24527;|P55264;|P68254;|P70349;|P99024;|Q04447;|Q8CG72;|Q8CHP8;|Q8VEE0;|Q91X96;|Q9CPU0;|Q9QUH0</t>
   </si>
   <si>
     <t xml:space="preserve">M46</t>
   </si>
   <si>
-    <t xml:space="preserve">Gstk1|Q9DCM2;Sdsl|Q8R238;Epn1|Q80VP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gusb|P12265;Ctsd|P18242;Pnp|P23492;Pitpna|P53810;Pitpnb|P53811;Ywhae|P62259;Garem1|Q3UFT3;Epn1|Q80VP1;Pef1|Q8BFY6;Sdsl|Q8R238;Fam114a2|Q8VE88;Gstk1|Q9DCM2</t>
+    <t xml:space="preserve">|Q9DCM2;|Q8R238;|Q80VP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P12265;|P18242;|P23492;|P53810;|P53811;|P62259;|Q3UFT3;|Q80VP1;|Q8BFY6;|Q8R238;|Q8VE88;|Q9DCM2</t>
   </si>
   <si>
     <t xml:space="preserve">M47</t>
   </si>
   <si>
-    <t xml:space="preserve">Nrbp2|Q91V36;Gda|Q9R111;Cmbl|Q8R1G2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fbxl16|A2RT62;Crym|O54983;Pcmt1|P23506;Gstm5|P48774;Strada|Q3UUJ4;Pank4|Q80YV4;Fam49a|Q8BHZ0;Cmbl|Q8R1G2;Lgalsl|Q8VED9;Nrbp2|Q91V36;Gda|Q9R111</t>
+    <t xml:space="preserve">|Q91V36;|Q9R111;|Q8R1G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2RT62;|O54983;|P23506;|P48774;|Q3UUJ4;|Q80YV4;|Q8BHZ0;|Q8R1G2;|Q8VED9;|Q91V36;|Q9R111</t>
   </si>
   <si>
     <t xml:space="preserve">M48</t>
   </si>
   <si>
-    <t xml:space="preserve">Ncald|Q91X97;Cpne6|Q9Z140;Rps6kb1|Q8BSK8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crkl|P47941;Hpca|P84075;Crk|Q64010;Sri|Q6P069;Gga3|Q8BMI3;Rps6kb1|Q8BSK8;Tbcd|Q8BYA0;Tbc1d13|Q8R3D1;Ncald|Q91X97;Cpne6|Q9Z140</t>
+    <t xml:space="preserve">|Q91X97;|Q9Z140;|Q8BSK8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P47941;|P84075;|Q64010;|Q6P069;|Q8BMI3;|Q8BSK8;|Q8BYA0;|Q8R3D1;|Q91X97;|Q9Z140</t>
   </si>
   <si>
     <t xml:space="preserve">M49</t>
   </si>
   <si>
-    <t xml:space="preserve">Galk1|Q9R0N0;Dstn|Q9R0P5;Uap1l1|Q3TW96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ppia|P17742;Slc9a3r1|P70441;Uap1l1|Q3TW96;Tsg101|Q61187;Cstb|Q62426;Ppme1|Q8BVQ5;Galk1|Q9R0N0;Dstn|Q9R0P5</t>
+    <t xml:space="preserve">|Q9R0N0;|Q9R0P5;|Q3TW96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P17742;|P70441;|Q3TW96;|Q61187;|Q62426;|Q8BVQ5;|Q9R0N0;|Q9R0P5</t>
   </si>
   <si>
     <t xml:space="preserve">M50</t>
   </si>
   <si>
-    <t xml:space="preserve">Diras1|Q91Z61;Atic|Q9CWJ9;Cpne1|Q8C166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pex5|O09012;Aprt|P08030;Gnl1|P36916;Gdpgp1|Q3TLS3;Spr|Q64105;Cpne1|Q8C166;Diras1|Q91Z61;Atic|Q9CWJ9</t>
+    <t xml:space="preserve">|Q91Z61;|Q9CWJ9;|Q8C166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09012;|P08030;|P36916;|Q3TLS3;|Q64105;|Q8C166;|Q91Z61;|Q9CWJ9</t>
   </si>
   <si>
     <t xml:space="preserve">M51</t>
   </si>
   <si>
-    <t xml:space="preserve">Rbck1|Q9WUB0;Faim|Q9WUD8;Gale|Q8R059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frmpd4|A2AFR3;Hprt|P00493;Cfl2|P45591;Ankfy1|Q810B6;Gale|Q8R059;Acbd6|Q9D061;Rbck1|Q9WUB0;Faim|Q9WUD8</t>
+    <t xml:space="preserve">|Q9WUB0;|Q9WUD8;|Q8R059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AFR3;|P00493;|P45591;|Q810B6;|Q8R059;|Q9D061;|Q9WUB0;|Q9WUD8</t>
   </si>
   <si>
     <t xml:space="preserve">M52</t>
   </si>
   <si>
-    <t xml:space="preserve">Wdr54|Q9R0D8;Ppp3r1|Q63810;Ppm1a|P49443</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pten|O08586;Arl6|O88848;Inpp1|P49442;Ppm1a|P49443;Pak3|Q61036;Ppp3r1|Q63810;Wdr54|Q9R0D8</t>
+    <t xml:space="preserve">|Q9R0D8;|Q63810;|P49443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08586;|O88848;|P49442;|P49443;|Q61036;|Q63810;|Q9R0D8</t>
   </si>
   <si>
     <t xml:space="preserve">M53</t>
   </si>
   <si>
-    <t xml:space="preserve">Ptpn23|Q6PB44;Prkd1|Q62101;Ripor1|Q68FE6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pdcd6|P12815;Rgs14|P97492;Otulin|Q3UCV8;Prkd1|Q62101;Ripor1|Q68FE6;Ptpn23|Q6PB44</t>
+    <t xml:space="preserve">|Q6PB44;|Q62101;|Q68FE6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P12815;|P97492;|Q3UCV8;|Q62101;|Q68FE6;|Q6PB44</t>
   </si>
   <si>
     <t xml:space="preserve">M54</t>
   </si>
   <si>
-    <t xml:space="preserve">Stau1|Q9Z108;Rpl11|Q9CXW4;Trip4|Q9QXN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rpl27a|P14115;Lipe|P54310;Rpl27|P61358;Nfia|Q02780;Nufip2|Q5F2E7;Dyrk1a|Q61214;Rbm12b2|Q66JV4;Gnl3l|Q6PGG6;Dzip3|Q7TPV2;Dapk1|Q80YE7;Cnot10|Q8BH15;Mical2|Q8BML1;Larp6|Q8BN59;Anapc2|Q8BZQ7;Camsap2|Q8C1B1;Cnot2|Q8C5L3;Cnot6l|Q8VEG6;Ddx41|Q91VN6;Cnot11|Q9CWN7;Rbm33|Q9CXK9;Rpl11|Q9CXW4;Mtrex|Q9CZU3;Mrto4|Q9D0I8;Rpf2|Q9JJ80;Trip4|Q9QXN3;Stau1|Q9Z108;Unkl|Q5FWH2;Clasp1|Q80TV8;Ago3|Q8CJF9;Nifk|Q91VE6;Smg9|Q9DB90;Pelp1|Q9DBD5;Cdc40|Q9DC48</t>
+    <t xml:space="preserve">|Q9Z108;|Q9CXW4;|Q9QXN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P14115;|P54310;|P61358;|Q02780;|Q5F2E7;|Q61214;|Q66JV4;|Q6PGG6;|Q7TPV2;|Q80YE7;|Q8BH15;|Q8BML1;|Q8BN59;|Q8BZQ7;|Q8C1B1;|Q8C5L3;|Q8VEG6;|Q91VN6;|Q9CWN7;|Q9CXK9;|Q9CXW4;|Q9CZU3;|Q9D0I8;|Q9JJ80;|Q9QXN3;|Q9Z108;|Q5FWH2;|Q80TV8;|Q8CJF9;|Q91VE6;|Q9DB90;|Q9DBD5;|Q9DC48</t>
   </si>
   <si>
     <t xml:space="preserve">M55</t>
   </si>
   <si>
-    <t xml:space="preserve">Adar|Q99MU3;Eif4enif1|Q9EST3;Msi2|Q920Q6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zcchc24|B2RVL6;Fry|E9Q8I9;Srp54a|P14576;Pura|P42669;Ddx6|P54823;Pcbp4|P57724;Crnkl1|P63154;Smg5|Q6ZPY2;Pum2|Q80U58;Shfl|Q8CAK3;Sltm|Q8CH25;Adar|Q99MU3;Ftsj3|Q9DBE9;Eif4enif1|Q9EST3;Dctn5|Q9QZB9;Trappc11|B2RXC1;Dcx|O88809;Ybx1|P62960;Mark2|Q05512;Trappc13|Q3TIR1;Tex10|Q3URQ0;Fam120a|Q6A0A9;Fam120b|Q6RI63;Vac14|Q80WQ2;Rbfox3|Q8BIF2;Fam120c|Q8C3F2;Msi2|Q920Q6;Mlf2|Q99KX1;Ddx20|Q9JJY4;Son|Q9QX47</t>
+    <t xml:space="preserve">|Q99MU3;|Q9EST3;|Q920Q6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RVL6;|E9Q8I9;|P14576;|P42669;|P54823;|P57724;|P63154;|Q6ZPY2;|Q80U58;|Q8CAK3;|Q8CH25;|Q99MU3;|Q9DBE9;|Q9EST3;|Q9QZB9;|B2RXC1;|O88809;|P62960;|Q05512;|Q3TIR1;|Q3URQ0;|Q6A0A9;|Q6RI63;|Q80WQ2;|Q8BIF2;|Q8C3F2;|Q920Q6;|Q99KX1;|Q9JJY4;|Q9QX47</t>
   </si>
   <si>
     <t xml:space="preserve">M56</t>
   </si>
   <si>
-    <t xml:space="preserve">Klhl26|Q8BGY4;Tdrd7|Q8K1H1;Ints10|Q8K2A7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otud4|B2RRE7;Tut4|B2RX14;Strn|O55106;Ercc3|P49135;Fam91a1|Q3UVG3;Herc2|Q4U2R1;Rtl6|Q505G4;Lrrk2|Q5S006;Klhl26|Q8BGY4;Wdr59|Q8C0M0;Eloa|Q8CB77;Eif4e|P63073;Tubg1|P83887;Bzw2|Q2L4X1;Tnrc6c|Q3UHC0;Armcx2|Q6A058;Eif4g1|Q6NZJ6;Dhx57|Q6P5D3;Eid2|Q6X7S9;Cpeb4|Q7TN98;Nop53|Q8BK35;Jakmip1|Q8BVL9;Bbs4|Q8C1Z7;Tdrd7|Q8K1H1;Ints10|Q8K2A7;Dock7|Q8R1A4;Smg8|Q8VE18;Nudt16l1|Q8VHN8;Nvl|Q9DBY8</t>
+    <t xml:space="preserve">|Q8BGY4;|Q8K1H1;|Q8K2A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RRE7;|B2RX14;|O55106;|P49135;|Q3UVG3;|Q4U2R1;|Q505G4;|Q5S006;|Q8BGY4;|Q8C0M0;|Q8CB77;|P63073;|P83887;|Q2L4X1;|Q3UHC0;|Q6A058;|Q6NZJ6;|Q6P5D3;|Q6X7S9;|Q7TN98;|Q8BK35;|Q8BVL9;|Q8C1Z7;|Q8K1H1;|Q8K2A7;|Q8R1A4;|Q8VE18;|Q8VHN8;|Q9DBY8</t>
   </si>
   <si>
     <t xml:space="preserve">M57</t>
   </si>
   <si>
-    <t xml:space="preserve">Prkra|Q9WTX2;Ankrd17|Q99NH0;Tpd52l2|Q9CYZ2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usp10|P52479;Rps15a|P62245;Cluh|Q5SW19;Arhgef2|Q60875;Larp4b|Q6A0A2;Ints1|Q6P4S8;Dhx29|Q6PGC1;Dclk2|Q6PGN3;Eif2s1|Q6ZWX6;Atxn2l|Q7TQH0;Znfx1|Q8R151;Eif2s2|Q99L45;Ankrd17|Q99NH0;Srsf9|Q9D0B0;Pak1ip1|Q9DCE5;Prkra|Q9WTX2;Map7d1|A2AJI0;Ythdc2|B2RR83;Atxn2|O70305;Usp39|Q3TIX9;Rbm27|Q5SFM8;Cnot1|Q6ZQ08;Eif4g3|Q80XI3;Coro2b|Q8BH44;Cnot3|Q8K0V4;Luzp1|Q8R4U7;Prpf6|Q91YR7;Tpd52l2|Q9CYZ2</t>
+    <t xml:space="preserve">|Q9WTX2;|Q99NH0;|Q9CYZ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P52479;|P62245;|Q5SW19;|Q60875;|Q6A0A2;|Q6P4S8;|Q6PGC1;|Q6PGN3;|Q6ZWX6;|Q7TQH0;|Q8R151;|Q99L45;|Q99NH0;|Q9D0B0;|Q9DCE5;|Q9WTX2;|A2AJI0;|B2RR83;|O70305;|Q3TIX9;|Q5SFM8;|Q6ZQ08;|Q80XI3;|Q8BH44;|Q8K0V4;|Q8R4U7;|Q91YR7;|Q9CYZ2</t>
   </si>
   <si>
     <t xml:space="preserve">M58</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubgcp5|Q8BKN5;Ncor2|Q9WU42;Mthfd1|Q922D8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las1l|A2BE28;Soga1|E1U8D0;Ascc3|E9PZJ8;Ccnk|O88874;Dnajb5|O89114;Dnmt1|P13864;Ighmbp2|P40694;Prkdc|P97313;Dync2h1|Q45VK7;Tut7|Q5BLK4;Cnot7|Q60809;Rictor|Q6QI06;Scaf4|Q7TSH6;Tubgcp5|Q8BKN5;Gtdc1|Q8BW56;Bbs7|Q8K2G4;Tspyl4|Q8VD63;Mios|Q8VE19;Mthfd1|Q922D8;Bbs5|Q9CZQ9;Nmnat1|Q9EPA7;Dgcr8|Q9EQM6;Mtor|Q9JLN9;Ncor2|Q9WU42;Smarcb1|Q9Z0H3</t>
+    <t xml:space="preserve">|Q8BKN5;|Q9WU42;|Q922D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2BE28;|E1U8D0;|E9PZJ8;|O88874;|O89114;|P13864;|P40694;|P97313;|Q45VK7;|Q5BLK4;|Q60809;|Q6QI06;|Q7TSH6;|Q8BKN5;|Q8BW56;|Q8K2G4;|Q8VD63;|Q8VE19;|Q922D8;|Q9CZQ9;|Q9EPA7;|Q9EQM6;|Q9JLN9;|Q9WU42;|Q9Z0H3</t>
   </si>
   <si>
     <t xml:space="preserve">M59</t>
   </si>
   <si>
-    <t xml:space="preserve">Tfip11|Q9ERA6;Rbfox1|Q9JJ43;Adarb1|Q91ZS8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prrc2c|Q3TLH4;Cdc5l|Q6A068;Prrc2a|Q7TSC1;Adarb1|Q91ZS8;Tfip11|Q9ERA6;Rc3h2|P0C090;U2af2|P26369;Pcbp3|P57722;Prpf4b|Q61136;U2surp|Q6NV83;Snrnp200|Q6P4T2;Prrc2b|Q7TPM1;Pum1|Q80U78;Zfp598|Q80YR4;Smg1|Q8BKX6;Gemin5|Q8BX17;Ago1|Q8CJG1;Trappc12|Q8K2L8;Purg|Q8R4E6;Dhx36|Q8VHK9;Tdrd3|Q91W18;Ddx50|Q99MJ9;Xab2|Q9DCD2;Rbfox1|Q9JJ43;Qk|Q9QYS9</t>
+    <t xml:space="preserve">|Q9ERA6;|Q9JJ43;|Q91ZS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3TLH4;|Q6A068;|Q7TSC1;|Q91ZS8;|Q9ERA6;|P0C090;|P26369;|P57722;|Q61136;|Q6NV83;|Q6P4T2;|Q7TPM1;|Q80U78;|Q80YR4;|Q8BKX6;|Q8BX17;|Q8CJG1;|Q8K2L8;|Q8R4E6;|Q8VHK9;|Q91W18;|Q99MJ9;|Q9DCD2;|Q9JJ43;|Q9QYS9</t>
   </si>
   <si>
     <t xml:space="preserve">M60</t>
   </si>
   <si>
-    <t xml:space="preserve">Smc3|Q9CW03;Prelp|Q9JK53;Numb|Q9QZS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gfod1|Q3UHD2;Stox2|Q499E5;Neurl4|Q5NCX5;Ralgapa1|Q6GYP7;Mapkap1|Q8BKH7;Ints4|Q8CIM8;Actr8|Q8R2S9;Smc1a|Q9CU62;Smc3|Q9CW03;Gfod2|Q9CYH5;Hspa12b|Q9CZJ2;Trim2|Q9ESN6;Prelp|Q9JK53;Zmym3|Q9JLM4;Actr10|Q9QZB7;Numb|Q9QZS3</t>
+    <t xml:space="preserve">|Q9CW03;|Q9JK53;|Q9QZS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3UHD2;|Q499E5;|Q5NCX5;|Q6GYP7;|Q8BKH7;|Q8CIM8;|Q8R2S9;|Q9CU62;|Q9CW03;|Q9CYH5;|Q9CZJ2;|Q9ESN6;|Q9JK53;|Q9JLM4;|Q9QZB7;|Q9QZS3</t>
   </si>
   <si>
     <t xml:space="preserve">M61</t>
   </si>
   <si>
-    <t xml:space="preserve">Wrap53|Q8VC51;Cpeb2|Q812E0;Upf1|Q9EPU0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rbbp6|P97868;Alkbh5|Q3TSG4;Ncbp1|Q3UYV9;Ggnbp2|Q5SV77;Larp1|Q6ZQ58;Cpeb2|Q812E0;Wrap53|Q8VC51;Purb|O35295;Pabpc1|P29341;Eif4g2|Q62448;Rbm26|Q6NZN0;Aqr|Q8CFQ3;Ago2|Q8CJG0;Prpf8|Q99PV0;Upf1|Q9EPU0</t>
+    <t xml:space="preserve">|Q8VC51;|Q812E0;|Q9EPU0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P97868;|Q3TSG4;|Q3UYV9;|Q5SV77;|Q6ZQ58;|Q812E0;|Q8VC51;|O35295;|P29341;|Q62448;|Q6NZN0;|Q8CFQ3;|Q8CJG0;|Q99PV0;|Q9EPU0</t>
   </si>
   <si>
     <t xml:space="preserve">M62</t>
   </si>
   <si>
-    <t xml:space="preserve">Mtmr9|Q9Z2D0;Fig4|Q91WF7;Nat10|Q8K224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tpd52l1|O54818;Irs1|P35569;Tpd52|Q62393;Trim9|Q8C7M3;Nat10|Q8K224;Fig4|Q91WF7;Ybx3|Q9JKB3;Mtmr7|Q9Z2C9;Cdkl5|Q3UTQ8;Gas2l1|Q8JZP9;Mtmr6|Q8VE11;Clvs1|Q9D4C9;Mtmr9|Q9Z2D0</t>
+    <t xml:space="preserve">|Q9Z2D0;|Q91WF7;|Q8K224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54818;|P35569;|Q62393;|Q8C7M3;|Q8K224;|Q91WF7;|Q9JKB3;|Q9Z2C9;|Q3UTQ8;|Q8JZP9;|Q8VE11;|Q9D4C9;|Q9Z2D0</t>
   </si>
   <si>
     <t xml:space="preserve">M63</t>
   </si>
   <si>
-    <t xml:space="preserve">Dhx30|Q99PU8;Top3b|Q9Z321;Tspoap1|Q7TNF8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trrap|Q80YV3;Spats2l|Q91WJ7;Ccdc9b|A3KGF9;Exosc10|P56960;Nol9|Q3TZX8;Tspoap1|Q7TNF8;Trim56|Q80VI1;Parp12|Q8BZ20;Utp15|Q8C7V3;Dhx30|Q99PU8;Senp3|Q9EP97;Top3b|Q9Z321</t>
+    <t xml:space="preserve">|Q99PU8;|Q9Z321;|Q7TNF8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q80YV3;|Q91WJ7;|A3KGF9;|P56960;|Q3TZX8;|Q7TNF8;|Q80VI1;|Q8BZ20;|Q8C7V3;|Q99PU8;|Q9EP97;|Q9Z321</t>
   </si>
   <si>
     <t xml:space="preserve">M64</t>
   </si>
   <si>
-    <t xml:space="preserve">Eefsec|Q9JHW4;Cc2d1a|Q8K1A6;Dclk1|Q9JLM8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rps5|P97461;Rbm15|Q0VBL3;Gprasp1|Q5U4C1;Tpp2|Q64514;Ctif|Q6PEE2;Naa30|Q8CES0;Stau2|Q8CJ67;Cc2d1a|Q8K1A6;Rps19|Q9CZX8;Eefsec|Q9JHW4;Dclk1|Q9JLM8;Myo9a|Q8C170</t>
+    <t xml:space="preserve">|Q9JHW4;|Q8K1A6;|Q9JLM8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P97461;|Q0VBL3;|Q5U4C1;|Q64514;|Q6PEE2;|Q8CES0;|Q8CJ67;|Q8K1A6;|Q9CZX8;|Q9JHW4;|Q9JLM8;|Q8C170</t>
   </si>
   <si>
     <t xml:space="preserve">M65</t>
   </si>
   <si>
-    <t xml:space="preserve">Riox1|Q9JJF3;Rcl1|Q9JJT0;Flywch1|Q8CI03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dnajb6|O54946;Rsl1d1|Q8BVY0;Flywch1|Q8CI03;Riox1|Q9JJF3;Med14|A2ABV5;Rcl1|Q9JJT0</t>
+    <t xml:space="preserve">|Q9JJF3;|Q9JJT0;|Q8CI03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54946;|Q8BVY0;|Q8CI03;|Q9JJF3;|A2ABV5;|Q9JJT0</t>
   </si>
   <si>
     <t xml:space="preserve">M66</t>
   </si>
   <si>
-    <t xml:space="preserve">Alg2|Q9DBE8;Apmap|Q9D7N9;Ergic1|Q9DC16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cx3cr1|Q9Z0D9;Sec22b|O08547;Dnajb14|Q149L6;Cers6|Q8C172;Tmx1|Q8VBT0;Cds2|Q99L43;Cisd2|Q9CQB5;Ergic3|Q9CQE7;Pcyox1|Q9CQF9;Ergic2|Q9CR89;Ergic1|Q9DC16;Porcn|Q9JJJ7;Dnajb12|Q9QYI4;Tmub2|Q3V209;Tmx3|Q8BXZ1;Nipa1|Q8BHK1;Slc29a4|Q8R139;Pigk|Q9CXY9;Gosr2|O35166;Atp2a2|O55143;Stim1|P70302;Cds1|P98191;Sort1|Q6PHU5;Nceh1|Q8BLF1;Scfd1|Q8BRF7;Sec62|Q8BU14;Agpat4|Q8K4X7;Rnf121|Q8R1Z9;Abhd6|Q8R2Y0;Rnf185|Q91YT2;Ghdc|Q99J23;Tmed9|Q99KF1;Vmp1|Q99KU0;Abhd12|Q99LR1;Use1|Q9CQ56;Dhrs7|Q9CXR1;Tmed10|Q9D1D4;Tmem35a|Q9D328;Cers4|Q9D6J1;Apmap|Q9D7N9;Alg2|Q9DBE8;Tmed2|Q9R0Q3</t>
+    <t xml:space="preserve">|Q9DBE8;|Q9D7N9;|Q9DC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9Z0D9;|O08547;|Q149L6;|Q8C172;|Q8VBT0;|Q99L43;|Q9CQB5;|Q9CQE7;|Q9CQF9;|Q9CR89;|Q9DC16;|Q9JJJ7;|Q9QYI4;|Q3V209;|Q8BXZ1;|Q8BHK1;|Q8R139;|Q9CXY9;|O35166;|O55143;|P70302;|P98191;|Q6PHU5;|Q8BLF1;|Q8BRF7;|Q8BU14;|Q8K4X7;|Q8R1Z9;|Q8R2Y0;|Q91YT2;|Q99J23;|Q99KF1;|Q99KU0;|Q99LR1;|Q9CQ56;|Q9CXR1;|Q9D1D4;|Q9D328;|Q9D6J1;|Q9D7N9;|Q9DBE8;|Q9R0Q3</t>
   </si>
   <si>
     <t xml:space="preserve">M67</t>
   </si>
   <si>
-    <t xml:space="preserve">Dolpp1|Q9JMF7;Tmem33|Q9CR67;Sacm1l|Q9EP69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M6pr|P24668;Por|P37040;Cav1|P49817;Nat8l|Q3UGX3;G6pc3|Q6NSQ9;Ankle2|Q6P1H6;Ano8|Q6PB70;Lnpk|Q7TQ95;Them6|Q80ZW2;Cpt1c|Q8BGD5;Scfd2|Q8BTY8;Cnst|Q8CBC4;Wrb|Q8K0D7;Ubac2|Q8R1K1;Cdipt|Q8VDP6;BC017158|Q91W34;Rer1|Q9CQU3;Lman1|Q9D0F3;Sacm1l|Q9EP69;Dolpp1|Q9JMF7;Faah|O08914;Ptpn1|P35821;Dhrs13|Q5SS80;Gramd1b|Q80TI0;Ano10|Q8BH79;Ppm1l|Q8BHN0;Tmem33|Q9CR67;Tmx2|Q9D710;Alg5|Q9DB25</t>
+    <t xml:space="preserve">|Q9JMF7;|Q9CR67;|Q9EP69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P24668;|P37040;|P49817;|Q3UGX3;|Q6NSQ9;|Q6P1H6;|Q6PB70;|Q7TQ95;|Q80ZW2;|Q8BGD5;|Q8BTY8;|Q8CBC4;|Q8K0D7;|Q8R1K1;|Q8VDP6;|Q91W34;|Q9CQU3;|Q9D0F3;|Q9EP69;|Q9JMF7;|O08914;|P35821;|Q5SS80;|Q80TI0;|Q8BH79;|Q8BHN0;|Q9CR67;|Q9D710;|Q9DB25</t>
   </si>
   <si>
     <t xml:space="preserve">M68</t>
   </si>
   <si>
-    <t xml:space="preserve">Vapb|Q9QY76;Ptdss2|Q9Z1X2;Vapa|Q9WV55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inf2|Q0GNC1;Otulinl|Q3TVP5;Bcap31|Q61335;Slc6a15|Q8BG16;Wdr20rt|Q9D5R2;Emd|O08579;Cybc1|Q3TYS2;Cerk|Q8K4Q7;Tapbpl|Q8VD31;Rabl3|Q9D4V7;Aig1|Q9D8B1;Paqr4|Q9JJE4;Vapb|Q9QY76;Vapa|Q9WV55;Ptdss2|Q9Z1X2;Hmox2|O70252;Kdsr|Q6GV12;Tmem56|Q8CGF5;Hacd3|Q8K2C9;Slc33a1|Q99J27;Agpat3|Q9D517</t>
+    <t xml:space="preserve">|Q9QY76;|Q9Z1X2;|Q9WV55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q0GNC1;|Q3TVP5;|Q61335;|Q8BG16;|Q9D5R2;|O08579;|Q3TYS2;|Q8K4Q7;|Q8VD31;|Q9D4V7;|Q9D8B1;|Q9JJE4;|Q9QY76;|Q9WV55;|Q9Z1X2;|O70252;|Q6GV12;|Q8CGF5;|Q8K2C9;|Q99J27;|Q9D517</t>
   </si>
   <si>
     <t xml:space="preserve">M69</t>
   </si>
   <si>
-    <t xml:space="preserve">Dgke|Q9R1C6;Rdh11|Q9QYF1;Acsl4|Q9QUJ7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nacad|Q5SWP3;Rdh11|Q9QYF1;Pgrmc1|O55022;Caml|P49070;Bcap29|Q61334;Surf4|Q64310;Pgrmc2|Q80UU9;Arel1|Q8CHG5;Cyp51|Q8K0C4;Clptm1|Q8VBZ3;Stx18|Q8VDS8;Ctnnbl1|Q9CWL8;Dpm3|Q9D1Q4;Plpp6|Q9D4F2;Lman2|Q9DBH5;Acsl4|Q9QUJ7;Dgke|Q9R1C6;Comt|O88587;Ptpn5|P54830;Ubxn4|Q8VCH8;Kdelr1|Q99JH8</t>
+    <t xml:space="preserve">|Q9R1C6;|Q9QYF1;|Q9QUJ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q5SWP3;|Q9QYF1;|O55022;|P49070;|Q61334;|Q64310;|Q80UU9;|Q8CHG5;|Q8K0C4;|Q8VBZ3;|Q8VDS8;|Q9CWL8;|Q9D1Q4;|Q9D4F2;|Q9DBH5;|Q9QUJ7;|Q9R1C6;|O88587;|P54830;|Q8VCH8;|Q99JH8</t>
   </si>
   <si>
     <t xml:space="preserve">M70</t>
   </si>
   <si>
-    <t xml:space="preserve">Nsdhl|Q9R1J0;Slc39a11|Q8BWY7;Amfr|Q9R049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slc39a11|Q8BWY7;5730455P16Rik|Q9CYI0;Tmem245|B1AZA5;Hsd17b7|O88736;Lmna|P48678;Smpd4|Q6ZPR5;Vma21|Q78T54;Yipf6|Q8BR70;Lmbrd2|Q8C561;Scamp1|Q8K021;Gramd1a|Q8VEF1;Clint1|Q99KN9;Trp53i11|Q4QQM4;Gde1|Q9JL56;Amfr|Q9R049;Nsdhl|Q9R1J0</t>
+    <t xml:space="preserve">|Q9R1J0;|Q8BWY7;|Q9R049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8BWY7;|Q9CYI0;|B1AZA5;|O88736;|P48678;|Q6ZPR5;|Q78T54;|Q8BR70;|Q8C561;|Q8K021;|Q8VEF1;|Q99KN9;|Q4QQM4;|Q9JL56;|Q9R049;|Q9R1J0</t>
   </si>
   <si>
     <t xml:space="preserve">M71</t>
   </si>
   <si>
-    <t xml:space="preserve">Tmem189|Q99LQ7;Vkorc1|Q9CRC0;Sgpp1|Q9JI99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cep350|E9Q309;Zw10|O54692;Sptlc2|P97363;Lpcat1|Q3TFD2;Alg11|Q3TZM9;Nyap1|Q6PFX7;Gpat3|Q8C0N2;Rnf170|Q8CBG9;Tmem63c|Q8CBX0;Stx5a|Q8K1E0;Plpp7|Q91WB2;Tmem189|Q99LQ7;Ubl5|Q9EPV8;Sgpp1|Q9JI99;Clcc1|Q99LI2;Vkorc1|Q9CRC0</t>
+    <t xml:space="preserve">|Q99LQ7;|Q9CRC0;|Q9JI99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9Q309;|O54692;|P97363;|Q3TFD2;|Q3TZM9;|Q6PFX7;|Q8C0N2;|Q8CBG9;|Q8CBX0;|Q8K1E0;|Q91WB2;|Q99LQ7;|Q9EPV8;|Q9JI99;|Q99LI2;|Q9CRC0</t>
   </si>
   <si>
     <t xml:space="preserve">M72</t>
   </si>
   <si>
-    <t xml:space="preserve">Tmem230|Q8CIB6;Tmed5|Q9CXE7;Ric3|Q8BPM6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pomk|Q3TUA9;Hgsnat|Q3UDW8;Cyb5d2|Q5SSH8;March6|Q6ZQ89;Bscl2|Q9Z2E9;Ddrgk1|Q80WW9;Ric3|Q8BPM6;Bet1|O35623;Odr4|Q4PJX1;Slc9a7|Q8BLV3;Tmem230|Q8CIB6;Dolk|Q8R2Y3;Derl1|Q99J56;Tmed5|Q9CXE7;Slc39a7|Q31125</t>
+    <t xml:space="preserve">|Q8CIB6;|Q9CXE7;|Q8BPM6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3TUA9;|Q3UDW8;|Q5SSH8;|Q6ZQ89;|Q9Z2E9;|Q80WW9;|Q8BPM6;|O35623;|Q4PJX1;|Q8BLV3;|Q8CIB6;|Q8R2Y3;|Q99J56;|Q9CXE7;|Q31125</t>
   </si>
   <si>
     <t xml:space="preserve">M73</t>
   </si>
   <si>
-    <t xml:space="preserve">Ufsp2|Q99K23;Cdkal1|Q91WE6;Tmem68|Q9D850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stim2|P83093;Lbr|Q3U9G9;Jagn1|Q5XKN4;Tmem62|Q8BXJ9;Tmed4|Q8R1V4;Dhcr24|Q8VCH6;Cdkal1|Q91WE6;Ufsp2|Q99K23;Tmem68|Q9D850;Tmed3|Q78IS1;Rhbdd2|Q8VEK2;Tor1b|Q9ER41</t>
+    <t xml:space="preserve">|Q99K23;|Q91WE6;|Q9D850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P83093;|Q3U9G9;|Q5XKN4;|Q8BXJ9;|Q8R1V4;|Q8VCH6;|Q91WE6;|Q99K23;|Q9D850;|Q78IS1;|Q8VEK2;|Q9ER41</t>
   </si>
   <si>
     <t xml:space="preserve">M74</t>
   </si>
   <si>
-    <t xml:space="preserve">Ephx1|Q9D379;Macroh2a1|Q9QZQ8;Alg1|Q921Q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alg1|Q921Q3;Macroh2a1|Q9QZQ8;Ryr3|A2AGL3;Ly6c2|P0CW03;Lpcat4|Q6NVG1;Ilvbl|Q8BU33;Tmcc3|Q8R310;Hsd17b12|O70503;Fads6|Q80UG1;Cyp2u1|Q9CX98;Ephx1|Q9D379</t>
+    <t xml:space="preserve">|Q9D379;|Q9QZQ8;|Q921Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q921Q3;|Q9QZQ8;|A2AGL3;|P0CW03;|Q6NVG1;|Q8BU33;|Q8R310;|O70503;|Q80UG1;|Q9CX98;|Q9D379</t>
   </si>
   <si>
     <t xml:space="preserve">M75</t>
   </si>
   <si>
-    <t xml:space="preserve">Atp13a1|Q9EPE9;Gpaa1|Q9WTK3;Acsl3|Q9CZW4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spcs2|Q9CYN2;Dpm1|O70152;Vkorc1l1|Q6TEK5;Pigt|Q8BXQ2;Pcyox1l|Q8C7K6;Creld1|Q91XD7;Mospd2|Q9CWP6;Acsl3|Q9CZW4;Atp13a1|Q9EPE9;Gpaa1|Q9WTK3</t>
+    <t xml:space="preserve">|Q9EPE9;|Q9WTK3;|Q9CZW4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9CYN2;|O70152;|Q6TEK5;|Q8BXQ2;|Q8C7K6;|Q91XD7;|Q9CWP6;|Q9CZW4;|Q9EPE9;|Q9WTK3</t>
   </si>
   <si>
     <t xml:space="preserve">M76</t>
   </si>
   <si>
-    <t xml:space="preserve">Mpdu1|Q9R0Q9;Osbpl5|Q9ER64;Lpgat1|Q91YX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dpagt1|P42867;Ephx4|Q6IE26;Tap1|P21958;Lclat1|Q3UN02;Pla2g7|Q60963;Tmem120a|Q8C1E7;Ndc1|Q8VCB1;Lpgat1|Q91YX5;Osbpl5|Q9ER64;Mpdu1|Q9R0Q9</t>
+    <t xml:space="preserve">|Q9R0Q9;|Q9ER64;|Q91YX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P42867;|Q6IE26;|P21958;|Q3UN02;|Q60963;|Q8C1E7;|Q8VCB1;|Q91YX5;|Q9ER64;|Q9R0Q9</t>
   </si>
   <si>
     <t xml:space="preserve">M77</t>
   </si>
   <si>
-    <t xml:space="preserve">Pigz|Q8BTP0;Nat14|Q8BVG8;Rint1|Q8BZ36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pkd2|O35245;Asna1|O54984;Aup1|P70295;Pnpla6|Q3TRM4;Sidt1|Q6AXF6;Pigz|Q8BTP0;Nat14|Q8BVG8;Rint1|Q8BZ36;Prkch|P23298</t>
+    <t xml:space="preserve">|Q8BTP0;|Q8BVG8;|Q8BZ36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35245;|O54984;|P70295;|Q3TRM4;|Q6AXF6;|Q8BTP0;|Q8BVG8;|Q8BZ36;|P23298</t>
   </si>
   <si>
     <t xml:space="preserve">M78</t>
   </si>
   <si>
-    <t xml:space="preserve">Ank|Q9JHZ2;Tvp23b|Q9D8T4;Gpr108|Q91WD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nbr1|P97432;Gpr108|Q91WD0;Tvp23b|Q9D8T4;Lman2l|P59481;Vps45|P97390;Fam234b|Q8BYI8;Tmx4|Q8C0L0;Ank|Q9JHZ2</t>
+    <t xml:space="preserve">|Q9JHZ2;|Q9D8T4;|Q91WD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P97432;|Q91WD0;|Q9D8T4;|P59481;|P97390;|Q8BYI8;|Q8C0L0;|Q9JHZ2</t>
   </si>
   <si>
     <t xml:space="preserve">M79</t>
   </si>
   <si>
-    <t xml:space="preserve">Selenok|Q9JLJ1;H13|Q9D8V0;Fmnl3|Q6ZPF4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenok|Q9JLJ1;Agpat1|O35083;Fmo5|P97872;Fmnl3|Q6ZPF4;Tmem259|Q8CIV2;Tor1aip1|Q921T2;H13|Q9D8V0</t>
+    <t xml:space="preserve">|Q9JLJ1;|Q9D8V0;|Q6ZPF4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9JLJ1;|O35083;|P97872;|Q6ZPF4;|Q8CIV2;|Q921T2;|Q9D8V0</t>
   </si>
   <si>
     <t xml:space="preserve">M80</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc12a7|Q9WVL3;Tecr|Q9CY27;Jph3|Q9ET77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tmem260|Q8BMD6;Slc12a7|Q9WVL3;Nucb1|Q02819;Mospd1|Q8VEL0;Tecr|Q9CY27;Jph3|Q9ET77</t>
+    <t xml:space="preserve">|Q9WVL3;|Q9CY27;|Q9ET77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8BMD6;|Q9WVL3;|Q02819;|Q8VEL0;|Q9CY27;|Q9ET77</t>
   </si>
   <si>
     <t xml:space="preserve">M81</t>
   </si>
   <si>
-    <t xml:space="preserve">Erp44|Q9D1Q6;Emc7|Q9EP72;Mia2|Q91ZV0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ppib|P24369;Aatk|Q80YE4;Sumf2|Q8BPG6;Poglut3|G5E897;Prkcsh|O08795;Calu|O35887;Ddost|O54734;Emc8|O70378;Itgam|P05555;Serpinh1|P19324;Fkbp2|P45878;Erp29|P57759;Sec61a1|P61620;Dad1|P61804;Anpep|P97449;Rundc1|Q0VDN7;Stt3b|Q3TDQ1;Lmtk3|Q5XJV6;Pon2|Q62086;Uggt1|Q6P5E4;Picalm|Q7M6Y3;Mogs|Q80UM7;Ganab|Q8BHN3;Rcn2|Q8BP92;Tusc3|Q8BTV1;Poglut1|Q8BYB9;Os9|Q8K2C7;Ncln|Q8VCM8;Erlec1|Q8VEH8;Txndc5|Q91W90;Rpn1|Q91YQ5;Mia2|Q91ZV0;Pofut1|Q91ZW2;Lrrc59|Q922Q8;Chid1|Q922Q9;Emc3|Q99KI3;Dnajb11|Q99KV1;Ptdss1|Q99LH2;Sec61b|Q9CQS8;Creld2|Q9CYA0;Ccdc47|Q9D024;Erp44|Q9D1Q6;Rpn2|Q9DBG6;Syvn1|Q9DBY1;Sdf2|Q9DCT5;Emc7|Q9EP72;Ube2j1|Q9JJZ4;Hyou1|Q9JKR6;Sec61a2|Q9JLR1;Pld1|Q9Z280;Minpp1|Q9Z2L6;Erlin2|Q8BFZ9;Emc1|Q8C7X2;Erlin1|Q91X78;Calr|P14211;Pm20d1|Q8C165;Erap1|Q9EQH2</t>
+    <t xml:space="preserve">|Q9D1Q6;|Q9EP72;|Q91ZV0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P24369;|Q80YE4;|Q8BPG6;|G5E897;|O08795;|O35887;|O54734;|O70378;|P05555;|P19324;|P45878;|P57759;|P61620;|P61804;|P97449;|Q0VDN7;|Q3TDQ1;|Q5XJV6;|Q62086;|Q6P5E4;|Q7M6Y3;|Q80UM7;|Q8BHN3;|Q8BP92;|Q8BTV1;|Q8BYB9;|Q8K2C7;|Q8VCM8;|Q8VEH8;|Q91W90;|Q91YQ5;|Q91ZV0;|Q91ZW2;|Q922Q8;|Q922Q9;|Q99KI3;|Q99KV1;|Q99LH2;|Q9CQS8;|Q9CYA0;|Q9D024;|Q9D1Q6;|Q9DBG6;|Q9DBY1;|Q9DCT5;|Q9EP72;|Q9JJZ4;|Q9JKR6;|Q9JLR1;|Q9Z280;|Q9Z2L6;|Q8BFZ9;|Q8C7X2;|Q91X78;|P14211;|Q8C165;|Q9EQH2</t>
   </si>
   <si>
     <t xml:space="preserve">M82</t>
   </si>
   <si>
-    <t xml:space="preserve">Pex3|Q9QXY9;Plod3|Q9R0E1;Ogfod3|Q9D136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sema5a|Q62217;Tgoln1|Q62313;Ctso|Q8BM88;Gpr107|Q8BUV8;Ssr3|Q9DCF9;Lrp6|O88572;Entpd1|P55772;Rbp4|Q00724;Edem3|Q2HXL6;Slc22a15|Q504N2;Lrrn1|Q61809;Tmem87a|Q8BXN9;Sidt2|Q8CIF6;Herpud2|Q9JJC9;Acp2|P24638;Alg10b|Q3UGP8;Endou|Q3V188;Myof|Q69ZN7;Fut11|Q8BHC9;AU040320|Q8K135;Abca9|Q8K449;Sumf1|Q8R0F3;Pex6|Q99LC9;Cdk5rap3|Q99LM2;Ssr1|Q9CY50;Ogfod3|Q9D136;Cnpy2|Q9QXT0;Pex3|Q9QXY9;Plod3|Q9R0E1;Spcs3|Q6ZWQ7</t>
+    <t xml:space="preserve">|Q9QXY9;|Q9R0E1;|Q9D136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q62217;|Q62313;|Q8BM88;|Q8BUV8;|Q9DCF9;|O88572;|P55772;|Q00724;|Q2HXL6;|Q504N2;|Q61809;|Q8BXN9;|Q8CIF6;|Q9JJC9;|P24638;|Q3UGP8;|Q3V188;|Q69ZN7;|Q8BHC9;|Q8K135;|Q8K449;|Q8R0F3;|Q99LC9;|Q99LM2;|Q9CY50;|Q9D136;|Q9QXT0;|Q9QXY9;|Q9R0E1;|Q6ZWQ7</t>
   </si>
   <si>
     <t xml:space="preserve">M83</t>
   </si>
   <si>
-    <t xml:space="preserve">Rgs10|Q9CQE5;Itpr2|Q9Z329;Sel1l|Q9Z2G6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplp1|Q03157;Sec63|Q8VHE0;Sel1l|Q9Z2G6;P4hb|P09103;Itgb2|P11835;Icam1|P13597;Pdia3|P27773;Stt3a|P46978;Lrpap1|P55302;Stmn4|P63042;Nomo1|Q6GQT9;Hspa13|Q8BM72;Eogt|Q8BYW9;Dnajc3|Q91YW3;Pdia6|Q922R8;Sar1b|Q9CQC9;Rgs10|Q9CQE5;Clstn1|Q9EPL2;Clstn2|Q9ER65;Selenof|Q9ERR7;Plek|Q9JHK5;Manf|Q9CXI5;Pdia4|P08003;Hspa5|P20029;Itpr2|Q9Z329</t>
+    <t xml:space="preserve">|Q9CQE5;|Q9Z329;|Q9Z2G6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q03157;|Q8VHE0;|Q9Z2G6;|P09103;|P11835;|P13597;|P27773;|P46978;|P55302;|P63042;|Q6GQT9;|Q8BM72;|Q8BYW9;|Q91YW3;|Q922R8;|Q9CQC9;|Q9CQE5;|Q9EPL2;|Q9ER65;|Q9ERR7;|Q9JHK5;|Q9CXI5;|P08003;|P20029;|Q9Z329</t>
   </si>
   <si>
     <t xml:space="preserve">M84</t>
   </si>
   <si>
-    <t xml:space="preserve">Emc4|Q9CZX9;Pex26|Q8BGI5;Bri3bp|Q8BXV2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugt8a|Q64676;Bri3bp|Q8BXV2;P2ry12|Q9CPV9;Tmem131|O70472;Dpep1|P31428;Aplp2|Q06335;D130043K22Rik|Q5SZV5;Mlec|Q6ZQI3;P4htm|Q8BG58;Pex26|Q8BGI5;Tmtc3|Q8BRH0;St7|Q99M96;Emc4|Q9CZX9;Sts|P50427;Selenot|P62342;Cept1|Q8BGS7;Pomgnt2|Q8BW41;St3gal5|O88829</t>
+    <t xml:space="preserve">|Q9CZX9;|Q8BGI5;|Q8BXV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q64676;|Q8BXV2;|Q9CPV9;|O70472;|P31428;|Q06335;|Q5SZV5;|Q6ZQI3;|Q8BG58;|Q8BGI5;|Q8BRH0;|Q99M96;|Q9CZX9;|P50427;|P62342;|Q8BGS7;|Q8BW41;|O88829</t>
   </si>
   <si>
     <t xml:space="preserve">M85</t>
   </si>
   <si>
-    <t xml:space="preserve">Nmnat2|Q8BNJ3;Abca5|Q8K448;Lrp1|Q91ZX7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lrp1|Q91ZX7;Vti1b|O88384;Atp8a2|P98200;Lmtk2|Q3TYD6;Sdf4|Q61112;Clcn4|Q61418;Mon1a|Q6PDG8;Nmnat2|Q8BNJ3;Itfg1|Q99KW9;Arl8b|Q9CQW2;Rundc3a|O08576;Rab11b|P46638;Pcsk1|P63239;Abca5|Q8K448;Stx7|O70439;Stx8|O88983;Tfrc|Q62351</t>
+    <t xml:space="preserve">|Q8BNJ3;|Q8K448;|Q91ZX7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q91ZX7;|O88384;|P98200;|Q3TYD6;|Q61112;|Q61418;|Q6PDG8;|Q8BNJ3;|Q99KW9;|Q9CQW2;|O08576;|P46638;|P63239;|Q8K448;|O70439;|O88983;|Q62351</t>
   </si>
   <si>
     <t xml:space="preserve">M86</t>
   </si>
   <si>
-    <t xml:space="preserve">Rrbp1|Q99PL5;Acbd3|Q8BMP6;Colgalt1|Q8K297</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptgds|O09114;Anxa2|P07356;Lamb1|P02469;Pex1|Q5BL07;P4ha1|Q60715;Cp|Q61147;Slc26a2|Q62273;Colgalt1|Q8K297;App|P12023;Synrg|Q5SV85;Ktn1|Q61595;Acbd3|Q8BMP6;Rrbp1|Q99PL5;Tbl2|Q9R099;Decr2|Q9WV68;Pex11b|Q9Z210</t>
+    <t xml:space="preserve">|Q99PL5;|Q8BMP6;|Q8K297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09114;|P07356;|P02469;|Q5BL07;|Q60715;|Q61147;|Q62273;|Q8K297;|P12023;|Q5SV85;|Q61595;|Q8BMP6;|Q99PL5;|Q9R099;|Q9WV68;|Q9Z210</t>
   </si>
   <si>
     <t xml:space="preserve">M87</t>
   </si>
   <si>
-    <t xml:space="preserve">Dnajc18|Q9CZJ9;Alg9|Q8VDI9;Mydgf|Q9CPT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dgat1|Q9Z2A7;Dpy19l1|A6X919;Ube4a|E9Q735;Sorl1|O88307;Alpl|P09242;Pigs|Q6PD26;Pomt2|Q8BGQ4;Cnpy4|Q8BQ47;Alg9|Q8VDI9;Mydgf|Q9CPT4;Nenf|Q9CQ45;Dnajc18|Q9CZJ9;Hmgcr|Q01237</t>
+    <t xml:space="preserve">|Q9CZJ9;|Q8VDI9;|Q9CPT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9Z2A7;|A6X919;|E9Q735;|O88307;|P09242;|Q6PD26;|Q8BGQ4;|Q8BQ47;|Q8VDI9;|Q9CPT4;|Q9CQ45;|Q9CZJ9;|Q01237</t>
   </si>
   <si>
     <t xml:space="preserve">M88</t>
   </si>
   <si>
-    <t xml:space="preserve">Lamtor5|Q9D1L9;Lrp8|Q924X6;Megf9|Q8BH27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2m|P01887;Podxl2|Q8CAE9;Ptprc|P06800;Scg3|P47867;Tmem38a|Q3TMP8;Atraid|Q6PGD0;Megf9|Q8BH27;Lmbrd1|Q8K0B2;Lrp8|Q924X6;Tmem147|Q9CQG6;Lamtor5|Q9D1L9;Spock2|Q9ER58;Triqk|B2B9E1</t>
+    <t xml:space="preserve">|Q9D1L9;|Q924X6;|Q8BH27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P01887;|Q8CAE9;|P06800;|P47867;|Q3TMP8;|Q6PGD0;|Q8BH27;|Q8K0B2;|Q924X6;|Q9CQG6;|Q9D1L9;|Q9ER58;|B2B9E1</t>
   </si>
   <si>
     <t xml:space="preserve">M89</t>
   </si>
   <si>
-    <t xml:space="preserve">Dnajc10|Q9DC23;Far1|Q922J9;Entpd5|Q9WUZ9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stam2|O88811;Folr1|P35846;Far1|Q922J9;Pakap|O54931;Mtdh|Q80WJ7;Ckap4|Q8BMK4;Agps|Q8C0I1;Tmco1|Q921L3;Dnajc10|Q9DC23;Entpd5|Q9WUZ9</t>
+    <t xml:space="preserve">|Q9DC23;|Q922J9;|Q9WUZ9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88811;|P35846;|Q922J9;|O54931;|Q80WJ7;|Q8BMK4;|Q8C0I1;|Q921L3;|Q9DC23;|Q9WUZ9</t>
   </si>
   <si>
     <t xml:space="preserve">M90</t>
   </si>
   <si>
-    <t xml:space="preserve">Pex13|Q9D0K1;Ccdc134|Q8C7V8;Ssr4|Q62186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tmtc1|Q3UV71;Ssr4|Q62186;Tgfb2|P27090;Txndc11|Q8K2W3;Sil1|Q9EPK6;Nt5e|Q61503;Ccdc134|Q8C7V8;Pex13|Q9D0K1</t>
+    <t xml:space="preserve">|Q9D0K1;|Q8C7V8;|Q62186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3UV71;|Q62186;|P27090;|Q8K2W3;|Q9EPK6;|Q61503;|Q8C7V8;|Q9D0K1</t>
   </si>
   <si>
     <t xml:space="preserve">M91</t>
   </si>
   <si>
-    <t xml:space="preserve">Txndc12|Q9CQU0;Asph|Q8BSY0;Hs6st2|Q80UW0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golph3|Q9CRA5;Tmem109|Q3UBX0;Mrc2|Q64449;Chpf|Q6IQX7;Hs6st2|Q80UW0;Asph|Q8BSY0;Txndc12|Q9CQU0</t>
+    <t xml:space="preserve">|Q9CQU0;|Q8BSY0;|Q80UW0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9CRA5;|Q3UBX0;|Q64449;|Q6IQX7;|Q80UW0;|Q8BSY0;|Q9CQU0</t>
   </si>
   <si>
     <t xml:space="preserve">M92</t>
   </si>
   <si>
-    <t xml:space="preserve">Txnrd1|Q9JMH6;Acss2|Q9QXG4;Arih1|Q9Z1K5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pgk1|P09411;Eno3|P21550;Brcc3|P46737;Uros|P51163;Ran|P62827;Babam1|Q3UI43;Xpo1|Q6P5F9;Nars|Q8BP47;Usp47|Q8BY87;Uba6|Q8C7R4;Babam2|Q8K3W0;Gspt1|Q8R050;Usp15|Q8R5H1;Acot7|Q91V12;Tubb6|Q922F4;Ppp6c|Q9CQR6;Ppid|Q9CR16;Nsfl1c|Q9CZ44;Cse1l|Q9ERK4;Isyna1|Q9JHU9;Txnrd1|Q9JMH6;Acss2|Q9QXG4;Arih1|Q9Z1K5</t>
+    <t xml:space="preserve">|Q9JMH6;|Q9QXG4;|Q9Z1K5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P09411;|P21550;|P46737;|P51163;|P62827;|Q3UI43;|Q6P5F9;|Q8BP47;|Q8BY87;|Q8C7R4;|Q8K3W0;|Q8R050;|Q8R5H1;|Q91V12;|Q922F4;|Q9CQR6;|Q9CR16;|Q9CZ44;|Q9ERK4;|Q9JHU9;|Q9JMH6;|Q9QXG4;|Q9Z1K5</t>
   </si>
   <si>
     <t xml:space="preserve">M93</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubqln2|Q9QZM0;St13|Q99L47;Nudt5|Q9JKX6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ppip5k1|A2ARP1;Capn1|O35350;Hsp90aa1|P07901;Umps|P13439;Stat3|P42227;Pepd|Q11136;Gmps|Q3THK7;Grb2|Q60631;Asns|Q61024;Igbp1|Q61249;Ube2r2|Q6ZWZ2;Ahsa1|Q8BK64;Tcp11l1|Q8BTG3;Gpcpd1|Q8C0L9;Fam160b1|Q8CDM8;Setd7|Q8VHL1;Irgq|Q8VIM9;Usp11|Q99K46;St13|Q99L47;Myg1|Q9JK81;Nudt5|Q9JKX6;Ubqln2|Q9QZM0</t>
+    <t xml:space="preserve">|Q9QZM0;|Q99L47;|Q9JKX6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2ARP1;|O35350;|P07901;|P13439;|P42227;|Q11136;|Q3THK7;|Q60631;|Q61024;|Q61249;|Q6ZWZ2;|Q8BK64;|Q8BTG3;|Q8C0L9;|Q8CDM8;|Q8VHL1;|Q8VIM9;|Q99K46;|Q99L47;|Q9JK81;|Q9JKX6;|Q9QZM0</t>
   </si>
   <si>
     <t xml:space="preserve">M94</t>
   </si>
   <si>
-    <t xml:space="preserve">Ppa1|Q9D819;Ptges3|Q9R0Q7;Chordc1|Q9D1P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ttc38|A3KMP2;Gclm|O09172;Hsp90ab1|P11499;Fkbp4|P30416;Ube2d3|P61079;Ube2k|P61087;Hspa8|P63017;Pde1b|Q01065;Cab39|Q06138;Stip1|Q60864;Oxsr1|Q6P9R2;Pgm1|Q7TSV4;Nae1|Q8VBW6;Abhd14b|Q8VCR7;Blvrb|Q923D2;Glrx3|Q9CQM9;Blvra|Q9CY64;Chordc1|Q9D1P4;Ppa1|Q9D819;Crot|Q9DC50;Ptges3|Q9R0Q7</t>
+    <t xml:space="preserve">|Q9D819;|Q9R0Q7;|Q9D1P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A3KMP2;|O09172;|P11499;|P30416;|P61079;|P61087;|P63017;|Q01065;|Q06138;|Q60864;|Q6P9R2;|Q7TSV4;|Q8VBW6;|Q8VCR7;|Q923D2;|Q9CQM9;|Q9CY64;|Q9D1P4;|Q9D819;|Q9DC50;|Q9R0Q7</t>
   </si>
   <si>
     <t xml:space="preserve">M95</t>
   </si>
   <si>
-    <t xml:space="preserve">Chmp5|Q9D7S9;Ttc1|Q91Z38;Rufy3|Q9D394</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aip|O08915;Nudc|O35685;Adprh|P54923;Arf4|P61750;Cdc37|Q61081;Zpr1|Q62384;Thop1|Q8C1A5;Tbcel|Q8C5W3;Hmgcs1|Q8JZK9;Nudcd3|Q8R1N4;Tbcc|Q8VCN9;Ciapin1|Q8WTY4;Ttc1|Q91Z38;Taldo1|Q93092;Adi1|Q99JT9;Txndc17|Q9CQM5;Coro7|Q9D2V7;Rufy3|Q9D394;Chmp5|Q9D7S9</t>
+    <t xml:space="preserve">|Q9D7S9;|Q91Z38;|Q9D394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08915;|O35685;|P54923;|P61750;|Q61081;|Q62384;|Q8C1A5;|Q8C5W3;|Q8JZK9;|Q8R1N4;|Q8VCN9;|Q8WTY4;|Q91Z38;|Q93092;|Q99JT9;|Q9CQM5;|Q9D2V7;|Q9D394;|Q9D7S9</t>
   </si>
   <si>
     <t xml:space="preserve">M96</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubb3|Q9ERD7;Scrn1|Q9CZC8;Ggct|Q9D7X8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capn2|O08529;Ldhb|P16125;Akt1|P31750;Nat2|P50295;Acyp2|P56375;Tuba1c|P68373;G6pdx|Q00612;Stk38l|Q7TSE6;Enoph1|Q8BGB7;Aars|Q8BGQ7;Czib|Q8BHG2;Uba3|Q8C878;Appl1|Q8K3H0;Cryl1|Q99KP3;Mtap|Q9CQ65;Scrn1|Q9CZC8;Tbcb|Q9D1E6;Ggct|Q9D7X8;Tubb3|Q9ERD7</t>
+    <t xml:space="preserve">|Q9ERD7;|Q9CZC8;|Q9D7X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08529;|P16125;|P31750;|P50295;|P56375;|P68373;|Q00612;|Q7TSE6;|Q8BGB7;|Q8BGQ7;|Q8BHG2;|Q8C878;|Q8K3H0;|Q99KP3;|Q9CQ65;|Q9CZC8;|Q9D1E6;|Q9D7X8;|Q9ERD7</t>
   </si>
   <si>
     <t xml:space="preserve">M97</t>
   </si>
   <si>
-    <t xml:space="preserve">Akap12|Q9WTQ5;Arl3|Q9WUL7;Tbc1d17|Q8BYH7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camk4|P08414;Limk1|P53668;Faf1|P54731;Fgf1|P61148;Sms|P97355;Calb2|Q08331;Fchsd2|Q3USJ8;Fnta|Q61239;N6amt1|Q6SKR2;Sgta|Q8BJU0;Tbc1d17|Q8BYH7;Brox|Q8K2Q7;Pbdc1|Q9D0B6;Mdp1|Q9D967;Haghl|Q9DB32;Akap12|Q9WTQ5;Arl3|Q9WUL7</t>
+    <t xml:space="preserve">|Q9WTQ5;|Q9WUL7;|Q8BYH7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P08414;|P53668;|P54731;|P61148;|P97355;|Q08331;|Q3USJ8;|Q61239;|Q6SKR2;|Q8BJU0;|Q8BYH7;|Q8K2Q7;|Q9D0B6;|Q9D967;|Q9DB32;|Q9WTQ5;|Q9WUL7</t>
   </si>
   <si>
     <t xml:space="preserve">M98</t>
   </si>
   <si>
-    <t xml:space="preserve">Psat1|Q99K85;Tubb4a|Q9D6F9;Sugt1|Q9CX34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bpgm|P15327;Gstp1|P19157;Pvalb|P32848;Prdx1|P35700;Nedd4|P46935;Cdk5|P49615;Gss|P51855;Phgdh|Q61753;Nqo1|Q64669;Ptpdc1|Q6NZK8;Kif1bp|Q6ZPU9;Flnb|Q80X90;Ppp1r11|Q8K1L5;Nans|Q99J77;Psat1|Q99K85;Sugt1|Q9CX34;Tubb4a|Q9D6F9</t>
+    <t xml:space="preserve">|Q99K85;|Q9D6F9;|Q9CX34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P15327;|P19157;|P32848;|P35700;|P46935;|P49615;|P51855;|Q61753;|Q64669;|Q6NZK8;|Q6ZPU9;|Q80X90;|Q8K1L5;|Q99J77;|Q99K85;|Q9CX34;|Q9D6F9</t>
   </si>
   <si>
     <t xml:space="preserve">M99</t>
   </si>
   <si>
-    <t xml:space="preserve">Camkk1|Q8VBY2;Uap1|Q91YN5;Xpot|Q9CRT8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gapdh|P16858;Tkt|P40142;Ahcy|P50247;Mat2a|Q3THS6;Ppp5c|Q60676;Sord|Q64442;Dpp8|Q80YA7;8030462N17Rik|Q8BH50;Kyat1|Q8BTY1;Phyhip|Q8K0S0;Camkk1|Q8VBY2;Isoc1|Q91V64;Uap1|Q91YN5;Xpot|Q9CRT8;Pycrl|Q9DCC4</t>
+    <t xml:space="preserve">|Q8VBY2;|Q91YN5;|Q9CRT8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P16858;|P40142;|P50247;|Q3THS6;|Q60676;|Q64442;|Q80YA7;|Q8BH50;|Q8BTY1;|Q8K0S0;|Q8VBY2;|Q91V64;|Q91YN5;|Q9CRT8;|Q9DCC4</t>
   </si>
   <si>
     <t xml:space="preserve">M100</t>
   </si>
   <si>
-    <t xml:space="preserve">Nqo2|Q9JI75;Chm|Q9QXG2;Uba5|Q8VE47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ppm1b|P36993;Map2k2|Q63932;D3Ertd751e|Q8BGN2;Tbce|Q8CIV8;Ubqln1|Q8R317;Uba5|Q8VE47;Lactb2|Q99KR3;Psph|Q99LS3;Nqo2|Q9JI75;Chm|Q9QXG2</t>
+    <t xml:space="preserve">|Q9JI75;|Q9QXG2;|Q8VE47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P36993;|Q63932;|Q8BGN2;|Q8CIV8;|Q8R317;|Q8VE47;|Q99KR3;|Q99LS3;|Q9JI75;|Q9QXG2</t>
   </si>
   <si>
     <t xml:space="preserve">M101</t>
   </si>
   <si>
-    <t xml:space="preserve">U2af1|Q9D883;Zfp346|Q9R0B7;Ilf3|Q9Z1X4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptbp1|P17225;Tia1|P52912;Tial1|P70318;Khsrp|Q3U0V1;Smu1|Q3UKJ7;Ddx17|Q501J6;Pcbp2|Q61990;Sf1|Q64213;Snrnp40|Q6PE01;Rbm15b|Q6PHZ5;Sympk|Q80X82;Rnf41|Q8BH75;Cpsf7|Q8BTV2;Rbms3|Q8BWL5;Lsm14b|Q8CGC4;Tcerg1|Q8CGF7;Cherp|Q8CGZ0;Sugp2|Q8CH09;Rbm17|Q8JZX4;Lsm14a|Q8K2F8;Sf3b4|Q8QZY9;Fubp1|Q91WJ8;Strbp|Q91WM1;Plrg1|Q922V4;Prpf19|Q99KP6;Snrpb2|Q9CQI7;Hnrnpa0|Q9CX86;Ilf2|Q9CXY6;Fip1l1|Q9D824;U2af1|Q9D883;Dazap1|Q9JII5;Alyref2|Q9JJW6;Mbnl1|Q9JKP5;Zfp346|Q9R0B7;Hnrnpdl|Q9Z130;Ilf3|Q9Z1X4</t>
+    <t xml:space="preserve">|Q9D883;|Q9R0B7;|Q9Z1X4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P17225;|P52912;|P70318;|Q3U0V1;|Q3UKJ7;|Q501J6;|Q61990;|Q64213;|Q6PE01;|Q6PHZ5;|Q80X82;|Q8BH75;|Q8BTV2;|Q8BWL5;|Q8CGC4;|Q8CGF7;|Q8CGZ0;|Q8CH09;|Q8JZX4;|Q8K2F8;|Q8QZY9;|Q91WJ8;|Q91WM1;|Q922V4;|Q99KP6;|Q9CQI7;|Q9CX86;|Q9CXY6;|Q9D824;|Q9D883;|Q9JII5;|Q9JJW6;|Q9JKP5;|Q9R0B7;|Q9Z130;|Q9Z1X4</t>
   </si>
   <si>
     <t xml:space="preserve">M102</t>
   </si>
   <si>
-    <t xml:space="preserve">Ddx39b|Q9Z1N5;Trappc6b|Q9D289;Acin1|Q9JIX8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alyref|O08583;Pnn|O35691;Api5|O35841;Sap18|O55128;Zfp326|O88291;Elavl1|P70372;Pnkd|Q69ZP3;Sec23ip|Q6NZC7;Pabpn1|Q8CCS6;AI597479|Q922M7;Magohb|Q9CQL1;Raver1|Q9CW46;Dcp2|Q9CYC6;Sarnp|Q9D1J3;Trappc6b|Q9D289;Trappc4|Q9ES56;Acin1|Q9JIX8;Celf2|Q9Z0H4;Ddx39b|Q9Z1N5;Trappc10|Q3TLI0;Edc4|Q3UJB9;Sec31a|Q3UPL0;Thoc6|Q5U4D9;Zc3h11a|Q6NZF1;Poldip3|Q8BG81;Zc3h14|Q8BJ05;Thoc5|Q8BKT7;Edc3|Q8K2D3;Ddx39|Q8VDW0;Eif4a3|Q91VC3;Dcp1a|Q91YD3;Rbm8a|Q9CWZ3</t>
+    <t xml:space="preserve">|Q9Z1N5;|Q9D289;|Q9JIX8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08583;|O35691;|O35841;|O55128;|O88291;|P70372;|Q69ZP3;|Q6NZC7;|Q8CCS6;|Q922M7;|Q9CQL1;|Q9CW46;|Q9CYC6;|Q9D1J3;|Q9D289;|Q9ES56;|Q9JIX8;|Q9Z0H4;|Q9Z1N5;|Q3TLI0;|Q3UJB9;|Q3UPL0;|Q5U4D9;|Q6NZF1;|Q8BG81;|Q8BJ05;|Q8BKT7;|Q8K2D3;|Q8VDW0;|Q91VC3;|Q91YD3;|Q9CWZ3</t>
   </si>
   <si>
     <t xml:space="preserve">M103</t>
   </si>
   <si>
-    <t xml:space="preserve">Sf3b1|Q99NB9;Lsm4|Q9QXA5;Sf3b3|Q921M3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eftud2|O08810;Hnrnph1|O35737;Lsm2|O35900;Snrpb|P27048;Snrpa1|P57784;Sf3b6|P59708;Snrpf|P62307;Snrpg|P62309;Lsm6|P62313;Snrpd2|P62317;Snrpd3|P62320;Tra2b|P62996;Hnrnph2|P70333;Phf5a|P83870;Puf60|Q3UEB3;Tra2a|Q6PFR5;Smndc1|Q8BGT7;Hook3|Q8BUK6;Srek1|Q8BZX4;Hnrnpu|Q8VEK3;Hnrnpll|Q921F4;Sf3b3|Q921M3;Hnrnpab|Q99020;Sf3b1|Q99NB9;Ncbp2|Q9CQ49;Trir|Q9D735;Lsm4|Q9QXA5;Srsf10|Q9R0U0</t>
+    <t xml:space="preserve">|Q99NB9;|Q9QXA5;|Q921M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08810;|O35737;|O35900;|P27048;|P57784;|P59708;|P62307;|P62309;|P62313;|P62317;|P62320;|P62996;|P70333;|P83870;|Q3UEB3;|Q6PFR5;|Q8BGT7;|Q8BUK6;|Q8BZX4;|Q8VEK3;|Q921F4;|Q921M3;|Q99020;|Q99NB9;|Q9CQ49;|Q9D735;|Q9QXA5;|Q9R0U0</t>
   </si>
   <si>
     <t xml:space="preserve">M104</t>
   </si>
   <si>
-    <t xml:space="preserve">Fxr2|Q9WVR4;Nova1|Q9JKN6;Ccar1|Q8CH18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cobl|Q5NBX1;Celf6|Q7TN33;Ik|Q9Z1M8;Thoc2|B1AZI6;Celf1|P28659;Apoc3|P33622;Fmr1|P35922;Smn1|P97801;Tnrc6a|Q3UHK8;Trappc1|Q5NCF2;Elavl2|Q60899;Elavl3|Q60900;Fxr1|Q61584;Elavl4|Q61701;Bud31|Q6PGH1;Syncrip|Q7TMK9;Ccar1|Q8CH18;Cstf3|Q99LI7;Trappc5|Q9CQA1;Gemin6|Q9CX53;Nova1|Q9JKN6;Fxr2|Q9WVR4</t>
+    <t xml:space="preserve">|Q9WVR4;|Q9JKN6;|Q8CH18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q5NBX1;|Q7TN33;|Q9Z1M8;|B1AZI6;|P28659;|P33622;|P35922;|P97801;|Q3UHK8;|Q5NCF2;|Q60899;|Q60900;|Q61584;|Q61701;|Q6PGH1;|Q7TMK9;|Q8CH18;|Q99LI7;|Q9CQA1;|Q9CX53;|Q9JKN6;|Q9WVR4</t>
   </si>
   <si>
     <t xml:space="preserve">M105</t>
   </si>
   <si>
-    <t xml:space="preserve">Snw1|Q9CSN1;Rbmx|Q9WV02;Cpsf1|Q9EPU4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safb|D3YXK2;Dhx9|O70133;Zfr|O88532;Hnrnpa2b1|O88569;Hnrnpa1|P49312;Hnrnpul2|Q00PI9;Khdrbs1|Q60749;Hnrnpa3|Q8BG05;Rbm14|Q8C2Q3;Heatr5b|Q8C547;Matr3|Q8K310;Pspc1|Q8R326;Sfpq|Q8VIJ6;Ptbp2|Q91Z31;Tardbp|Q921F2;Nono|Q99K48;Snw1|Q9CSN1;Cpsf1|Q9EPU4;Rbmx|Q9WV02</t>
+    <t xml:space="preserve">|Q9CSN1;|Q9WV02;|Q9EPU4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|D3YXK2;|O70133;|O88532;|O88569;|P49312;|Q00PI9;|Q60749;|Q8BG05;|Q8C2Q3;|Q8C547;|Q8K310;|Q8R326;|Q8VIJ6;|Q91Z31;|Q921F2;|Q99K48;|Q9CSN1;|Q9EPU4;|Q9WV02</t>
   </si>
   <si>
     <t xml:space="preserve">M106</t>
   </si>
   <si>
-    <t xml:space="preserve">Rsrc1|Q9DBU6;Ylpm1|Q9R0I7;Nudt21|Q9CQF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hnrnpk|P61979;Erh|P84089;Map9|Q3TRR0;Hnrnpd|Q60668;Sf3a2|Q62203;Cpeb3|Q7TN99;Dzank1|Q8C008;Sf3a1|Q8K4Z5;Ccsap|Q8QZT2;Wbp11|Q923D5;Rbm10|Q99KG3;Nudt21|Q9CQF3;Lsm7|Q9CQQ8;Bcas2|Q9D287;Sf3a3|Q9D554;Rsrc1|Q9DBU6;Ylpm1|Q9R0I7</t>
+    <t xml:space="preserve">|Q9DBU6;|Q9R0I7;|Q9CQF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P61979;|P84089;|Q3TRR0;|Q60668;|Q62203;|Q7TN99;|Q8C008;|Q8K4Z5;|Q8QZT2;|Q923D5;|Q99KG3;|Q9CQF3;|Q9CQQ8;|Q9D287;|Q9D554;|Q9DBU6;|Q9R0I7</t>
   </si>
   <si>
     <t xml:space="preserve">M107</t>
   </si>
   <si>
-    <t xml:space="preserve">Rtca|Q9D7H3;Rps9|Q6ZWN5;Keap1|Q9Z2X8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rps16|P14131;Rps2|P25444;Pcbp1|P60335;Smg6|P61406;Rps4x|P62702;Zswim8|Q3UHH1;Tiam1|Q60610;Rps9|Q6ZWN5;Celf4|Q7TSY6;Rnf214|Q8BFU3;Itfg2|Q91WI7;Abcf2|Q99LE6;Rtca|Q9D7H3;Keap1|Q9Z2X8</t>
+    <t xml:space="preserve">|Q9D7H3;|Q6ZWN5;|Q9Z2X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P14131;|P25444;|P60335;|P61406;|P62702;|Q3UHH1;|Q60610;|Q6ZWN5;|Q7TSY6;|Q8BFU3;|Q91WI7;|Q99LE6;|Q9D7H3;|Q9Z2X8</t>
   </si>
   <si>
     <t xml:space="preserve">M108</t>
   </si>
   <si>
-    <t xml:space="preserve">Rnps1|Q99M28;Ppp1r8|Q8R3G1;Ppil1|Q9D0W5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mknk1|O08605;Zc3h18|Q0P678;Smg7|Q5RJH6;Rbm22|Q8BHS3;Ppp1r8|Q8R3G1;Rnps1|Q99M28;Ppil1|Q9D0W5;Sec13|Q9D1M0;Cep131|Q62036</t>
+    <t xml:space="preserve">|Q99M28;|Q8R3G1;|Q9D0W5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08605;|Q0P678;|Q5RJH6;|Q8BHS3;|Q8R3G1;|Q99M28;|Q9D0W5;|Q9D1M0;|Q62036</t>
   </si>
   <si>
     <t xml:space="preserve">M109</t>
   </si>
   <si>
-    <t xml:space="preserve">Tpgs1|Q99MS8;Cstf1|Q99LC2;Thoc1|Q8R3N6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cstf1|Q99LC2;Mfap1b|C0HKD9;Thoc7|Q7TMY4;Ppwd1|Q8CEC6;Thoc1|Q8R3N6;Ssx2ip|Q8VC66;Tpgs1|Q99MS8</t>
+    <t xml:space="preserve">|Q99MS8;|Q99LC2;|Q8R3N6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q99LC2;|C0HKD9;|Q7TMY4;|Q8CEC6;|Q8R3N6;|Q8VC66;|Q99MS8</t>
   </si>
   <si>
     <t xml:space="preserve">M110</t>
   </si>
   <si>
-    <t xml:space="preserve">Extl3|Q9WVL6;Rab5a|Q9CQD1;Gabbr1|Q9WV18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam10|O35598;Hcn2|O88703;Sstr2|P30875;Rab8b|P61028;Lpar1|P61793;Kcnab2|P62482;Trpc6|Q61143;Rhof|Q8BYP3;Snx30|Q8CE50;Gabbr1|Q9WV18;Lpcat2|Q8BYI6;Extl3|Q9WVL6;Stmn3|O70166;Clec2l|P0C7M9;Rab8a|P55258;Mblac2|Q8BL86;Zdhhc14|Q8BQQ1;Abhd17c|Q8VCV1;Xpr1|Q9Z0U0;Rab5a|Q9CQD1</t>
+    <t xml:space="preserve">|Q9WVL6;|Q9CQD1;|Q9WV18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35598;|O88703;|P30875;|P61028;|P61793;|P62482;|Q61143;|Q8BYP3;|Q8CE50;|Q9WV18;|Q8BYI6;|Q9WVL6;|O70166;|P0C7M9;|P55258;|Q8BL86;|Q8BQQ1;|Q8VCV1;|Q9Z0U0;|Q9CQD1</t>
   </si>
   <si>
     <t xml:space="preserve">M111</t>
   </si>
   <si>
-    <t xml:space="preserve">Gprc5b|Q923Z0;Aldh3b1|Q80VQ0;Mindy1|Q76LS9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cntnap1|O54991;Kcna1|P16388;Efnb1|P52795;Tyro3|P55144;Rala|P63321;Atp1b3|P97370;Ttyh2|Q3TH73;5031439G07Rik|Q3UE31;Cep164|Q5DU05;Fzd7|Q61090;D630045J12Rik|Q68FD9;Dagla|Q6WQJ1;Mindy1|Q76LS9;Aldh3b1|Q80VQ0;Astn2|Q80Z10;Fam234a|Q8C0Z1;Iglon5|Q8HW98;Igsf8|Q8R366;Gprc5b|Q923Z0</t>
+    <t xml:space="preserve">|Q923Z0;|Q80VQ0;|Q76LS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54991;|P16388;|P52795;|P55144;|P63321;|P97370;|Q3TH73;|Q3UE31;|Q5DU05;|Q61090;|Q68FD9;|Q6WQJ1;|Q76LS9;|Q80VQ0;|Q80Z10;|Q8C0Z1;|Q8HW98;|Q8R366;|Q923Z0</t>
   </si>
   <si>
     <t xml:space="preserve">M112</t>
   </si>
   <si>
-    <t xml:space="preserve">Adcy2|Q80TL1;Fam126a|Q6P9N1;Rab31|Q921E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rras|P10833;Slc16a1|P53986;Gaa|P70699;Nrp1|P97333;Egfr|Q01279;Lrrc8b|Q5DU41;Slc20a1|Q61609;Fam126a|Q6P9N1;Adcy2|Q80TL1;Rab31|Q921E2;Epha6|Q62413;Ntrk3|Q6VNS1;Lynx1|P0DP60;Slc4a3|P16283;Cnnm2|Q3TWN3;Ptprj|Q64455;Rab9|Q9R0M6;Slc20a2|Q80UP8</t>
+    <t xml:space="preserve">|Q80TL1;|Q6P9N1;|Q921E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P10833;|P53986;|P70699;|P97333;|Q01279;|Q5DU41;|Q61609;|Q6P9N1;|Q80TL1;|Q921E2;|Q62413;|Q6VNS1;|P0DP60;|P16283;|Q3TWN3;|Q64455;|Q9R0M6;|Q80UP8</t>
   </si>
   <si>
     <t xml:space="preserve">M113</t>
   </si>
   <si>
-    <t xml:space="preserve">Dnajb2|Q9QYI5;Gpr37|Q9QY42;Slc12a5|Q91V14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabrd|P22933;Rap1a|P62835;Rhog|P84096;Grm1|P97772;Cacna2d2|Q6PHS9;Slitrk1|Q810C1;Serinc5|Q8BHJ6;Gnal|Q8CGK7;Slc12a5|Q91V14;Rap1b|Q99JI6;Jam3|Q9D8B7;Gpr37|Q9QY42;Dnajb2|Q9QYI5;Tollip|Q9QZ06</t>
+    <t xml:space="preserve">|Q9QYI5;|Q9QY42;|Q91V14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P22933;|P62835;|P84096;|P97772;|Q6PHS9;|Q810C1;|Q8BHJ6;|Q8CGK7;|Q91V14;|Q99JI6;|Q9D8B7;|Q9QY42;|Q9QYI5;|Q9QZ06</t>
   </si>
   <si>
     <t xml:space="preserve">M114</t>
   </si>
   <si>
-    <t xml:space="preserve">Scn8a|Q9WTU3;Plscr3|Q9JIZ9;Gabra5|Q8BHJ7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nectin2|P32507;Stx4a|P70452;Abcg2|Q7TMS5;Ptk7|Q8BKG3;Neto2|Q8BNJ6;Frs2|Q8C180;Slco3a1|Q8R3L5;Plscr3|Q9JIZ9;Lamtor1|Q9CQ22;Chrm4|P32211;Mvb12b|Q6KAU4;Gabra5|Q8BHJ7;Scn8a|Q9WTU3</t>
+    <t xml:space="preserve">|Q9WTU3;|Q9JIZ9;|Q8BHJ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P32507;|P70452;|Q7TMS5;|Q8BKG3;|Q8BNJ6;|Q8C180;|Q8R3L5;|Q9JIZ9;|Q9CQ22;|P32211;|Q6KAU4;|Q8BHJ7;|Q9WTU3</t>
   </si>
   <si>
     <t xml:space="preserve">M115</t>
   </si>
   <si>
-    <t xml:space="preserve">Atp1a1|Q8VDN2;Atp2b2|Q9R0K7;Kcnd2|Q9Z0V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robo1|O89026;Gnas|P63094;Gabrb2|P63137;Nptn|P97300;Adcy8|P97490;Trpm1|Q2TV84;Prkg2|Q61410;Plppr3|Q7TPB0;Plppr1|Q8BFZ2;Atp1a1|Q8VDN2;Golga7|Q91W53;Atp2b2|Q9R0K7;Kcnd2|Q9Z0V2</t>
+    <t xml:space="preserve">|Q8VDN2;|Q9R0K7;|Q9Z0V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O89026;|P63094;|P63137;|P97300;|P97490;|Q2TV84;|Q61410;|Q7TPB0;|Q8BFZ2;|Q8VDN2;|Q91W53;|Q9R0K7;|Q9Z0V2</t>
   </si>
   <si>
     <t xml:space="preserve">M116</t>
   </si>
   <si>
-    <t xml:space="preserve">Rgs7bp|Q8BQP9;Faim2|Q8K097;Grm5|Q3UVX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plxnb2|B2RXS4;Atp2b1|G5E829;Pld3|O35405;Ptpra|P18052;Gabra3|P26049;Adcy5|P84309;Cacna1c|Q01815;Grm5|Q3UVX5;Cr1l|Q64735;Kcnt1|Q6ZPR4;Rgs7bp|Q8BQP9;Faim2|Q8K097;Oprm1|P42866</t>
+    <t xml:space="preserve">|Q8BQP9;|Q8K097;|Q3UVX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RXS4;|G5E829;|O35405;|P18052;|P26049;|P84309;|Q01815;|Q3UVX5;|Q64735;|Q6ZPR4;|Q8BQP9;|Q8K097;|P42866</t>
   </si>
   <si>
     <t xml:space="preserve">M117</t>
   </si>
   <si>
-    <t xml:space="preserve">Celsr2|Q9R0M0;Sppl2a|Q9JJF9;Abcc10|Q8R4P9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insr|P15208;Ntrk2|P15209;Gba|P17439;Lyn|P25911;Itgav|P43406;Acvr1b|Q61271;Nsg1|Q62092;Abcg1|Q64343;Abcc10|Q8R4P9;Tnfrsf21|Q9EPU5;Sppl2a|Q9JJF9;Celsr2|Q9R0M0</t>
+    <t xml:space="preserve">|Q9R0M0;|Q9JJF9;|Q8R4P9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P15208;|P15209;|P17439;|P25911;|P43406;|Q61271;|Q62092;|Q64343;|Q8R4P9;|Q9EPU5;|Q9JJF9;|Q9R0M0</t>
   </si>
   <si>
     <t xml:space="preserve">M118</t>
   </si>
   <si>
-    <t xml:space="preserve">Sft2d2|Q8VD57;Stxbp6|Q8R3T5;Plxna3|P70208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nlgn4l|B0F2B4;Emp2|O88662;Dcc|P70211;Asic1|Q6NXK8;Rab35|Q6PHN9;Sft2d2|Q8VD57;Gria1|P23818;Gria2|P23819;Abcc9|P70170;Plxna3|P70208;Kcnj11|Q61743;Stxbp6|Q8R3T5</t>
+    <t xml:space="preserve">|Q8VD57;|Q8R3T5;|P70208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B0F2B4;|O88662;|P70211;|Q6NXK8;|Q6PHN9;|Q8VD57;|P23818;|P23819;|P70170;|P70208;|Q61743;|Q8R3T5</t>
   </si>
   <si>
     <t xml:space="preserve">M119</t>
   </si>
   <si>
-    <t xml:space="preserve">Ctsz|Q9WUU7;Gabra4|Q9D6F4;Cspg5|Q71M36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kcnb2|A6H8H5;Grik3|B1AS29;Plxna2|P70207;Gprin1|Q3UNH4;Cspg5|Q71M36;Amigo1|Q80ZD8;Pcdhga4|Q91XY4;Gabra4|Q9D6F4;Ndrg3|Q9QYF9;Ctsz|Q9WUU7</t>
+    <t xml:space="preserve">|Q9WUU7;|Q9D6F4;|Q71M36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A6H8H5;|B1AS29;|P70207;|Q3UNH4;|Q71M36;|Q80ZD8;|Q91XY4;|Q9D6F4;|Q9QYF9;|Q9WUU7</t>
   </si>
   <si>
     <t xml:space="preserve">M120</t>
   </si>
   <si>
-    <t xml:space="preserve">Kcnip3|Q9QXT8;Tesc|Q9JKL5;Slc39a6|Q8C145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nrp2|O35375;Prnp|P04925;1500009L16Rik|P0C913;Fgfr1|P16092;Aqp4|P55088;Adcyap1r1|P70205;Slc39a6|Q8C145;Tesc|Q9JKL5;Cntn6|Q9JMB8;Kcnip3|Q9QXT8</t>
+    <t xml:space="preserve">|Q9QXT8;|Q9JKL5;|Q8C145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35375;|P04925;|P0C913;|P16092;|P55088;|P70205;|Q8C145;|Q9JKL5;|Q9JMB8;|Q9QXT8</t>
   </si>
   <si>
     <t xml:space="preserve">M121</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc43a2|Q8CGA3;Lhfpl2|Q8BGA2;Cntnap5a|Q0V8T9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gna12|P27600;Cd81|P35762;Cntnap5a|Q0V8T9;Lhfpl2|Q8BGA2;Chmp6|P0C0A3;Lrrc4b|P0C192;Slc43a2|Q8CGA3</t>
+    <t xml:space="preserve">|Q8CGA3;|Q8BGA2;|Q0V8T9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P27600;|P35762;|Q0V8T9;|Q8BGA2;|P0C0A3;|P0C192;|Q8CGA3</t>
   </si>
   <si>
     <t xml:space="preserve">M122</t>
   </si>
   <si>
-    <t xml:space="preserve">Cmtr1|Q9DBC3;Sart3|Q9JLI8;Strap|Q9Z1Z2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nmt1|O70310;Map2|P20357;Aimp1|P31230;Pcif1|P59114;Rps15|P62843;Rps28|P62858;Larp7|Q05CL8;Srsf6|Q3TWW8;Ddx46|Q569Z5;Ctc1|Q5SUQ9;Mars|Q68FL6;Kdm1a|Q6ZQ88;Dcaf1|Q80TR8;Nelfa|Q8BG30;Htatsf1|Q8BGC0;Tarsl2|Q8BLY2;Lars|Q8BMJ2;Trmt2a|Q8BNV1;Iars|Q8BU30;Eprs|Q8CGC7;Irf2bpl|Q8K3X4;Aimp2|Q8R010;Setd3|Q91WC0;Yars|Q91WQ3;Dars|Q922B2;Kars|Q99MN1;Luc7l|Q9CYI4;Rars|Q9D0I9;Eef1e1|Q9D1M4;Cmtr1|Q9DBC3;Wdr61|Q9ERF3;Habp4|Q9JKS5;Sart3|Q9JLI8;Strap|Q9Z1Z2</t>
+    <t xml:space="preserve">|Q9DBC3;|Q9JLI8;|Q9Z1Z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O70310;|P20357;|P31230;|P59114;|P62843;|P62858;|Q05CL8;|Q3TWW8;|Q569Z5;|Q5SUQ9;|Q68FL6;|Q6ZQ88;|Q80TR8;|Q8BG30;|Q8BGC0;|Q8BLY2;|Q8BMJ2;|Q8BNV1;|Q8BU30;|Q8CGC7;|Q8K3X4;|Q8R010;|Q91WC0;|Q91WQ3;|Q922B2;|Q99MN1;|Q9CYI4;|Q9D0I9;|Q9D1M4;|Q9DBC3;|Q9ERF3;|Q9JKS5;|Q9JLI8;|Q9Z1Z2</t>
   </si>
   <si>
     <t xml:space="preserve">M123</t>
   </si>
   <si>
-    <t xml:space="preserve">Ap3b1|Q9Z1T1;Bud23|Q9CY21;Rnf25|Q9QZR0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chd5|A2A8L1;Shoc2|O88520;Eef2|P58252;Inpp5j|P59644;Hcfc1|Q61191;Prkci|Q62074;Ubr5|Q80TP3;Arhgef17|Q80U35;Polr2e|Q80UW8;Wdr82|Q8BFQ4;Gtf3c4|Q8BMQ2;Cwf19l1|Q8CI33;Rassf8|Q8CJ96;Otud6b|Q8K2H2;Klhdc8a|Q91XA8;Egln1|Q91YE3;1110059E24Rik|Q9CQ90;Pin4|Q9CWW6;Bud23|Q9CY21;Polr3c|Q9D483;Rpap3|Q9D706;Ccnt1|Q9QWV9;Rnf25|Q9QZR0;Ap3b1|Q9Z1T1</t>
+    <t xml:space="preserve">|Q9Z1T1;|Q9CY21;|Q9QZR0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A8L1;|O88520;|P58252;|P59644;|Q61191;|Q62074;|Q80TP3;|Q80U35;|Q80UW8;|Q8BFQ4;|Q8BMQ2;|Q8CI33;|Q8CJ96;|Q8K2H2;|Q91XA8;|Q91YE3;|Q9CQ90;|Q9CWW6;|Q9CY21;|Q9D483;|Q9D706;|Q9QWV9;|Q9QZR0;|Q9Z1T1</t>
   </si>
   <si>
     <t xml:space="preserve">M124</t>
   </si>
   <si>
-    <t xml:space="preserve">Parn|Q8VDG3;Cog1|Q9Z160;Naa38|Q9D2U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hdac1|O09106;Srp14|P16254;Rangap1|P46061;Xdh|Q00519;Klhdc2|Q4G5Y1;Trim28|Q62318;Sbno1|Q689Z5;Prepl|Q8C167;Dido1|Q8C9B9;Pym1|Q8CHP5;Mta1|Q8K4B0;Tprkb|Q8QZZ7;Tut1|Q8R3F9;Parn|Q8VDG3;D1Ertd622e|Q8VEB3;Actl6b|Q99MR0;Hdac9|Q99N13;Naa38|Q9D2U5;Tssc4|Q9JHE7;Cog1|Q9Z160</t>
+    <t xml:space="preserve">|Q8VDG3;|Q9Z160;|Q9D2U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09106;|P16254;|P46061;|Q00519;|Q4G5Y1;|Q62318;|Q689Z5;|Q8C167;|Q8C9B9;|Q8CHP5;|Q8K4B0;|Q8QZZ7;|Q8R3F9;|Q8VDG3;|Q8VEB3;|Q99MR0;|Q99N13;|Q9D2U5;|Q9JHE7;|Q9Z160</t>
   </si>
   <si>
     <t xml:space="preserve">M125</t>
   </si>
   <si>
-    <t xml:space="preserve">Cutc|Q9D8X1;Rcor1|Q8CFE3;Naa10|Q9QY36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sec16a|E9QAT4;Foxk1|P42128;Msh2|P43247;Srp9|P49962;Msh6|P54276;Ufd1|P70362;Arnt2|Q61324;Ddx58|Q6Q899;Mon2|Q80TL7;Elac2|Q80Y81;Rcor1|Q8CFE3;Cog2|Q921L5;Unc45a|Q99KD5;Bccip|Q9CWI3;Ttc33|Q9D6K7;Cutc|Q9D8X1;Naa10|Q9QY36</t>
+    <t xml:space="preserve">|Q9D8X1;|Q8CFE3;|Q9QY36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9QAT4;|P42128;|P43247;|P49962;|P54276;|P70362;|Q61324;|Q6Q899;|Q80TL7;|Q80Y81;|Q8CFE3;|Q921L5;|Q99KD5;|Q9CWI3;|Q9D6K7;|Q9D8X1;|Q9QY36</t>
   </si>
   <si>
     <t xml:space="preserve">M126</t>
   </si>
   <si>
-    <t xml:space="preserve">Akap8|Q9DBR0;Snu13|Q9D0T1;Zcrb1|Q9CZ96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhx15|O35286;Apex1|P28352;Fau|P62862;Gtf2f1|Q3THK3;Snrpa|Q62189;Snrpc|Q62241;Snrnp70|Q62376;Srrm2|Q8BTI8;Mettl3|Q8C3P7;Rbm12|Q8R4X3;Rtraf|Q9CQE8;Zcrb1|Q9CZ96;Thumpd2|Q9CZB3;Snu13|Q9D0T1;Akap8|Q9DBR0</t>
+    <t xml:space="preserve">|Q9DBR0;|Q9D0T1;|Q9CZ96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35286;|P28352;|P62862;|Q3THK3;|Q62189;|Q62241;|Q62376;|Q8BTI8;|Q8C3P7;|Q8R4X3;|Q9CQE8;|Q9CZ96;|Q9CZB3;|Q9D0T1;|Q9DBR0</t>
   </si>
   <si>
     <t xml:space="preserve">M127</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruvbl2|Q9WTM5;Aar2|Q9D2V5;Rwdd4a|Q9CPR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruvbl1|P60122;Trmt1|Q3TX08;Ddb1|Q3U1J4;Iqgap2|Q3UQ44;Ctr9|Q62018;Usp34|Q6ZQ93;Ctdp1|Q7TSG2;R3hcc1|Q8BSI6;Xpo5|Q924C1;Rwdd4a|Q9CPR1;Aar2|Q9D2V5;Prmt1|Q9JIF0;Ruvbl2|Q9WTM5</t>
+    <t xml:space="preserve">|Q9WTM5;|Q9D2V5;|Q9CPR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P60122;|Q3TX08;|Q3U1J4;|Q3UQ44;|Q62018;|Q6ZQ93;|Q7TSG2;|Q8BSI6;|Q924C1;|Q9CPR1;|Q9D2V5;|Q9JIF0;|Q9WTM5</t>
   </si>
   <si>
     <t xml:space="preserve">M128</t>
   </si>
   <si>
-    <t xml:space="preserve">Taf10|Q8K0H5;Tcaf1|Q8BNE1;Gtf2f2|Q8R0A0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dennd5b|A2RSQ0;Btbd1|P58544;Hdac2|P70288;Fam160a2|Q3U2I3;Zmiz1|Q6P1E1;Tox3|Q80W03;Srp68|Q8BMA6;Tcaf1|Q8BNE1;Taf10|Q8K0H5;Gtf2f2|Q8R0A0;Cog8|Q9JJA2</t>
+    <t xml:space="preserve">|Q8K0H5;|Q8BNE1;|Q8R0A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2RSQ0;|P58544;|P70288;|Q3U2I3;|Q6P1E1;|Q80W03;|Q8BMA6;|Q8BNE1;|Q8K0H5;|Q8R0A0;|Q9JJA2</t>
   </si>
   <si>
     <t xml:space="preserve">M129</t>
   </si>
   <si>
-    <t xml:space="preserve">Eif4e2|Q8BMB3;Rprd1a|Q8VDS4;Rps21|Q9CQR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rpsa|P14206;Vim|P20152;Psme3|P61290;Rack1|P68040;Naa50|Q6PGB6;Eif4e2|Q8BMB3;Rprd1a|Q8VDS4;Srsf4|Q8VE97;Rps21|Q9CQR2</t>
+    <t xml:space="preserve">|Q8BMB3;|Q8VDS4;|Q9CQR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P14206;|P20152;|P61290;|P68040;|Q6PGB6;|Q8BMB3;|Q8VDS4;|Q8VE97;|Q9CQR2</t>
   </si>
   <si>
     <t xml:space="preserve">M130</t>
   </si>
   <si>
-    <t xml:space="preserve">Brap|Q99MP8;Tbl1xr1|Q8BHJ5;Eif5a|P63242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Map4|P27546;Rxrb|P28704;Dnajc2|P54103;Rps24|P62849;Eif5a|P63242;Tbl1xr1|Q8BHJ5;Brap|Q99MP8</t>
+    <t xml:space="preserve">|Q99MP8;|Q8BHJ5;|P63242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P27546;|P28704;|P54103;|P62849;|P63242;|Q8BHJ5;|Q99MP8</t>
   </si>
   <si>
     <t xml:space="preserve">M131</t>
   </si>
   <si>
-    <t xml:space="preserve">Bag6|Q9Z1R2;Rnmt|Q9D0L8;Tcea1|P10711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ncl|P09405;Tcea1|P10711;Pde4dip|Q80YT7;Rps6ka5|Q8C050;Rnmt|Q9D0L8;Bag6|Q9Z1R2</t>
+    <t xml:space="preserve">|Q9Z1R2;|Q9D0L8;|P10711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P09405;|P10711;|Q80YT7;|Q8C050;|Q9D0L8;|Q9Z1R2</t>
   </si>
   <si>
     <t xml:space="preserve">M132</t>
   </si>
   <si>
-    <t xml:space="preserve">Clic4|Q9QYB1;Prkar1a|Q9DBC7;Pmm2|Q9Z2M7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fmnl2|A2APV2;Myo1e|E9Q634;Folh1|O35409;Gamt|O35969;Car2|P00920;Cntn1|P12960;Gsn|P13020;Rdx|P26043;Fah|P35505;Dnm2|P39054;Arf6|P62331;Vsnl1|P62761;Padi2|Q08642;Plcl1|Q3USB7;Pls1|Q3V0K9;Ermn|Q5EBJ4;Taok1|Q5F2E8;Il1rap|Q61730;Kctd12|Q6WVG3;Gstm7|Q80W21;Cpne3|Q8BT60;Qdpr|Q8BVI4;Arhgef10|Q8C033;Pex5l|Q8C437;Acy1|Q99JW2;Carhsp1|Q9CR86;Prkar1a|Q9DBC7;Akr1e1|Q9DCT1;Kcnip1|Q9JJ57;Clic4|Q9QYB1;Pmm2|Q9Z2M7</t>
+    <t xml:space="preserve">|Q9QYB1;|Q9DBC7;|Q9Z2M7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2APV2;|E9Q634;|O35409;|O35969;|P00920;|P12960;|P13020;|P26043;|P35505;|P39054;|P62331;|P62761;|Q08642;|Q3USB7;|Q3V0K9;|Q5EBJ4;|Q5F2E8;|Q61730;|Q6WVG3;|Q80W21;|Q8BT60;|Q8BVI4;|Q8C033;|Q8C437;|Q99JW2;|Q9CR86;|Q9DBC7;|Q9DCT1;|Q9JJ57;|Q9QYB1;|Q9Z2M7</t>
   </si>
   <si>
     <t xml:space="preserve">M133</t>
   </si>
   <si>
-    <t xml:space="preserve">Car14|Q9WVT6;Plxnb3|Q9QY40;Sirt2|Q8VDQ8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efnb3|O35393;Fv1|P70213;Sema5b|Q60519;Ndrg1|Q62433;Thsd7a|Q69ZU6;Opalin|Q7M750;Lypd1|Q8BLC3;Fam177a|Q8BR63;Mcam|Q8R2Y2;Aspa|Q8R3P0;Serpinb1a|Q9D154;Plin3|Q9DBG5;Kcnip2|Q9JJ69;Car14|Q9WVT6;Cd34|Q64314;Scn4b|Q7M729;Dock5|B2RY04;Sypl|O09117;Itpr1|P11881;Cnp|P16330;Cd82|P40237;Ufm1|P61961;E330009J07Rik|Q3UHG7;Myo1d|Q5SYD0;Shh|Q62226;Slc44a1|Q6X893;Sirt2|Q8VDQ8;Tspan2|Q922J6;Plxnb3|Q9QY40</t>
+    <t xml:space="preserve">|Q9WVT6;|Q9QY40;|Q8VDQ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35393;|P70213;|Q60519;|Q62433;|Q69ZU6;|Q7M750;|Q8BLC3;|Q8BR63;|Q8R2Y2;|Q8R3P0;|Q9D154;|Q9DBG5;|Q9JJ69;|Q9WVT6;|Q64314;|Q7M729;|B2RY04;|O09117;|P11881;|P16330;|P40237;|P61961;|Q3UHG7;|Q5SYD0;|Q62226;|Q6X893;|Q8VDQ8;|Q922J6;|Q9QY40</t>
   </si>
   <si>
     <t xml:space="preserve">M134</t>
   </si>
   <si>
-    <t xml:space="preserve">Tbc1d10b|Q8BHL3;Cpq|Q9WVJ3;Fnbp1|Q80TY0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exoc6b|A6H5Z3;Exoc7|O35250;Gucy1b1|O54865;Prkca|P20444;Marcks|P26645;Marcksl1|P28667;Gnb5|P62881;Fer|P70451;Exoc5|Q3TPX4;Camkv|Q3UHL1;Gas7|Q60780;Ankrd13d|Q6PD24;Carns1|Q6ZPS2;Cyfip1|Q7TMB8;Prcp|Q7TMR0;Csmd3|Q80T79;Fnbp1|Q80TY0;Bcas1|Q80YN3;Tbc1d10b|Q8BHL3;Nmral1|Q8K2T1;Gpt|Q8QZR5;Cpq|Q9WVJ3;Myo6|Q64331</t>
+    <t xml:space="preserve">|Q8BHL3;|Q9WVJ3;|Q80TY0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A6H5Z3;|O35250;|O54865;|P20444;|P26645;|P28667;|P62881;|P70451;|Q3TPX4;|Q3UHL1;|Q60780;|Q6PD24;|Q6ZPS2;|Q7TMB8;|Q7TMR0;|Q80T79;|Q80TY0;|Q80YN3;|Q8BHL3;|Q8K2T1;|Q8QZR5;|Q9WVJ3;|Q64331</t>
   </si>
   <si>
     <t xml:space="preserve">M135</t>
   </si>
   <si>
-    <t xml:space="preserve">Abcb9|Q9JJ59;Pllp|Q9DCU2;Kcnc3|Q63959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scarb2|O35114;Slc1a6|O35544;Snx12|O70493;Hsp90b1|P08113;Ace|P09470;Kras|P32883;Snx27|Q3UHD6;Fat2|Q5F226;Igf1r|Q60751;Itga3|Q62470;Tmem67|Q8BR76;Spg20|Q8R1X6;Dusp15|Q8R4V2;Lrp1b|Q9JI18;Abcb9|Q9JJ59;Tspan3|Q9QY33;Clcn2|Q9R0A1;Rab21|P35282;Gabra6|P16305;Lgi2|Q8K4Z0;Pllp|Q9DCU2;Itgb5|O70309;Kcnc3|Q63959</t>
+    <t xml:space="preserve">|Q9JJ59;|Q9DCU2;|Q63959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35114;|O35544;|O70493;|P08113;|P09470;|P32883;|Q3UHD6;|Q5F226;|Q60751;|Q62470;|Q8BR76;|Q8R1X6;|Q8R4V2;|Q9JI18;|Q9JJ59;|Q9QY33;|Q9R0A1;|P35282;|P16305;|Q8K4Z0;|Q9DCU2;|O70309;|Q63959</t>
   </si>
   <si>
     <t xml:space="preserve">M136</t>
   </si>
   <si>
-    <t xml:space="preserve">Myo1c|Q9WTI7;Clcn5|Q9WVD4;Kcnj3|P63250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cpd|O89001;Enpp1|P06802;Abca2|P41234;Atp11a|P98197;Myo1c|Q9WTI7;Kcnh2|O35219;Cd151|O35566;Rnf13|O54965;Tesk1|O70146;Lamp1|P11438;Chrm1|P12657;Kcnj6|P48542;Stom|P54116;Kcnj3|P63250;Tmem88b|Q3TYP4;Ermp1|Q3UVK0;Igsf3|Q6ZQA6;Enpp4|Q8BTJ4;Clcn5|Q9WVD4</t>
+    <t xml:space="preserve">|Q9WTI7;|Q9WVD4;|P63250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O89001;|P06802;|P41234;|P98197;|Q9WTI7;|O35219;|O35566;|O54965;|O70146;|P11438;|P12657;|P48542;|P54116;|P63250;|Q3TYP4;|Q3UVK0;|Q6ZQA6;|Q8BTJ4;|Q9WVD4</t>
   </si>
   <si>
     <t xml:space="preserve">M137</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorcs2|Q9EPR5;Tmem145|Q8C4U2;H6pd|Q8CFX1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kcnj9|P48543;Sez6l2|Q4V9Z5;Sez6l|Q6P1D5;Tmem145|Q8C4U2;Ece2|B2RQR8;Lmnb1|P14733;Rab7|P51150;Slc1a1|P51906;Atp7a|Q64430;Tmem151a|Q6GQT5;Cachd1|Q6PDJ1;Steap2|Q8BWB6;H6pd|Q8CFX1;Sorcs2|Q9EPR5</t>
+    <t xml:space="preserve">|Q9EPR5;|Q8C4U2;|Q8CFX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P48543;|Q4V9Z5;|Q6P1D5;|Q8C4U2;|B2RQR8;|P14733;|P51150;|P51906;|Q64430;|Q6GQT5;|Q6PDJ1;|Q8BWB6;|Q8CFX1;|Q9EPR5</t>
   </si>
   <si>
     <t xml:space="preserve">M138</t>
   </si>
   <si>
-    <t xml:space="preserve">Lrrc75a|Q7TSF4;Rgs8|Q8BXT1;Arhgap26|Q6ZQ82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osbpl9|A2A8Z1;Cpne9|Q1RLL3;Arhgap26|Q6ZQ82;Usp6nl|Q80XC3;Rgs8|Q8BXT1;Ptpru|B1AUH1;Cbln3|Q9JHG0;Inpp4b|Q6P1Y8;Krit1|Q6S5J6;Lrrc75a|Q7TSF4;Nubp1|Q9R060</t>
+    <t xml:space="preserve">|Q7TSF4;|Q8BXT1;|Q6ZQ82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A8Z1;|Q1RLL3;|Q6ZQ82;|Q80XC3;|Q8BXT1;|B1AUH1;|Q9JHG0;|Q6P1Y8;|Q6S5J6;|Q7TSF4;|Q9R060</t>
   </si>
   <si>
     <t xml:space="preserve">M139</t>
   </si>
   <si>
-    <t xml:space="preserve">Icmt|Q9EQK7;Wwox|Q91WL8;Cers2|Q924Z4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kcnk1|O08581;Ugt1a7c|Q6ZQM8;Slc38a2|Q8CFE6;Cers2|Q924Z4;Icmt|Q9EQK7;Frmd5|Q6P5H6;Slc38a1|Q8K2P7;Wwox|Q91WL8;Xxylt1|Q3U4G3</t>
+    <t xml:space="preserve">|Q9EQK7;|Q91WL8;|Q924Z4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08581;|Q6ZQM8;|Q8CFE6;|Q924Z4;|Q9EQK7;|Q6P5H6;|Q8K2P7;|Q91WL8;|Q3U4G3</t>
   </si>
   <si>
     <t xml:space="preserve">M140</t>
   </si>
   <si>
-    <t xml:space="preserve">Ralb|Q9JIW9;P2rx7|Q9Z1M0;Rabgef1|Q9JM13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Npr1|P18293;Slc7a1|Q09143;Lrrc24|Q8BHA1;Slc13a3|Q91Y63;Abcb6|Q9DC29;Ralb|Q9JIW9;Rabgef1|Q9JM13;P2rx7|Q9Z1M0</t>
+    <t xml:space="preserve">|Q9JIW9;|Q9Z1M0;|Q9JM13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P18293;|Q09143;|Q8BHA1;|Q91Y63;|Q9DC29;|Q9JIW9;|Q9JM13;|Q9Z1M0</t>
   </si>
   <si>
     <t xml:space="preserve">M141</t>
   </si>
   <si>
-    <t xml:space="preserve">Sept5|Q9Z2Q6;Sept6|Q9R1T4;Slc22a4|Q9Z306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slc4a4|O88343;Slc6a11|P31650;Cnrip1|Q5M8N0;Pacsin1|Q61644;Lgi1|Q9JIA1;Cdc42ep4|Q9JM96;Mpp3|O88910;Scn2a|B1AWN6;Flot1|O08917;Slc6a6|O35316;Stx1a|O35526;Sept7|O55131;Slc6a9|P28571;Cd38|P56528;Flot2|Q60634;Cd47|Q61735;Nlgn2|Q69ZK9;Exoc3l4|Q6DIA2;Sept11|Q8C1B7;Sept8|Q8CHH9;Brinp1|Q920P3;Sept6|Q9R1T4;Heph|Q9Z0Z4;Sept5|Q9Z2Q6;Slc22a4|Q9Z306</t>
+    <t xml:space="preserve">|Q9Z2Q6;|Q9R1T4;|Q9Z306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88343;|P31650;|Q5M8N0;|Q61644;|Q9JIA1;|Q9JM96;|O88910;|B1AWN6;|O08917;|O35316;|O35526;|O55131;|P28571;|P56528;|Q60634;|Q61735;|Q69ZK9;|Q6DIA2;|Q8C1B7;|Q8CHH9;|Q920P3;|Q9R1T4;|Q9Z0Z4;|Q9Z2Q6;|Q9Z306</t>
   </si>
   <si>
     <t xml:space="preserve">M142</t>
   </si>
   <si>
-    <t xml:space="preserve">Mpp2|Q9WV34;Adam23|Q9R1V7;Dnm3|Q8BZ98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kctd8|Q50H33;Llgl1|Q80Y17;Lin7a|Q8JZS0;Plxnc1|Q9QZC2;Prrt2|E9PUL5;Sept4|P28661;Gnb4|P29387;Ephb2|P54763;Grm2|Q14BI2;Arsg|Q3TYD4;Plxnd1|Q3UH93;Shisa6|Q3UH99;Ctnna3|Q65CL1;Tmem132e|Q6IEE6;Igsf1|Q7TQA1;Phf24|Q80TL4;Spag1|Q80ZX8;Scn3b|Q8BHK2;Dnm3|Q8BZ98;Anln|Q8K298;Nectin1|Q9JKF6;Syt7|Q9R0N7;Adam23|Q9R1V7;Mpp2|Q9WV34;Plcb1|Q9Z1B3</t>
+    <t xml:space="preserve">|Q9WV34;|Q9R1V7;|Q8BZ98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q50H33;|Q80Y17;|Q8JZS0;|Q9QZC2;|E9PUL5;|P28661;|P29387;|P54763;|Q14BI2;|Q3TYD4;|Q3UH93;|Q3UH99;|Q65CL1;|Q6IEE6;|Q7TQA1;|Q80TL4;|Q80ZX8;|Q8BHK2;|Q8BZ98;|Q8K298;|Q9JKF6;|Q9R0N7;|Q9R1V7;|Q9WV34;|Q9Z1B3</t>
   </si>
   <si>
     <t xml:space="preserve">M143</t>
   </si>
   <si>
-    <t xml:space="preserve">Cadm3|Q99N28;Mlc1|Q8VHK5;Gpr158|Q8C419</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slc1a4|O35874;Slc3a2|P10852;L1cam|P11627;Atp1b2|P14231;F3|P20352;Gja1|P23242;Slc1a3|P56564;Gjb6|P70689;Sirpa|P97797;Prex2|Q3LAC4;Atp1a2|Q6PIE5;Nfasc|Q810U3;Gpr158|Q8C419;Cadm4|Q8R464;Mlc1|Q8VHK5;Plpp3|Q99JY8;Cadm3|Q99N28;Kcnj10|Q9JM63;Zdhhc5|Q8VDZ4;Ppp1r16a|Q923M0;Kcnj16|Q9Z307</t>
+    <t xml:space="preserve">|Q99N28;|Q8VHK5;|Q8C419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35874;|P10852;|P11627;|P14231;|P20352;|P23242;|P56564;|P70689;|P97797;|Q3LAC4;|Q6PIE5;|Q810U3;|Q8C419;|Q8R464;|Q8VHK5;|Q99JY8;|Q99N28;|Q9JM63;|Q8VDZ4;|Q923M0;|Q9Z307</t>
   </si>
   <si>
     <t xml:space="preserve">M144</t>
   </si>
   <si>
-    <t xml:space="preserve">Sec14l2|Q99J08;Ddah1|Q9CWS0;Magi2|Q9WVQ1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin1|O08539;Lin7c|O88952;Ldha|P06151;Gstm1|P10649;Gsta4|P24472;Ppp3cb|P48453;Rida|P52760;Actb|P60710;Ppp3ca|P63328;Tnpo3|Q6P2B1;Mtss2|Q6P9S0;Ahcyl1|Q80SW1;Fbxo2|Q80UW2;Asrgl1|Q8C0M9;Nhsl1|Q8CAF4;Plcd1|Q8R3B1;Tkfc|Q8VC30;Sec14l2|Q99J08;Ddah1|Q9CWS0;Magi2|Q9WVQ1</t>
+    <t xml:space="preserve">|Q99J08;|Q9CWS0;|Q9WVQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08539;|O88952;|P06151;|P10649;|P24472;|P48453;|P52760;|P60710;|P63328;|Q6P2B1;|Q6P9S0;|Q80SW1;|Q80UW2;|Q8C0M9;|Q8CAF4;|Q8R3B1;|Q8VC30;|Q99J08;|Q9CWS0;|Q9WVQ1</t>
   </si>
   <si>
     <t xml:space="preserve">M145</t>
   </si>
   <si>
-    <t xml:space="preserve">Ntm|Q99PJ0;Jam2|Q9JI59;Cadm2|Q8BLQ9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scn1a|A2APX8;Farp1|F8VPU2;Epb41l2|O70318;Aifm3|Q3TY86;Slc39a12|Q5FWH7;Rgma|Q6PCX7;Myh14|Q6URW6;Negr1|Q80Z24;Lsamp|Q8BLK3;Cadm2|Q8BLQ9;Appl2|Q8K3G9;Ntm|Q99PJ0;Jam2|Q9JI59</t>
+    <t xml:space="preserve">|Q99PJ0;|Q9JI59;|Q8BLQ9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2APX8;|F8VPU2;|O70318;|Q3TY86;|Q5FWH7;|Q6PCX7;|Q6URW6;|Q80Z24;|Q8BLK3;|Q8BLQ9;|Q8K3G9;|Q99PJ0;|Q9JI59</t>
   </si>
   <si>
     <t xml:space="preserve">M146</t>
   </si>
   <si>
-    <t xml:space="preserve">Pakap|Q8BR92;Rgs12|Q8CGE9;Naga|Q9QWR8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ddc|O88533;Igsf21|Q7TNR6;Robo2|Q7TPD3;Erbin|Q80TH2;Pakap|Q8BR92;Manba|Q8K2I4;Naga|Q9QWR8;Slc6a3|Q61327;Ptprd|Q64487;Kirrel2|Q7TSU7;Rgs12|Q8CGE9</t>
+    <t xml:space="preserve">|Q8BR92;|Q8CGE9;|Q9QWR8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88533;|Q7TNR6;|Q7TPD3;|Q80TH2;|Q8BR92;|Q8K2I4;|Q9QWR8;|Q61327;|Q64487;|Q7TSU7;|Q8CGE9</t>
   </si>
   <si>
     <t xml:space="preserve">M147</t>
   </si>
   <si>
-    <t xml:space="preserve">Cdh20|Q9Z0M3;Cacnb4|Q8R0S4;Daam2|Q80U19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rgs7|O54829;Dao|P18894;Ctnna1|P26231;Plcb3|P51432;Ahcyl2|Q68FL4;Psd2|Q6P1I6;Pcdh19|Q80TF3;Daam2|Q80U19;Slitrk4|Q810B8;Cacnb4|Q8R0S4;Cdh20|Q9Z0M3</t>
+    <t xml:space="preserve">|Q9Z0M3;|Q8R0S4;|Q80U19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54829;|P18894;|P26231;|P51432;|Q68FL4;|Q6P1I6;|Q80TF3;|Q80U19;|Q810B8;|Q8R0S4;|Q9Z0M3</t>
   </si>
   <si>
     <t xml:space="preserve">M148</t>
   </si>
   <si>
-    <t xml:space="preserve">Snx18|Q91ZR2;Aida|Q8C4Q6;Tenm1|Q9WTS4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lxn|P70202;Tspan9|Q8BJU2;Rps6kc1|Q8BLK9;Aida|Q8C4Q6;Snx18|Q91ZR2;Tenm1|Q9WTS4;Epb41l1|Q9Z2H5;Gjc2|Q8BQU6</t>
+    <t xml:space="preserve">|Q91ZR2;|Q8C4Q6;|Q9WTS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P70202;|Q8BJU2;|Q8BLK9;|Q8C4Q6;|Q91ZR2;|Q9WTS4;|Q9Z2H5;|Q8BQU6</t>
   </si>
   <si>
     <t xml:space="preserve">M149</t>
   </si>
   <si>
-    <t xml:space="preserve">Lrrc57|Q9D1G5;Sept3|Q9Z1S5;Sept10|Q8C650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sept2|P42208;Kctd16|Q5DTY9;Rnf31|Q924T7;Lrrc57|Q9D1G5;Sept3|Q9Z1S5;Brinp2|Q6DFY8;Sept10|Q8C650</t>
+    <t xml:space="preserve">|Q9D1G5;|Q9Z1S5;|Q8C650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P42208;|Q5DTY9;|Q924T7;|Q9D1G5;|Q9Z1S5;|Q6DFY8;|Q8C650</t>
   </si>
   <si>
     <t xml:space="preserve">M150</t>
   </si>
   <si>
-    <t xml:space="preserve">Iah1|Q9DB29;Bpnt1|Q9Z0S1;Nt5c3|Q9D020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vat1l|Q80TB8;Glod4|Q9CPV4;Aldh9a1|Q9JLJ2;Bpnt1|Q9Z0S1;Nt5c3|Q9D020;Iah1|Q9DB29</t>
+    <t xml:space="preserve">|Q9DB29;|Q9Z0S1;|Q9D020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q80TB8;|Q9CPV4;|Q9JLJ2;|Q9Z0S1;|Q9D020;|Q9DB29</t>
   </si>
   <si>
     <t xml:space="preserve">M151</t>
   </si>
   <si>
-    <t xml:space="preserve">Trpv2|Q9WTR1;Arl15|Q8BGR6;Adgrl1|Q80TR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slc7a2|P18581;Gna13|P27601;Fyn|P39688;Cnr1|P47746;Yes1|Q04736;Lrfn1|Q2WF71;Slc22a23|Q3UHH2;Gpr162|Q3UN16;Slc30a1|Q60738;Ttyh3|Q6P5F7;Ubtd2|Q6PGH0;Atp2b4|Q6Q477;Adgrl1|Q80TR1;Arl15|Q8BGR6;Plxnb1|Q8CJH3;Golga7b|Q9D428;Trpv2|Q9WTR1;Scn1b|P97952;Zdhhc8|Q5Y5T5;Tmem169|Q8BG50</t>
+    <t xml:space="preserve">|Q9WTR1;|Q8BGR6;|Q80TR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P18581;|P27601;|P39688;|P47746;|Q04736;|Q2WF71;|Q3UHH2;|Q3UN16;|Q60738;|Q6P5F7;|Q6PGH0;|Q6Q477;|Q80TR1;|Q8BGR6;|Q8CJH3;|Q9D428;|Q9WTR1;|P97952;|Q5Y5T5;|Q8BG50</t>
   </si>
   <si>
     <t xml:space="preserve">M152</t>
   </si>
   <si>
-    <t xml:space="preserve">Cacna2d3|Q9Z1L5;Nlgn3|Q8BYM5;Ly6h|Q9WUC3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gnai1|B2RSH2;Prkaca|P05132;Gnai2|P08752;Gabrg2|P22723;Gpm6a|P35802;Gpm6b|P35803;Stx1b|P61264;Gabra1|P62812;Gabrb3|P63080;Epha4|Q03137;Scn2b|Q56A07;Dpp10|Q6NXK7;Lrtm2|Q8BGX3;Nlgn3|Q8BYM5;Gnai3|Q9DC51;Ly6h|Q9WUC3;Atp1a4|Q9WV27;Cacna2d3|Q9Z1L5</t>
+    <t xml:space="preserve">|Q9Z1L5;|Q8BYM5;|Q9WUC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RSH2;|P05132;|P08752;|P22723;|P35802;|P35803;|P61264;|P62812;|P63080;|Q03137;|Q56A07;|Q6NXK7;|Q8BGX3;|Q8BYM5;|Q9DC51;|Q9WUC3;|Q9WV27;|Q9Z1L5</t>
   </si>
   <si>
     <t xml:space="preserve">M153</t>
   </si>
   <si>
-    <t xml:space="preserve">Cntnap2|Q9CPW0;Daam1|Q8BPM0;Spred1|Q924S8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fam171a2|A2A699;Bmpr1a|P36895;Rhob|P62746;Gnb1|P62874;Gnb2|P62880;Plxna1|P70206;Cnnm1|Q0GA42;Cntn2|Q61330;Kcna4|Q61423;Atp1a3|Q6PIC6;Daam1|Q8BPM0;Slc44a2|Q8BY89;Spred1|Q924S8;Cntnap2|Q9CPW0;Dpp6|Q9Z218;Cacng8|Q8VHW2</t>
+    <t xml:space="preserve">|Q9CPW0;|Q8BPM0;|Q924S8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A699;|P36895;|P62746;|P62874;|P62880;|P70206;|Q0GA42;|Q61330;|Q61423;|Q6PIC6;|Q8BPM0;|Q8BY89;|Q924S8;|Q9CPW0;|Q9Z218;|Q8VHW2</t>
   </si>
   <si>
     <t xml:space="preserve">M154</t>
   </si>
   <si>
-    <t xml:space="preserve">Rgs17|Q9QZB0;Lrrc8a|Q80WG5;Plxna4|Q80UG2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cacna2d1|O08532;Gnaz|O70443;Kit|P05532;Adcy9|P51830;Rap2b|P61226;Rras2|P62071;Slc8a1|P70414;Smpd1|Q04519;Fgfr3|Q61851;Slc39a10|Q6P5F6;Plxna4|Q80UG2;Lrrc8a|Q80WG5;Rell2|Q8BRJ3;Clmp|Q8R373;Ist1|Q9CX00;Rgs17|Q9QZB0</t>
+    <t xml:space="preserve">|Q9QZB0;|Q80WG5;|Q80UG2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08532;|O70443;|P05532;|P51830;|P61226;|P62071;|P70414;|Q04519;|Q61851;|Q6P5F6;|Q80UG2;|Q80WG5;|Q8BRJ3;|Q8R373;|Q9CX00;|Q9QZB0</t>
   </si>
   <si>
     <t xml:space="preserve">M155</t>
   </si>
   <si>
-    <t xml:space="preserve">Adam22|Q9R1V6;Tenm2|Q9WTS5;Gabbr2|Q80T41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prrt1|O35449;Cd200|O54901;Kcnc1|P15388;Kcna3|P16390;Rab23|P35288;Astn1|Q61137;Kcna6|Q61923;Tspan7|Q62283;Fbxo41|Q6NS60;Gabbr2|Q80T41;Adam11|Q9R1V4;Adam22|Q9R1V6;Tenm2|Q9WTS5</t>
+    <t xml:space="preserve">|Q9R1V6;|Q9WTS5;|Q80T41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35449;|O54901;|P15388;|P16390;|P35288;|Q61137;|Q61923;|Q62283;|Q6NS60;|Q80T41;|Q9R1V4;|Q9R1V6;|Q9WTS5</t>
   </si>
   <si>
     <t xml:space="preserve">M156</t>
   </si>
   <si>
-    <t xml:space="preserve">Slco1c1|Q9ERB5;Lrrc8d|Q8BGR2;Kcnq2|Q9Z351</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ano3|A2AHL1;Nrxn2|E9Q7X7;Ctsa|P16675;Gm2a|Q60648;Mertk|Q60805;Pla2g15|Q8VEB4;Slco1c1|Q9ERB5;Axl|Q00993;Lrrc8d|Q8BGR2;Kcnq2|Q9Z351</t>
+    <t xml:space="preserve">|Q9ERB5;|Q8BGR2;|Q9Z351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AHL1;|E9Q7X7;|P16675;|Q60648;|Q60805;|Q8VEB4;|Q9ERB5;|Q00993;|Q8BGR2;|Q9Z351</t>
   </si>
   <si>
     <t xml:space="preserve">M157</t>
   </si>
   <si>
-    <t xml:space="preserve">Rgs20|Q9QZB1;Gng12|Q9DAS9;Palm|Q9Z0P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ncam2|O35136;Ncam1|P13595;Gnao1|P18872;Snap25|P60879;Neo1|P97798;Fam171b|Q14CH0;Gng12|Q9DAS9;Rgs20|Q9QZB1;Palm|Q9Z0P4</t>
+    <t xml:space="preserve">|Q9QZB1;|Q9DAS9;|Q9Z0P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35136;|P13595;|P18872;|P60879;|P97798;|Q14CH0;|Q9DAS9;|Q9QZB1;|Q9Z0P4</t>
   </si>
   <si>
     <t xml:space="preserve">M158</t>
   </si>
   <si>
-    <t xml:space="preserve">Tmem51|Q99LG1;Ankib1|Q6ZPS6;Grm3|Q9QYS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nras|P08556;Rac3|P60764;Sema4b|Q62179;Hepacam|Q640R3;Ankib1|Q6ZPS6;Tmem51|Q99LG1;Antxr1|Q9CZ52;Grm3|Q9QYS2</t>
+    <t xml:space="preserve">|Q99LG1;|Q6ZPS6;|Q9QYS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P08556;|P60764;|Q62179;|Q640R3;|Q6ZPS6;|Q99LG1;|Q9CZ52;|Q9QYS2</t>
   </si>
   <si>
     <t xml:space="preserve">M159</t>
   </si>
   <si>
-    <t xml:space="preserve">Pcnx|Q9QYC1;Spry2|Q9QXV8;Cdip1|Q9DB75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hcn1|O88704;Slc2a1|P17809;Ache|P21836;Efr3a|Q8BG67;Cdip1|Q9DB75;Spry2|Q9QXV8;Pcnx|Q9QYC1</t>
+    <t xml:space="preserve">|Q9QYC1;|Q9QXV8;|Q9DB75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88704;|P17809;|P21836;|Q8BG67;|Q9DB75;|Q9QXV8;|Q9QYC1</t>
   </si>
   <si>
     <t xml:space="preserve">M160</t>
   </si>
   <si>
-    <t xml:space="preserve">Rpl15|Q9CZM2;Bzw1|Q9CQC6;Rpl19|P84099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ttll7|A4Q9F0;Rpl21|O09167;Rpl7a|P12970;Rpl7|P14148;Rpl3|P27659;Rpl28|P41105;Rpl6|P47911;Rpl13|P47963;Rpl36|P47964;Rpl10a|P53026;Rpl26|P61255;Rpl18a|P62717;Rpl30|P62889;Rpl31|P62900;Rpl32|P62911;Rpl8|P62918;Rpl36a|P83882;Rpl19|P84099;Fam98a|Q3TJZ6;Kin|Q8K339;Seh1l|Q8R2U0;Bzw1|Q9CQC6;Mettl16|Q9CQG2;Rpl15|Q9CZM2;Rpl34|Q9D1R9</t>
+    <t xml:space="preserve">|Q9CZM2;|Q9CQC6;|P84099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A4Q9F0;|O09167;|P12970;|P14148;|P27659;|P41105;|P47911;|P47963;|P47964;|P53026;|P61255;|P62717;|P62889;|P62900;|P62911;|P62918;|P83882;|P84099;|Q3TJZ6;|Q8K339;|Q8R2U0;|Q9CQC6;|Q9CQG2;|Q9CZM2;|Q9D1R9</t>
   </si>
   <si>
     <t xml:space="preserve">M161</t>
   </si>
   <si>
-    <t xml:space="preserve">Ddx47|Q9CWX9;Ccdc92|Q8VDN4;Nob1|Q8BW10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sars|P26638;Rpl18|P35980;Rps8|P62242;Rps26|P62855;Rpl22|P67984;Irs2|P81122;Rps3a1|P97351;Nxt2|Q3UNA4;Scaf1|Q5U4C3;Ddx19a|Q61655;Smarcc2|Q6PDG5;Trim46|Q7TNM2;Rsbn1|Q80T69;Rpl24|Q8BP67;Utp25|Q8BTT6;Nob1|Q8BW10;Strip2|Q8C9H6;Gtf3c1|Q8K284;Ccdc92|Q8VDN4;Nelfcd|Q922L6;Ddx47|Q9CWX9;Lsm12|Q9D0R8;Aatf|Q9JKX4</t>
+    <t xml:space="preserve">|Q9CWX9;|Q8VDN4;|Q8BW10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P26638;|P35980;|P62242;|P62855;|P67984;|P81122;|P97351;|Q3UNA4;|Q5U4C3;|Q61655;|Q6PDG5;|Q7TNM2;|Q80T69;|Q8BP67;|Q8BTT6;|Q8BW10;|Q8C9H6;|Q8K284;|Q8VDN4;|Q922L6;|Q9CWX9;|Q9D0R8;|Q9JKX4</t>
   </si>
   <si>
     <t xml:space="preserve">M162</t>
   </si>
   <si>
-    <t xml:space="preserve">Rpl22l1|Q9D7S7;Rpl4|Q9D8E6;Rpl17|Q9CPR4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Szt2|A2A9C3;Rpl35a|O55142;Rplp0|P14869;Rpl13a|P19253;Drg1|P32233;Rpl12|P35979;Eef1d|P57776;Rpl37a|P61514;Rpl23a|P62751;Rpl23|P62830;Kndc1|Q0KK55;Tcf25|Q8R3L2;C330007P06Rik|Q8VDP2;Rbm39|Q8VH51;Eif3m|Q99JX4;Rpl17|Q9CPR4;Nop16|Q9CPT5;Phf6|Q9D4J7;Rpl22l1|Q9D7S7;Rpl4|Q9D8E6</t>
+    <t xml:space="preserve">|Q9D7S7;|Q9D8E6;|Q9CPR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A9C3;|O55142;|P14869;|P19253;|P32233;|P35979;|P57776;|P61514;|P62751;|P62830;|Q0KK55;|Q8R3L2;|Q8VDP2;|Q8VH51;|Q99JX4;|Q9CPR4;|Q9CPT5;|Q9D4J7;|Q9D7S7;|Q9D8E6</t>
   </si>
   <si>
     <t xml:space="preserve">M163</t>
   </si>
   <si>
-    <t xml:space="preserve">Vars|Q9Z1Q9;Eef1g|Q9D8N0;Prpf3|Q922U1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gcn1|E9PVA8;Ttc3|O88196;Rpl9|P51410;Rps10|P63325;Luc7l3|Q5SUF2;Ddx3x|Q62167;Pcid2|Q8BFV2;Csnk1a1|Q8BK63;Ythdf3|Q8BYK6;Farsa|Q8C0C7;Bclaf1|Q8K019;Hdlbp|Q8VDJ3;Ccar2|Q8VDP4;Prpf3|Q922U1;Rtcb|Q99LF4;Eef1g|Q9D8N0;Farsb|Q9WUA2;Vars|Q9Z1Q9</t>
+    <t xml:space="preserve">|Q9Z1Q9;|Q9D8N0;|Q922U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9PVA8;|O88196;|P51410;|P63325;|Q5SUF2;|Q62167;|Q8BFV2;|Q8BK63;|Q8BYK6;|Q8C0C7;|Q8K019;|Q8VDJ3;|Q8VDP4;|Q922U1;|Q99LF4;|Q9D8N0;|Q9WUA2;|Q9Z1Q9</t>
   </si>
   <si>
     <t xml:space="preserve">M164</t>
   </si>
   <si>
-    <t xml:space="preserve">Serbp1|Q9CY58;Cars|Q9ER72;Gigyf2|Q6Y7W8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eef1a1|P10126;Rpl5|P47962;Pold1|P52431;Rps23|P62267;Eef1a2|P62631;Rps6|P62754;Eif5b|Q05D44;Zc3h15|Q3TIV5;Fkbp3|Q62446;Abcf1|Q6P542;Gigyf2|Q6Y7W8;Csde1|Q91W50;Serbp1|Q9CY58;Cars|Q9ER72</t>
+    <t xml:space="preserve">|Q9CY58;|Q9ER72;|Q6Y7W8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P10126;|P47962;|P52431;|P62267;|P62631;|P62754;|Q05D44;|Q3TIV5;|Q62446;|Q6P542;|Q6Y7W8;|Q91W50;|Q9CY58;|Q9ER72</t>
   </si>
   <si>
     <t xml:space="preserve">M165</t>
   </si>
   <si>
-    <t xml:space="preserve">Eif2s3x|Q9Z0N1;Nxf1|Q99JX7;Toe1|Q9D2E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pa2g4|P50580;Rps20|P60867;Rps7|P62082;G3bp2|P97379;Rps27|Q6ZWU9;Prpf38b|Q80SY5;Fam98b|Q80VD1;Smarcal1|Q8BJL0;Tyw3|Q8BSA9;Nxf1|Q99JX7;Toe1|Q9D2E2;Eif2s3x|Q9Z0N1</t>
+    <t xml:space="preserve">|Q9Z0N1;|Q99JX7;|Q9D2E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P50580;|P60867;|P62082;|P97379;|Q6ZWU9;|Q80SY5;|Q80VD1;|Q8BJL0;|Q8BSA9;|Q99JX7;|Q9D2E2;|Q9Z0N1</t>
   </si>
   <si>
     <t xml:space="preserve">M166</t>
   </si>
   <si>
-    <t xml:space="preserve">Rpl14|Q9CR57;Clip4|Q8CI96;Xrn2|Q9DBR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camta1|A2A891;Abce1|P61222;Rps14|P62264;Rnf40|Q3U319;Nrde2|Q80XC6;Vxn|Q8BG31;Clip4|Q8CI96;Ddx1|Q91VR5;Rpl14|Q9CR57;Ppil2|Q9D787;Xrn2|Q9DBR1</t>
+    <t xml:space="preserve">|Q9CR57;|Q8CI96;|Q9DBR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A891;|P61222;|P62264;|Q3U319;|Q80XC6;|Q8BG31;|Q8CI96;|Q91VR5;|Q9CR57;|Q9D787;|Q9DBR1</t>
   </si>
   <si>
     <t xml:space="preserve">M167</t>
   </si>
   <si>
-    <t xml:space="preserve">Hnrnpul1|Q8VDM6;Cpsf6|Q6NVF9;Ddx5|Q61656</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Map7|O88735;Rbm3|O89086;Cirbp|P60824;Srsf3|P84104;Hp1bp3|Q3TEA8;Ddx5|Q61656;Cpsf6|Q6NVF9;Hnrnpul1|Q8VDM6</t>
+    <t xml:space="preserve">|Q8VDM6;|Q6NVF9;|Q61656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88735;|O89086;|P60824;|P84104;|Q3TEA8;|Q61656;|Q6NVF9;|Q8VDM6</t>
   </si>
   <si>
     <t xml:space="preserve">M168</t>
   </si>
   <si>
-    <t xml:space="preserve">Map1a|Q9QYR6;Specc1|Q5SXY1;Mob4|Q6PEB6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srpk2|O54781;Fus|P56959;Arglu1|Q3UL36;Specc1|Q5SXY1;Mob4|Q6PEB6;Map1a|Q9QYR6</t>
+    <t xml:space="preserve">|Q9QYR6;|Q5SXY1;|Q6PEB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54781;|P56959;|Q3UL36;|Q5SXY1;|Q6PEB6;|Q9QYR6</t>
   </si>
   <si>
     <t xml:space="preserve">M169</t>
   </si>
   <si>
-    <t xml:space="preserve">Naa25|Q8BWZ3;Eif4b|Q8BGD9;Ltn1|Q6A009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parg|O88622;Deptor|Q570Y9;Ltn1|Q6A009;Eif4b|Q8BGD9;Naa25|Q8BWZ3</t>
+    <t xml:space="preserve">|Q8BWZ3;|Q8BGD9;|Q6A009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88622;|Q570Y9;|Q6A009;|Q8BGD9;|Q8BWZ3</t>
   </si>
   <si>
     <t xml:space="preserve">M170</t>
   </si>
   <si>
-    <t xml:space="preserve">Morf4l2|Q9R0Q4;Ubap2|Q91VX2;Nemf|Q8CCP0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srsf5|O35326;Naa20|P61600;Nemf|Q8CCP0;Ubap2|Q91VX2;Morf4l2|Q9R0Q4</t>
+    <t xml:space="preserve">|Q9R0Q4;|Q91VX2;|Q8CCP0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35326;|P61600;|Q8CCP0;|Q91VX2;|Q9R0Q4</t>
   </si>
   <si>
     <t xml:space="preserve">M171</t>
   </si>
   <si>
-    <t xml:space="preserve">Agap3|Q8VHH5;Camsap3|Q80VC9;Fn3k|Q9ER35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanc2|A2A690;Sbf2|E9PXF8;Cyth3|O08967;Diaph2|O70566;Phkg1|P07934;Phka1|P18826;Arhgap39|P59281;Dock4|P59764;Cyth2|P63034;Carmil2|Q3V3V9;Ccdc85a|Q5SP85;Cyfip2|Q5SQX6;Tsc2|Q61037;Apc|Q61315;Fgd6|Q69ZL1;Camk2d|Q6PHZ2;Dmxl1|Q6PNC0;Wdfy3|Q6VNB8;Phkb|Q7TSH2;Camsap3|Q80VC9;Elmo2|Q8BHL5;Ppfia2|Q8BSS9;Abi1|Q8CBW3;Agap3|Q8VHH5;Ampd2|Q9DBT5;Fn3k|Q9ER35;Arhgef7|Q9ES28;Cul3|Q9JLV5;Ulk2|Q9QY01</t>
+    <t xml:space="preserve">|Q8VHH5;|Q80VC9;|Q9ER35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A690;|E9PXF8;|O08967;|O70566;|P07934;|P18826;|P59281;|P59764;|P63034;|Q3V3V9;|Q5SP85;|Q5SQX6;|Q61037;|Q61315;|Q69ZL1;|Q6PHZ2;|Q6PNC0;|Q6VNB8;|Q7TSH2;|Q80VC9;|Q8BHL5;|Q8BSS9;|Q8CBW3;|Q8VHH5;|Q9DBT5;|Q9ER35;|Q9ES28;|Q9JLV5;|Q9QY01</t>
   </si>
   <si>
     <t xml:space="preserve">M172</t>
   </si>
   <si>
-    <t xml:space="preserve">Mtmr1|Q9Z2C4;Ap3b2|Q9JME5;Myo18a|Q9JMH9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ap3d1|O54774;Akap10|O88845;Nckap1|P28660;Ptk2|P34152;Htt|P42859;Pfkm|P47857;Abi2|P62484;Lyst|P97412;Abl2|Q4JIM5;Ppp2r5c|Q60996;Git1|Q68FF6;Sbf1|Q6ZPE2;Epg5|Q80TA9;Srgap3|Q812A2;Ap3s2|Q8BSZ2;Stk32c|Q8QZV4;Ap3m2|Q8R2R9;Ap3s1|Q9DCR2;Tsc1|Q9EP53;Ap3b2|Q9JME5;Myo18a|Q9JMH9;Bcar3|Q9QZK2;Mtmr1|Q9Z2C4</t>
+    <t xml:space="preserve">|Q9Z2C4;|Q9JME5;|Q9JMH9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O54774;|O88845;|P28660;|P34152;|P42859;|P47857;|P62484;|P97412;|Q4JIM5;|Q60996;|Q68FF6;|Q6ZPE2;|Q80TA9;|Q812A2;|Q8BSZ2;|Q8QZV4;|Q8R2R9;|Q9DCR2;|Q9EP53;|Q9JME5;|Q9JMH9;|Q9QZK2;|Q9Z2C4</t>
   </si>
   <si>
     <t xml:space="preserve">M173</t>
   </si>
   <si>
-    <t xml:space="preserve">Ophn1|Q99J31;Iqsec1|Q8R0S2;Erc1|Q99MI1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sh3pxd2b|A2AAY5;Nck2|O55033;Abl1|P00520;Cit|P49025;Ppfia3|P60469;Trio|Q0KL02;Baiap2|Q8BKX1;Wdr37|Q8CBE3;Pacs1|Q8K212;Iqsec1|Q8R0S2;Ophn1|Q99J31;Erc1|Q99MI1;Rims1|Q99NE5;Rb1cc1|Q9ESK9</t>
+    <t xml:space="preserve">|Q99J31;|Q8R0S2;|Q99MI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AAY5;|O55033;|P00520;|P49025;|P60469;|Q0KL02;|Q8BKX1;|Q8CBE3;|Q8K212;|Q8R0S2;|Q99J31;|Q99MI1;|Q99NE5;|Q9ESK9</t>
   </si>
   <si>
     <t xml:space="preserve">M174</t>
   </si>
   <si>
-    <t xml:space="preserve">Pip4k2c|Q91XU3;Pank1|Q8K4K6;Asap2|Q7SIG6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capza2|P47754;Capzb|P47757;Map4k4|P97820;Eps8|Q08509;Phactr1|Q2M3X8;C530008M17Rik|Q5PR69;Taok2|Q6ZQ29;Syne2|Q6ZWQ0;Asap2|Q7SIG6;Rapgef2|Q8CHG7;Pank1|Q8K4K6;Pip4k2c|Q91XU3;Lrrc40|Q9CRC8</t>
+    <t xml:space="preserve">|Q91XU3;|Q8K4K6;|Q7SIG6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P47754;|P47757;|P97820;|Q08509;|Q2M3X8;|Q5PR69;|Q6ZQ29;|Q6ZWQ0;|Q7SIG6;|Q8CHG7;|Q8K4K6;|Q91XU3;|Q9CRC8</t>
   </si>
   <si>
     <t xml:space="preserve">M175</t>
   </si>
   <si>
-    <t xml:space="preserve">Carmil1|Q6EDY6;Caskin1|Q6P9K8;Atat1|Q8K341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sash1|P59808;Tnik|P83510;Agbl4|Q09LZ8;Dennd4b|Q3U1Y4;Dab2ip|Q3UHC7;Grk3|Q3UYH7;Wdr34|Q5U4F6;Actr3b|Q641P0;Carmil1|Q6EDY6;Caskin1|Q6P9K8;Atat1|Q8K341;D230025D16Rik|Q922R1;Spast|Q9QYY8</t>
+    <t xml:space="preserve">|Q6EDY6;|Q6P9K8;|Q8K341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P59808;|P83510;|Q09LZ8;|Q3U1Y4;|Q3UHC7;|Q3UYH7;|Q5U4F6;|Q641P0;|Q6EDY6;|Q6P9K8;|Q8K341;|Q922R1;|Q9QYY8</t>
   </si>
   <si>
     <t xml:space="preserve">M176</t>
   </si>
   <si>
-    <t xml:space="preserve">Nos1|Q9Z0J4;Coro1c|Q9WUM4;Sh3kbp1|Q8R550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ampd3|O08739;Pfkl|P12382;Bcr|Q6PAJ1;Sh2d5|Q8JZW5;Dennd1a|Q8K382;Sh3kbp1|Q8R550;Necap1|Q9CR95;Magi3|Q9EQJ9;Flii|Q9JJ28;Coro1c|Q9WUM4;Nos1|Q9Z0J4</t>
+    <t xml:space="preserve">|Q9Z0J4;|Q9WUM4;|Q8R550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08739;|P12382;|Q6PAJ1;|Q8JZW5;|Q8K382;|Q8R550;|Q9CR95;|Q9EQJ9;|Q9JJ28;|Q9WUM4;|Q9Z0J4</t>
   </si>
   <si>
     <t xml:space="preserve">M177</t>
   </si>
   <si>
-    <t xml:space="preserve">Dlc1|Q9R0Z9;Arhgap22|Q8BL80;Slain2|Q8CI08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camsap1|A2AHC3;Specc1l|Q2KN98;Sin3a|Q60520;Tbc1d1|Q60949;Heatr6|Q6P1G0;Morn4|Q6PGF2;Ppip5k2|Q6ZQB6;Arhgap22|Q8BL80;Slain2|Q8CI08;Arhgef6|Q8K4I3;Dlc1|Q9R0Z9</t>
+    <t xml:space="preserve">|Q9R0Z9;|Q8BL80;|Q8CI08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AHC3;|Q2KN98;|Q60520;|Q60949;|Q6P1G0;|Q6PGF2;|Q6ZQB6;|Q8BL80;|Q8CI08;|Q8K4I3;|Q9R0Z9</t>
   </si>
   <si>
     <t xml:space="preserve">M178</t>
   </si>
   <si>
-    <t xml:space="preserve">Sipa1l2|Q80TE4;Anapc7|Q9WVM3;Trim66|Q924W6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kif5a|P33175;Arhgap5|P97393;Arhgef28|P97433;Jcad|Q5DTX6;Chuk|Q60680;Sipa1l2|Q80TE4;Chn2|Q80XD1;Ppp4r4|Q8C0Y0;Trim66|Q924W6;Anapc7|Q9WVM3</t>
+    <t xml:space="preserve">|Q80TE4;|Q9WVM3;|Q924W6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P33175;|P97393;|P97433;|Q5DTX6;|Q60680;|Q80TE4;|Q80XD1;|Q8C0Y0;|Q924W6;|Q9WVM3</t>
   </si>
   <si>
     <t xml:space="preserve">M179</t>
   </si>
   <si>
-    <t xml:space="preserve">Prps2|Q9CS42;Txndc9|Q9CQ79;Nek9|Q8K1R7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uprt|B1AVZ0;Nmt2|O70311;Birc6|O88738;Fth1|P09528;Tcp1|P11983;Pik3r1|P26450;Cct8|P42932;Anapc1|P53995;Cct7|P80313;Cct2|P80314;Cct4|P80315;Cct5|P80316;Cct6a|P80317;Cct3|P80318;Fhl1|P97447;Hectd3|Q3U487;Eml4|Q3UMY5;Eif2b4|Q61749;Wdr91|Q7TMQ7;Kcmf1|Q80UY2;Cdc23|Q8BGZ4;Tbc1d4|Q8BYJ6;Wdr26|Q8C6G8;Eif2b5|Q8CHW4;Nek9|Q8K1R7;Anapc4|Q91W96;Dgkg|Q91WG7;Uckl1|Q91YL3;Eif2b1|Q99LC8;Txndc9|Q9CQ79;Prps2|Q9CS42;Psma1|Q9R1P4</t>
+    <t xml:space="preserve">|Q9CS42;|Q9CQ79;|Q8K1R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B1AVZ0;|O70311;|O88738;|P09528;|P11983;|P26450;|P42932;|P53995;|P80313;|P80314;|P80315;|P80316;|P80317;|P80318;|P97447;|Q3U487;|Q3UMY5;|Q61749;|Q7TMQ7;|Q80UY2;|Q8BGZ4;|Q8BYJ6;|Q8C6G8;|Q8CHW4;|Q8K1R7;|Q91W96;|Q91WG7;|Q91YL3;|Q99LC8;|Q9CQ79;|Q9CS42;|Q9R1P4</t>
   </si>
   <si>
     <t xml:space="preserve">M180</t>
   </si>
   <si>
-    <t xml:space="preserve">Prps1|Q9D7G0;Map1lc3b|Q9CQV6;Psma7|Q9Z2U0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trip12|G5E870;Psmd14|O35593;Pja1|O55176;Psma3|O70435;Psmc3|O88685;Ndn|P25233;Psmc2|P46471;Psma2|P49722;Psmc5|P62196;Psmc6|P62334;Psmb7|P70195;Psmb4|P99026;Psmd1|Q3TXS7;Fam117b|Q3U3E2;Psmb6|Q60692;Ccp110|Q7TSH4;Psmd11|Q8BG32;Phactr3|Q8BYK5;Amer2|Q8CCJ4;Map1lc3b|Q9CQV6;Prpsap1|Q9D0M1;Prps1|Q9D7G0;Psma4|Q9R1P0;Psma7|Q9Z2U0</t>
+    <t xml:space="preserve">|Q9D7G0;|Q9CQV6;|Q9Z2U0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|G5E870;|O35593;|O55176;|O70435;|O88685;|P25233;|P46471;|P49722;|P62196;|P62334;|P70195;|P99026;|Q3TXS7;|Q3U3E2;|Q60692;|Q7TSH4;|Q8BG32;|Q8BYK5;|Q8CCJ4;|Q9CQV6;|Q9D0M1;|Q9D7G0;|Q9R1P0;|Q9Z2U0</t>
   </si>
   <si>
     <t xml:space="preserve">M181</t>
   </si>
   <si>
-    <t xml:space="preserve">Elp3|Q9CZX0;Psmb2|Q9R1P3;Osbpl6|Q8BXR9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psmd4|O35226;Map1b|P14873;Agtpbp1|Q641K1;Elp1|Q7TT37;Usp8|Q80U87;Eif2a|Q8BJW6;Osbpl6|Q8BXR9;Txnl1|Q8CDN6;Dis3l2|Q8CI75;Psmd2|Q8VDM4;Clip1|Q922J3;Trim33|Q99PP7;Elp3|Q9CZX0;Armc8|Q9DBR3;Adrm1|Q9JKV1;Psmb2|Q9R1P3</t>
+    <t xml:space="preserve">|Q9CZX0;|Q9R1P3;|Q8BXR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35226;|P14873;|Q641K1;|Q7TT37;|Q80U87;|Q8BJW6;|Q8BXR9;|Q8CDN6;|Q8CI75;|Q8VDM4;|Q922J3;|Q99PP7;|Q9CZX0;|Q9DBR3;|Q9JKV1;|Q9R1P3</t>
   </si>
   <si>
     <t xml:space="preserve">M182</t>
   </si>
   <si>
-    <t xml:space="preserve">Sphk2|Q9JIA7;Mib2|Q8R516;Git2|Q9JLQ2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sec14l1|A8Y5H7;Becn1|O88597;Polr2a|P08775;Actr1a|P61164;Rps18|P62270;Agap1|Q8BXK8;Nkiras1|Q8CEC5;Wdr11|Q8K1X1;Mib2|Q8R516;Prpsap2|Q8R574;Phkg2|Q9DB30;Inpp4a|Q9EPW0;Sphk2|Q9JIA7;Git2|Q9JLQ2</t>
+    <t xml:space="preserve">|Q9JIA7;|Q8R516;|Q9JLQ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A8Y5H7;|O88597;|P08775;|P61164;|P62270;|Q8BXK8;|Q8CEC5;|Q8K1X1;|Q8R516;|Q8R574;|Q9DB30;|Q9EPW0;|Q9JIA7;|Q9JLQ2</t>
   </si>
   <si>
     <t xml:space="preserve">M183</t>
   </si>
   <si>
-    <t xml:space="preserve">Eml3|Q8VC03;Stat2|Q9WVL2;Elp5|Q99L85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ttc39a|A2ACP1;Ikbkb|O88351;Wnk1|P83741;Tgfbrap1|Q3UR70;Lrrc47|Q505F5;Hbs1l|Q69ZS7;Arhgef18|Q6P9R4;Gatd1|Q8BFQ8;Ttc26|Q8BS45;Eml3|Q8VC03;Elp5|Q99L85;Stat2|Q9WVL2</t>
+    <t xml:space="preserve">|Q8VC03;|Q9WVL2;|Q99L85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2ACP1;|O88351;|P83741;|Q3UR70;|Q505F5;|Q69ZS7;|Q6P9R4;|Q8BFQ8;|Q8BS45;|Q8VC03;|Q99L85;|Q9WVL2</t>
   </si>
   <si>
     <t xml:space="preserve">M184</t>
   </si>
   <si>
-    <t xml:space="preserve">Map1lc3a|Q91VR7;Eef1aknmt|Q91YR5;Dctn2|Q99KJ8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cdk14|O35495;Plin4|O88492;Psmd7|P26516;Scube1|Q6NZL8;Dpp9|Q8BVG4;Map1lc3a|Q91VR7;Elp2|Q91WG4;Eef1aknmt|Q91YR5;Dctn2|Q99KJ8;Polr3e|Q9CZT4</t>
+    <t xml:space="preserve">|Q91VR7;|Q91YR5;|Q99KJ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35495;|O88492;|P26516;|Q6NZL8;|Q8BVG4;|Q91VR7;|Q91WG4;|Q91YR5;|Q99KJ8;|Q9CZT4</t>
   </si>
   <si>
     <t xml:space="preserve">M185</t>
   </si>
   <si>
-    <t xml:space="preserve">Kcnq5|Q9JK45;Syt11|Q9R0N3;Saraf|Q8R3Q0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vps41|Q5KU39;Vps39|Q8R5L3;Ptprk|P35822;Vamp7|P70280;Pip4p1|Q3TWL2;Lrig2|Q52KR2;Kxd1|Q80XH1;Mon1b|Q8BMQ8;Derl2|Q8BNI4;Disp2|Q8CIP5;Slc22a17|Q9D9E0;Kcnq5|Q9JK45;Syt11|Q9R0N3;Dhcr7|O88455;Nsf|P46460;Pi4k2a|Q2TBE6;Srebf2|Q3U1N2;Pgap1|Q3UUQ7;Tapt1|Q4VBD2;Ankrd46|Q8BTZ5;Ufl1|Q8CCJ3;Saraf|Q8R3Q0;Slc12a9|Q99MR3;Tmem43|Q9DBS1;Bok|O35425;Clcn6|O35454;Atp9a|O70228</t>
+    <t xml:space="preserve">|Q9JK45;|Q9R0N3;|Q8R3Q0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q5KU39;|Q8R5L3;|P35822;|P70280;|Q3TWL2;|Q52KR2;|Q80XH1;|Q8BMQ8;|Q8BNI4;|Q8CIP5;|Q9D9E0;|Q9JK45;|Q9R0N3;|O88455;|P46460;|Q2TBE6;|Q3U1N2;|Q3UUQ7;|Q4VBD2;|Q8BTZ5;|Q8CCJ3;|Q8R3Q0;|Q99MR3;|Q9DBS1;|O35425;|O35454;|O70228</t>
   </si>
   <si>
     <t xml:space="preserve">M186</t>
   </si>
   <si>
-    <t xml:space="preserve">Tor1a|Q9ER39;Hsd17b11|Q9EQ06;Cyp4f14|Q9EP75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptpn2|Q06180;Lemd2|Q6DVA0;Mboat2|Q8R3I2;Emc6|Q9CQW0;Cyp4f14|Q9EP75;Cln8|Q9QUK3;Fbxl20|Q9CZV8;Tmem229a|B9EJI9;Bcl2|P10417;Faf2|Q3TDN2;Chpt1|Q8C025;Tlcd1|Q99JT6;Prxl2a|Q9CYH2;Tor1a|Q9ER39;Smpd2|O70572;Aldh3a2|P47740;Chp1|P61022;Slc27a1|Q60714;Adam9|Q61072;Sgpl1|Q8R0X7;Acsl6|Q91WC3;Abhd3|Q91ZH7;Hsd17b11|Q9EQ06;Erg28|Q9ERY9</t>
+    <t xml:space="preserve">|Q9ER39;|Q9EQ06;|Q9EP75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q06180;|Q6DVA0;|Q8R3I2;|Q9CQW0;|Q9EP75;|Q9QUK3;|Q9CZV8;|B9EJI9;|P10417;|Q3TDN2;|Q8C025;|Q99JT6;|Q9CYH2;|Q9ER39;|O70572;|P47740;|P61022;|Q60714;|Q61072;|Q8R0X7;|Q91WC3;|Q91ZH7;|Q9EQ06;|Q9ERY9</t>
   </si>
   <si>
     <t xml:space="preserve">M187</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc35f6|Q8VE96;Tspan13|Q9D8C2;Syt13|Q9EQT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penk|P22005;Rab2a|P53994;Syt13|Q9EQT6;Man1a|P45700;Stmn2|P55821;Slc45a1|Q8BIV7;Slc35f6|Q8VE96;Tmub1|Q9JMG3;Pdyn|O35417;Napb|P28663;Pam|P97467;Pid1|Q3UBG2;Slc2a13|Q3UHK1;Ankrd13c|Q3UX43;Npdc1|Q64322;St8sia3|Q64689;Svop|Q8BFT9;Arl8a|Q8VEH3;Rab14|Q91V41;Tmem50b|Q9D1X9;Tspan13|Q9D8C2</t>
+    <t xml:space="preserve">|Q8VE96;|Q9D8C2;|Q9EQT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P22005;|P53994;|Q9EQT6;|P45700;|P55821;|Q8BIV7;|Q8VE96;|Q9JMG3;|O35417;|P28663;|P97467;|Q3UBG2;|Q3UHK1;|Q3UX43;|Q64322;|Q64689;|Q8BFT9;|Q8VEH3;|Q91V41;|Q9D1X9;|Q9D8C2</t>
   </si>
   <si>
     <t xml:space="preserve">M188</t>
   </si>
   <si>
-    <t xml:space="preserve">Nat8f1|Q9JIZ0;Fads2|Q9Z0R9;Sec11a|Q9R0P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyb5a|P56395;Pbxip1|Q3TVI8;Mb21d2|Q8C525;Dner|Q8JZM4;Cers1|P27545;Unc79|Q0KK59;Lmf1|Q3U3R4;Nalcn|Q8BXR5;Hacd2|Q9D3B1;Sec11a|Q9R0P6;Tapbp|Q9R233;Canx|P35564;Magt1|Q9CQY5;Hhatl|Q9D1G3;Scamp2|Q9ERN0;Nat8f1|Q9JIZ0;Fads2|Q9Z0R9</t>
+    <t xml:space="preserve">|Q9JIZ0;|Q9Z0R9;|Q9R0P6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P56395;|Q3TVI8;|Q8C525;|Q8JZM4;|P27545;|Q0KK59;|Q3U3R4;|Q8BXR5;|Q9D3B1;|Q9R0P6;|Q9R233;|P35564;|Q9CQY5;|Q9D1G3;|Q9ERN0;|Q9JIZ0;|Q9Z0R9</t>
   </si>
   <si>
     <t xml:space="preserve">M189</t>
   </si>
   <si>
-    <t xml:space="preserve">Ptgfrn|Q9WV91;Rab1b|Q9D1G1;Itch|Q8C863</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tmem151b|Q68FE7;Ptgfrn|Q9WV91;Cckbr|P56481;Rab5b|P61021;Rab1b|Q9D1G1;Bace1|P56818;Rundc3b|Q6PDC0;Lrrc1|Q80VQ1;Itch|Q8C863;Vps26a|P40336;Bloc1s3|Q5U5M8</t>
+    <t xml:space="preserve">|Q9WV91;|Q9D1G1;|Q8C863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q68FE7;|Q9WV91;|P56481;|P61021;|Q9D1G1;|P56818;|Q6PDC0;|Q80VQ1;|Q8C863;|P40336;|Q5U5M8</t>
   </si>
   <si>
     <t xml:space="preserve">M190</t>
   </si>
   <si>
-    <t xml:space="preserve">Pip4p2|Q9CZX7;Pign|Q9R1S3;Snap47|Q8R570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dpp4|P28843;Fdft1|P53798;Rab2b|P59279;Rab9b|Q8BHH2;Snap47|Q8R570;Clip3|B9EHT4;Pnpla7|A2AJ88;Tmed8|Q3UHI4;Pip4p2|Q9CZX7;Pign|Q9R1S3</t>
+    <t xml:space="preserve">|Q9CZX7;|Q9R1S3;|Q8R570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P28843;|P53798;|P59279;|Q8BHH2;|Q8R570;|B9EHT4;|A2AJ88;|Q3UHI4;|Q9CZX7;|Q9R1S3</t>
   </si>
   <si>
     <t xml:space="preserve">M191</t>
   </si>
   <si>
-    <t xml:space="preserve">C1qtnf4|Q8R066;Abcc5|Q9R1X5;Stoml1|Q8CI66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ldlr|P35951;Soat1|Q61263;Epha7|Q61772;C1qtnf4|Q8R066;Araf|P04627;Prkce|P16054;Dgcr2|P98154;Ube2j2|Q6P073;Stoml1|Q8CI66;Abcc5|Q9R1X5</t>
+    <t xml:space="preserve">|Q8R066;|Q9R1X5;|Q8CI66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P35951;|Q61263;|Q61772;|Q8R066;|P04627;|P16054;|P98154;|Q6P073;|Q8CI66;|Q9R1X5</t>
   </si>
   <si>
     <t xml:space="preserve">M192</t>
   </si>
   <si>
-    <t xml:space="preserve">Stx12|Q9ER00;Ggt7|Q99JP7;Plxdc2|Q9DC11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fkbp8|O35465;Rab4b|Q91ZR1;Ggt7|Q99JP7;Napa|Q9DB05;Vti1a|O89116;Plxdc2|Q9DC11;Stx12|Q9ER00</t>
+    <t xml:space="preserve">|Q9ER00;|Q99JP7;|Q9DC11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35465;|Q91ZR1;|Q99JP7;|Q9DB05;|O89116;|Q9DC11;|Q9ER00</t>
   </si>
   <si>
     <t xml:space="preserve">M193</t>
   </si>
   <si>
-    <t xml:space="preserve">D17H6S53E|Q9Z1R4;Tmem167|Q9CR64;Jph1|Q9ET80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mctp1|E9PV86;Ccdc136|Q3TVA9;Zfyve27|Q3TXX3;Reep5|Q60870;Ei24|Q61070;Tex2|Q6ZPJ0;C2cd2l|Q80X80;Reep1|Q8BGH4;Atl1|Q8BH66;Ldah|Q8BVA5;Acsl5|Q8JZR0;Rtn1|Q8K0T0;Reep2|Q8VCD6;Slc27a4|Q91VE0;Ncoa5|Q91W39;Rtn4|Q99P72;Retreg3|Q9CQV4;Tmem167|Q9CR64;Praf2|Q9JIG8;D17H6S53E|Q9Z1R4;Fkbp1b|Q9Z2I2;Atg9a|Q68FE2;Snx1|Q9WV80;Slmap|Q3URD3;Tmcc1|Q69ZZ6;Gpat4|Q8K2C8;Jph1|Q9ET80;Pdzd8|B9EJ80;Ctdnep1|Q3TP92;Arl6ip5|Q8R5J9</t>
+    <t xml:space="preserve">|Q9Z1R4;|Q9CR64;|Q9ET80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9PV86;|Q3TVA9;|Q3TXX3;|Q60870;|Q61070;|Q6ZPJ0;|Q80X80;|Q8BGH4;|Q8BH66;|Q8BVA5;|Q8JZR0;|Q8K0T0;|Q8VCD6;|Q91VE0;|Q91W39;|Q99P72;|Q9CQV4;|Q9CR64;|Q9JIG8;|Q9Z1R4;|Q9Z2I2;|Q68FE2;|Q9WV80;|Q3URD3;|Q69ZZ6;|Q8K2C8;|Q9ET80;|B9EJ80;|Q3TP92;|Q8R5J9</t>
   </si>
   <si>
     <t xml:space="preserve">M194</t>
   </si>
   <si>
-    <t xml:space="preserve">Hnrnpm|Q9D0E1;Khdrbs3|Q9R226;Hnrnpc|Q9Z204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osbpl8|B9EJ86;Ap1g1|P22892;Igf2r|Q07113;Trappc9|Q3U0M1;Map11|Q3UTZ3;Vezt|Q3ZK22;Raly|Q64012;Atl2|Q6PA06;Pitpnm2|Q6ZPQ6;Tmcc2|Q80W04;Rbm45|Q8BHN5;Snx14|Q8BHY8;Ralyl|Q8BTF8;Ncbp3|Q8BZR9;Myef2|Q8C854;Hnrnpl|Q8R081;Rbmxl1|Q91VM5;Hnrnpm|Q9D0E1;Sec23b|Q9D662;Fam241b|Q9D882;Khdrbs3|Q9R226;Hnrnpc|Q9Z204</t>
+    <t xml:space="preserve">|Q9D0E1;|Q9R226;|Q9Z204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B9EJ86;|P22892;|Q07113;|Q3U0M1;|Q3UTZ3;|Q3ZK22;|Q64012;|Q6PA06;|Q6ZPQ6;|Q80W04;|Q8BHN5;|Q8BHY8;|Q8BTF8;|Q8BZR9;|Q8C854;|Q8R081;|Q91VM5;|Q9D0E1;|Q9D662;|Q9D882;|Q9R226;|Q9Z204</t>
   </si>
   <si>
     <t xml:space="preserve">M195</t>
   </si>
   <si>
-    <t xml:space="preserve">Fyttd1|Q91Z49;Chtop|Q9CY57;Pcm1|Q9R0L6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thoc3|Q8VE80;Ryr2|E9Q401;Rab18|P35293;Sec23a|Q01405;Asphd1|Q2TA57;Esyt2|Q3TZZ7;Sec24a|Q3U2P1;Gba2|Q69ZF3;Cyp4x1|Q6A152;Snx13|Q6PHS6;Mib1|Q80SY4;Usp20|Q8C6M1;Casc3|Q8K3W3;Fyttd1|Q91Z49;Fgfr1op2|Q9CRA9;Chtop|Q9CY57;Mvp|Q9EQK5;Pcm1|Q9R0L6;Slc35g2|D3YVE8;Atp9b|P98195;Prrc1|Q3UPH1</t>
+    <t xml:space="preserve">|Q91Z49;|Q9CY57;|Q9R0L6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8VE80;|E9Q401;|P35293;|Q01405;|Q2TA57;|Q3TZZ7;|Q3U2P1;|Q69ZF3;|Q6A152;|Q6PHS6;|Q80SY4;|Q8C6M1;|Q8K3W3;|Q91Z49;|Q9CRA9;|Q9CY57;|Q9EQK5;|Q9R0L6;|D3YVE8;|P98195;|Q3UPH1</t>
   </si>
   <si>
     <t xml:space="preserve">M196</t>
   </si>
   <si>
-    <t xml:space="preserve">Snx2|Q9CWK8;Cyp2s1|Q9DBX6;Endod1|Q8C522</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esyt1|Q3U7R1;Fam57b|Q7TNV1;Tbc1d5|Q80XQ2;Vps26b|Q8C0E2;Endod1|Q8C522;Hdac11|Q91WA3;Cyp2s1|Q9DBX6;Slc27a2|O35488;Usp33|Q8R5K2;Snx2|Q9CWK8;Tacc2|Q9JJG0;Bag2|Q91YN9</t>
+    <t xml:space="preserve">|Q9CWK8;|Q9DBX6;|Q8C522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3U7R1;|Q7TNV1;|Q80XQ2;|Q8C0E2;|Q8C522;|Q91WA3;|Q9DBX6;|O35488;|Q8R5K2;|Q9CWK8;|Q9JJG0;|Q91YN9</t>
   </si>
   <si>
     <t xml:space="preserve">M197</t>
   </si>
   <si>
-    <t xml:space="preserve">Rtn3|Q9ES97;Arl6ip1|Q9JKW0;Snap29|Q9ERB0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scamp3|O35609;Trappc3|O55013;Snx25|Q3ZT31;Soga3|Q6NZL0;Snx19|Q6P4T1;Myo5a|Q99104;Snap29|Q9ERB0;Rtn3|Q9ES97;Ppp1r3f|Q9JIG4;Arl6ip1|Q9JKW0;Asphd2|Q80VP9;Retreg2|Q6NS82</t>
+    <t xml:space="preserve">|Q9ES97;|Q9JKW0;|Q9ERB0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35609;|O55013;|Q3ZT31;|Q6NZL0;|Q6P4T1;|Q99104;|Q9ERB0;|Q9ES97;|Q9JIG4;|Q9JKW0;|Q80VP9;|Q6NS82</t>
   </si>
   <si>
     <t xml:space="preserve">M198</t>
   </si>
   <si>
-    <t xml:space="preserve">Auh|Q9JLZ3;Dap3|Q9ER88;Sars2|Q9JJL8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tars2|Q3UQ84;Gcdh|Q60759;Glud1|P26443;Ckmt1|P30275;Acadvl|P50544;Mthfd1l|Q3V3R1;Ogdh|Q60597;Mrps27|Q8BK72;Mrps23|Q8VE22;Pccb|Q99MN9;Mrpl3|Q99N95;Mrpl24|Q9CQ06;Mrps22|Q9CXW2;Dlst|Q9D2G2;Mrps11|Q9DCA2;Sars2|Q9JJL8;Auh|Q9JLZ3;Nwd2|Q6P5U7;Pnpt1|Q8K1R3;Fastkd2|Q922E6;Gadd45gip1|Q9CR59;Mrps30|Q9D0G0;Mrpl2|Q9D773;Dap3|Q9ER88</t>
+    <t xml:space="preserve">|Q9JLZ3;|Q9ER88;|Q9JJL8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3UQ84;|Q60759;|P26443;|P30275;|P50544;|Q3V3R1;|Q60597;|Q8BK72;|Q8VE22;|Q99MN9;|Q99N95;|Q9CQ06;|Q9CXW2;|Q9D2G2;|Q9DCA2;|Q9JJL8;|Q9JLZ3;|Q6P5U7;|Q8K1R3;|Q922E6;|Q9CR59;|Q9D0G0;|Q9D773;|Q9ER88</t>
   </si>
   <si>
     <t xml:space="preserve">M199</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrpl19|Q9D338;1700021F05Rik|Q9CQF4;Mrps34|Q9JIK9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cisd3|B1AR13;Fam81a|Q3UXZ6;Coq6|Q8R1S0;1700021F05Rik|Q9CQF4;Ndufaf1|Q9CWX2;Shmt2|Q9CZN7;Mrps34|Q9JIK9;Bcat2|O35855;Clpp|O88696;Dbt|P53395;Mrps6|P58064;Coq9|Q8K1Z0;Mcat|Q8R3F5;Spryd4|Q91WK1;Mrpl44|Q9CY73;Mrpl19|Q9D338;Arhgap25|Q8BYW1</t>
+    <t xml:space="preserve">|Q9D338;|Q9CQF4;|Q9JIK9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B1AR13;|Q3UXZ6;|Q8R1S0;|Q9CQF4;|Q9CWX2;|Q9CZN7;|Q9JIK9;|O35855;|O88696;|P53395;|P58064;|Q8K1Z0;|Q8R3F5;|Q91WK1;|Q9CY73;|Q9D338;|Q8BYW1</t>
   </si>
   <si>
     <t xml:space="preserve">M200</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrpl40|Q9Z2Q5;Mrps9|Q9D7N3;Mrps15|Q9DC71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wdr47|Q8CGF6;Mrps21|P58059;Madd|Q80U28;Mrps26|Q80ZS3;Pcca|Q91ZA3;Wars2|Q9CYK1;Ssbp1|Q9CYR0;Mrpl28|Q9D1B9;Mrps9|Q9D7N3;Mrpl40|Q9Z2Q5;Selenow|P63300;Mrps35|Q8BJZ4;Mrpl11|Q9CQF0;Mrps15|Q9DC71;Mrpl39|Q9JKF7</t>
+    <t xml:space="preserve">|Q9Z2Q5;|Q9D7N3;|Q9DC71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q8CGF6;|P58059;|Q80U28;|Q80ZS3;|Q91ZA3;|Q9CYK1;|Q9CYR0;|Q9D1B9;|Q9D7N3;|Q9Z2Q5;|P63300;|Q8BJZ4;|Q9CQF0;|Q9DC71;|Q9JKF7</t>
   </si>
   <si>
     <t xml:space="preserve">M201</t>
   </si>
   <si>
-    <t xml:space="preserve">Anks1b|Q8BIZ1;Prickle2|Q80Y24;Shank2|Q80Z38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shank1|D3YZU1;Syngap1|F6SEU4;Dlg3|P70175;Arhgap44|Q5SSM3;Dlgap3|Q6PFD5;Prickle2|Q80Y24;Anks1b|Q8BIZ1;Nln|Q91YP2;Etl4|A2AQ25;Dlgap4|B1AZP2;Shank3|Q4ACU6;Mrps31|Q61733;Shank2|Q80Z38;Homer1|Q9Z2Y3</t>
+    <t xml:space="preserve">|Q8BIZ1;|Q80Y24;|Q80Z38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|D3YZU1;|F6SEU4;|P70175;|Q5SSM3;|Q6PFD5;|Q80Y24;|Q8BIZ1;|Q91YP2;|A2AQ25;|B1AZP2;|Q4ACU6;|Q61733;|Q80Z38;|Q9Z2Y3</t>
   </si>
   <si>
     <t xml:space="preserve">M202</t>
   </si>
   <si>
-    <t xml:space="preserve">Iscu|Q9D7P6;Dguok|Q9QX60;Ppa2|Q91VM9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs2|Q5NCE8;Pdhx|Q8BKZ9;Bckdha|P50136;Timm13|P62075;Afg1l|Q3V384;Supv3l1|Q80YD1;Slc25a16|Q8C0K5;Ppa2|Q91VM9;Rtn4ip1|Q924D0;Iscu|Q9D7P6;Cacng3|Q9JJV5;Dguok|Q9QX60</t>
+    <t xml:space="preserve">|Q9D7P6;|Q9QX60;|Q91VM9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q5NCE8;|Q8BKZ9;|P50136;|P62075;|Q3V384;|Q80YD1;|Q8C0K5;|Q91VM9;|Q924D0;|Q9D7P6;|Q9JJV5;|Q9QX60</t>
   </si>
   <si>
     <t xml:space="preserve">M203</t>
   </si>
   <si>
-    <t xml:space="preserve">Ecsit|Q9QZH6;Ndufa11|Q9D8B4;Timm22|Q9CQ85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clpb|Q60649;Msrb2|Q78J03;Maip1|Q8BHE8;Slc25a29|Q8BL03;Guf1|Q8C3X4;Pars2|Q8CFI5;Oxnad1|Q8VE38;Timm22|Q9CQ85;Ndufa11|Q9D8B4;Trmu|Q9DAT5;Acot2|Q9QYR9;Ecsit|Q9QZH6</t>
+    <t xml:space="preserve">|Q9QZH6;|Q9D8B4;|Q9CQ85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q60649;|Q78J03;|Q8BHE8;|Q8BL03;|Q8C3X4;|Q8CFI5;|Q8VE38;|Q9CQ85;|Q9D8B4;|Q9DAT5;|Q9QYR9;|Q9QZH6</t>
   </si>
   <si>
     <t xml:space="preserve">M204</t>
   </si>
   <si>
-    <t xml:space="preserve">Acox1|Q9R0H0;Acaa1a|Q921H8;Acad11|Q80XL6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phyh|O35386;Nudt19|P11930;Anxa6|P14824;Cat|P24270;Msn|P26041;Scp2|P32020;Anxa5|P48036;Hsd17b4|P51660;Abcd3|P55096;Hpcal1|P62748;Anxa11|P97384;Aqp1|Q02013;Osbp|Q3B7Z2;Acbd5|Q5XG73;Abcd2|Q61285;Acad11|Q80XL6;Cpne5|Q8JZW4;Acaa1a|Q921H8;Ddah2|Q99LD8;Tmem135|Q9CYV5;Tysnd1|Q9DBA6;Rilpl1|Q9JJC6;Acox1|Q9R0H0</t>
+    <t xml:space="preserve">|Q9R0H0;|Q921H8;|Q80XL6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35386;|P11930;|P14824;|P24270;|P26041;|P32020;|P48036;|P51660;|P55096;|P62748;|P97384;|Q02013;|Q3B7Z2;|Q5XG73;|Q61285;|Q80XL6;|Q8JZW4;|Q921H8;|Q99LD8;|Q9CYV5;|Q9DBA6;|Q9JJC6;|Q9R0H0</t>
   </si>
   <si>
     <t xml:space="preserve">M205</t>
   </si>
   <si>
-    <t xml:space="preserve">Atrn|Q9WU60;Gprin3|Q8BWS5;Rftn1|Q6A0D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akap5|D3YVF0;Anxa3|O35639;Itm2b|O89051;Cd55|Q61475;Spock1|Q62288;Rftn1|Q6A0D4;Gprin3|Q8BWS5;Actn2|Q9JI91;Atrn|Q9WU60;Gfra1|P97785;Epha5|Q60629;Omg|Q63912;Mgrn1|Q9D074</t>
+    <t xml:space="preserve">|Q9WU60;|Q8BWS5;|Q6A0D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|D3YVF0;|O35639;|O89051;|Q61475;|Q62288;|Q6A0D4;|Q8BWS5;|Q9JI91;|Q9WU60;|P97785;|Q60629;|Q63912;|Q9D074</t>
   </si>
   <si>
     <t xml:space="preserve">M206</t>
   </si>
   <si>
-    <t xml:space="preserve">Dtna|Q9D2N4;Tenm3|Q9WTS6;Ehhadh|Q9DBM2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dmd|P11531;Ezr|P26040;Rasa3|Q60790;Psap|Q61207;Snta1|Q61234;Dag1|Q62165;Nrcam|Q810U4;Fat3|Q8BNA6;Snx16|Q8C080;Sntb1|Q99L88;Dtna|Q9D2N4;Ehhadh|Q9DBM2;Tenm3|Q9WTS6</t>
+    <t xml:space="preserve">|Q9D2N4;|Q9WTS6;|Q9DBM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P11531;|P26040;|Q60790;|Q61207;|Q61234;|Q62165;|Q810U4;|Q8BNA6;|Q8C080;|Q99L88;|Q9D2N4;|Q9DBM2;|Q9WTS6</t>
   </si>
   <si>
     <t xml:space="preserve">M207</t>
   </si>
   <si>
-    <t xml:space="preserve">Pcnx3|Q8VI59;Tpbg|Q9Z0L0;Lrp4|Q8VI56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edil3|O35474;Clcn7|O70496;Ctnnal1|O88327;Cacna1h|O88427;Prkar1b|P12849;Slc4a2|P13808;Nsg2|P47759;Cxadr|P97792;Lrp4|Q8VI56;Pcnx3|Q8VI59;Tpbg|Q9Z0L0;Myorg|Q69ZQ1</t>
+    <t xml:space="preserve">|Q8VI59;|Q9Z0L0;|Q8VI56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35474;|O70496;|O88327;|O88427;|P12849;|P13808;|P47759;|P97792;|Q8VI56;|Q8VI59;|Q9Z0L0;|Q69ZQ1</t>
   </si>
   <si>
     <t xml:space="preserve">M208</t>
   </si>
   <si>
-    <t xml:space="preserve">Crybb1|Q9WVJ5;Gsdmd|Q9D8T2;Gns|Q8BFR4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin2|D3Z6Q9;Glb1|P23780;Myo1f|P70248;Lcp1|Q61233;Gsdmd|Q9D8T2;Plbd2|Q3TCN2;Cntfr|O88507;Ctsb|P10605;Actn1|Q7TPR4;Gns|Q8BFR4;Crybb1|Q9WVJ5;Man2b2|O54782</t>
+    <t xml:space="preserve">|Q9WVJ5;|Q9D8T2;|Q8BFR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|D3Z6Q9;|P23780;|P70248;|Q61233;|Q9D8T2;|Q3TCN2;|O88507;|P10605;|Q7TPR4;|Q8BFR4;|Q9WVJ5;|O54782</t>
   </si>
   <si>
     <t xml:space="preserve">M209</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc15a4|Q91W98;Tmem63a|Q91YT8;Tmem214|Q8BM55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sparc|P07214;Kcnj13|P86046;Stxbp2|Q64324;Slc15a4|Q91W98;Tmem63a|Q91YT8;Fam129a|Q3UW53;Tmem214|Q8BM55;Slc22a6|Q8VC69</t>
+    <t xml:space="preserve">|Q91W98;|Q91YT8;|Q8BM55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P07214;|P86046;|Q64324;|Q91W98;|Q91YT8;|Q3UW53;|Q8BM55;|Q8VC69</t>
   </si>
   <si>
     <t xml:space="preserve">M210</t>
   </si>
   <si>
-    <t xml:space="preserve">Dis3|Q9CSH3;Ints5|Q8CHT3;Usp45|Q8K387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhx8|A2A4P0;Lmo4|P61969;Snrpe|P62305;Frg1|P97376;Rp9|P97762;Wdr19|Q3UGF1;Peg3|Q3URU2;Zfp638|Q61464;Nudt16|Q6P3D0;Naa35|Q6PHQ8;Fhod3|Q76LL6;Med23|Q80YQ2;Unk|Q8BL48;Dop1a|Q8BL99;Leng8|Q8CBY3;Fam193a|Q8CGI1;Ints5|Q8CHT3;Usp45|Q8K387;Rpp25l|Q99JH1;Dis3|Q9CSH3;Gtf2e1|Q9D0D5;Rita1|Q9D1H0</t>
+    <t xml:space="preserve">|Q9CSH3;|Q8CHT3;|Q8K387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A4P0;|P61969;|P62305;|P97376;|P97762;|Q3UGF1;|Q3URU2;|Q61464;|Q6P3D0;|Q6PHQ8;|Q76LL6;|Q80YQ2;|Q8BL48;|Q8BL99;|Q8CBY3;|Q8CGI1;|Q8CHT3;|Q8K387;|Q99JH1;|Q9CSH3;|Q9D0D5;|Q9D1H0</t>
   </si>
   <si>
     <t xml:space="preserve">M211</t>
   </si>
   <si>
-    <t xml:space="preserve">Inpp5e|Q9JII1;Wdr24|Q8CFJ9;Ccdc124|Q9D8X2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nfx1|B1AY10;Kif1c|O35071;Tnk2|O54967;Crebbp|P45481;Ttc21b|Q0HA38;Dact3|Q0PHV7;Txlng|Q8BHN1;Cfap410|Q8C6G1;Wdr24|Q8CFJ9;Pno1|Q9CPS7;Nkiras2|Q9CR56;Sesn3|Q9CYP7;Ccdc124|Q9D8X2;Inpp5e|Q9JII1</t>
+    <t xml:space="preserve">|Q9JII1;|Q8CFJ9;|Q9D8X2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B1AY10;|O35071;|O54967;|P45481;|Q0HA38;|Q0PHV7;|Q8BHN1;|Q8C6G1;|Q8CFJ9;|Q9CPS7;|Q9CR56;|Q9CYP7;|Q9D8X2;|Q9JII1</t>
   </si>
   <si>
     <t xml:space="preserve">M212</t>
   </si>
   <si>
-    <t xml:space="preserve">Exosc5|Q9CRA8;Ddx21|Q9JIK5;Thap11|Q9JJD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralgapa2|A3KGS3;Terf2|O35144;Spata5|Q3UMC0;Scaf8|Q6DID3;Samd4|Q8CBY1;Ddx18|Q8K363;Rbm4b|Q8VE92;Wac|Q924H7;Map4k3|Q99JP0;Exosc5|Q9CRA8;Ddx21|Q9JIK5;Thap11|Q9JJD0</t>
+    <t xml:space="preserve">|Q9CRA8;|Q9JIK5;|Q9JJD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A3KGS3;|O35144;|Q3UMC0;|Q6DID3;|Q8CBY1;|Q8K363;|Q8VE92;|Q924H7;|Q99JP0;|Q9CRA8;|Q9JIK5;|Q9JJD0</t>
   </si>
   <si>
     <t xml:space="preserve">M213</t>
   </si>
   <si>
-    <t xml:space="preserve">Fam50a|Q9WV03;Fbll1|Q80WS3;Zfp593|Q9DB42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rngtt|O55236;Rps17|P63276;G3bp1|P97855;Selenoh|Q3UQA7;Rnf20|Q5DTM8;Fbll1|Q80WS3;Camta2|Q80Y50;Gprasp2|Q8BUY8;Zfp593|Q9DB42;Fam50a|Q9WV03</t>
+    <t xml:space="preserve">|Q9WV03;|Q80WS3;|Q9DB42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55236;|P63276;|P97855;|Q3UQA7;|Q5DTM8;|Q80WS3;|Q80Y50;|Q8BUY8;|Q9DB42;|Q9WV03</t>
   </si>
   <si>
     <t xml:space="preserve">M214</t>
   </si>
   <si>
-    <t xml:space="preserve">Ebna1bp2|Q9D903;Nup214|Q80U93;Smarca5|Q91ZW3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Per1|O35973;Depdc5|P61460;Hivep2|Q3UHF7;Top2b|Q64511;Pds5a|Q6A026;Nup214|Q80U93;Mtmr3|Q8K296;Smarca5|Q91ZW3;Exosc4|Q921I9;Ebna1bp2|Q9D903</t>
+    <t xml:space="preserve">|Q9D903;|Q80U93;|Q91ZW3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35973;|P61460;|Q3UHF7;|Q64511;|Q6A026;|Q80U93;|Q8K296;|Q91ZW3;|Q921I9;|Q9D903</t>
   </si>
   <si>
     <t xml:space="preserve">M215</t>
   </si>
   <si>
-    <t xml:space="preserve">Syt6|Q9R0N8;Csnk1e|Q9JMK2;Rasgrp1|Q9Z1S3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chadl|E9Q7T7;Tanc1|Q0VGY8;Pdap1|Q3UHX2;Shb|Q6PD21;Rpgrip1l|Q8CG73;Cdk17|Q8K0D0;Csnk1e|Q9JMK2;Syt6|Q9R0N8;Rasgrp1|Q9Z1S3</t>
+    <t xml:space="preserve">|Q9R0N8;|Q9JMK2;|Q9Z1S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9Q7T7;|Q0VGY8;|Q3UHX2;|Q6PD21;|Q8CG73;|Q8K0D0;|Q9JMK2;|Q9R0N8;|Q9Z1S3</t>
   </si>
   <si>
     <t xml:space="preserve">M216</t>
   </si>
   <si>
-    <t xml:space="preserve">Ddx56|Q9D0R4;Wdr6|Q99ME2;Rfc4|Q99J62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nek1|P51954;Rps29|P62274;Spin1|Q61142;Rad21|Q61550;Tspyl2|Q7TQI8;Rfc4|Q99J62;Wdr6|Q99ME2;Ddx56|Q9D0R4</t>
+    <t xml:space="preserve">|Q9D0R4;|Q99ME2;|Q99J62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P51954;|P62274;|Q61142;|Q61550;|Q7TQI8;|Q99J62;|Q99ME2;|Q9D0R4</t>
   </si>
   <si>
     <t xml:space="preserve">M217</t>
   </si>
   <si>
-    <t xml:space="preserve">Eif2ak4|Q9QZ05;Exosc1|Q9DAA6;Glyr1|Q922P9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bod1l|E9Q6J5;Ldb1|P70662;Rassf5|Q5EBH1;Trim25|Q61510;Peak1|Q69Z38;Ints7|Q7TQK1;Bbs9|Q811G0;Rae1|Q8C570;Mepce|Q8K3A9;Ahsa2|Q8N9S3;Ptov1|Q91VU8;Synpo2|Q91YE8;Glyr1|Q922P9;Aven|Q9D9K3;Exosc1|Q9DAA6;Dkc1|Q9ESX5;Eif2ak4|Q9QZ05</t>
+    <t xml:space="preserve">|Q9QZ05;|Q9DAA6;|Q922P9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|E9Q6J5;|P70662;|Q5EBH1;|Q61510;|Q69Z38;|Q7TQK1;|Q811G0;|Q8C570;|Q8K3A9;|Q8N9S3;|Q91VU8;|Q91YE8;|Q922P9;|Q9D9K3;|Q9DAA6;|Q9ESX5;|Q9QZ05</t>
   </si>
   <si>
     <t xml:space="preserve">M218</t>
   </si>
   <si>
-    <t xml:space="preserve">Myo9b|Q9QY06;Azi2|Q9QYP6;Pikfyve|Q9Z1T6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ppfibp2|O35711;Sos2|Q02384;Dennd5a|Q6PAL8;Cul9|Q80TT8;Ift57|Q8BXG3;Bbs2|Q9CWF6;Cyth1|Q9QX11;Myo9b|Q9QY06;Azi2|Q9QYP6;Pikfyve|Q9Z1T6</t>
+    <t xml:space="preserve">|Q9QY06;|Q9QYP6;|Q9Z1T6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35711;|Q02384;|Q6PAL8;|Q80TT8;|Q8BXG3;|Q9CWF6;|Q9QX11;|Q9QY06;|Q9QYP6;|Q9Z1T6</t>
   </si>
   <si>
     <t xml:space="preserve">M219</t>
   </si>
   <si>
-    <t xml:space="preserve">Srgap1|Q91Z69;Ift122|Q6NWV3;Ttc8|Q8VD72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nt5c1a|A3KFX0;Dlg5|E9Q9R9;Pik3r2|O08908;Pik3ca|P42337;Arpc4|P59999;Mtus2|Q3UHD3;Ift122|Q6NWV3;Ttc8|Q8VD72;Srgap1|Q91Z69</t>
+    <t xml:space="preserve">|Q91Z69;|Q6NWV3;|Q8VD72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A3KFX0;|E9Q9R9;|O08908;|P42337;|P59999;|Q3UHD3;|Q6NWV3;|Q8VD72;|Q91Z69</t>
   </si>
   <si>
     <t xml:space="preserve">M220</t>
   </si>
   <si>
-    <t xml:space="preserve">Hecw1|Q8K4P8;Rptor|Q8K4Q0;Khnyn|Q80U38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nudt18|Q3U2V3;Dvl3|Q61062;Map4k2|Q61161;Smad2|Q62432;Mtmr10|Q7TPM9;Khnyn|Q80U38;Rbsn|Q80Y56;Hecw1|Q8K4P8;Rptor|Q8K4Q0</t>
+    <t xml:space="preserve">|Q8K4P8;|Q8K4Q0;|Q80U38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q3U2V3;|Q61062;|Q61161;|Q62432;|Q7TPM9;|Q80U38;|Q80Y56;|Q8K4P8;|Q8K4Q0</t>
   </si>
   <si>
     <t xml:space="preserve">M221</t>
   </si>
   <si>
-    <t xml:space="preserve">Vps36|Q91XD6;Mtmr2|Q9Z2D1;Elac1|Q8VEB6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arfgef1|G3X9K3;Wwc2|Q6NXJ0;Pik3cb|Q8BTI9;AI837181|Q8VD62;Snrk|Q8VDU5;Elac1|Q8VEB6;Vps36|Q91XD6;Mtmr2|Q9Z2D1</t>
+    <t xml:space="preserve">|Q91XD6;|Q9Z2D1;|Q8VEB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|G3X9K3;|Q6NXJ0;|Q8BTI9;|Q8VD62;|Q8VDU5;|Q8VEB6;|Q91XD6;|Q9Z2D1</t>
   </si>
   <si>
     <t xml:space="preserve">M222</t>
   </si>
   <si>
-    <t xml:space="preserve">Set|Q9EQU5;Thumpd1|Q99J36;Btf3l4|Q9CQH7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pnisr|A2AJT4;Rtf1|A2AQ19;Anp32a|O35381;Supt5|O55201;Hbb-b1|P02088;Gc|P21614;Cbx3|P23198;Hdgf|P51859;Anp32e|P97822;Apoa1|Q00623;Nsun2|Q1HFZ0;Ogfod1|Q3U0K8;Hdgfl2|Q3UMU9;Pfas|Q5SUR0;Fam169a|Q5XG69;Ppm1g|Q61074;Nab2|Q61127;Itih2|Q61703;Fbxo22|Q78JE5;Fto|Q8BGW1;Prpf39|Q8K2Z2;Thumpd1|Q99J36;Btf3l4|Q9CQH7;Drap1|Q9D6N5;Set|Q9EQU5;Anp32b|Q9EST5;Dnajc7|Q9QYI3</t>
+    <t xml:space="preserve">|Q9EQU5;|Q99J36;|Q9CQH7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AJT4;|A2AQ19;|O35381;|O55201;|P02088;|P21614;|P23198;|P51859;|P97822;|Q00623;|Q1HFZ0;|Q3U0K8;|Q3UMU9;|Q5SUR0;|Q5XG69;|Q61074;|Q61127;|Q61703;|Q78JE5;|Q8BGW1;|Q8K2Z2;|Q99J36;|Q9CQH7;|Q9D6N5;|Q9EQU5;|Q9EST5;|Q9QYI3</t>
   </si>
   <si>
     <t xml:space="preserve">M223</t>
   </si>
   <si>
-    <t xml:space="preserve">Nrip2|Q9JHR9;2410004B18Rik|Q9CWU4;Sumo3|Q9Z172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cfdp1|O88271;Ttr|P07309;Ces1c|P23953;Ptma|P26350;Cdkn1b|P46414;Rad23a|P54726;Uevld|Q3U1V6;Qrich1|Q3UA37;Arhgap17|Q3UIA2;Spag9|Q58A65;Serpinf2|Q61247;Snd1|Q78PY7;Smap2|Q7TN29;Chmp2b|Q8BJF9;Nup54|Q8BTS4;Agfg1|Q8K2K6;Trf|Q921I1;Arfgap2|Q99K28;2410004B18Rik|Q9CWU4;Nrip2|Q9JHR9;Palmd|Q9JHU2;Enpp2|Q9R1E6;Sncg|Q9Z0F7;Sumo3|Q9Z172;Stk39|Q9Z1W9</t>
+    <t xml:space="preserve">|Q9JHR9;|Q9CWU4;|Q9Z172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88271;|P07309;|P23953;|P26350;|P46414;|P54726;|Q3U1V6;|Q3UA37;|Q3UIA2;|Q58A65;|Q61247;|Q78PY7;|Q7TN29;|Q8BJF9;|Q8BTS4;|Q8K2K6;|Q921I1;|Q99K28;|Q9CWU4;|Q9JHR9;|Q9JHU2;|Q9R1E6;|Q9Z0F7;|Q9Z172;|Q9Z1W9</t>
   </si>
   <si>
     <t xml:space="preserve">M224</t>
   </si>
   <si>
-    <t xml:space="preserve">Cthrc1|Q9D1D6;Ppp1r14a|Q91VC7;Serpina1b|P22599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eif6|O55135;Apoa4|P06728;Apoe|P08226;Sub1|P11031;Hspb1|P14602;Cst3|P21460;Serpina1b|P22599;Atxn10|P28658;Pltp|P55065;Serpina1d|Q00897;Gcc2|Q8CHG3;Ppp1r14a|Q91VC7;Hid1|Q8R1F6;Cthrc1|Q9D1D6</t>
+    <t xml:space="preserve">|Q9D1D6;|Q91VC7;|P22599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55135;|P06728;|P08226;|P11031;|P14602;|P21460;|P22599;|P28658;|P55065;|Q00897;|Q8CHG3;|Q91VC7;|Q8R1F6;|Q9D1D6</t>
   </si>
   <si>
     <t xml:space="preserve">M225</t>
   </si>
   <si>
-    <t xml:space="preserve">Nudt12|Q9DCN1;Sae1|Q9R1T2;Uba2|Q9Z1F9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sod3|O09164;Serpina1a|P07758;Ahsg|P29699;Serpinc1|P32261;Ppp1cc|P63087;Eloc|P83940;Papss1|Q60967;Ranbp3|Q9CT10;Nudt12|Q9DCN1;Sae1|Q9R1T2;Uba2|Q9Z1F9</t>
+    <t xml:space="preserve">|Q9DCN1;|Q9R1T2;|Q9Z1F9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O09164;|P07758;|P29699;|P32261;|P63087;|P83940;|Q60967;|Q9CT10;|Q9DCN1;|Q9R1T2;|Q9Z1F9</t>
   </si>
   <si>
     <t xml:space="preserve">M226</t>
   </si>
   <si>
-    <t xml:space="preserve">Trim44|Q9QXA7;Mtss1|Q8R1S4;Eps8l2|Q99K30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cdr2l|A2A6T1;Prkg1|P0C605;Car1|P13634;Car8|P28651;Rab6b|P61294;Gabpa|Q00422;Mtss1|Q8R1S4;Eps8l2|Q99K30;Dcps|Q9DAR7;Slc9a3r2|Q9JHL1;Trim44|Q9QXA7</t>
+    <t xml:space="preserve">|Q9QXA7;|Q8R1S4;|Q99K30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2A6T1;|P0C605;|P13634;|P28651;|P61294;|Q00422;|Q8R1S4;|Q99K30;|Q9DAR7;|Q9JHL1;|Q9QXA7</t>
   </si>
   <si>
     <t xml:space="preserve">M227</t>
   </si>
   <si>
-    <t xml:space="preserve">Tubgcp4|Q9D4F8;Ascc1|Q9D8Z1;Spats2|Q8K1N4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virma|A2AIV2;Trmt1l|A2RSY6;Tubgcp6|G5E8P0;Ythdf1|P59326;Rims4|P60191;Snrpd1|P62315;Gtpbp2|Q3UJK4;Zscan26|Q5RJ54;Tsr1|Q5SWD9;Samhd1|Q60710;Rexo4|Q6PAQ4;Btbd10|Q80X66;Krr1|Q8BGA5;Larp4|Q8BWW4;Zc3h6|Q8BYK8;Spats2|Q8K1N4;Kctd10|Q922M3;Cdk9|Q99J95;Dimt1|Q9D0D4;Tubgcp4|Q9D4F8;Ascc1|Q9D8Z1</t>
+    <t xml:space="preserve">|Q9D4F8;|Q9D8Z1;|Q8K1N4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AIV2;|A2RSY6;|G5E8P0;|P59326;|P60191;|P62315;|Q3UJK4;|Q5RJ54;|Q5SWD9;|Q60710;|Q6PAQ4;|Q80X66;|Q8BGA5;|Q8BWW4;|Q8BYK8;|Q8K1N4;|Q922M3;|Q99J95;|Q9D0D4;|Q9D4F8;|Q9D8Z1</t>
   </si>
   <si>
     <t xml:space="preserve">M228</t>
   </si>
   <si>
-    <t xml:space="preserve">Dgkz|Q80UP3;Sh3bp4|Q921I6;Dip2a|Q8BWT5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptpn3|A2ALK8;Ankrd63|A2ARS0;Nhsl2|B1AXH1;Rasgrf1|P27671;Sbds|P70122;Fmn1|Q05860;Ppp1r21|Q3TDD9;Dip2b|Q3UH60;Ksr2|Q3UVC0;Grb10|Q60760;Smarcd1|Q61466;Dgkb|Q6NS52;Phldb1|Q6PDH0;R3hdm2|Q80TM6;Dgkz|Q80UP3;Dip2a|Q8BWT5;Sbk1|Q8QZX0;Sh3bp4|Q921I6;Strn3|Q9ERG2</t>
+    <t xml:space="preserve">|Q80UP3;|Q921I6;|Q8BWT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2ALK8;|A2ARS0;|B1AXH1;|P27671;|P70122;|Q05860;|Q3TDD9;|Q3UH60;|Q3UVC0;|Q60760;|Q61466;|Q6NS52;|Q6PDH0;|Q80TM6;|Q80UP3;|Q8BWT5;|Q8QZX0;|Q921I6;|Q9ERG2</t>
   </si>
   <si>
     <t xml:space="preserve">M229</t>
   </si>
   <si>
-    <t xml:space="preserve">Rrs1|Q9CYH6;Ddx24|Q9ESV0;Cmss1|Q9CZT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dcaf7|P61963;Ewsr1|Q61545;Cdk13|Q69ZA1;Cdk19|Q8BWD8;Nop14|Q8R3N1;Oard1|Q8R5F3;Coro6|Q920M5;Fam76a|Q922G2;2310033P09Rik|Q99LX5;Rrs1|Q9CYH6;Cmss1|Q9CZT6;Ppih|Q9D868;Leng1|Q9DB98;Ddx24|Q9ESV0;Mta2|Q9R190</t>
+    <t xml:space="preserve">|Q9CYH6;|Q9ESV0;|Q9CZT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P61963;|Q61545;|Q69ZA1;|Q8BWD8;|Q8R3N1;|Q8R5F3;|Q920M5;|Q922G2;|Q99LX5;|Q9CYH6;|Q9CZT6;|Q9D868;|Q9DB98;|Q9ESV0;|Q9R190</t>
   </si>
   <si>
     <t xml:space="preserve">M230</t>
   </si>
   <si>
-    <t xml:space="preserve">Nek7|Q9ES74;Grb14|Q9JLM9;Ercc4|Q9QZD4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tspyl1|O88852;Rps13|P62301;Morc2a|Q69ZX6;Fbxo11|Q7TPD1;Exosc3|Q7TQK4;Tlk1|Q8C0V0;Nmd3|Q99L48;Ints11|Q9CWS4;Ppil4|Q9CXG3;Nek7|Q9ES74;Exosc9|Q9JHI7;Grb14|Q9JLM9;Ercc4|Q9QZD4</t>
+    <t xml:space="preserve">|Q9ES74;|Q9JLM9;|Q9QZD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88852;|P62301;|Q69ZX6;|Q7TPD1;|Q7TQK4;|Q8C0V0;|Q99L48;|Q9CWS4;|Q9CXG3;|Q9ES74;|Q9JHI7;|Q9JLM9;|Q9QZD4</t>
   </si>
   <si>
     <t xml:space="preserve">M231</t>
   </si>
   <si>
-    <t xml:space="preserve">Pnkp|Q9JLV6;Dbr1|Q923B1;Neurl1a|Q923S6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hap1|O35668;Bysl|O54825;Uri1|Q3TLD5;Ccnh|Q61458;Ddx55|Q6ZPL9;Heatr3|Q8BQM4;Dbr1|Q923B1;Neurl1a|Q923S6;Pnkp|Q9JLV6</t>
+    <t xml:space="preserve">|Q9JLV6;|Q923B1;|Q923S6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35668;|O54825;|Q3TLD5;|Q61458;|Q6ZPL9;|Q8BQM4;|Q923B1;|Q923S6;|Q9JLV6</t>
   </si>
   <si>
     <t xml:space="preserve">M232</t>
   </si>
   <si>
-    <t xml:space="preserve">Eif4h|Q9WUK2;Nle1|Q8VEJ4;Exosc8|Q9D753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matk|P41242;Nfic|P70255;Hexim2|Q3TVI4;Spg11|Q3UHA3;Ncor1|Q60974;Ahi1|Q8K3E5;Nle1|Q8VEJ4;Exosc8|Q9D753;Eif4h|Q9WUK2</t>
+    <t xml:space="preserve">|Q9WUK2;|Q8VEJ4;|Q9D753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P41242;|P70255;|Q3TVI4;|Q3UHA3;|Q60974;|Q8K3E5;|Q8VEJ4;|Q9D753;|Q9WUK2</t>
   </si>
   <si>
     <t xml:space="preserve">M233</t>
   </si>
   <si>
-    <t xml:space="preserve">Srgap2|Q91Z67;Kank3|Q9Z1P7;D6Wsu163e|Q91YN0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dock11|A2AF47;Strn4|P58404;Psd3|Q2PFD7;Kazn|Q69ZS8;Sowaha|Q8BLS7;D6Wsu163e|Q91YN0;Srgap2|Q91Z67;Kank3|Q9Z1P7;Hdac5|Q9Z2V6</t>
+    <t xml:space="preserve">|Q91Z67;|Q9Z1P7;|Q91YN0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AF47;|P58404;|Q2PFD7;|Q69ZS8;|Q8BLS7;|Q91YN0;|Q91Z67;|Q9Z1P7;|Q9Z2V6</t>
   </si>
   <si>
     <t xml:space="preserve">M234</t>
   </si>
   <si>
-    <t xml:space="preserve">Mlst8|Q9DCJ1;Wwp2|Q9DBH0;Tns2|Q8CGB6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plekhd1|B2RPU2;Tent4b|Q68ED3;Tbck|Q8BM85;Tns2|Q8CGB6;Wwp2|Q9DBH0;Mlst8|Q9DCJ1;Itsn1|Q9Z0R4</t>
+    <t xml:space="preserve">|Q9DCJ1;|Q9DBH0;|Q8CGB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RPU2;|Q68ED3;|Q8BM85;|Q8CGB6;|Q9DBH0;|Q9DCJ1;|Q9Z0R4</t>
   </si>
   <si>
     <t xml:space="preserve">M235</t>
   </si>
   <si>
-    <t xml:space="preserve">Ehd3|Q9QXY6;Crtac1|Q8R555;Syt10|Q9R0N4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adgrl3|Q80TS3;Ptp4a3|Q9D658;Slc24a4|Q8CGQ8;Ptprt|Q99M80;Fam13c|Q9DBR2;Cpne8|Q9DC53;Syt10|Q9R0N4;Ephb6|O08644;Gfra2|O08842;Ptprf|A2A8L5;Kcnh1|Q60603;Kirrel3|Q8BR86;Rtn4rl1|Q8K0S5;Crtac1|Q8R555;Ehd3|Q9QXY6;Hexa|P29416;Rtn4rl2|Q7M6Z0</t>
+    <t xml:space="preserve">|Q9QXY6;|Q8R555;|Q9R0N4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q80TS3;|Q9D658;|Q8CGQ8;|Q99M80;|Q9DBR2;|Q9DC53;|Q9R0N4;|O08644;|O08842;|A2A8L5;|Q60603;|Q8BR86;|Q8K0S5;|Q8R555;|Q9QXY6;|P29416;|Q7M6Z0</t>
   </si>
   <si>
     <t xml:space="preserve">M236</t>
   </si>
   <si>
-    <t xml:space="preserve">Pde2a|Q922S4;Fmnl1|Q9JL26;Slc7a8|Q9QXW9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slc2a3|P32037;Pi4ka|E9Q3L2;Ttc7b|E9Q6P5;Tenm4|Q3UHK6;Tbc1d24|Q3UUG6;Fam126b|Q8C729;Slc14a1|Q8VHL0;Pde2a|Q922S4;Fmnl1|Q9JL26;Src|P05480;Prrt3|Q6PE13;Efr3b|Q6ZQ18;Shisa4|Q8CA71;Tmem178|Q9CZ16;Apbb1|Q9QXJ1;Unc5a|Q8K1S4;Slc7a8|Q9QXW9</t>
+    <t xml:space="preserve">|Q922S4;|Q9JL26;|Q9QXW9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P32037;|E9Q3L2;|E9Q6P5;|Q3UHK6;|Q3UUG6;|Q8C729;|Q8VHL0;|Q922S4;|Q9JL26;|P05480;|Q6PE13;|Q6ZQ18;|Q8CA71;|Q9CZ16;|Q9QXJ1;|Q8K1S4;|Q9QXW9</t>
   </si>
   <si>
     <t xml:space="preserve">M237</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc38a3|Q9DCP2;Glipr2|Q9CYL5;Fibp|Q9JI19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entpd2|O55026;Slc1a2|P43006;Cntn4|Q69Z26;C2cd5|Q7TPS5;Rftn2|Q8CHX7;Gpr37l1|Q99JG2;Glipr2|Q9CYL5;Slc38a3|Q9DCP2;Fibp|Q9JI19;Ttyh1|Q9D3A9;Vcam1|P29533;Rhbdf1|Q6PIX5;Nrxn1|Q9CS84;Fmn2|Q9JL04;Slc7a5|Q9Z127;Ednrb|P48302</t>
+    <t xml:space="preserve">|Q9DCP2;|Q9CYL5;|Q9JI19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O55026;|P43006;|Q69Z26;|Q7TPS5;|Q8CHX7;|Q99JG2;|Q9CYL5;|Q9DCP2;|Q9JI19;|Q9D3A9;|P29533;|Q6PIX5;|Q9CS84;|Q9JL04;|Q9Z127;|P48302</t>
   </si>
   <si>
     <t xml:space="preserve">M238</t>
   </si>
   <si>
-    <t xml:space="preserve">Lancl2|Q9JJK2;Necab2|Q91ZP9;Prkag2|Q91WG5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngp|O08692;Tbc1d10a|P58802;Pdlim4|P70271;Rap1gap2|Q5SVL6;Doc2a|Q7TNF0;Lrsam1|Q80ZI6;Necab2|Q91ZP9;Cetn2|Q9R1K9;Prkaa2|Q8BRK8;Prkag2|Q91WG5;Lancl2|Q9JJK2;Prkab2|Q6PAM0;Cacnb1|Q8R3Z5</t>
+    <t xml:space="preserve">|Q9JJK2;|Q91ZP9;|Q91WG5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08692;|P58802;|P70271;|Q5SVL6;|Q7TNF0;|Q80ZI6;|Q91ZP9;|Q9R1K9;|Q8BRK8;|Q91WG5;|Q9JJK2;|Q6PAM0;|Q8R3Z5</t>
   </si>
   <si>
     <t xml:space="preserve">M239</t>
   </si>
   <si>
-    <t xml:space="preserve">Hagh|Q99KB8;Plpbp|Q9Z2Y8;Naprt|Q8CC86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arhgef10l|A2AWP8;Pgam2|O70250;Nme1|P15532;Kif1a|P33173;Nme2|Q01768;Naprt|Q8CC86;6430548M08Rik|Q8R0A7;Nit1|Q8VDK1;Hagh|Q99KB8;Plpbp|Q9Z2Y8;Pde4a|O89084</t>
+    <t xml:space="preserve">|Q99KB8;|Q9Z2Y8;|Q8CC86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2AWP8;|O70250;|P15532;|P33173;|Q01768;|Q8CC86;|Q8R0A7;|Q8VDK1;|Q99KB8;|Q9Z2Y8;|O89084</t>
   </si>
   <si>
     <t xml:space="preserve">M240</t>
   </si>
   <si>
-    <t xml:space="preserve">Rap2a|Q80ZJ1;Ctsf|Q9R013;Nrxn3|Q6P9K9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabra2|P26048;Ppt1|O88531;Adora1|Q60612;Nrxn3|Q6P9K9;Rap2a|Q80ZJ1;Lrfn3|Q8BLY3;Ctsf|Q9R013</t>
+    <t xml:space="preserve">|Q80ZJ1;|Q9R013;|Q6P9K9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P26048;|O88531;|Q60612;|Q6P9K9;|Q80ZJ1;|Q8BLY3;|Q9R013</t>
   </si>
   <si>
     <t xml:space="preserve">M241</t>
   </si>
   <si>
-    <t xml:space="preserve">Adam17|Q9Z0F8;Fxyd6|Q9D164;2810459M11Rik|Q9CYS6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prmt8|Q6PAK3;2810459M11Rik|Q9CYS6;Tbc1d8b|A3KGB4;Gng3|P63216;Fxyd6|Q9D164;Adam17|Q9Z0F8</t>
+    <t xml:space="preserve">|Q9Z0F8;|Q9D164;|Q9CYS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q6PAK3;|Q9CYS6;|A3KGB4;|P63216;|Q9D164;|Q9Z0F8</t>
   </si>
   <si>
     <t xml:space="preserve">M242</t>
   </si>
   <si>
-    <t xml:space="preserve">Sgsm1|Q8BPQ7;Gad1|P48318;Snap91|Q61548</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yjefn3|F6W8I0;Gad1|P48318;Snap91|Q61548;Sgsm1|Q8BPQ7;Olfm1|O88998</t>
+    <t xml:space="preserve">|Q8BPQ7;|P48318;|Q61548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|F6W8I0;|P48318;|Q61548;|Q8BPQ7;|O88998</t>
   </si>
   <si>
     <t xml:space="preserve">M243</t>
   </si>
   <si>
-    <t xml:space="preserve">Fdps|Q920E5;Arpp21|Q9DCB4;Ak5|Q920P5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfdn2|O70591;Nedd8|P29595;Ensa|P60840;Vbp1|P61759;Elob|P62869;Ywhah|P68510;Dnal1|Q05A62;Msto1|Q2YDW2;Bola2|Q8BGS2;Nrd1|Q8BHG1;Epm2aip1|Q8VEH5;Fdps|Q920E5;Ak5|Q920P5;Pls3|Q99K51;Hspbp1|Q99P31;1700037H04Rik|Q9D1K7;Arpp21|Q9DCB4</t>
+    <t xml:space="preserve">|Q920E5;|Q9DCB4;|Q920P5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O70591;|P29595;|P60840;|P61759;|P62869;|P68510;|Q05A62;|Q2YDW2;|Q8BGS2;|Q8BHG1;|Q8VEH5;|Q920E5;|Q920P5;|Q99K51;|Q99P31;|Q9D1K7;|Q9DCB4</t>
   </si>
   <si>
     <t xml:space="preserve">M244</t>
   </si>
   <si>
-    <t xml:space="preserve">Uchl1|Q9R0P9;Rnh1|Q91VI7;Nrbp1|Q99J45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap1gap|A2ALS5;Shroom2|A2ALU4;Rbp1|Q00915;Cpne7|Q0VE82;Ppp1r1b|Q60829;Srm|Q64674;Necab1|Q8BG18;Rnh1|Q91VI7;Nrbp1|Q99J45;Pmvk|Q9D1G2;Ift22|Q9DAI2;Rnf14|Q9JI90;Uchl1|Q9R0P9;Clic1|Q9Z1Q5</t>
+    <t xml:space="preserve">|Q9R0P9;|Q91VI7;|Q99J45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|A2ALS5;|A2ALU4;|Q00915;|Q0VE82;|Q60829;|Q64674;|Q8BG18;|Q91VI7;|Q99J45;|Q9D1G2;|Q9DAI2;|Q9JI90;|Q9R0P9;|Q9Z1Q5</t>
   </si>
   <si>
     <t xml:space="preserve">M245</t>
   </si>
   <si>
-    <t xml:space="preserve">Skp1a|Q9WTX5;Pea15a|Q62048;Cplx1|P63040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dbi|P31786;Stmn1|P54227;Pdcd5|P56812;Nrgn|P60761;Mtpn|P62774;Cplx1|P63040;Tbc1d15|Q9CXF4;Tmod2|Q9JKK7;Skp1a|Q9WTX5;Idi1|P58044;Pea15a|Q62048;Dynll2|Q9D0M5</t>
+    <t xml:space="preserve">|Q9WTX5;|Q62048;|P63040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P31786;|P54227;|P56812;|P60761;|P62774;|P63040;|Q9CXF4;|Q9JKK7;|Q9WTX5;|P58044;|Q62048;|Q9D0M5</t>
   </si>
   <si>
     <t xml:space="preserve">M246</t>
   </si>
   <si>
-    <t xml:space="preserve">Uso1|Q9Z1Z0;Vps4a|Q8VEJ9;Gorasp2|Q99JX3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lgals1|P16045;Vps4b|P46467;Arl1|P61211;Wbp2|P97765;Cfap36|Q8C6E0;Vps4a|Q8VEJ9;Chmp1a|Q921W0;Gorasp2|Q99JX3;Pdxdc1|Q99K01;Col4a3bp|Q9EQG9;Uso1|Q9Z1Z0</t>
+    <t xml:space="preserve">|Q9Z1Z0;|Q8VEJ9;|Q99JX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P16045;|P46467;|P61211;|P97765;|Q8C6E0;|Q8VEJ9;|Q921W0;|Q99JX3;|Q99K01;|Q9EQG9;|Q9Z1Z0</t>
   </si>
   <si>
     <t xml:space="preserve">M247</t>
   </si>
   <si>
-    <t xml:space="preserve">Ppp1r2|Q9DCL8;Chmp4b|Q9D8B3;Ube2l3|P68037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atox1|O08997;Calb1|P12658;Ube2l3|P68037;Zyx|Q62523;Dap|Q91XC8;Ufc1|Q9CR09;Chmp4b|Q9D8B3;Ppp1r2|Q9DCL8</t>
+    <t xml:space="preserve">|Q9DCL8;|Q9D8B3;|P68037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08997;|P12658;|P68037;|Q62523;|Q91XC8;|Q9CR09;|Q9D8B3;|Q9DCL8</t>
   </si>
   <si>
     <t xml:space="preserve">M248</t>
   </si>
   <si>
-    <t xml:space="preserve">Ttc27|Q8CD92;Myh9|Q8VDD5;Itpk1|Q8BYN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crabp2|P22935;Nub1|P54729;Cda|P56389;Itpk1|Q8BYN3;Ttc27|Q8CD92;Dym|Q8CHY3;Myh9|Q8VDD5</t>
+    <t xml:space="preserve">|Q8CD92;|Q8VDD5;|Q8BYN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|P22935;|P54729;|P56389;|Q8BYN3;|Q8CD92;|Q8CHY3;|Q8VDD5</t>
   </si>
   <si>
     <t xml:space="preserve">M249</t>
   </si>
   <si>
-    <t xml:space="preserve">Ntng2|Q8R4F1;Arvcf|P98203;Osbpl10|S4R1M9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stxbp1|O08599;Syt3|O35681;Grin1|P35438;Rab3a|P63011;Slc7a10|P63115;Cacna1a|P97445;Kcnma1|Q08460;Grm7|Q68ED2;Grm4|Q68EF4;Mfn2|Q80U63;Lrrtm4|Q80XG9;Adgrb3|Q80ZF8;Ntng2|Q8R4F1;Osbpl10|S4R1M9;Cacna1b|O55017;Cacng2|O88602;Grm8|P47743;Il1rapl1|P59823;Arvcf|P98203;Pkp4|Q68FH0;Lrrc4|Q99PH1</t>
+    <t xml:space="preserve">|Q8R4F1;|P98203;|S4R1M9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O08599;|O35681;|P35438;|P63011;|P63115;|P97445;|Q08460;|Q68ED2;|Q68EF4;|Q80U63;|Q80XG9;|Q80ZF8;|Q8R4F1;|S4R1M9;|O55017;|O88602;|P47743;|P59823;|P98203;|Q68FH0;|Q99PH1</t>
   </si>
   <si>
     <t xml:space="preserve">M250</t>
   </si>
   <si>
-    <t xml:space="preserve">Slc8a2|Q8K596;Ctnnb1|Q02248;Sept9|Q80UG5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptprs|B0V2N1;Ctnnd2|O35927;Cdh2|P15116;Ctnnd1|P30999;Slc6a1|P31648;Cacnb3|P54285;Cdh11|P55288;Ctnnb1|Q02248;Ctnna2|Q61301;Sept9|Q80UG5;Slitrk5|Q810B7;Dlg1|Q811D0;Trhde|Q8K093;Slc8a2|Q8K596;Lingo1|Q9D1T0;Sema4d|O09126;Adcy1|O88444</t>
+    <t xml:space="preserve">|Q8K596;|Q02248;|Q80UG5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B0V2N1;|O35927;|P15116;|P30999;|P31648;|P54285;|P55288;|Q02248;|Q61301;|Q80UG5;|Q810B7;|Q811D0;|Q8K093;|Q8K596;|Q9D1T0;|O09126;|O88444</t>
   </si>
   <si>
     <t xml:space="preserve">M251</t>
   </si>
   <si>
-    <t xml:space="preserve">Rnf141|Q99MB7;Armc1|Q9D7A8;Amt|Q8CFA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gdap1|O88741;Bcl2l13|P59017;Mtch2|Q791V5;Rhot2|Q8JZN7;Ydjc|Q14BV6;Acp6|Q8BP40;Hsdl1|Q8BTX9;Amt|Q8CFA2;Rnf141|Q99MB7;Ociad1|Q9CRD0;Armc1|Q9D7A8</t>
+    <t xml:space="preserve">|Q99MB7;|Q9D7A8;|Q8CFA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O88741;|P59017;|Q791V5;|Q8JZN7;|Q14BV6;|Q8BP40;|Q8BTX9;|Q8CFA2;|Q99MB7;|Q9CRD0;|Q9D7A8</t>
   </si>
   <si>
     <t xml:space="preserve">M252</t>
   </si>
   <si>
-    <t xml:space="preserve">Tomm20|Q9DCC8;Prodh|Q9WU79;Tomm40|Q9QYA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abcb8|Q9CXJ4;Cpox|P36552;Rmnd1|Q8CI78;Tomm20|Q9DCC8;Tomm40|Q9QYA2;Prodh|Q9WU79;Dnajc19|Q9CQV7</t>
+    <t xml:space="preserve">|Q9DCC8;|Q9WU79;|Q9QYA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q9CXJ4;|P36552;|Q8CI78;|Q9DCC8;|Q9QYA2;|Q9WU79;|Q9CQV7</t>
   </si>
   <si>
     <t xml:space="preserve">M253</t>
   </si>
   <si>
-    <t xml:space="preserve">Prxl2b|Q9DB60;Slc25a18|Q9DB41;Naxd|Q9CZ42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gk|Q64516;Sfxn5|Q925N0;Naxd|Q9CZ42;Slc25a18|Q9DB41;Prxl2b|Q9DB60</t>
+    <t xml:space="preserve">|Q9DB60;|Q9DB41;|Q9CZ42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Q64516;|Q925N0;|Q9CZ42;|Q9DB41;|Q9DB60</t>
   </si>
   <si>
     <t xml:space="preserve">M254</t>
   </si>
   <si>
-    <t xml:space="preserve">Hacl1|Q9QXE0;Tax1bp1|Q3UKC1;Rln3|Q8CHK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sdc4|O35988;Pdgfrb|P05622;Prkar2b|P31324;Nf2|P46662;Golga3|P55937;Gmeb2|P58929;Pafah1b1|P63005;Rock1|P70335;Irf3|P70671;Arhgef9|Q3UTH8;Ifit3|Q64345;Galk2|Q68FH4;Arf2|Q8BSL7;Rln3|Q8CHK2;Aamdc|Q8R0P4;Dph7|Q9CYU6;Rcan3|Q9JKK0;Hacl1|Q9QXE0;Rnf7|Q9WTZ1;Ephb3|P54754;Eps15|P42567;Tax1bp1|Q3UKC1</t>
+    <t xml:space="preserve">|Q9QXE0;|Q3UKC1;|Q8CHK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|O35988;|P05622;|P31324;|P46662;|P55937;|P58929;|P63005;|P70335;|P70671;|Q3UTH8;|Q64345;|Q68FH4;|Q8BSL7;|Q8CHK2;|Q8R0P4;|Q9CYU6;|Q9JKK0;|Q9QXE0;|Q9WTZ1;|P54754;|P42567;|Q3UKC1</t>
   </si>
   <si>
     <t xml:space="preserve">M255</t>
   </si>
   <si>
-    <t xml:space="preserve">Fbxo6|Q9QZN4;Ogfrl1|Q8VE52;Gab2|Q9Z1S8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ankrd44|B2RXR6;Hace1|Q3U0D9;Rnf123|Q5XPI3;Gmds|Q8K0C9;Plekho2|Q8K124;Pygl|Q9ET01;Gab2|Q9Z1S8;Nt5c3b|Q3UFY7;Prkaa1|Q5EG47;Ogfrl1|Q8VE52;Nlgn1|Q99K10;Fbxo6|Q9QZN4;Osbp2|Q5QNQ6;Alk|P97793;Ric8b|Q80XE1;Smcr8|Q3UMB5</t>
+    <t xml:space="preserve">|Q9QZN4;|Q8VE52;|Q9Z1S8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|B2RXR6;|Q3U0D9;|Q5XPI3;|Q8K0C9;|Q8K124;|Q9ET01;|Q9Z1S8;|Q3UFY7;|Q5EG47;|Q8VE52;|Q99K10;|Q9QZN4;|Q5QNQ6;|P97793;|Q80XE1;|Q3UMB5</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>

</xml_diff>

<commit_message>
module mean and sem added
</commit_message>
<xml_diff>
--- a/tables/Swip_TMT_Module_GLM_Results.xlsx
+++ b/tables/Swip_TMT_Module_GLM_Results.xlsx
@@ -2828,13 +2828,13 @@
         <v>11.9459703207529</v>
       </c>
       <c r="E2" t="n">
-        <v>0.436035521730554</v>
+        <v>0.00113152888289592</v>
       </c>
       <c r="F2" t="n">
         <v>12.0942804240309</v>
       </c>
       <c r="G2" t="n">
-        <v>0.443104964328822</v>
+        <v>0.00112057690188383</v>
       </c>
       <c r="H2" t="n">
         <v>0.141807677279323</v>
@@ -2917,13 +2917,13 @@
         <v>10.6534977896004</v>
       </c>
       <c r="E3" t="n">
-        <v>0.396394162125504</v>
+        <v>0.00155890873904421</v>
       </c>
       <c r="F3" t="n">
         <v>10.7604602930145</v>
       </c>
       <c r="G3" t="n">
-        <v>0.248622908299779</v>
+        <v>0.00049275183553426</v>
       </c>
       <c r="H3" t="n">
         <v>0.10291004008678</v>
@@ -3006,13 +3006,13 @@
         <v>11.6923954864326</v>
       </c>
       <c r="E4" t="n">
-        <v>0.393221304803772</v>
+        <v>0.000903923533143549</v>
       </c>
       <c r="F4" t="n">
         <v>11.80749700036</v>
       </c>
       <c r="G4" t="n">
-        <v>0.387981497429984</v>
+        <v>0.000814433415465343</v>
       </c>
       <c r="H4" t="n">
         <v>0.109622943752374</v>
@@ -3095,13 +3095,13 @@
         <v>13.7447114010815</v>
       </c>
       <c r="E5" t="n">
-        <v>0.519856238420701</v>
+        <v>0.00108031037110326</v>
       </c>
       <c r="F5" t="n">
         <v>13.8547026429146</v>
       </c>
       <c r="G5" t="n">
-        <v>0.506540190256519</v>
+        <v>0.000911268421431756</v>
       </c>
       <c r="H5" t="n">
         <v>0.104395405778132</v>
@@ -3184,13 +3184,13 @@
         <v>11.7076687645261</v>
       </c>
       <c r="E6" t="n">
-        <v>0.426696985817655</v>
+        <v>0.00117019638482672</v>
       </c>
       <c r="F6" t="n">
         <v>11.8307176401334</v>
       </c>
       <c r="G6" t="n">
-        <v>0.431679920838462</v>
+        <v>0.00115712544146788</v>
       </c>
       <c r="H6" t="n">
         <v>0.118145117773206</v>
@@ -3273,13 +3273,13 @@
         <v>13.2081658156044</v>
       </c>
       <c r="E7" t="n">
-        <v>0.593443126818564</v>
+        <v>0.00265447494649397</v>
       </c>
       <c r="F7" t="n">
         <v>12.9883752085735</v>
       </c>
       <c r="G7" t="n">
-        <v>0.583114421607089</v>
+        <v>0.00258714505483691</v>
       </c>
       <c r="H7" t="n">
         <v>-0.23033849977401</v>
@@ -3362,13 +3362,13 @@
         <v>13.8386173612644</v>
       </c>
       <c r="E8" t="n">
-        <v>0.482394597143735</v>
+        <v>0.000726115481746587</v>
       </c>
       <c r="F8" t="n">
         <v>13.7687771514215</v>
       </c>
       <c r="G8" t="n">
-        <v>0.492639905592292</v>
+        <v>0.00082685788916311</v>
       </c>
       <c r="H8" t="n">
         <v>-0.0764648404342189</v>
@@ -3451,13 +3451,13 @@
         <v>10.9118526297007</v>
       </c>
       <c r="E9" t="n">
-        <v>0.446080249174169</v>
+        <v>0.00200520912023133</v>
       </c>
       <c r="F9" t="n">
         <v>11.0376835819113</v>
       </c>
       <c r="G9" t="n">
-        <v>0.439103343718143</v>
+        <v>0.00178781417723862</v>
       </c>
       <c r="H9" t="n">
         <v>0.119901491231807</v>
@@ -3540,13 +3540,13 @@
         <v>13.5390127307638</v>
       </c>
       <c r="E10" t="n">
-        <v>0.687431173940146</v>
+        <v>0.00583627267151234</v>
       </c>
       <c r="F10" t="n">
         <v>13.0585017614089</v>
       </c>
       <c r="G10" t="n">
-        <v>0.677416911370794</v>
+        <v>0.00579183380748666</v>
       </c>
       <c r="H10" t="n">
         <v>-0.504178888811042</v>
@@ -3629,13 +3629,13 @@
         <v>12.1104391705803</v>
       </c>
       <c r="E11" t="n">
-        <v>0.488402042421524</v>
+        <v>0.00162163459344215</v>
       </c>
       <c r="F11" t="n">
         <v>12.2348820611237</v>
       </c>
       <c r="G11" t="n">
-        <v>0.480449928639572</v>
+        <v>0.00143910848152116</v>
       </c>
       <c r="H11" t="n">
         <v>0.118246414101239</v>
@@ -3718,13 +3718,13 @@
         <v>14.1866034951198</v>
       </c>
       <c r="E12" t="n">
-        <v>0.536033739180276</v>
+        <v>0.00105649485328582</v>
       </c>
       <c r="F12" t="n">
         <v>14.1026182289369</v>
       </c>
       <c r="G12" t="n">
-        <v>0.531808045509688</v>
+        <v>0.00105720137707521</v>
       </c>
       <c r="H12" t="n">
         <v>-0.0925479371399358</v>
@@ -3807,13 +3807,13 @@
         <v>11.5142523632264</v>
       </c>
       <c r="E13" t="n">
-        <v>0.41422192089895</v>
+        <v>0.00117343605762382</v>
       </c>
       <c r="F13" t="n">
         <v>11.6034785945227</v>
       </c>
       <c r="G13" t="n">
-        <v>0.417932274202749</v>
+        <v>0.00114900434022219</v>
       </c>
       <c r="H13" t="n">
         <v>0.0830100472783941</v>
@@ -3896,13 +3896,13 @@
         <v>12.1750914501208</v>
       </c>
       <c r="E14" t="n">
-        <v>0.528560811181844</v>
+        <v>0.00220877100152332</v>
       </c>
       <c r="F14" t="n">
         <v>12.3255991075202</v>
       </c>
       <c r="G14" t="n">
-        <v>0.53000193311595</v>
+        <v>0.00211738718726406</v>
       </c>
       <c r="H14" t="n">
         <v>0.145094600543358</v>
@@ -3985,13 +3985,13 @@
         <v>12.807406443624</v>
       </c>
       <c r="E15" t="n">
-        <v>0.482805351708683</v>
+        <v>0.00114651687416116</v>
       </c>
       <c r="F15" t="n">
         <v>12.7082748603931</v>
       </c>
       <c r="G15" t="n">
-        <v>0.500382022094158</v>
+        <v>0.00138451623542876</v>
       </c>
       <c r="H15" t="n">
         <v>-0.106932017861287</v>
@@ -4074,13 +4074,13 @@
         <v>12.3956570660535</v>
       </c>
       <c r="E16" t="n">
-        <v>0.508551369759917</v>
+        <v>0.00170461748562455</v>
       </c>
       <c r="F16" t="n">
         <v>12.2808283392204</v>
       </c>
       <c r="G16" t="n">
-        <v>0.483858310680753</v>
+        <v>0.00145021087490652</v>
       </c>
       <c r="H16" t="n">
         <v>-0.12103989588742</v>
@@ -4163,13 +4163,13 @@
         <v>12.3751708100658</v>
       </c>
       <c r="E17" t="n">
-        <v>0.502463203095254</v>
+        <v>0.00164764824332165</v>
       </c>
       <c r="F17" t="n">
         <v>12.4975910780255</v>
       </c>
       <c r="G17" t="n">
-        <v>0.515178346001414</v>
+        <v>0.00171965470105726</v>
       </c>
       <c r="H17" t="n">
         <v>0.118025343296817</v>
@@ -4252,13 +4252,13 @@
         <v>12.6620597158175</v>
       </c>
       <c r="E18" t="n">
-        <v>0.500995413915186</v>
+        <v>0.00143661429322703</v>
       </c>
       <c r="F18" t="n">
         <v>12.5559035213472</v>
       </c>
       <c r="G18" t="n">
-        <v>0.50804150393772</v>
+        <v>0.00157765999758645</v>
       </c>
       <c r="H18" t="n">
         <v>-0.113789025025537</v>
@@ -4341,13 +4341,13 @@
         <v>12.5047367289007</v>
       </c>
       <c r="E19" t="n">
-        <v>0.49006285043008</v>
+        <v>0.00139055066923123</v>
       </c>
       <c r="F19" t="n">
         <v>12.4111010502611</v>
       </c>
       <c r="G19" t="n">
-        <v>0.483148904173524</v>
+        <v>0.00135892697379587</v>
       </c>
       <c r="H19" t="n">
         <v>-0.0996850105930181</v>
@@ -4430,13 +4430,13 @@
         <v>14.8788195446246</v>
       </c>
       <c r="E20" t="n">
-        <v>0.488392864243195</v>
+        <v>0.000495234257928527</v>
       </c>
       <c r="F20" t="n">
         <v>14.9488277433591</v>
       </c>
       <c r="G20" t="n">
-        <v>0.515548893519664</v>
+        <v>0.000637060916727681</v>
       </c>
       <c r="H20" t="n">
         <v>0.0584939577700861</v>
@@ -4519,13 +4519,13 @@
         <v>10.8965371131824</v>
       </c>
       <c r="E21" t="n">
-        <v>0.350073988519369</v>
+        <v>0.000977243561127861</v>
       </c>
       <c r="F21" t="n">
         <v>10.9765099615747</v>
       </c>
       <c r="G21" t="n">
-        <v>0.344131304743843</v>
+        <v>0.000894681435121786</v>
       </c>
       <c r="H21" t="n">
         <v>0.0742891858279291</v>
@@ -4608,13 +4608,13 @@
         <v>11.8713357183211</v>
       </c>
       <c r="E22" t="n">
-        <v>0.413792490672128</v>
+        <v>0.000974460520802922</v>
       </c>
       <c r="F22" t="n">
         <v>11.8017148964948</v>
       </c>
       <c r="G22" t="n">
-        <v>0.420670549978874</v>
+        <v>0.00106945713328068</v>
       </c>
       <c r="H22" t="n">
         <v>-0.0759042746103075</v>
@@ -4697,13 +4697,13 @@
         <v>14.4567129540122</v>
       </c>
       <c r="E23" t="n">
-        <v>0.669887167405822</v>
+        <v>0.00358666058643489</v>
       </c>
       <c r="F23" t="n">
         <v>14.6972077581216</v>
       </c>
       <c r="G23" t="n">
-        <v>0.670477471604231</v>
+        <v>0.00348013244864369</v>
       </c>
       <c r="H23" t="n">
         <v>0.237062861069231</v>
@@ -4786,13 +4786,13 @@
         <v>13.3078662175562</v>
       </c>
       <c r="E24" t="n">
-        <v>0.475381094755206</v>
+        <v>0.000855161049584821</v>
       </c>
       <c r="F24" t="n">
         <v>13.2495803308588</v>
       </c>
       <c r="G24" t="n">
-        <v>0.465924405291943</v>
+        <v>0.000809001785177319</v>
       </c>
       <c r="H24" t="n">
         <v>-0.0651730893838965</v>
@@ -4875,13 +4875,13 @@
         <v>12.0722203887165</v>
       </c>
       <c r="E25" t="n">
-        <v>0.476302695274916</v>
+        <v>0.00149558393241092</v>
       </c>
       <c r="F25" t="n">
         <v>11.9888193392477</v>
       </c>
       <c r="G25" t="n">
-        <v>0.479294953348541</v>
+        <v>0.00158695564217534</v>
       </c>
       <c r="H25" t="n">
         <v>-0.0907058322810206</v>
@@ -4964,13 +4964,13 @@
         <v>10.9335231635231</v>
       </c>
       <c r="E26" t="n">
-        <v>0.286574653869058</v>
+        <v>0.000590916698921038</v>
       </c>
       <c r="F26" t="n">
         <v>10.8756013479639</v>
       </c>
       <c r="G26" t="n">
-        <v>0.297619244629866</v>
+        <v>0.000666626226915533</v>
       </c>
       <c r="H26" t="n">
         <v>-0.0642805458437355</v>
@@ -5053,13 +5053,13 @@
         <v>12.338641575948</v>
       </c>
       <c r="E27" t="n">
-        <v>0.442292266781788</v>
+        <v>0.000994421064621984</v>
       </c>
       <c r="F27" t="n">
         <v>12.4150193017555</v>
       </c>
       <c r="G27" t="n">
-        <v>0.44822907082842</v>
+        <v>0.00100477801248894</v>
       </c>
       <c r="H27" t="n">
         <v>0.0708390671235903</v>
@@ -5142,13 +5142,13 @@
         <v>14.0268706722576</v>
       </c>
       <c r="E28" t="n">
-        <v>0.585807572303552</v>
+        <v>0.00183268637757821</v>
       </c>
       <c r="F28" t="n">
         <v>13.9221362202791</v>
       </c>
       <c r="G28" t="n">
-        <v>0.580274278018762</v>
+        <v>0.00180502806465209</v>
       </c>
       <c r="H28" t="n">
         <v>-0.112026683646522</v>
@@ -5231,13 +5231,13 @@
         <v>10.9584160215137</v>
       </c>
       <c r="E29" t="n">
-        <v>0.366610810618837</v>
+        <v>0.00106866067317922</v>
       </c>
       <c r="F29" t="n">
         <v>10.9059777637166</v>
       </c>
       <c r="G29" t="n">
-        <v>0.347351178040991</v>
+        <v>0.000951027938406214</v>
       </c>
       <c r="H29" t="n">
         <v>-0.0608973837306934</v>
@@ -5320,13 +5320,13 @@
         <v>13.8540624572339</v>
       </c>
       <c r="E30" t="n">
-        <v>0.55111920339313</v>
+        <v>0.00139736869807868</v>
       </c>
       <c r="F30" t="n">
         <v>13.7811809658303</v>
       </c>
       <c r="G30" t="n">
-        <v>0.539474726045092</v>
+        <v>0.00128650894035819</v>
       </c>
       <c r="H30" t="n">
         <v>-0.0791128506231767</v>
@@ -5409,13 +5409,13 @@
         <v>13.9417855143749</v>
       </c>
       <c r="E31" t="n">
-        <v>0.602231633905021</v>
+        <v>0.00221763666095675</v>
       </c>
       <c r="F31" t="n">
         <v>13.8204343664375</v>
       </c>
       <c r="G31" t="n">
-        <v>0.594677731543638</v>
+        <v>0.00214927386282712</v>
       </c>
       <c r="H31" t="n">
         <v>-0.130325513646761</v>
@@ -5498,13 +5498,13 @@
         <v>12.0612398410645</v>
       </c>
       <c r="E32" t="n">
-        <v>0.54805442143872</v>
+        <v>0.00273851479348868</v>
       </c>
       <c r="F32" t="n">
         <v>11.9212571518356</v>
       </c>
       <c r="G32" t="n">
-        <v>0.546310207161105</v>
+        <v>0.00284176786307498</v>
       </c>
       <c r="H32" t="n">
         <v>-0.154036464461193</v>
@@ -5587,13 +5587,13 @@
         <v>11.1081652537483</v>
       </c>
       <c r="E33" t="n">
-        <v>0.402399143709546</v>
+        <v>0.00130464738108775</v>
       </c>
       <c r="F33" t="n">
         <v>11.039314027999</v>
       </c>
       <c r="G33" t="n">
-        <v>0.394407905084572</v>
+        <v>0.00126949830720757</v>
       </c>
       <c r="H33" t="n">
         <v>-0.075082563893624</v>
@@ -5676,13 +5676,13 @@
         <v>12.728075284378</v>
       </c>
       <c r="E34" t="n">
-        <v>0.458298972473808</v>
+        <v>0.000956890997038697</v>
       </c>
       <c r="F34" t="n">
         <v>12.6557916033036</v>
       </c>
       <c r="G34" t="n">
-        <v>0.477343599324567</v>
+        <v>0.00115543394478606</v>
       </c>
       <c r="H34" t="n">
         <v>-0.0781940783945619</v>
@@ -5765,13 +5765,13 @@
         <v>10.833080959629</v>
       </c>
       <c r="E35" t="n">
-        <v>0.466320719701352</v>
+        <v>0.00240742884532379</v>
       </c>
       <c r="F35" t="n">
         <v>10.9459798325508</v>
       </c>
       <c r="G35" t="n">
-        <v>0.454282420012095</v>
+        <v>0.00210760138940213</v>
       </c>
       <c r="H35" t="n">
         <v>0.108093041401453</v>
@@ -5854,13 +5854,13 @@
         <v>12.2390238898317</v>
       </c>
       <c r="E36" t="n">
-        <v>0.594628613355748</v>
+        <v>0.00374175602521775</v>
       </c>
       <c r="F36" t="n">
         <v>12.4194353694828</v>
       </c>
       <c r="G36" t="n">
-        <v>0.58639973765866</v>
+        <v>0.00333215433532385</v>
       </c>
       <c r="H36" t="n">
         <v>0.174908669891507</v>
@@ -5943,13 +5943,13 @@
         <v>10.8987625329606</v>
       </c>
       <c r="E37" t="n">
-        <v>0.397439038418284</v>
+        <v>0.00139410839505225</v>
       </c>
       <c r="F37" t="n">
         <v>10.8273508497123</v>
       </c>
       <c r="G37" t="n">
-        <v>0.430618803609506</v>
+        <v>0.00185593045464693</v>
       </c>
       <c r="H37" t="n">
         <v>-0.0809802676830322</v>
@@ -6032,13 +6032,13 @@
         <v>14.4122604772724</v>
       </c>
       <c r="E38" t="n">
-        <v>0.518570431774379</v>
+        <v>0.000816245074593619</v>
       </c>
       <c r="F38" t="n">
         <v>14.362606981914</v>
       </c>
       <c r="G38" t="n">
-        <v>0.523093884009571</v>
+        <v>0.000870423830390903</v>
       </c>
       <c r="H38" t="n">
         <v>-0.0562293956314363</v>
@@ -6121,13 +6121,13 @@
         <v>11.897072876024</v>
       </c>
       <c r="E39" t="n">
-        <v>0.48500614726058</v>
+        <v>0.00173009798229618</v>
       </c>
       <c r="F39" t="n">
         <v>11.9805973963447</v>
       </c>
       <c r="G39" t="n">
-        <v>0.452386315771287</v>
+        <v>0.00127587466753536</v>
       </c>
       <c r="H39" t="n">
         <v>0.077440080420803</v>
@@ -6210,13 +6210,13 @@
         <v>10.8192086855701</v>
       </c>
       <c r="E40" t="n">
-        <v>0.488005611823065</v>
+        <v>0.00289675244369552</v>
       </c>
       <c r="F40" t="n">
         <v>10.7153992253614</v>
       </c>
       <c r="G40" t="n">
-        <v>0.489628732569179</v>
+        <v>0.00300601688861549</v>
       </c>
       <c r="H40" t="n">
         <v>-0.111313062984727</v>
@@ -6299,13 +6299,13 @@
         <v>12.2039887452306</v>
       </c>
       <c r="E41" t="n">
-        <v>0.592514058009782</v>
+        <v>0.00378702177645145</v>
       </c>
       <c r="F41" t="n">
         <v>12.0443770085959</v>
       </c>
       <c r="G41" t="n">
-        <v>0.589385299501303</v>
+        <v>0.00386457170330494</v>
       </c>
       <c r="H41" t="n">
         <v>-0.171553603017118</v>
@@ -6388,13 +6388,13 @@
         <v>11.4998783885094</v>
       </c>
       <c r="E42" t="n">
-        <v>0.407519740438121</v>
+        <v>0.00111779146091241</v>
       </c>
       <c r="F42" t="n">
         <v>11.4488667383502</v>
       </c>
       <c r="G42" t="n">
-        <v>0.421434068187836</v>
+        <v>0.00127442404287185</v>
       </c>
       <c r="H42" t="n">
         <v>-0.0592302889770245</v>
@@ -6477,13 +6477,13 @@
         <v>10.7092995724082</v>
       </c>
       <c r="E43" t="n">
-        <v>0.485979094263737</v>
+        <v>0.0029594575517946</v>
       </c>
       <c r="F43" t="n">
         <v>10.8221113063374</v>
       </c>
       <c r="G43" t="n">
-        <v>0.486937859469571</v>
+        <v>0.00285528408480364</v>
       </c>
       <c r="H43" t="n">
         <v>0.106942814192951</v>
@@ -6566,13 +6566,13 @@
         <v>14.3124503177586</v>
       </c>
       <c r="E44" t="n">
-        <v>0.616232269702655</v>
+        <v>0.00222471093108656</v>
       </c>
       <c r="F44" t="n">
         <v>14.2170391287918</v>
       </c>
       <c r="G44" t="n">
-        <v>0.616175135669443</v>
+        <v>0.00232606038842654</v>
       </c>
       <c r="H44" t="n">
         <v>-0.105155299786269</v>
@@ -6655,13 +6655,13 @@
         <v>12.9527805789121</v>
       </c>
       <c r="E45" t="n">
-        <v>0.511659343408755</v>
+        <v>0.00139294822277071</v>
       </c>
       <c r="F45" t="n">
         <v>13.0321203630418</v>
       </c>
       <c r="G45" t="n">
-        <v>0.512862316509612</v>
+        <v>0.00135343508464395</v>
       </c>
       <c r="H45" t="n">
         <v>0.0728971739530882</v>
@@ -6744,13 +6744,13 @@
         <v>13.8866038290758</v>
       </c>
       <c r="E46" t="n">
-        <v>0.49680290693886</v>
+        <v>0.000821061829290604</v>
       </c>
       <c r="F46" t="n">
         <v>13.9332985887486</v>
       </c>
       <c r="G46" t="n">
-        <v>0.502498098305223</v>
+        <v>0.000846488981814193</v>
       </c>
       <c r="H46" t="n">
         <v>0.0399294544990009</v>
@@ -6833,13 +6833,13 @@
         <v>12.4651689586346</v>
       </c>
       <c r="E47" t="n">
-        <v>0.526637156059679</v>
+        <v>0.00193308326214971</v>
       </c>
       <c r="F47" t="n">
         <v>12.3849585079415</v>
       </c>
       <c r="G47" t="n">
-        <v>0.524856611424443</v>
+        <v>0.00197568049138947</v>
       </c>
       <c r="H47" t="n">
         <v>-0.0874429734910449</v>
@@ -6922,13 +6922,13 @@
         <v>12.5461483580798</v>
       </c>
       <c r="E48" t="n">
-        <v>0.55062062973921</v>
+        <v>0.00230482515586212</v>
       </c>
       <c r="F48" t="n">
         <v>12.4617588559978</v>
       </c>
       <c r="G48" t="n">
-        <v>0.548989672928422</v>
+        <v>0.00235761092388309</v>
       </c>
       <c r="H48" t="n">
         <v>-0.0918364495266369</v>
@@ -7011,13 +7011,13 @@
         <v>14.5411876247845</v>
       </c>
       <c r="E49" t="n">
-        <v>0.604391916644212</v>
+        <v>0.0018395217301639</v>
       </c>
       <c r="F49" t="n">
         <v>14.4596468614834</v>
       </c>
       <c r="G49" t="n">
-        <v>0.604532629063192</v>
+        <v>0.00189453541610119</v>
       </c>
       <c r="H49" t="n">
         <v>-0.0887430211705379</v>
@@ -7100,13 +7100,13 @@
         <v>12.7946043715874</v>
       </c>
       <c r="E50" t="n">
-        <v>0.518154465937942</v>
+        <v>0.00156830280883879</v>
       </c>
       <c r="F50" t="n">
         <v>12.8674349666839</v>
       </c>
       <c r="G50" t="n">
-        <v>0.497562558829485</v>
+        <v>0.00126825691161284</v>
       </c>
       <c r="H50" t="n">
         <v>0.0668192918562548</v>
@@ -7189,13 +7189,13 @@
         <v>13.3389822946128</v>
       </c>
       <c r="E51" t="n">
-        <v>0.447545036376354</v>
+        <v>0.000654858121603337</v>
       </c>
       <c r="F51" t="n">
         <v>13.2970200704049</v>
       </c>
       <c r="G51" t="n">
-        <v>0.46674648020422</v>
+        <v>0.000794595682810311</v>
       </c>
       <c r="H51" t="n">
         <v>-0.0488348682025467</v>
@@ -7278,13 +7278,13 @@
         <v>13.2424287336602</v>
       </c>
       <c r="E52" t="n">
-        <v>0.541357362972877</v>
+        <v>0.00160916031291661</v>
       </c>
       <c r="F52" t="n">
         <v>13.1819632387339</v>
       </c>
       <c r="G52" t="n">
-        <v>0.534422426640112</v>
+        <v>0.00156223788518655</v>
       </c>
       <c r="H52" t="n">
         <v>-0.0672290648312434</v>
@@ -7367,13 +7367,13 @@
         <v>14.3556992101039</v>
       </c>
       <c r="E53" t="n">
-        <v>0.560445357667628</v>
+        <v>0.00126583496965315</v>
       </c>
       <c r="F53" t="n">
         <v>14.413999221094</v>
       </c>
       <c r="G53" t="n">
-        <v>0.564715529954376</v>
+        <v>0.00129449960562903</v>
       </c>
       <c r="H53" t="n">
         <v>0.0655988084671432</v>
@@ -7456,13 +7456,13 @@
         <v>9.49547600452414</v>
       </c>
       <c r="E54" t="n">
-        <v>0.304564049711176</v>
+        <v>0.0015691332449358</v>
       </c>
       <c r="F54" t="n">
         <v>9.43926871333851</v>
       </c>
       <c r="G54" t="n">
-        <v>0.342715097015689</v>
+        <v>0.00205837993473816</v>
       </c>
       <c r="H54" t="n">
         <v>-0.0643559616168755</v>
@@ -7545,13 +7545,13 @@
         <v>13.4178386253875</v>
       </c>
       <c r="E55" t="n">
-        <v>0.505135066709687</v>
+        <v>0.00107483920137538</v>
       </c>
       <c r="F55" t="n">
         <v>13.4762405368579</v>
       </c>
       <c r="G55" t="n">
-        <v>0.494025560145501</v>
+        <v>0.000949247318050733</v>
       </c>
       <c r="H55" t="n">
         <v>0.052086365140858</v>
@@ -7634,13 +7634,13 @@
         <v>13.7981228259909</v>
       </c>
       <c r="E56" t="n">
-        <v>0.424467553252155</v>
+        <v>0.000425372010655834</v>
       </c>
       <c r="F56" t="n">
         <v>13.8386143156776</v>
       </c>
       <c r="G56" t="n">
-        <v>0.419702881270574</v>
+        <v>0.000398670740558231</v>
       </c>
       <c r="H56" t="n">
         <v>0.0365641969312908</v>
@@ -7723,13 +7723,13 @@
         <v>12.0438627908014</v>
       </c>
       <c r="E57" t="n">
-        <v>0.516580823421472</v>
+        <v>0.00212490264092293</v>
       </c>
       <c r="F57" t="n">
         <v>11.9702350049034</v>
       </c>
       <c r="G57" t="n">
-        <v>0.51221138214879</v>
+        <v>0.00209725052461214</v>
       </c>
       <c r="H57" t="n">
         <v>-0.0796617543025219</v>
@@ -7812,13 +7812,13 @@
         <v>14.6997816655392</v>
       </c>
       <c r="E58" t="n">
-        <v>0.483768470851043</v>
+        <v>0.000508900942418492</v>
       </c>
       <c r="F58" t="n">
         <v>14.7405606597602</v>
       </c>
       <c r="G58" t="n">
-        <v>0.477899666827536</v>
+        <v>0.000473222945612541</v>
       </c>
       <c r="H58" t="n">
         <v>0.0335764061283446</v>
@@ -7901,13 +7901,13 @@
         <v>15.0702238844789</v>
       </c>
       <c r="E59" t="n">
-        <v>0.646947083240242</v>
+        <v>0.00237029277520653</v>
       </c>
       <c r="F59" t="n">
         <v>15.1727925419199</v>
       </c>
       <c r="G59" t="n">
-        <v>0.642627680860067</v>
+        <v>0.00223723544235838</v>
       </c>
       <c r="H59" t="n">
         <v>0.097771493487289</v>
@@ -7990,13 +7990,13 @@
         <v>13.6186954360523</v>
       </c>
       <c r="E60" t="n">
-        <v>0.592445967924186</v>
+        <v>0.00225309652694509</v>
       </c>
       <c r="F60" t="n">
         <v>13.5388162804747</v>
       </c>
       <c r="G60" t="n">
-        <v>0.594789285958017</v>
+        <v>0.00238121970037879</v>
       </c>
       <c r="H60" t="n">
         <v>-0.0865673124753144</v>
@@ -8079,13 +8079,13 @@
         <v>14.3515402681234</v>
       </c>
       <c r="E61" t="n">
-        <v>0.57237361907178</v>
+        <v>0.0014291795770859</v>
       </c>
       <c r="F61" t="n">
         <v>14.3057396939322</v>
       </c>
       <c r="G61" t="n">
-        <v>0.575007965773688</v>
+        <v>0.00149061190650205</v>
       </c>
       <c r="H61" t="n">
         <v>-0.0519407437958999</v>
@@ -8168,13 +8168,13 @@
         <v>12.6137246239852</v>
       </c>
       <c r="E62" t="n">
-        <v>0.501068792711227</v>
+        <v>0.00145901544680408</v>
       </c>
       <c r="F62" t="n">
         <v>12.6792184670087</v>
       </c>
       <c r="G62" t="n">
-        <v>0.505765356428284</v>
+        <v>0.00147699857578129</v>
       </c>
       <c r="H62" t="n">
         <v>0.0568911373795916</v>
@@ -8257,13 +8257,13 @@
         <v>11.3767050928124</v>
       </c>
       <c r="E63" t="n">
-        <v>0.345477695411747</v>
+        <v>0.00072597936929126</v>
       </c>
       <c r="F63" t="n">
         <v>11.3442627395472</v>
       </c>
       <c r="G63" t="n">
-        <v>0.347792107456914</v>
+        <v>0.000755157920584618</v>
       </c>
       <c r="H63" t="n">
         <v>-0.038904619057741</v>
@@ -8346,13 +8346,13 @@
         <v>12.7337663082099</v>
       </c>
       <c r="E64" t="n">
-        <v>0.517237596343005</v>
+        <v>0.00160217421983567</v>
       </c>
       <c r="F64" t="n">
         <v>12.6850270456348</v>
       </c>
       <c r="G64" t="n">
-        <v>0.513652343082244</v>
+        <v>0.00157275421453976</v>
       </c>
       <c r="H64" t="n">
         <v>-0.0547771079891822</v>
@@ -8435,13 +8435,13 @@
         <v>11.2849059158359</v>
       </c>
       <c r="E65" t="n">
-        <v>0.462466681993579</v>
+        <v>0.00191545899677125</v>
       </c>
       <c r="F65" t="n">
         <v>11.2262998702997</v>
       </c>
       <c r="G65" t="n">
-        <v>0.469859705039608</v>
+        <v>0.00207174171547649</v>
       </c>
       <c r="H65" t="n">
         <v>-0.0654071920021823</v>
@@ -8524,13 +8524,13 @@
         <v>11.3852957987646</v>
       </c>
       <c r="E66" t="n">
-        <v>0.530004550578845</v>
+        <v>0.003074593755189</v>
       </c>
       <c r="F66" t="n">
         <v>11.4735889219344</v>
       </c>
       <c r="G66" t="n">
-        <v>0.506797803389237</v>
+        <v>0.00250321713135394</v>
       </c>
       <c r="H66" t="n">
         <v>0.0825126092411525</v>
@@ -8613,13 +8613,13 @@
         <v>12.3750847654418</v>
       </c>
       <c r="E67" t="n">
-        <v>0.484053745030457</v>
+        <v>0.00139299876071002</v>
       </c>
       <c r="F67" t="n">
         <v>12.3310704650274</v>
       </c>
       <c r="G67" t="n">
-        <v>0.487768147340057</v>
+        <v>0.00147003667011553</v>
       </c>
       <c r="H67" t="n">
         <v>-0.0506983879333271</v>
@@ -8702,13 +8702,13 @@
         <v>13.7066529959938</v>
       </c>
       <c r="E68" t="n">
-        <v>0.630667791646422</v>
+        <v>0.00315424824765224</v>
       </c>
       <c r="F68" t="n">
         <v>13.6053066276648</v>
       </c>
       <c r="G68" t="n">
-        <v>0.624903863156885</v>
+        <v>0.00308258057772852</v>
       </c>
       <c r="H68" t="n">
         <v>-0.110255731293158</v>
@@ -8791,13 +8791,13 @@
         <v>14.1252589183329</v>
       </c>
       <c r="E69" t="n">
-        <v>0.452519461726478</v>
+        <v>0.000480205124354569</v>
       </c>
       <c r="F69" t="n">
         <v>14.1619615124154</v>
       </c>
       <c r="G69" t="n">
-        <v>0.432802478291745</v>
+        <v>0.000389018609663876</v>
       </c>
       <c r="H69" t="n">
         <v>0.0300950144963251</v>
@@ -8880,13 +8880,13 @@
         <v>13.9110735246225</v>
       </c>
       <c r="E70" t="n">
-        <v>0.575309597748556</v>
+        <v>0.00172419191617586</v>
       </c>
       <c r="F70" t="n">
         <v>13.9746093443596</v>
       </c>
       <c r="G70" t="n">
-        <v>0.564398391336304</v>
+        <v>0.0015173489125651</v>
       </c>
       <c r="H70" t="n">
         <v>0.0572553202861004</v>
@@ -8969,13 +8969,13 @@
         <v>13.0309157812814</v>
       </c>
       <c r="E71" t="n">
-        <v>0.570868019213926</v>
+        <v>0.00227045337418223</v>
       </c>
       <c r="F71" t="n">
         <v>13.1089748015328</v>
       </c>
       <c r="G71" t="n">
-        <v>0.554090091540518</v>
+        <v>0.00193064714942476</v>
       </c>
       <c r="H71" t="n">
         <v>0.0708609727558795</v>
@@ -9058,13 +9058,13 @@
         <v>10.7929572486979</v>
       </c>
       <c r="E72" t="n">
-        <v>0.430263397136454</v>
+        <v>0.00187267596268823</v>
       </c>
       <c r="F72" t="n">
         <v>10.8479796011054</v>
       </c>
       <c r="G72" t="n">
-        <v>0.416905051596245</v>
+        <v>0.00166809505831762</v>
       </c>
       <c r="H72" t="n">
         <v>0.0499420096826934</v>
@@ -9147,13 +9147,13 @@
         <v>14.393738713899</v>
       </c>
       <c r="E73" t="n">
-        <v>0.573867728507179</v>
+        <v>0.00143255567636262</v>
       </c>
       <c r="F73" t="n">
         <v>14.4432920739053</v>
       </c>
       <c r="G73" t="n">
-        <v>0.582123606129002</v>
+        <v>0.00151771147812683</v>
       </c>
       <c r="H73" t="n">
         <v>0.0555101802606869</v>
@@ -9236,13 +9236,13 @@
         <v>13.666427272666</v>
       </c>
       <c r="E74" t="n">
-        <v>0.576388837277164</v>
+        <v>0.00190539232160005</v>
       </c>
       <c r="F74" t="n">
         <v>13.6120670198862</v>
       </c>
       <c r="G74" t="n">
-        <v>0.578607323975292</v>
+        <v>0.00199139168069614</v>
       </c>
       <c r="H74" t="n">
         <v>-0.0612055129156085</v>
@@ -9325,13 +9325,13 @@
         <v>14.8076576924805</v>
       </c>
       <c r="E75" t="n">
-        <v>0.530815121080601</v>
+        <v>0.000791297480730508</v>
       </c>
       <c r="F75" t="n">
         <v>14.8477948964191</v>
       </c>
       <c r="G75" t="n">
-        <v>0.531489524392567</v>
+        <v>0.000780471982444897</v>
       </c>
       <c r="H75" t="n">
         <v>0.0328108447258312</v>
@@ -9414,13 +9414,13 @@
         <v>11.8838265041369</v>
       </c>
       <c r="E76" t="n">
-        <v>0.417608771683105</v>
+        <v>0.000997616956193893</v>
       </c>
       <c r="F76" t="n">
         <v>11.9277333554695</v>
       </c>
       <c r="G76" t="n">
-        <v>0.349059225115632</v>
+        <v>0.000556258333239487</v>
       </c>
       <c r="H76" t="n">
         <v>0.0376806592881791</v>
@@ -9503,13 +9503,13 @@
         <v>11.9085945698403</v>
       </c>
       <c r="E77" t="n">
-        <v>0.393860934369972</v>
+        <v>0.000811874559251924</v>
       </c>
       <c r="F77" t="n">
         <v>11.8761885343989</v>
       </c>
       <c r="G77" t="n">
-        <v>0.402659237761275</v>
+        <v>0.000891769488457884</v>
       </c>
       <c r="H77" t="n">
         <v>-0.0391034184458468</v>
@@ -9592,13 +9592,13 @@
         <v>13.2760360579654</v>
       </c>
       <c r="E78" t="n">
-        <v>0.547129384752941</v>
+        <v>0.00168225496849413</v>
       </c>
       <c r="F78" t="n">
         <v>13.3335447798195</v>
       </c>
       <c r="G78" t="n">
-        <v>0.540911502162156</v>
+        <v>0.00155190934782303</v>
       </c>
       <c r="H78" t="n">
         <v>0.0512815550758172</v>
@@ -9681,13 +9681,13 @@
         <v>12.2424311663423</v>
       </c>
       <c r="E79" t="n">
-        <v>0.550499475522043</v>
+        <v>0.00257067566559323</v>
       </c>
       <c r="F79" t="n">
         <v>12.3171937184079</v>
       </c>
       <c r="G79" t="n">
-        <v>0.533682706942356</v>
+        <v>0.00220595226027186</v>
       </c>
       <c r="H79" t="n">
         <v>0.0681637026425925</v>
@@ -9770,13 +9770,13 @@
         <v>12.8614386178493</v>
       </c>
       <c r="E80" t="n">
-        <v>0.474876664685671</v>
+        <v>0.00104199142960425</v>
       </c>
       <c r="F80" t="n">
         <v>12.9018382639038</v>
       </c>
       <c r="G80" t="n">
-        <v>0.470898120717852</v>
+        <v>0.000983252376885172</v>
       </c>
       <c r="H80" t="n">
         <v>0.0338473980896381</v>
@@ -9859,13 +9859,13 @@
         <v>9.12319429788691</v>
       </c>
       <c r="E81" t="n">
-        <v>0.44197643290995</v>
+        <v>0.00457775990023673</v>
       </c>
       <c r="F81" t="n">
         <v>9.19551034767121</v>
       </c>
       <c r="G81" t="n">
-        <v>0.366595117772433</v>
+        <v>0.00278543975308864</v>
       </c>
       <c r="H81" t="n">
         <v>0.0679436552790502</v>
@@ -9948,13 +9948,13 @@
         <v>13.7024827070516</v>
       </c>
       <c r="E82" t="n">
-        <v>0.494444843354624</v>
+        <v>0.000864324628655963</v>
       </c>
       <c r="F82" t="n">
         <v>13.7380918795779</v>
       </c>
       <c r="G82" t="n">
-        <v>0.50046612927393</v>
+        <v>0.000903949058283976</v>
       </c>
       <c r="H82" t="n">
         <v>0.0287524813127283</v>
@@ -10037,13 +10037,13 @@
         <v>12.2518649670466</v>
       </c>
       <c r="E83" t="n">
-        <v>0.530681911456557</v>
+        <v>0.00218015876123428</v>
       </c>
       <c r="F83" t="n">
         <v>12.2027154260286</v>
       </c>
       <c r="G83" t="n">
-        <v>0.517548788060181</v>
+        <v>0.00200293593949073</v>
       </c>
       <c r="H83" t="n">
         <v>-0.054745724887303</v>
@@ -10126,13 +10126,13 @@
         <v>12.3289371377502</v>
       </c>
       <c r="E84" t="n">
-        <v>0.53687788992605</v>
+        <v>0.00223392032306082</v>
       </c>
       <c r="F84" t="n">
         <v>12.2614016207835</v>
       </c>
       <c r="G84" t="n">
-        <v>0.541247135045901</v>
+        <v>0.00238409358423649</v>
       </c>
       <c r="H84" t="n">
         <v>-0.0655694283178274</v>
@@ -10215,13 +10215,13 @@
         <v>11.4831387786311</v>
       </c>
       <c r="E85" t="n">
-        <v>0.511127780314952</v>
+        <v>0.00256646576394013</v>
       </c>
       <c r="F85" t="n">
         <v>11.4320183961106</v>
       </c>
       <c r="G85" t="n">
-        <v>0.515130779628095</v>
+        <v>0.00270534891082447</v>
       </c>
       <c r="H85" t="n">
         <v>-0.0582289634770041</v>
@@ -10304,13 +10304,13 @@
         <v>10.3455483812155</v>
       </c>
       <c r="E86" t="n">
-        <v>0.145022452540942</v>
+        <v>0.000302981914248478</v>
       </c>
       <c r="F86" t="n">
         <v>10.3284705966431</v>
       </c>
       <c r="G86" t="n">
-        <v>0.385936458777053</v>
+        <v>0.00171727297634344</v>
       </c>
       <c r="H86" t="n">
         <v>-0.0288722072220614</v>
@@ -10393,13 +10393,13 @@
         <v>14.3962240525131</v>
       </c>
       <c r="E87" t="n">
-        <v>0.576970730658183</v>
+        <v>0.00148781491222357</v>
       </c>
       <c r="F87" t="n">
         <v>14.4399014468767</v>
       </c>
       <c r="G87" t="n">
-        <v>0.579317161966966</v>
+        <v>0.0014664799166306</v>
       </c>
       <c r="H87" t="n">
         <v>0.0373536528043127</v>
@@ -10482,13 +10482,13 @@
         <v>13.0433559780532</v>
       </c>
       <c r="E88" t="n">
-        <v>0.482910931553498</v>
+        <v>0.00103220620292902</v>
       </c>
       <c r="F88" t="n">
         <v>13.0183924105912</v>
       </c>
       <c r="G88" t="n">
-        <v>0.479641951019688</v>
+        <v>0.00101207225662777</v>
       </c>
       <c r="H88" t="n">
         <v>-0.0311038203785823</v>
@@ -10571,13 +10571,13 @@
         <v>10.3308447630981</v>
       </c>
       <c r="E89" t="n">
-        <v>0.329076512816671</v>
+        <v>0.00114627524811941</v>
       </c>
       <c r="F89" t="n">
         <v>10.3055895697967</v>
       </c>
       <c r="G89" t="n">
-        <v>0.340189302524146</v>
+        <v>0.00125501014853575</v>
       </c>
       <c r="H89" t="n">
         <v>-0.0325905656741866</v>
@@ -10660,13 +10660,13 @@
         <v>13.6032814775494</v>
       </c>
       <c r="E90" t="n">
-        <v>0.520676817650213</v>
+        <v>0.00115795875520766</v>
       </c>
       <c r="F90" t="n">
         <v>13.5793186544332</v>
       </c>
       <c r="G90" t="n">
-        <v>0.53389104781302</v>
+        <v>0.00131840463351072</v>
       </c>
       <c r="H90" t="n">
         <v>-0.0300650564469412</v>
@@ -10749,13 +10749,13 @@
         <v>13.4631482316389</v>
       </c>
       <c r="E91" t="n">
-        <v>0.533785550837761</v>
+        <v>0.00139060083358974</v>
       </c>
       <c r="F91" t="n">
         <v>13.5027623669248</v>
       </c>
       <c r="G91" t="n">
-        <v>0.53160912962957</v>
+        <v>0.001324423029658</v>
       </c>
       <c r="H91" t="n">
         <v>0.034391707647064</v>
@@ -10838,13 +10838,13 @@
         <v>12.7969633838486</v>
       </c>
       <c r="E92" t="n">
-        <v>0.520541905644427</v>
+        <v>0.00160076848002763</v>
       </c>
       <c r="F92" t="n">
         <v>12.7616059106269</v>
       </c>
       <c r="G92" t="n">
-        <v>0.519416451542238</v>
+        <v>0.00161375584541372</v>
       </c>
       <c r="H92" t="n">
         <v>-0.0415465454546953</v>
@@ -10927,13 +10927,13 @@
         <v>11.6011645591145</v>
       </c>
       <c r="E93" t="n">
-        <v>0.50680604893741</v>
+        <v>0.00236535347562334</v>
       </c>
       <c r="F93" t="n">
         <v>11.5561843142832</v>
       </c>
       <c r="G93" t="n">
-        <v>0.514311613922573</v>
+        <v>0.00254315841253332</v>
       </c>
       <c r="H93" t="n">
         <v>-0.0545173429187346</v>
@@ -11016,13 +11016,13 @@
         <v>14.0272759335818</v>
       </c>
       <c r="E94" t="n">
-        <v>0.417089545730257</v>
+        <v>0.000355357362000454</v>
       </c>
       <c r="F94" t="n">
         <v>14.0145426330808</v>
       </c>
       <c r="G94" t="n">
-        <v>0.427060769234919</v>
+        <v>0.000394406458036939</v>
       </c>
       <c r="H94" t="n">
         <v>-0.0208287174366762</v>
@@ -11105,13 +11105,13 @@
         <v>13.0357582335812</v>
       </c>
       <c r="E95" t="n">
-        <v>0.511119448759209</v>
+        <v>0.00133237077434619</v>
       </c>
       <c r="F95" t="n">
         <v>13.0757983759491</v>
       </c>
       <c r="G95" t="n">
-        <v>0.477173282970245</v>
+        <v>0.000964898217941335</v>
       </c>
       <c r="H95" t="n">
         <v>0.0337464918481359</v>
@@ -11194,13 +11194,13 @@
         <v>12.7822154566238</v>
       </c>
       <c r="E96" t="n">
-        <v>0.490872226467688</v>
+        <v>0.00123916862722481</v>
       </c>
       <c r="F96" t="n">
         <v>12.7527217535454</v>
       </c>
       <c r="G96" t="n">
-        <v>0.493606162431931</v>
+        <v>0.00128796557666866</v>
       </c>
       <c r="H96" t="n">
         <v>-0.0364493911281627</v>
@@ -11283,13 +11283,13 @@
         <v>11.1405289590217</v>
       </c>
       <c r="E97" t="n">
-        <v>0.530980593550985</v>
+        <v>0.00347337964014062</v>
       </c>
       <c r="F97" t="n">
         <v>11.0763401249584</v>
       </c>
       <c r="G97" t="n">
-        <v>0.5269796612304</v>
+        <v>0.00343154378325489</v>
       </c>
       <c r="H97" t="n">
         <v>-0.068820610135396</v>
@@ -11372,13 +11372,13 @@
         <v>14.4107342423225</v>
       </c>
       <c r="E98" t="n">
-        <v>0.546768076186059</v>
+        <v>0.00107788186924531</v>
       </c>
       <c r="F98" t="n">
         <v>14.4497982303512</v>
       </c>
       <c r="G98" t="n">
-        <v>0.551526000122502</v>
+        <v>0.0011221591778119</v>
       </c>
       <c r="H98" t="n">
         <v>0.0323635271952273</v>
@@ -11461,13 +11461,13 @@
         <v>15.9314255961783</v>
       </c>
       <c r="E99" t="n">
-        <v>0.58171515643575</v>
+        <v>0.000892136524224196</v>
       </c>
       <c r="F99" t="n">
         <v>15.9617225227035</v>
       </c>
       <c r="G99" t="n">
-        <v>0.582533154206142</v>
+        <v>0.00089259463367033</v>
       </c>
       <c r="H99" t="n">
         <v>0.0246488563246752</v>
@@ -11550,13 +11550,13 @@
         <v>13.0048840734394</v>
       </c>
       <c r="E100" t="n">
-        <v>0.471813330029271</v>
+        <v>0.000949406295328843</v>
       </c>
       <c r="F100" t="n">
         <v>13.0419805417323</v>
       </c>
       <c r="G100" t="n">
-        <v>0.469205726581918</v>
+        <v>0.000914052375655796</v>
       </c>
       <c r="H100" t="n">
         <v>0.0292785112757476</v>
@@ -11639,13 +11639,13 @@
         <v>10.1606079045992</v>
       </c>
       <c r="E101" t="n">
-        <v>0.380027575665848</v>
+        <v>0.00179883260178578</v>
       </c>
       <c r="F101" t="n">
         <v>10.1992593421621</v>
       </c>
       <c r="G101" t="n">
-        <v>0.346811218526044</v>
+        <v>0.001399042913113</v>
       </c>
       <c r="H101" t="n">
         <v>0.0333624019167661</v>
@@ -11728,13 +11728,13 @@
         <v>13.2155910707314</v>
       </c>
       <c r="E102" t="n">
-        <v>0.530513991027047</v>
+        <v>0.00147774924522609</v>
       </c>
       <c r="F102" t="n">
         <v>13.1841712607896</v>
       </c>
       <c r="G102" t="n">
-        <v>0.522862728910952</v>
+        <v>0.0013990796746274</v>
       </c>
       <c r="H102" t="n">
         <v>-0.0322019923827784</v>
@@ -11817,13 +11817,13 @@
         <v>11.8898138427808</v>
       </c>
       <c r="E103" t="n">
-        <v>0.422526826774931</v>
+        <v>0.00103761084195869</v>
       </c>
       <c r="F103" t="n">
         <v>11.8674036550653</v>
       </c>
       <c r="G103" t="n">
-        <v>0.424630784300262</v>
+        <v>0.00107217091209276</v>
       </c>
       <c r="H103" t="n">
         <v>-0.0296611467869172</v>
@@ -11906,13 +11906,13 @@
         <v>10.5152277324449</v>
       </c>
       <c r="E104" t="n">
-        <v>0.3903988875336</v>
+        <v>0.00160933329562163</v>
       </c>
       <c r="F104" t="n">
         <v>10.4884470220021</v>
       </c>
       <c r="G104" t="n">
-        <v>0.394734345427406</v>
+        <v>0.00169387498760345</v>
       </c>
       <c r="H104" t="n">
         <v>-0.0331366388004213</v>
@@ -11995,13 +11995,13 @@
         <v>16.2939477266444</v>
       </c>
       <c r="E105" t="n">
-        <v>0.60582997078875</v>
+        <v>0.00103147308625415</v>
       </c>
       <c r="F105" t="n">
         <v>16.2740204862801</v>
       </c>
       <c r="G105" t="n">
-        <v>0.606142687218626</v>
+        <v>0.00104363955799225</v>
       </c>
       <c r="H105" t="n">
         <v>-0.026638269866859</v>
@@ -12084,13 +12084,13 @@
         <v>9.48219915930276</v>
       </c>
       <c r="E106" t="n">
-        <v>0.39085106546636</v>
+        <v>0.00278093694854195</v>
       </c>
       <c r="F106" t="n">
         <v>9.44228098785293</v>
       </c>
       <c r="G106" t="n">
-        <v>0.42022944845525</v>
+        <v>0.00342696847910879</v>
       </c>
       <c r="H106" t="n">
         <v>-0.053962895196899</v>
@@ -12173,13 +12173,13 @@
         <v>11.9978320516847</v>
       </c>
       <c r="E107" t="n">
-        <v>0.442682675708252</v>
+        <v>0.00116896225672773</v>
       </c>
       <c r="F107" t="n">
         <v>12.0342377267951</v>
       </c>
       <c r="G107" t="n">
-        <v>0.438315143370067</v>
+        <v>0.00110523014414131</v>
       </c>
       <c r="H107" t="n">
         <v>0.0276577087578042</v>
@@ -12262,13 +12262,13 @@
         <v>10.1493463796147</v>
       </c>
       <c r="E108" t="n">
-        <v>0.322960158249849</v>
+        <v>0.00121443782668024</v>
       </c>
       <c r="F108" t="n">
         <v>10.1265725229843</v>
       </c>
       <c r="G108" t="n">
-        <v>0.307349907758363</v>
+        <v>0.00110118646517063</v>
       </c>
       <c r="H108" t="n">
         <v>-0.0292965523932603</v>
@@ -12351,13 +12351,13 @@
         <v>12.5212781497425</v>
       </c>
       <c r="E109" t="n">
-        <v>0.449391227971634</v>
+        <v>0.000967205906390293</v>
       </c>
       <c r="F109" t="n">
         <v>12.498088228582</v>
       </c>
       <c r="G109" t="n">
-        <v>0.443471977083089</v>
+        <v>0.000931742602872808</v>
       </c>
       <c r="H109" t="n">
         <v>-0.0300452863506884</v>
@@ -12440,13 +12440,13 @@
         <v>13.427761636397</v>
       </c>
       <c r="E110" t="n">
-        <v>0.496107463815362</v>
+        <v>0.000992256999798155</v>
       </c>
       <c r="F110" t="n">
         <v>13.4578561568761</v>
       </c>
       <c r="G110" t="n">
-        <v>0.491152609793507</v>
+        <v>0.000925501071458681</v>
       </c>
       <c r="H110" t="n">
         <v>0.0222945325283048</v>
@@ -12529,13 +12529,13 @@
         <v>10.959919054977</v>
       </c>
       <c r="E111" t="n">
-        <v>0.478619269215345</v>
+        <v>0.00247860547586837</v>
       </c>
       <c r="F111" t="n">
         <v>11.0125346577735</v>
       </c>
       <c r="G111" t="n">
-        <v>0.482929298429515</v>
+        <v>0.00255333424542119</v>
       </c>
       <c r="H111" t="n">
         <v>0.0466601619245422</v>
@@ -12618,13 +12618,13 @@
         <v>12.1597513684013</v>
       </c>
       <c r="E112" t="n">
-        <v>0.508590331429693</v>
+        <v>0.00188281178077946</v>
       </c>
       <c r="F112" t="n">
         <v>12.1286744294877</v>
       </c>
       <c r="G112" t="n">
-        <v>0.510973090560089</v>
+        <v>0.00195205775073617</v>
       </c>
       <c r="H112" t="n">
         <v>-0.0414096803368071</v>
@@ -12707,13 +12707,13 @@
         <v>14.5012628272113</v>
       </c>
       <c r="E113" t="n">
-        <v>0.599458827819037</v>
+        <v>0.00175751544377151</v>
       </c>
       <c r="F113" t="n">
         <v>14.5489304025643</v>
       </c>
       <c r="G113" t="n">
-        <v>0.588257429909774</v>
+        <v>0.0015734369537224</v>
       </c>
       <c r="H113" t="n">
         <v>0.0410701619894593</v>
@@ -12796,13 +12796,13 @@
         <v>11.2426993071505</v>
       </c>
       <c r="E114" t="n">
-        <v>0.360349584525501</v>
+        <v>0.000878467535088213</v>
       </c>
       <c r="F114" t="n">
         <v>11.2247829545838</v>
       </c>
       <c r="G114" t="n">
-        <v>0.375921360470646</v>
+        <v>0.000999053907150644</v>
       </c>
       <c r="H114" t="n">
         <v>-0.0240008389107983</v>
@@ -12885,13 +12885,13 @@
         <v>15.0276136714004</v>
       </c>
       <c r="E115" t="n">
-        <v>0.547149749279227</v>
+        <v>0.000856596617179553</v>
       </c>
       <c r="F115" t="n">
         <v>15.0108015828075</v>
       </c>
       <c r="G115" t="n">
-        <v>0.545388214154744</v>
+        <v>0.000850308087437582</v>
       </c>
       <c r="H115" t="n">
         <v>-0.0234663266831728</v>
@@ -12974,13 +12974,13 @@
         <v>11.9827186171009</v>
       </c>
       <c r="E116" t="n">
-        <v>0.498948351175476</v>
+        <v>0.00187006426737795</v>
       </c>
       <c r="F116" t="n">
         <v>11.9529146482764</v>
       </c>
       <c r="G116" t="n">
-        <v>0.50206006080467</v>
+        <v>0.00195637573478954</v>
       </c>
       <c r="H116" t="n">
         <v>-0.0367874869600924</v>
@@ -13063,13 +13063,13 @@
         <v>11.7688226439709</v>
       </c>
       <c r="E117" t="n">
-        <v>0.50069811801946</v>
+        <v>0.00208165999530812</v>
       </c>
       <c r="F117" t="n">
         <v>11.8115359953205</v>
       </c>
       <c r="G117" t="n">
-        <v>0.498579902857584</v>
+        <v>0.00201964412299567</v>
       </c>
       <c r="H117" t="n">
         <v>0.0353421189713978</v>
@@ -13152,13 +13152,13 @@
         <v>14.7055591537642</v>
       </c>
       <c r="E118" t="n">
-        <v>0.612950344240992</v>
+        <v>0.00189963063848496</v>
       </c>
       <c r="F118" t="n">
         <v>14.672799628986</v>
       </c>
       <c r="G118" t="n">
-        <v>0.615468146334662</v>
+        <v>0.00196632916057589</v>
       </c>
       <c r="H118" t="n">
         <v>-0.0410708908674552</v>
@@ -13241,13 +13241,13 @@
         <v>12.0769214791518</v>
       </c>
       <c r="E119" t="n">
-        <v>0.495473424346423</v>
+        <v>0.0017454568019058</v>
       </c>
       <c r="F119" t="n">
         <v>12.1172592917729</v>
       </c>
       <c r="G119" t="n">
-        <v>0.4756533547232</v>
+        <v>0.00145846100861718</v>
       </c>
       <c r="H119" t="n">
         <v>0.0349020115072087</v>
@@ -13330,13 +13330,13 @@
         <v>10.634472743322</v>
       </c>
       <c r="E120" t="n">
-        <v>0.245040418237272</v>
+        <v>0.000519924913382273</v>
       </c>
       <c r="F120" t="n">
         <v>10.6197314731356</v>
       </c>
       <c r="G120" t="n">
-        <v>0.327600859473299</v>
+        <v>0.000961565381218913</v>
       </c>
       <c r="H120" t="n">
         <v>-0.0218419689873696</v>
@@ -13419,13 +13419,13 @@
         <v>12.8680376078648</v>
       </c>
       <c r="E121" t="n">
-        <v>0.423445953087203</v>
+        <v>0.000654321894966505</v>
       </c>
       <c r="F121" t="n">
         <v>12.896934731662</v>
       </c>
       <c r="G121" t="n">
-        <v>0.429691568778131</v>
+        <v>0.000684019391549407</v>
       </c>
       <c r="H121" t="n">
         <v>0.021642931112981</v>
@@ -13508,13 +13508,13 @@
         <v>13.088557365143</v>
       </c>
       <c r="E122" t="n">
-        <v>0.600223503229658</v>
+        <v>0.00291446201037234</v>
       </c>
       <c r="F122" t="n">
         <v>13.1494234118154</v>
       </c>
       <c r="G122" t="n">
-        <v>0.599992563561488</v>
+        <v>0.00287752285974324</v>
       </c>
       <c r="H122" t="n">
         <v>0.0548920961228275</v>
@@ -13597,13 +13597,13 @@
         <v>13.1862771937858</v>
       </c>
       <c r="E123" t="n">
-        <v>0.432351121231916</v>
+        <v>0.00061204373189787</v>
       </c>
       <c r="F123" t="n">
         <v>13.2146963177318</v>
       </c>
       <c r="G123" t="n">
-        <v>0.45473776632846</v>
+        <v>0.000737076372125207</v>
       </c>
       <c r="H123" t="n">
         <v>0.0197806511039543</v>
@@ -13686,13 +13686,13 @@
         <v>9.68485993816161</v>
       </c>
       <c r="E124" t="n">
-        <v>0.377861572465627</v>
+        <v>0.00228660189570821</v>
       </c>
       <c r="F124" t="n">
         <v>9.65220454978022</v>
       </c>
       <c r="G124" t="n">
-        <v>0.386193161147121</v>
+        <v>0.00246121363319933</v>
       </c>
       <c r="H124" t="n">
         <v>-0.0397739657263365</v>
@@ -13775,13 +13775,13 @@
         <v>11.5071444293888</v>
       </c>
       <c r="E125" t="n">
-        <v>0.503655269113715</v>
+        <v>0.00238470144737387</v>
       </c>
       <c r="F125" t="n">
         <v>11.5499366412673</v>
       </c>
       <c r="G125" t="n">
-        <v>0.471468465015708</v>
+        <v>0.00180624138902133</v>
       </c>
       <c r="H125" t="n">
         <v>0.0376250929074739</v>
@@ -13864,13 +13864,13 @@
         <v>11.092465518731</v>
       </c>
       <c r="E126" t="n">
-        <v>0.507578986280941</v>
+        <v>0.00291667175376972</v>
       </c>
       <c r="F126" t="n">
         <v>11.1388471166209</v>
       </c>
       <c r="G126" t="n">
-        <v>0.486850166588748</v>
+        <v>0.00248599892356114</v>
       </c>
       <c r="H126" t="n">
         <v>0.0432117724903117</v>
@@ -13953,13 +13953,13 @@
         <v>9.60709635731555</v>
       </c>
       <c r="E127" t="n">
-        <v>0.477044940210922</v>
+        <v>0.00465893604487462</v>
       </c>
       <c r="F127" t="n">
         <v>9.53732667822738</v>
       </c>
       <c r="G127" t="n">
-        <v>0.483500473683634</v>
+        <v>0.00495631836111946</v>
       </c>
       <c r="H127" t="n">
         <v>-0.069233652003521</v>
@@ -14042,13 +14042,13 @@
         <v>13.1366659872023</v>
       </c>
       <c r="E128" t="n">
-        <v>0.548670734367774</v>
+        <v>0.00179028169856532</v>
       </c>
       <c r="F128" t="n">
         <v>13.1738847182868</v>
       </c>
       <c r="G128" t="n">
-        <v>0.524749683676777</v>
+        <v>0.00143324460776717</v>
       </c>
       <c r="H128" t="n">
         <v>0.0319843003279071</v>
@@ -14131,13 +14131,13 @@
         <v>14.4932278762976</v>
       </c>
       <c r="E129" t="n">
-        <v>0.584420936393428</v>
+        <v>0.00152961403425395</v>
       </c>
       <c r="F129" t="n">
         <v>14.532557724222</v>
       </c>
       <c r="G129" t="n">
-        <v>0.589420359554105</v>
+        <v>0.00158830370096717</v>
       </c>
       <c r="H129" t="n">
         <v>0.0327057113764472</v>
@@ -14220,13 +14220,13 @@
         <v>10.0225482884001</v>
       </c>
       <c r="E130" t="n">
-        <v>0.40302497907492</v>
+        <v>0.0022717996250516</v>
       </c>
       <c r="F130" t="n">
         <v>9.99210420623731</v>
       </c>
       <c r="G130" t="n">
-        <v>0.37925478807486</v>
+        <v>0.00196248294254133</v>
       </c>
       <c r="H130" t="n">
         <v>-0.0337300454090627</v>
@@ -14309,13 +14309,13 @@
         <v>12.5322820496826</v>
       </c>
       <c r="E131" t="n">
-        <v>0.555555043687852</v>
+        <v>0.00242539897013789</v>
       </c>
       <c r="F131" t="n">
         <v>12.5819050912628</v>
       </c>
       <c r="G131" t="n">
-        <v>0.559491083019421</v>
+        <v>0.00245926198156955</v>
       </c>
       <c r="H131" t="n">
         <v>0.0440240006342623</v>
@@ -14398,13 +14398,13 @@
         <v>14.9630188559499</v>
       </c>
       <c r="E132" t="n">
-        <v>0.5601816629007</v>
+        <v>0.00100561170941617</v>
       </c>
       <c r="F132" t="n">
         <v>14.9930640972978</v>
       </c>
       <c r="G132" t="n">
-        <v>0.558780703780595</v>
+        <v>0.000983198571304511</v>
       </c>
       <c r="H132" t="n">
         <v>0.0232776905142978</v>
@@ -14487,13 +14487,13 @@
         <v>10.3062338729865</v>
       </c>
       <c r="E133" t="n">
-        <v>0.270631292542153</v>
+        <v>0.00076464138969108</v>
       </c>
       <c r="F133" t="n">
         <v>10.2836176871248</v>
       </c>
       <c r="G133" t="n">
-        <v>0.440229167250605</v>
+        <v>0.0025666737043408</v>
       </c>
       <c r="H133" t="n">
         <v>-0.0310215708942132</v>
@@ -14576,13 +14576,13 @@
         <v>13.095173804204</v>
       </c>
       <c r="E134" t="n">
-        <v>0.581706753293032</v>
+        <v>0.00246220552020617</v>
       </c>
       <c r="F134" t="n">
         <v>13.1432144184054</v>
       </c>
       <c r="G134" t="n">
-        <v>0.565700248037869</v>
+        <v>0.00210527328685286</v>
       </c>
       <c r="H134" t="n">
         <v>0.0424751022561868</v>
@@ -14665,13 +14665,13 @@
         <v>8.8793737126314</v>
       </c>
       <c r="E135" t="n">
-        <v>0.424056106664492</v>
+        <v>0.00470982419850362</v>
       </c>
       <c r="F135" t="n">
         <v>8.8177337655912</v>
       </c>
       <c r="G135" t="n">
-        <v>0.42948215534617</v>
+        <v>0.00499704889170178</v>
       </c>
       <c r="H135" t="n">
         <v>-0.0608867847055953</v>
@@ -14754,13 +14754,13 @@
         <v>13.6899276024978</v>
       </c>
       <c r="E136" t="n">
-        <v>0.541431216633983</v>
+        <v>0.00136577661747435</v>
       </c>
       <c r="F136" t="n">
         <v>13.6719542544065</v>
       </c>
       <c r="G136" t="n">
-        <v>0.547854681984121</v>
+        <v>0.0014477488391907</v>
       </c>
       <c r="H136" t="n">
         <v>-0.024210238082274</v>
@@ -14843,13 +14843,13 @@
         <v>10.9425323498692</v>
       </c>
       <c r="E137" t="n">
-        <v>0.513438542904553</v>
+        <v>0.00330448511661191</v>
       </c>
       <c r="F137" t="n">
         <v>10.9942637082618</v>
       </c>
       <c r="G137" t="n">
-        <v>0.518187988588685</v>
+        <v>0.00332381689672936</v>
       </c>
       <c r="H137" t="n">
         <v>0.0453073440576855</v>
@@ -14932,13 +14932,13 @@
         <v>14.6446413368635</v>
       </c>
       <c r="E138" t="n">
-        <v>0.537946653498371</v>
+        <v>0.000904909624152822</v>
       </c>
       <c r="F138" t="n">
         <v>14.6706764051389</v>
       </c>
       <c r="G138" t="n">
-        <v>0.545096157707282</v>
+        <v>0.000963326220957306</v>
       </c>
       <c r="H138" t="n">
         <v>0.0185358698905001</v>
@@ -15021,13 +15021,13 @@
         <v>11.3264899086782</v>
       </c>
       <c r="E139" t="n">
-        <v>0.317701546639269</v>
+        <v>0.000601818519447496</v>
       </c>
       <c r="F139" t="n">
         <v>11.3508216821332</v>
       </c>
       <c r="G139" t="n">
-        <v>0.316365716347713</v>
+        <v>0.000586091434697582</v>
       </c>
       <c r="H139" t="n">
         <v>0.0176710652265304</v>
@@ -15110,13 +15110,13 @@
         <v>11.0478202821516</v>
       </c>
       <c r="E140" t="n">
-        <v>0.421940142451288</v>
+        <v>0.00155452468196071</v>
       </c>
       <c r="F140" t="n">
         <v>11.0752125409836</v>
       </c>
       <c r="G140" t="n">
-        <v>0.320767013645572</v>
+        <v>0.000707106145788318</v>
       </c>
       <c r="H140" t="n">
         <v>0.0221858466394156</v>
@@ -15199,13 +15199,13 @@
         <v>11.2043182990496</v>
       </c>
       <c r="E141" t="n">
-        <v>0.421465322547662</v>
+        <v>0.00143582874086353</v>
       </c>
       <c r="F141" t="n">
         <v>11.2352106438062</v>
       </c>
       <c r="G141" t="n">
-        <v>0.429908520374024</v>
+        <v>0.00151936377486157</v>
       </c>
       <c r="H141" t="n">
         <v>0.0236105505550661</v>
@@ -15288,13 +15288,13 @@
         <v>14.2891363605504</v>
       </c>
       <c r="E142" t="n">
-        <v>0.429005907118221</v>
+        <v>0.000353670036096279</v>
       </c>
       <c r="F142" t="n">
         <v>14.2793406169165</v>
       </c>
       <c r="G142" t="n">
-        <v>0.397294296426101</v>
+        <v>0.000259150290251505</v>
       </c>
       <c r="H142" t="n">
         <v>-0.0156606762161363</v>
@@ -15377,13 +15377,13 @@
         <v>13.8786592284577</v>
       </c>
       <c r="E143" t="n">
-        <v>0.451361829010915</v>
+        <v>0.000529904240222872</v>
       </c>
       <c r="F143" t="n">
         <v>13.8705381087408</v>
       </c>
       <c r="G143" t="n">
-        <v>0.434630919024412</v>
+        <v>0.000453952931110692</v>
       </c>
       <c r="H143" t="n">
         <v>-0.0140814353237173</v>
@@ -15466,13 +15466,13 @@
         <v>11.5082337983865</v>
       </c>
       <c r="E144" t="n">
-        <v>0.357928619004123</v>
+        <v>0.000749401001798383</v>
       </c>
       <c r="F144" t="n">
         <v>11.5313950222227</v>
       </c>
       <c r="G144" t="n">
-        <v>0.345703119543258</v>
+        <v>0.000668745460933368</v>
       </c>
       <c r="H144" t="n">
         <v>0.0172510853272378</v>
@@ -15555,13 +15555,13 @@
         <v>12.1363723583739</v>
       </c>
       <c r="E145" t="n">
-        <v>0.61136019097147</v>
+        <v>0.00450218226411801</v>
       </c>
       <c r="F145" t="n">
         <v>12.2087086136696</v>
       </c>
       <c r="G145" t="n">
-        <v>0.6239183211387</v>
+        <v>0.00492053906439696</v>
       </c>
       <c r="H145" t="n">
         <v>0.0660972931305109</v>
@@ -15644,13 +15644,13 @@
         <v>13.6706152447376</v>
       </c>
       <c r="E146" t="n">
-        <v>0.483976051427325</v>
+        <v>0.000793843856565917</v>
       </c>
       <c r="F146" t="n">
         <v>13.6584362053363</v>
       </c>
       <c r="G146" t="n">
-        <v>0.49526670220018</v>
+        <v>0.000888235365260062</v>
       </c>
       <c r="H146" t="n">
         <v>-0.0188916516795999</v>
@@ -15733,13 +15733,13 @@
         <v>11.934162412831</v>
       </c>
       <c r="E147" t="n">
-        <v>0.449902036188131</v>
+        <v>0.00127686811275348</v>
       </c>
       <c r="F147" t="n">
         <v>11.919277239388</v>
       </c>
       <c r="G147" t="n">
-        <v>0.447567716172644</v>
+        <v>0.00126091649168945</v>
       </c>
       <c r="H147" t="n">
         <v>-0.0214756224225521</v>
@@ -15822,13 +15822,13 @@
         <v>12.2815589070933</v>
       </c>
       <c r="E148" t="n">
-        <v>0.508423443533788</v>
+        <v>0.0017831462721575</v>
       </c>
       <c r="F148" t="n">
         <v>12.3146719181091</v>
       </c>
       <c r="G148" t="n">
-        <v>0.476569825822872</v>
+        <v>0.00134234995415388</v>
       </c>
       <c r="H148" t="n">
         <v>0.0269878385945874</v>
@@ -15911,13 +15911,13 @@
         <v>13.4059272057219</v>
       </c>
       <c r="E149" t="n">
-        <v>0.555163450458082</v>
+        <v>0.00173429375394712</v>
       </c>
       <c r="F149" t="n">
         <v>13.3868087454605</v>
       </c>
       <c r="G149" t="n">
-        <v>0.557453394619086</v>
+        <v>0.00176664727561046</v>
       </c>
       <c r="H149" t="n">
         <v>-0.0256090276898568</v>
@@ -16000,13 +16000,13 @@
         <v>12.0844094821882</v>
       </c>
       <c r="E150" t="n">
-        <v>0.673455312312904</v>
+        <v>0.00777432235459172</v>
       </c>
       <c r="F150" t="n">
         <v>11.9897041163792</v>
       </c>
       <c r="G150" t="n">
-        <v>0.664389022939658</v>
+        <v>0.00737329298030615</v>
       </c>
       <c r="H150" t="n">
         <v>-0.104561175783633</v>
@@ -16089,13 +16089,13 @@
         <v>11.9155759031123</v>
       </c>
       <c r="E151" t="n">
-        <v>0.387751367194649</v>
+        <v>0.000773586259936166</v>
       </c>
       <c r="F151" t="n">
         <v>11.9383271225846</v>
       </c>
       <c r="G151" t="n">
-        <v>0.389472639483535</v>
+        <v>0.000770134281257786</v>
       </c>
       <c r="H151" t="n">
         <v>0.0162179249052449</v>
@@ -16178,13 +16178,13 @@
         <v>13.0078779828061</v>
       </c>
       <c r="E152" t="n">
-        <v>0.528332643060357</v>
+        <v>0.00158402399587983</v>
       </c>
       <c r="F152" t="n">
         <v>13.0419822740771</v>
       </c>
       <c r="G152" t="n">
-        <v>0.556336955003127</v>
+        <v>0.00199195407668385</v>
       </c>
       <c r="H152" t="n">
         <v>0.027048581054465</v>
@@ -16267,13 +16267,13 @@
         <v>12.4057677803256</v>
       </c>
       <c r="E153" t="n">
-        <v>0.61539605832596</v>
+        <v>0.004262625688981</v>
       </c>
       <c r="F153" t="n">
         <v>12.3493004362821</v>
       </c>
       <c r="G153" t="n">
-        <v>0.625303879652727</v>
+        <v>0.00473541425795593</v>
       </c>
       <c r="H153" t="n">
         <v>-0.0618194041684629</v>
@@ -16356,13 +16356,13 @@
         <v>11.2491778023362</v>
       </c>
       <c r="E154" t="n">
-        <v>0.423017057111403</v>
+        <v>0.00142975708750266</v>
       </c>
       <c r="F154" t="n">
         <v>11.237032413702</v>
       </c>
       <c r="G154" t="n">
-        <v>0.426667256450678</v>
+        <v>0.00147167813046054</v>
       </c>
       <c r="H154" t="n">
         <v>-0.0182849762894352</v>
@@ -16445,13 +16445,13 @@
         <v>9.95108451039732</v>
       </c>
       <c r="E155" t="n">
-        <v>0.329625462387687</v>
+        <v>0.00142098125363824</v>
       </c>
       <c r="F155" t="n">
         <v>9.94108574267598</v>
       </c>
       <c r="G155" t="n">
-        <v>0.30628962808882</v>
+        <v>0.00121513049123095</v>
       </c>
       <c r="H155" t="n">
         <v>-0.016104603438857</v>
@@ -16534,13 +16534,13 @@
         <v>12.7860084838373</v>
       </c>
       <c r="E156" t="n">
-        <v>0.477943488475291</v>
+        <v>0.00110496671096484</v>
       </c>
       <c r="F156" t="n">
         <v>12.8115821584085</v>
       </c>
       <c r="G156" t="n">
-        <v>0.442684113502077</v>
+        <v>0.000794768768442941</v>
       </c>
       <c r="H156" t="n">
         <v>0.0190478031678231</v>
@@ -16623,13 +16623,13 @@
         <v>10.5356516049816</v>
       </c>
       <c r="E157" t="n">
-        <v>0.367778200505716</v>
+        <v>0.00135179776734312</v>
       </c>
       <c r="F157" t="n">
         <v>10.5591448077748</v>
       </c>
       <c r="G157" t="n">
-        <v>0.353066801552304</v>
+        <v>0.00120052732983989</v>
       </c>
       <c r="H157" t="n">
         <v>0.0191442612888243</v>
@@ -16712,13 +16712,13 @@
         <v>13.7170891431099</v>
       </c>
       <c r="E158" t="n">
-        <v>0.58289259838523</v>
+        <v>0.00197454420893375</v>
       </c>
       <c r="F158" t="n">
         <v>13.751689710089</v>
       </c>
       <c r="G158" t="n">
-        <v>0.565485452112268</v>
+        <v>0.00167978121831901</v>
       </c>
       <c r="H158" t="n">
         <v>0.0271082652242737</v>
@@ -16801,13 +16801,13 @@
         <v>13.6224719626533</v>
       </c>
       <c r="E159" t="n">
-        <v>0.500029232765333</v>
+        <v>0.000947387512051571</v>
       </c>
       <c r="F159" t="n">
         <v>13.6429217944368</v>
       </c>
       <c r="G159" t="n">
-        <v>0.507926782649956</v>
+        <v>0.00100417818858333</v>
       </c>
       <c r="H159" t="n">
         <v>0.0142754030990973</v>
@@ -16890,13 +16890,13 @@
         <v>14.1661677933586</v>
       </c>
       <c r="E160" t="n">
-        <v>0.583693528384876</v>
+        <v>0.00170891621880999</v>
       </c>
       <c r="F160" t="n">
         <v>14.1484245487965</v>
       </c>
       <c r="G160" t="n">
-        <v>0.58580103104227</v>
+        <v>0.0017546844861544</v>
       </c>
       <c r="H160" t="n">
         <v>-0.0241188327358484</v>
@@ -16979,13 +16979,13 @@
         <v>15.7181252640391</v>
       </c>
       <c r="E161" t="n">
-        <v>0.604683123216085</v>
+        <v>0.00123801718112268</v>
       </c>
       <c r="F161" t="n">
         <v>15.7050689690398</v>
       </c>
       <c r="G161" t="n">
-        <v>0.609111871852606</v>
+        <v>0.00130247875391854</v>
       </c>
       <c r="H161" t="n">
         <v>-0.0191883343465312</v>
@@ -17068,13 +17068,13 @@
         <v>10.9076286036741</v>
       </c>
       <c r="E162" t="n">
-        <v>0.497141834946741</v>
+        <v>0.00297050764402322</v>
       </c>
       <c r="F162" t="n">
         <v>10.8770145534074</v>
       </c>
       <c r="G162" t="n">
-        <v>0.493846903749759</v>
+        <v>0.00290002436307319</v>
       </c>
       <c r="H162" t="n">
         <v>-0.0338601222417408</v>
@@ -17157,13 +17157,13 @@
         <v>9.91219431462172</v>
       </c>
       <c r="E163" t="n">
-        <v>0.292520624898699</v>
+        <v>0.0011273858365715</v>
       </c>
       <c r="F163" t="n">
         <v>9.90080405741709</v>
       </c>
       <c r="G163" t="n">
-        <v>0.340398400963781</v>
+        <v>0.00157034138391831</v>
       </c>
       <c r="H163" t="n">
         <v>-0.0184263652964671</v>
@@ -17246,13 +17246,13 @@
         <v>13.1977109210593</v>
       </c>
       <c r="E164" t="n">
-        <v>0.498566426894398</v>
+        <v>0.00111891591705614</v>
       </c>
       <c r="F164" t="n">
         <v>13.1891779276053</v>
       </c>
       <c r="G164" t="n">
-        <v>0.503348081511277</v>
+        <v>0.00116216842981491</v>
       </c>
       <c r="H164" t="n">
         <v>-0.0153639890943044</v>
@@ -17335,13 +17335,13 @@
         <v>14.4842735176591</v>
       </c>
       <c r="E165" t="n">
-        <v>0.577259862037706</v>
+        <v>0.00143272657921807</v>
       </c>
       <c r="F165" t="n">
         <v>14.4714879812658</v>
       </c>
       <c r="G165" t="n">
-        <v>0.580648209530064</v>
+        <v>0.00148217721601836</v>
       </c>
       <c r="H165" t="n">
         <v>-0.0188874839951311</v>
@@ -17424,13 +17424,13 @@
         <v>11.785922605134</v>
       </c>
       <c r="E166" t="n">
-        <v>0.356330721320171</v>
+        <v>0.000635774817707978</v>
       </c>
       <c r="F166" t="n">
         <v>11.7787495033891</v>
       </c>
       <c r="G166" t="n">
-        <v>0.351506828102102</v>
+        <v>0.000615902521200103</v>
       </c>
       <c r="H166" t="n">
         <v>-0.0137695730034939</v>
@@ -17513,13 +17513,13 @@
         <v>14.3276583836185</v>
       </c>
       <c r="E167" t="n">
-        <v>0.561403635048103</v>
+        <v>0.0013020676897211</v>
       </c>
       <c r="F167" t="n">
         <v>14.3510628542228</v>
       </c>
       <c r="G167" t="n">
-        <v>0.564660371341218</v>
+        <v>0.00131354938802274</v>
       </c>
       <c r="H167" t="n">
         <v>0.0169400619860418</v>
@@ -17602,13 +17602,13 @@
         <v>11.4922298165859</v>
       </c>
       <c r="E168" t="n">
-        <v>0.603906159581828</v>
+        <v>0.00538113813330983</v>
       </c>
       <c r="F168" t="n">
         <v>11.4348393266116</v>
       </c>
       <c r="G168" t="n">
-        <v>0.609778563911268</v>
+        <v>0.0056921770057828</v>
       </c>
       <c r="H168" t="n">
         <v>-0.0601111288904211</v>
@@ -17691,13 +17691,13 @@
         <v>13.4528832047037</v>
       </c>
       <c r="E169" t="n">
-        <v>0.519462727142526</v>
+        <v>0.0012154567194081</v>
       </c>
       <c r="F169" t="n">
         <v>13.4425938445457</v>
       </c>
       <c r="G169" t="n">
-        <v>0.525798316100113</v>
+        <v>0.00129217700317423</v>
       </c>
       <c r="H169" t="n">
         <v>-0.0165617652749714</v>
@@ -17780,13 +17780,13 @@
         <v>12.5958577224224</v>
       </c>
       <c r="E170" t="n">
-        <v>0.476344419437832</v>
+        <v>0.00117927619223898</v>
       </c>
       <c r="F170" t="n">
         <v>12.6209474918154</v>
       </c>
       <c r="G170" t="n">
-        <v>0.482836095421763</v>
+        <v>0.00124359775699166</v>
       </c>
       <c r="H170" t="n">
         <v>0.0184731990196562</v>
@@ -17869,13 +17869,13 @@
         <v>11.4512917107007</v>
       </c>
       <c r="E171" t="n">
-        <v>0.522019821439983</v>
+        <v>0.00285182240392365</v>
       </c>
       <c r="F171" t="n">
         <v>11.4259507486781</v>
       </c>
       <c r="G171" t="n">
-        <v>0.534202726042858</v>
+        <v>0.00313142003359504</v>
       </c>
       <c r="H171" t="n">
         <v>-0.0326767063846376</v>
@@ -17958,13 +17958,13 @@
         <v>13.1663847807396</v>
       </c>
       <c r="E172" t="n">
-        <v>0.50550589216372</v>
+        <v>0.00119756227116616</v>
       </c>
       <c r="F172" t="n">
         <v>13.1910875554977</v>
       </c>
       <c r="G172" t="n">
-        <v>0.515985575804942</v>
+        <v>0.00131463541009961</v>
       </c>
       <c r="H172" t="n">
         <v>0.0171691654861805</v>
@@ -18047,13 +18047,13 @@
         <v>13.19078092701</v>
       </c>
       <c r="E173" t="n">
-        <v>0.53038226849693</v>
+        <v>0.0014911556448234</v>
       </c>
       <c r="F173" t="n">
         <v>13.2166767816902</v>
       </c>
       <c r="G173" t="n">
-        <v>0.506405426270333</v>
+        <v>0.00118824830462525</v>
       </c>
       <c r="H173" t="n">
         <v>0.0186457165599064</v>
@@ -18136,13 +18136,13 @@
         <v>9.06411414583636</v>
       </c>
       <c r="E174" t="n">
-        <v>0.326241749964303</v>
+        <v>0.00231856098420973</v>
       </c>
       <c r="F174" t="n">
         <v>9.05016066394432</v>
       </c>
       <c r="G174" t="n">
-        <v>0.341713536458681</v>
+        <v>0.00255514095291702</v>
       </c>
       <c r="H174" t="n">
         <v>-0.0228960303726345</v>
@@ -18225,13 +18225,13 @@
         <v>13.1468488794846</v>
       </c>
       <c r="E175" t="n">
-        <v>0.589737520542819</v>
+        <v>0.00261464313004451</v>
       </c>
       <c r="F175" t="n">
         <v>13.1243125177854</v>
       </c>
       <c r="G175" t="n">
-        <v>0.595181942427014</v>
+        <v>0.00276626639808837</v>
       </c>
       <c r="H175" t="n">
         <v>-0.0299340915301011</v>
@@ -18314,13 +18314,13 @@
         <v>12.2339036566276</v>
       </c>
       <c r="E176" t="n">
-        <v>0.487306857757988</v>
+        <v>0.00151161057469657</v>
       </c>
       <c r="F176" t="n">
         <v>12.2600002815284</v>
       </c>
       <c r="G176" t="n">
-        <v>0.481665406660353</v>
+        <v>0.00144781801549564</v>
       </c>
       <c r="H176" t="n">
         <v>0.0189797162058925</v>
@@ -18403,13 +18403,13 @@
         <v>10.1645793438031</v>
       </c>
       <c r="E177" t="n">
-        <v>0.254385213292541</v>
+        <v>0.000742235470969989</v>
       </c>
       <c r="F177" t="n">
         <v>10.160790548584</v>
       </c>
       <c r="G177" t="n">
-        <v>0.237440756349981</v>
+        <v>0.000660656636019401</v>
       </c>
       <c r="H177" t="n">
         <v>-0.0125101410467255</v>
@@ -18492,13 +18492,13 @@
         <v>13.6642886004591</v>
       </c>
       <c r="E178" t="n">
-        <v>0.470456571806427</v>
+        <v>0.00070076219379302</v>
       </c>
       <c r="F178" t="n">
         <v>13.6833456228596</v>
       </c>
       <c r="G178" t="n">
-        <v>0.482634480484957</v>
+        <v>0.000778809393321869</v>
       </c>
       <c r="H178" t="n">
         <v>0.0117974358613421</v>
@@ -18581,13 +18581,13 @@
         <v>13.9058174393924</v>
       </c>
       <c r="E179" t="n">
-        <v>0.492068385702704</v>
+        <v>0.000774681559531085</v>
       </c>
       <c r="F179" t="n">
         <v>13.9241320304013</v>
       </c>
       <c r="G179" t="n">
-        <v>0.482289994200577</v>
+        <v>0.000701438481821413</v>
       </c>
       <c r="H179" t="n">
         <v>0.0106632586349954</v>
@@ -18670,13 +18670,13 @@
         <v>13.767217154796</v>
       </c>
       <c r="E180" t="n">
-        <v>0.541314716625779</v>
+        <v>0.0013188242043292</v>
       </c>
       <c r="F180" t="n">
         <v>13.7595206922201</v>
       </c>
       <c r="G180" t="n">
-        <v>0.537171244022401</v>
+        <v>0.00126833391871694</v>
       </c>
       <c r="H180" t="n">
         <v>-0.0148039868438609</v>
@@ -18759,13 +18759,13 @@
         <v>9.47040449155325</v>
       </c>
       <c r="E181" t="n">
-        <v>0.475977932640209</v>
+        <v>0.00476487029907382</v>
       </c>
       <c r="F181" t="n">
         <v>9.50425042137881</v>
       </c>
       <c r="G181" t="n">
-        <v>0.444545537864537</v>
+        <v>0.00399153088611198</v>
       </c>
       <c r="H181" t="n">
         <v>0.0319232149983576</v>
@@ -18848,13 +18848,13 @@
         <v>14.0456845523033</v>
       </c>
       <c r="E182" t="n">
-        <v>0.523592114986492</v>
+        <v>0.000997723719710558</v>
       </c>
       <c r="F182" t="n">
         <v>14.0628715841142</v>
       </c>
       <c r="G182" t="n">
-        <v>0.5285460291094</v>
+        <v>0.0010326043323119</v>
       </c>
       <c r="H182" t="n">
         <v>0.01090892906586</v>
@@ -18937,13 +18937,13 @@
         <v>9.97001201796832</v>
       </c>
       <c r="E183" t="n">
-        <v>0.268512186280793</v>
+        <v>0.00091946277186584</v>
       </c>
       <c r="F183" t="n">
         <v>9.96535441612608</v>
       </c>
       <c r="G183" t="n">
-        <v>0.286336557444031</v>
+        <v>0.00104981050211629</v>
       </c>
       <c r="H183" t="n">
         <v>-0.0113843311211373</v>
@@ -19026,13 +19026,13 @@
         <v>14.4459790469816</v>
       </c>
       <c r="E184" t="n">
-        <v>0.522706828653554</v>
+        <v>0.000835837634647035</v>
       </c>
       <c r="F184" t="n">
         <v>14.4411161762819</v>
       </c>
       <c r="G184" t="n">
-        <v>0.515590166364185</v>
+        <v>0.000785942547206942</v>
       </c>
       <c r="H184" t="n">
         <v>-0.0117902089456681</v>
@@ -19115,13 +19115,13 @@
         <v>10.9516462924114</v>
       </c>
       <c r="E185" t="n">
-        <v>0.441832059549884</v>
+        <v>0.00189491496057481</v>
       </c>
       <c r="F185" t="n">
         <v>10.9724474319461</v>
       </c>
       <c r="G185" t="n">
-        <v>0.39550940915414</v>
+        <v>0.00133190672204258</v>
       </c>
       <c r="H185" t="n">
         <v>0.0151958518379315</v>
@@ -19204,13 +19204,13 @@
         <v>13.5557602952659</v>
       </c>
       <c r="E186" t="n">
-        <v>0.548536346537809</v>
+        <v>0.00152286760994514</v>
       </c>
       <c r="F186" t="n">
         <v>13.5789512749469</v>
       </c>
       <c r="G186" t="n">
-        <v>0.540208171103423</v>
+        <v>0.00140675273850274</v>
       </c>
       <c r="H186" t="n">
         <v>0.0160559841974188</v>
@@ -19293,13 +19293,13 @@
         <v>12.5177094426831</v>
       </c>
       <c r="E187" t="n">
-        <v>0.554239304641933</v>
+        <v>0.00241787961033503</v>
       </c>
       <c r="F187" t="n">
         <v>12.5425579319325</v>
       </c>
       <c r="G187" t="n">
-        <v>0.551349137053773</v>
+        <v>0.00232136440105065</v>
       </c>
       <c r="H187" t="n">
         <v>0.020886614578079</v>
@@ -19382,13 +19382,13 @@
         <v>12.2436940810201</v>
       </c>
       <c r="E188" t="n">
-        <v>0.410050814124217</v>
+        <v>0.000789409466380403</v>
       </c>
       <c r="F188" t="n">
         <v>12.2385519328151</v>
       </c>
       <c r="G188" t="n">
-        <v>0.423613893552872</v>
+        <v>0.000887418210401831</v>
       </c>
       <c r="H188" t="n">
         <v>-0.0116279111944648</v>
@@ -19471,13 +19471,13 @@
         <v>11.204792837046</v>
       </c>
       <c r="E189" t="n">
-        <v>0.337384942177315</v>
+        <v>0.000748761745311061</v>
       </c>
       <c r="F189" t="n">
         <v>11.2224615440241</v>
       </c>
       <c r="G189" t="n">
-        <v>0.342919001224793</v>
+        <v>0.000774712998096811</v>
       </c>
       <c r="H189" t="n">
         <v>0.0104744803118531</v>
@@ -19560,13 +19560,13 @@
         <v>13.2907906771285</v>
       </c>
       <c r="E190" t="n">
-        <v>0.472642040399953</v>
+        <v>0.000841486059210485</v>
       </c>
       <c r="F190" t="n">
         <v>13.2871952791086</v>
       </c>
       <c r="G190" t="n">
-        <v>0.495890921568079</v>
+        <v>0.00104613130358001</v>
       </c>
       <c r="H190" t="n">
         <v>-0.0111017964854983</v>
@@ -19649,13 +19649,13 @@
         <v>14.9622074355701</v>
       </c>
       <c r="E191" t="n">
-        <v>0.717728023765303</v>
+        <v>0.00520911187942616</v>
       </c>
       <c r="F191" t="n">
         <v>14.9156373224438</v>
       </c>
       <c r="G191" t="n">
-        <v>0.719870765006282</v>
+        <v>0.00528149099696722</v>
       </c>
       <c r="H191" t="n">
         <v>-0.0502460267249051</v>
@@ -19738,13 +19738,13 @@
         <v>14.4182753778901</v>
       </c>
       <c r="E192" t="n">
-        <v>0.537941421038653</v>
+        <v>0.000983808905986942</v>
       </c>
       <c r="F192" t="n">
         <v>14.4354220800829</v>
       </c>
       <c r="G192" t="n">
-        <v>0.543483225891557</v>
+        <v>0.00104156814944813</v>
       </c>
       <c r="H192" t="n">
         <v>0.010652762969832</v>
@@ -19827,13 +19827,13 @@
         <v>11.3899831546119</v>
       </c>
       <c r="E193" t="n">
-        <v>0.416916685894593</v>
+        <v>0.00126768482824295</v>
       </c>
       <c r="F193" t="n">
         <v>11.3859491879319</v>
       </c>
       <c r="G193" t="n">
-        <v>0.421140847885057</v>
+        <v>0.00131557000865027</v>
       </c>
       <c r="H193" t="n">
         <v>-0.0103179565272442</v>
@@ -19916,13 +19916,13 @@
         <v>12.474228624116</v>
       </c>
       <c r="E194" t="n">
-        <v>0.575301658175892</v>
+        <v>0.00293280038217414</v>
       </c>
       <c r="F194" t="n">
         <v>12.5015474684878</v>
       </c>
       <c r="G194" t="n">
-        <v>0.574681607321478</v>
+        <v>0.00290718077962867</v>
       </c>
       <c r="H194" t="n">
         <v>0.0216412638612255</v>
@@ -20005,13 +20005,13 @@
         <v>8.98095814078999</v>
       </c>
       <c r="E195" t="n">
-        <v>0.322826053957144</v>
+        <v>0.00236845328968604</v>
       </c>
       <c r="F195" t="n">
         <v>9.00179924176249</v>
       </c>
       <c r="G195" t="n">
-        <v>0.307031803039336</v>
+        <v>0.0021205382744886</v>
       </c>
       <c r="H195" t="n">
         <v>0.0136161768292147</v>
@@ -20094,13 +20094,13 @@
         <v>11.4515577403286</v>
       </c>
       <c r="E196" t="n">
-        <v>0.456685079548183</v>
+        <v>0.00169145896296096</v>
       </c>
       <c r="F196" t="n">
         <v>11.4488950935338</v>
       </c>
       <c r="G196" t="n">
-        <v>0.469386264861861</v>
+        <v>0.00186567924892489</v>
       </c>
       <c r="H196" t="n">
         <v>-0.0137612500258034</v>
@@ -20183,13 +20183,13 @@
         <v>12.4043066100849</v>
       </c>
       <c r="E197" t="n">
-        <v>0.500495326959182</v>
+        <v>0.0015849000734755</v>
       </c>
       <c r="F197" t="n">
         <v>12.3990243122581</v>
       </c>
       <c r="G197" t="n">
-        <v>0.504358865220822</v>
+        <v>0.00164577352512558</v>
       </c>
       <c r="H197" t="n">
         <v>-0.0127012560487033</v>
@@ -20272,13 +20272,13 @@
         <v>13.1545178101187</v>
       </c>
       <c r="E198" t="n">
-        <v>0.461339523827808</v>
+        <v>0.000805406122265335</v>
       </c>
       <c r="F198" t="n">
         <v>13.1544687717306</v>
       </c>
       <c r="G198" t="n">
-        <v>0.457287417688603</v>
+        <v>0.000780540622163875</v>
       </c>
       <c r="H198" t="n">
         <v>-0.00780801178448974</v>
@@ -20361,13 +20361,13 @@
         <v>13.6184966760317</v>
       </c>
       <c r="E199" t="n">
-        <v>0.513567370029215</v>
+        <v>0.00107434269840103</v>
       </c>
       <c r="F199" t="n">
         <v>13.6338805805631</v>
       </c>
       <c r="G199" t="n">
-        <v>0.513987379570346</v>
+        <v>0.00107164725513208</v>
       </c>
       <c r="H199" t="n">
         <v>0.00924579766592046</v>
@@ -20450,13 +20450,13 @@
         <v>11.9415943629597</v>
       </c>
       <c r="E200" t="n">
-        <v>0.409171532652739</v>
+        <v>0.00091266369140554</v>
       </c>
       <c r="F200" t="n">
         <v>11.9573971011741</v>
       </c>
       <c r="G200" t="n">
-        <v>0.408924982323679</v>
+        <v>0.00089621824172818</v>
       </c>
       <c r="H200" t="n">
         <v>0.00978711873499112</v>
@@ -20539,13 +20539,13 @@
         <v>13.8066925298917</v>
       </c>
       <c r="E201" t="n">
-        <v>0.586408251452239</v>
+        <v>0.00198242002717904</v>
       </c>
       <c r="F201" t="n">
         <v>13.8285671425251</v>
       </c>
       <c r="G201" t="n">
-        <v>0.592570781456852</v>
+        <v>0.00211278785509996</v>
       </c>
       <c r="H201" t="n">
         <v>0.0144050386808026</v>
@@ -20628,13 +20628,13 @@
         <v>10.616158645423</v>
       </c>
       <c r="E202" t="n">
-        <v>0.358035893872139</v>
+        <v>0.0012049050635375</v>
       </c>
       <c r="F202" t="n">
         <v>10.6159608419904</v>
       </c>
       <c r="G202" t="n">
-        <v>0.363176299245793</v>
+        <v>0.00124860353400777</v>
       </c>
       <c r="H202" t="n">
         <v>-0.00680830827095372</v>
@@ -20717,13 +20717,13 @@
         <v>11.4902871310311</v>
       </c>
       <c r="E203" t="n">
-        <v>0.377680118959327</v>
+        <v>0.000885503388836252</v>
       </c>
       <c r="F203" t="n">
         <v>11.497752105195</v>
       </c>
       <c r="G203" t="n">
-        <v>0.389225924966471</v>
+        <v>0.000963069138690356</v>
       </c>
       <c r="H203" t="n">
         <v>0.00830787128918674</v>
@@ -20806,13 +20806,13 @@
         <v>11.676463959653</v>
       </c>
       <c r="E204" t="n">
-        <v>0.365931945487069</v>
+        <v>0.000728014703587782</v>
       </c>
       <c r="F204" t="n">
         <v>11.671262313608</v>
       </c>
       <c r="G204" t="n">
-        <v>0.271593276570508</v>
+        <v>0.000341022720005933</v>
       </c>
       <c r="H204" t="n">
         <v>-0.00714704864976116</v>
@@ -20895,13 +20895,13 @@
         <v>13.6267256711039</v>
       </c>
       <c r="E205" t="n">
-        <v>0.446769176780612</v>
+        <v>0.000569330725501591</v>
       </c>
       <c r="F205" t="n">
         <v>13.6394939258656</v>
       </c>
       <c r="G205" t="n">
-        <v>0.443341797804355</v>
+        <v>0.000547979435275219</v>
       </c>
       <c r="H205" t="n">
         <v>0.00629890219367829</v>
@@ -20984,13 +20984,13 @@
         <v>13.6959295184366</v>
       </c>
       <c r="E206" t="n">
-        <v>0.474341998916667</v>
+        <v>0.000715065071585479</v>
       </c>
       <c r="F206" t="n">
         <v>13.7094224088359</v>
       </c>
       <c r="G206" t="n">
-        <v>0.465080686744362</v>
+        <v>0.000653853293710481</v>
       </c>
       <c r="H206" t="n">
         <v>0.00675503094840167</v>
@@ -21073,13 +21073,13 @@
         <v>13.6898481571707</v>
       </c>
       <c r="E207" t="n">
-        <v>0.608035792525267</v>
+        <v>0.00258453531856109</v>
       </c>
       <c r="F207" t="n">
         <v>13.7169529652723</v>
       </c>
       <c r="G207" t="n">
-        <v>0.622619082325875</v>
+        <v>0.0028619138082525</v>
       </c>
       <c r="H207" t="n">
         <v>0.016765226201515</v>
@@ -21162,13 +21162,13 @@
         <v>12.5162954876301</v>
       </c>
       <c r="E208" t="n">
-        <v>0.552089276041785</v>
+        <v>0.00237189487726838</v>
       </c>
       <c r="F208" t="n">
         <v>12.5071032187666</v>
       </c>
       <c r="G208" t="n">
-        <v>0.564078173972618</v>
+        <v>0.00262500407094559</v>
       </c>
       <c r="H208" t="n">
         <v>-0.0155118179431241</v>
@@ -21251,13 +21251,13 @@
         <v>11.8901726812005</v>
       </c>
       <c r="E209" t="n">
-        <v>0.510033831003684</v>
+        <v>0.00215670702470052</v>
       </c>
       <c r="F209" t="n">
         <v>11.9113186015835</v>
       </c>
       <c r="G209" t="n">
-        <v>0.507922366601674</v>
+        <v>0.00206468436111178</v>
       </c>
       <c r="H209" t="n">
         <v>0.0137976349890094</v>
@@ -21340,13 +21340,13 @@
         <v>12.6311358485303</v>
       </c>
       <c r="E210" t="n">
-        <v>0.505036498307457</v>
+        <v>0.00149435420073231</v>
       </c>
       <c r="F210" t="n">
         <v>12.6268366415846</v>
       </c>
       <c r="G210" t="n">
-        <v>0.515190565851705</v>
+        <v>0.00164460581547581</v>
       </c>
       <c r="H210" t="n">
         <v>-0.0103297780479889</v>
@@ -21429,13 +21429,13 @@
         <v>13.0381303858069</v>
       </c>
       <c r="E211" t="n">
-        <v>0.465281041248407</v>
+        <v>0.000883731953021914</v>
       </c>
       <c r="F211" t="n">
         <v>13.052222398524</v>
       </c>
       <c r="G211" t="n">
-        <v>0.476818335427542</v>
+        <v>0.000970248860332903</v>
       </c>
       <c r="H211" t="n">
         <v>0.00709371550072435</v>
@@ -21518,13 +21518,13 @@
         <v>10.9593259986664</v>
       </c>
       <c r="E212" t="n">
-        <v>0.523008250148371</v>
+        <v>0.00349260367388209</v>
       </c>
       <c r="F212" t="n">
         <v>10.9817616100469</v>
       </c>
       <c r="G212" t="n">
-        <v>0.525339379740088</v>
+        <v>0.00356650438618134</v>
       </c>
       <c r="H212" t="n">
         <v>0.0162325009755452</v>
@@ -21607,13 +21607,13 @@
         <v>13.6176701356667</v>
       </c>
       <c r="E213" t="n">
-        <v>0.471105373827739</v>
+        <v>0.000719067245758364</v>
       </c>
       <c r="F213" t="n">
         <v>13.6179246666653</v>
       </c>
       <c r="G213" t="n">
-        <v>0.472349760843713</v>
+        <v>0.000727945297026219</v>
       </c>
       <c r="H213" t="n">
         <v>-0.00611265045461533</v>
@@ -21696,13 +21696,13 @@
         <v>10.5826405348754</v>
       </c>
       <c r="E214" t="n">
-        <v>0.367521177941638</v>
+        <v>0.00131481676129699</v>
       </c>
       <c r="F214" t="n">
         <v>10.5825398140136</v>
       </c>
       <c r="G214" t="n">
-        <v>0.41419688211138</v>
+        <v>0.00186316051781108</v>
       </c>
       <c r="H214" t="n">
         <v>-0.00911876666526447</v>
@@ -21785,13 +21785,13 @@
         <v>13.0610771134453</v>
       </c>
       <c r="E215" t="n">
-        <v>0.480447623516415</v>
+        <v>0.000999694347453171</v>
       </c>
       <c r="F215" t="n">
         <v>13.075037391189</v>
       </c>
       <c r="G215" t="n">
-        <v>0.481490541354998</v>
+        <v>0.00100516394613527</v>
       </c>
       <c r="H215" t="n">
         <v>0.00696014236332502</v>
@@ -21874,13 +21874,13 @@
         <v>13.7661113269356</v>
       </c>
       <c r="E216" t="n">
-        <v>0.487641375220934</v>
+        <v>0.000787043252735006</v>
       </c>
       <c r="F216" t="n">
         <v>13.7681330491857</v>
       </c>
       <c r="G216" t="n">
-        <v>0.487906975102741</v>
+        <v>0.000792355953943442</v>
       </c>
       <c r="H216" t="n">
         <v>-0.00620449374755381</v>
@@ -21963,13 +21963,13 @@
         <v>10.7121150865674</v>
       </c>
       <c r="E217" t="n">
-        <v>0.362144046533494</v>
+        <v>0.00118054076011324</v>
       </c>
       <c r="F217" t="n">
         <v>10.7122173230017</v>
       </c>
       <c r="G217" t="n">
-        <v>0.377139553610535</v>
+        <v>0.00132269185209173</v>
       </c>
       <c r="H217" t="n">
         <v>-0.0066177125479554</v>
@@ -22052,13 +22052,13 @@
         <v>11.4091320723572</v>
       </c>
       <c r="E218" t="n">
-        <v>0.375514639488199</v>
+        <v>0.000906492712926664</v>
       </c>
       <c r="F218" t="n">
         <v>11.4212279739831</v>
       </c>
       <c r="G218" t="n">
-        <v>0.392551646883259</v>
+        <v>0.00102909184033456</v>
       </c>
       <c r="H218" t="n">
         <v>0.00662235318420439</v>
@@ -22141,13 +22141,13 @@
         <v>14.2709172740099</v>
       </c>
       <c r="E219" t="n">
-        <v>0.503653880627385</v>
+        <v>0.000745259036321024</v>
       </c>
       <c r="F219" t="n">
         <v>14.2835551645676</v>
       </c>
       <c r="G219" t="n">
-        <v>0.499080049105977</v>
+        <v>0.00070872758911018</v>
       </c>
       <c r="H219" t="n">
         <v>0.00596396021015656</v>
@@ -22230,13 +22230,13 @@
         <v>15.1095631092304</v>
       </c>
       <c r="E220" t="n">
-        <v>0.584706493438373</v>
+        <v>0.00123274780834535</v>
       </c>
       <c r="F220" t="n">
         <v>15.1241327905826</v>
       </c>
       <c r="G220" t="n">
-        <v>0.586339730146627</v>
+        <v>0.0012506967738235</v>
       </c>
       <c r="H220" t="n">
         <v>0.00752091120254185</v>
@@ -22319,13 +22319,13 @@
         <v>10.1544293384228</v>
       </c>
       <c r="E221" t="n">
-        <v>0.336669120556893</v>
+        <v>0.00133308303901926</v>
       </c>
       <c r="F221" t="n">
         <v>10.1554374678058</v>
       </c>
       <c r="G221" t="n">
-        <v>0.296615570260632</v>
+        <v>0.00100594859730693</v>
       </c>
       <c r="H221" t="n">
         <v>-0.00572887520820003</v>
@@ -22408,13 +22408,13 @@
         <v>11.5914872689311</v>
       </c>
       <c r="E222" t="n">
-        <v>0.531942608577513</v>
+        <v>0.00287386483978526</v>
       </c>
       <c r="F222" t="n">
         <v>11.5868791017219</v>
       </c>
       <c r="G222" t="n">
-        <v>0.532846136185211</v>
+        <v>0.00294591369280717</v>
       </c>
       <c r="H222" t="n">
         <v>-0.0117567589402635</v>
@@ -22497,13 +22497,13 @@
         <v>13.9704383769764</v>
       </c>
       <c r="E223" t="n">
-        <v>0.562809366554292</v>
+        <v>0.00150019737237593</v>
       </c>
       <c r="F223" t="n">
         <v>13.9847914699112</v>
       </c>
       <c r="G223" t="n">
-        <v>0.560485044285652</v>
+        <v>0.00145344923973889</v>
       </c>
       <c r="H223" t="n">
         <v>0.0078203316165461</v>
@@ -22586,13 +22586,13 @@
         <v>11.287732943546</v>
       </c>
       <c r="E224" t="n">
-        <v>0.397467292892202</v>
+        <v>0.00114560805376921</v>
       </c>
       <c r="F224" t="n">
         <v>11.2873793111518</v>
       </c>
       <c r="G224" t="n">
-        <v>0.41939367162135</v>
+        <v>0.00135750986170919</v>
       </c>
       <c r="H224" t="n">
         <v>-0.00698625401183842</v>
@@ -22675,13 +22675,13 @@
         <v>11.9340546511899</v>
       </c>
       <c r="E225" t="n">
-        <v>0.558807884675487</v>
+        <v>0.00317342980712174</v>
       </c>
       <c r="F225" t="n">
         <v>11.9480228065239</v>
       </c>
       <c r="G225" t="n">
-        <v>0.559706411851648</v>
+        <v>0.00313279686053993</v>
       </c>
       <c r="H225" t="n">
         <v>0.0118049204045992</v>
@@ -22764,13 +22764,13 @@
         <v>14.1881604550055</v>
       </c>
       <c r="E226" t="n">
-        <v>0.62103838298024</v>
+        <v>0.0024431291514994</v>
       </c>
       <c r="F226" t="n">
         <v>14.1756544783158</v>
       </c>
       <c r="G226" t="n">
-        <v>0.627381545881526</v>
+        <v>0.00261929690835644</v>
       </c>
       <c r="H226" t="n">
         <v>-0.0121263789644174</v>
@@ -22853,13 +22853,13 @@
         <v>10.4457766424881</v>
       </c>
       <c r="E227" t="n">
-        <v>0.346470257801535</v>
+        <v>0.00121684682021493</v>
       </c>
       <c r="F227" t="n">
         <v>10.4466471840779</v>
       </c>
       <c r="G227" t="n">
-        <v>0.358563666651325</v>
+        <v>0.00132555592878575</v>
       </c>
       <c r="H227" t="n">
         <v>-0.00513734870964514</v>
@@ -22942,13 +22942,13 @@
         <v>13.911246072454</v>
       </c>
       <c r="E228" t="n">
-        <v>0.559958157036182</v>
+        <v>0.00149018109049042</v>
       </c>
       <c r="F228" t="n">
         <v>13.9233398208273</v>
       </c>
       <c r="G228" t="n">
-        <v>0.56515407881116</v>
+        <v>0.00155869780529333</v>
       </c>
       <c r="H228" t="n">
         <v>0.00569628238954919</v>
@@ -23031,13 +23031,13 @@
         <v>16.1956670414935</v>
       </c>
       <c r="E229" t="n">
-        <v>0.591368673860405</v>
+        <v>0.00091024658207398</v>
       </c>
       <c r="F229" t="n">
         <v>16.2055268436113</v>
       </c>
       <c r="G229" t="n">
-        <v>0.589563913128981</v>
+        <v>0.000882270297603323</v>
       </c>
       <c r="H229" t="n">
         <v>0.00419308947322231</v>
@@ -23120,13 +23120,13 @@
         <v>12.0097494298887</v>
       </c>
       <c r="E230" t="n">
-        <v>0.384763094620641</v>
+        <v>0.000717697408810427</v>
       </c>
       <c r="F230" t="n">
         <v>12.0113046880912</v>
       </c>
       <c r="G230" t="n">
-        <v>0.402299102033043</v>
+        <v>0.000828213979349846</v>
       </c>
       <c r="H230" t="n">
         <v>-0.00434238437600501</v>
@@ -23209,13 +23209,13 @@
         <v>12.1531420467048</v>
       </c>
       <c r="E231" t="n">
-        <v>0.56525400432004</v>
+        <v>0.00304270877042566</v>
       </c>
       <c r="F231" t="n">
         <v>12.1682366920545</v>
       </c>
       <c r="G231" t="n">
-        <v>0.566654167400719</v>
+        <v>0.00306665885265837</v>
       </c>
       <c r="H231" t="n">
         <v>0.00956477478541441</v>
@@ -23298,13 +23298,13 @@
         <v>13.9922541900478</v>
       </c>
       <c r="E232" t="n">
-        <v>0.613370997890048</v>
+        <v>0.00244763222017818</v>
       </c>
       <c r="F232" t="n">
         <v>13.9821888844803</v>
       </c>
       <c r="G232" t="n">
-        <v>0.620244637096197</v>
+        <v>0.00258858403643303</v>
       </c>
       <c r="H232" t="n">
         <v>-0.00986218838345608</v>
@@ -23387,13 +23387,13 @@
         <v>10.3358957602403</v>
       </c>
       <c r="E233" t="n">
-        <v>0.281517061543057</v>
+        <v>0.000807440657911462</v>
       </c>
       <c r="F233" t="n">
         <v>10.3470390241925</v>
       </c>
       <c r="G233" t="n">
-        <v>0.335753109720429</v>
+        <v>0.00118341668904361</v>
       </c>
       <c r="H233" t="n">
         <v>0.00366996755928671</v>
@@ -23476,13 +23476,13 @@
         <v>10.9747533190277</v>
       </c>
       <c r="E234" t="n">
-        <v>0.468616830530608</v>
+        <v>0.00228741187839711</v>
       </c>
       <c r="F234" t="n">
         <v>10.9742874664498</v>
       </c>
       <c r="G234" t="n">
-        <v>0.424578421356481</v>
+        <v>0.0016583263889349</v>
       </c>
       <c r="H234" t="n">
         <v>-0.00585347505315429</v>
@@ -23565,13 +23565,13 @@
         <v>12.9617727427967</v>
       </c>
       <c r="E235" t="n">
-        <v>0.368150604001151</v>
+        <v>0.000380978010451137</v>
       </c>
       <c r="F235" t="n">
         <v>12.9659743784996</v>
       </c>
       <c r="G235" t="n">
-        <v>0.357680670705318</v>
+        <v>0.000346514469443929</v>
       </c>
       <c r="H235" t="n">
         <v>-0.00321132876207847</v>
@@ -23654,13 +23654,13 @@
         <v>10.2913180879915</v>
       </c>
       <c r="E236" t="n">
-        <v>0.284442045519313</v>
+        <v>0.000848630365680608</v>
       </c>
       <c r="F236" t="n">
         <v>10.2938942025493</v>
       </c>
       <c r="G236" t="n">
-        <v>0.326315185193495</v>
+        <v>0.00114237302292366</v>
       </c>
       <c r="H236" t="n">
         <v>-0.00327671271648308</v>
@@ -23743,13 +23743,13 @@
         <v>14.4419010591289</v>
       </c>
       <c r="E237" t="n">
-        <v>0.487036289966509</v>
+        <v>0.0005870497463499</v>
       </c>
       <c r="F237" t="n">
         <v>14.4452611877441</v>
       </c>
       <c r="G237" t="n">
-        <v>0.50647576576596</v>
+        <v>0.000714754677999453</v>
       </c>
       <c r="H237" t="n">
         <v>-0.00293217370712769</v>
@@ -23832,13 +23832,13 @@
         <v>13.1373011368883</v>
       </c>
       <c r="E238" t="n">
-        <v>0.57217248561641</v>
+        <v>0.00221761808397055</v>
       </c>
       <c r="F238" t="n">
         <v>13.1501420064926</v>
       </c>
       <c r="G238" t="n">
-        <v>0.56968113678225</v>
+        <v>0.00218646311053197</v>
       </c>
       <c r="H238" t="n">
         <v>0.00654918831501103</v>
@@ -23921,13 +23921,13 @@
         <v>13.9310237876966</v>
       </c>
       <c r="E239" t="n">
-        <v>0.515978581895875</v>
+        <v>0.000968382451675778</v>
       </c>
       <c r="F239" t="n">
         <v>13.935954869453</v>
       </c>
       <c r="G239" t="n">
-        <v>0.518528756725705</v>
+        <v>0.000987838286413764</v>
       </c>
       <c r="H239" t="n">
         <v>-0.00256331090882753</v>
@@ -24010,13 +24010,13 @@
         <v>13.873125062562</v>
       </c>
       <c r="E240" t="n">
-        <v>0.513219374209022</v>
+        <v>0.000963228164885089</v>
       </c>
       <c r="F240" t="n">
         <v>13.882215474762</v>
       </c>
       <c r="G240" t="n">
-        <v>0.513950327357198</v>
+        <v>0.000967915896223208</v>
       </c>
       <c r="H240" t="n">
         <v>0.00273362850603821</v>
@@ -24099,13 +24099,13 @@
         <v>10.173553206791</v>
       </c>
       <c r="E241" t="n">
-        <v>0.414225904868932</v>
+        <v>0.00228001076441856</v>
       </c>
       <c r="F241" t="n">
         <v>10.1680840907118</v>
       </c>
       <c r="G241" t="n">
-        <v>0.469968235101806</v>
+        <v>0.00338593517564721</v>
       </c>
       <c r="H241" t="n">
         <v>-0.00551032518663548</v>
@@ -24188,13 +24188,13 @@
         <v>11.6143983603762</v>
       </c>
       <c r="E242" t="n">
-        <v>0.516741836099541</v>
+        <v>0.00252555613443216</v>
       </c>
       <c r="F242" t="n">
         <v>11.6147151780566</v>
       </c>
       <c r="G242" t="n">
-        <v>0.504040255144047</v>
+        <v>0.00230178594302164</v>
       </c>
       <c r="H242" t="n">
         <v>-0.00448280519363453</v>
@@ -24277,13 +24277,13 @@
         <v>12.474295012661</v>
       </c>
       <c r="E243" t="n">
-        <v>0.567725607986944</v>
+        <v>0.00276233107564957</v>
       </c>
       <c r="F243" t="n">
         <v>12.4849132596312</v>
       </c>
       <c r="G243" t="n">
-        <v>0.574723725810724</v>
+        <v>0.00290432879533958</v>
       </c>
       <c r="H243" t="n">
         <v>0.00474933811452739</v>
@@ -24366,13 +24366,13 @@
         <v>11.9146415451404</v>
       </c>
       <c r="E244" t="n">
-        <v>0.502039818867567</v>
+        <v>0.00199010005316121</v>
       </c>
       <c r="F244" t="n">
         <v>11.9193944578864</v>
       </c>
       <c r="G244" t="n">
-        <v>0.499600891866369</v>
+        <v>0.00192752679620957</v>
       </c>
       <c r="H244" t="n">
         <v>-0.00301680562661225</v>
@@ -24455,13 +24455,13 @@
         <v>9.31117898955504</v>
       </c>
       <c r="E245" t="n">
-        <v>0.264417319863232</v>
+        <v>0.00134030654799797</v>
       </c>
       <c r="F245" t="n">
         <v>9.32381857629777</v>
       </c>
       <c r="G245" t="n">
-        <v>0.410296803058757</v>
+        <v>0.00338273239616531</v>
       </c>
       <c r="H245" t="n">
         <v>0.00215490966981941</v>
@@ -24544,13 +24544,13 @@
         <v>14.6261770464886</v>
       </c>
       <c r="E246" t="n">
-        <v>0.524453491779492</v>
+        <v>0.000796341805751517</v>
       </c>
       <c r="F246" t="n">
         <v>14.6306170879463</v>
       </c>
       <c r="G246" t="n">
-        <v>0.516874896058224</v>
+        <v>0.000733184011357918</v>
       </c>
       <c r="H246" t="n">
         <v>-0.00134830635211716</v>
@@ -24633,13 +24633,13 @@
         <v>14.1414746993083</v>
       </c>
       <c r="E247" t="n">
-        <v>0.617972546094708</v>
+        <v>0.00239527367033938</v>
       </c>
       <c r="F247" t="n">
         <v>14.1506721894402</v>
       </c>
       <c r="G247" t="n">
-        <v>0.610109615361918</v>
+        <v>0.00224086557696466</v>
       </c>
       <c r="H247" t="n">
         <v>0.00271336372241293</v>
@@ -24722,13 +24722,13 @@
         <v>12.0537126511096</v>
       </c>
       <c r="E248" t="n">
-        <v>0.438187498425489</v>
+        <v>0.0010990714576087</v>
       </c>
       <c r="F248" t="n">
         <v>12.0614189158213</v>
       </c>
       <c r="G248" t="n">
-        <v>0.4452662752911</v>
+        <v>0.00115410597399907</v>
       </c>
       <c r="H248" t="n">
         <v>0.00125059531960011</v>
@@ -24811,13 +24811,13 @@
         <v>12.9610275410056</v>
       </c>
       <c r="E249" t="n">
-        <v>0.44089840331891</v>
+        <v>0.000733331424270385</v>
       </c>
       <c r="F249" t="n">
         <v>12.9685609635551</v>
       </c>
       <c r="G249" t="n">
-        <v>0.442243070477149</v>
+        <v>0.000738863491473514</v>
       </c>
       <c r="H249" t="n">
         <v>0.00110166951684211</v>
@@ -24900,13 +24900,13 @@
         <v>10.80909642079</v>
       </c>
       <c r="E250" t="n">
-        <v>0.399740631100559</v>
+        <v>0.00148860953607727</v>
       </c>
       <c r="F250" t="n">
         <v>10.8181685098191</v>
       </c>
       <c r="G250" t="n">
-        <v>0.416545682710474</v>
+        <v>0.00167541405311458</v>
       </c>
       <c r="H250" t="n">
         <v>0.00132126223344879</v>
@@ -24989,13 +24989,13 @@
         <v>10.9526874017642</v>
       </c>
       <c r="E251" t="n">
-        <v>0.33314488130745</v>
+        <v>0.000833771351335968</v>
       </c>
       <c r="F251" t="n">
         <v>10.9563283850463</v>
       </c>
       <c r="G251" t="n">
-        <v>0.422304947590859</v>
+        <v>0.00163229104777155</v>
       </c>
       <c r="H251" t="n">
         <v>-0.00104805552344608</v>
@@ -25078,13 +25078,13 @@
         <v>12.747520807691</v>
       </c>
       <c r="E252" t="n">
-        <v>0.405170220196638</v>
+        <v>0.000590659276546081</v>
       </c>
       <c r="F252" t="n">
         <v>12.7554111301396</v>
       </c>
       <c r="G252" t="n">
-        <v>0.410517258716288</v>
+        <v>0.000616193598313771</v>
       </c>
       <c r="H252" t="n">
         <v>0.00100873906994722</v>
@@ -25167,13 +25167,13 @@
         <v>8.45523138943321</v>
       </c>
       <c r="E253" t="n">
-        <v>0.309474173050304</v>
+        <v>0.00296124704346348</v>
       </c>
       <c r="F253" t="n">
         <v>8.46492090973451</v>
       </c>
       <c r="G253" t="n">
-        <v>0.327399974468222</v>
+        <v>0.00327172630480024</v>
       </c>
       <c r="H253" t="n">
         <v>-0.00114557767747842</v>
@@ -25256,13 +25256,13 @@
         <v>9.9928177962328</v>
       </c>
       <c r="E254" t="n">
-        <v>0.465786763078059</v>
+        <v>0.00359679522263014</v>
       </c>
       <c r="F254" t="n">
         <v>9.9945822150962</v>
       </c>
       <c r="G254" t="n">
-        <v>0.439139939930155</v>
+        <v>0.00296273190876805</v>
       </c>
       <c r="H254" t="n">
         <v>0.00184170809778295</v>
@@ -25345,13 +25345,13 @@
         <v>16.0779839102556</v>
       </c>
       <c r="E255" t="n">
-        <v>0.580834451914007</v>
+        <v>0.000836710945731928</v>
       </c>
       <c r="F255" t="n">
         <v>16.0863619413386</v>
       </c>
       <c r="G255" t="n">
-        <v>0.588594980099565</v>
+        <v>0.000916115162787109</v>
       </c>
       <c r="H255" t="n">
         <v>0.000552221646321488</v>
@@ -25434,13 +25434,13 @@
         <v>10.8723614551085</v>
       </c>
       <c r="E256" t="n">
-        <v>0.443693734512551</v>
+        <v>0.00201030457084315</v>
       </c>
       <c r="F256" t="n">
         <v>10.8784325760856</v>
       </c>
       <c r="G256" t="n">
-        <v>0.439970063700175</v>
+        <v>0.00194250293742414</v>
       </c>
       <c r="H256" t="n">
         <v>-0.000859781158514213</v>

</xml_diff>